<commit_message>
Update on 20250807 part 5
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="169">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -673,6 +673,10 @@
   </si>
   <si>
     <t>官网提供卫视,青海省频道在线观看,可使用酷9JS脚本的Webview方式观看*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>beijing.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -852,22 +856,22 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1203,7 +1207,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1212,20 +1216,20 @@
       <c r="C2" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="17" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="20"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="16"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="21"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>151</v>
@@ -1235,7 +1239,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1247,7 +1251,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="17"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1257,7 +1261,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="17"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1273,7 +1277,9 @@
       <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>168</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>21</v>
       </c>
@@ -1287,7 +1293,7 @@
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1299,7 +1305,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="17"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="1" t="s">
         <v>121</v>
       </c>
@@ -1309,7 +1315,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1321,7 +1327,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="17"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1331,7 +1337,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1343,7 +1349,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="17"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
@@ -1385,7 +1391,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="16" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1399,7 +1405,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="17"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="1" t="s">
         <v>50</v>
       </c>
@@ -1409,7 +1415,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="16" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1423,25 +1429,25 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="17"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="17" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="17"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="16"/>
+      <c r="D23" s="17"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="17"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1451,7 +1457,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="17"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="1" t="s">
         <v>45</v>
       </c>
@@ -1461,22 +1467,22 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="17"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="17" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="17"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="16"/>
+      <c r="D27" s="17"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="s">
@@ -1499,7 +1505,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="16" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1511,7 +1517,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="17"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="1" t="s">
         <v>55</v>
       </c>
@@ -1529,7 +1535,7 @@
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="18" t="s">
         <v>102</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1541,7 +1547,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="21"/>
+      <c r="A34" s="20"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
         <v>142</v>
@@ -1551,7 +1557,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="17" t="s">
+      <c r="A35" s="16" t="s">
         <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1563,7 +1569,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="17"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="1" t="s">
         <v>60</v>
       </c>
@@ -1613,27 +1619,27 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="16" t="s">
         <v>62</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C41" s="1"/>
-      <c r="D41" s="16" t="s">
+      <c r="D41" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="17"/>
+      <c r="A42" s="16"/>
       <c r="B42" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C42" s="1"/>
-      <c r="D42" s="16"/>
+      <c r="D42" s="17"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="17"/>
+      <c r="A43" s="16"/>
       <c r="B43" s="1" t="s">
         <v>91</v>
       </c>
@@ -1643,7 +1649,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="17"/>
+      <c r="A44" s="16"/>
       <c r="B44" s="1" t="s">
         <v>92</v>
       </c>
@@ -1653,7 +1659,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="16" t="s">
         <v>95</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1665,7 +1671,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="17"/>
+      <c r="A46" s="16"/>
       <c r="B46" s="1" t="s">
         <v>96</v>
       </c>
@@ -1675,35 +1681,35 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="18" t="s">
         <v>63</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C47" s="1"/>
-      <c r="D47" s="16" t="s">
+      <c r="D47" s="17" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="20"/>
+      <c r="A48" s="19"/>
       <c r="B48" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="16"/>
+      <c r="D48" s="17"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="20"/>
+      <c r="A49" s="19"/>
       <c r="B49" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C49" s="1"/>
-      <c r="D49" s="16"/>
+      <c r="D49" s="17"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="20"/>
+      <c r="A50" s="19"/>
       <c r="B50" s="1" t="s">
         <v>99</v>
       </c>
@@ -1713,7 +1719,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="20"/>
+      <c r="A51" s="19"/>
       <c r="B51" s="1" t="s">
         <v>101</v>
       </c>
@@ -1723,7 +1729,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="20"/>
+      <c r="A52" s="19"/>
       <c r="B52" s="1" t="s">
         <v>110</v>
       </c>
@@ -1733,7 +1739,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="20"/>
+      <c r="A53" s="19"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
         <v>145</v>
@@ -1743,7 +1749,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="20"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
         <v>146</v>
@@ -1753,7 +1759,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="21"/>
+      <c r="A55" s="20"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
         <v>147</v>
@@ -1763,7 +1769,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="16" t="s">
         <v>67</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -1775,7 +1781,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="17"/>
+      <c r="A57" s="16"/>
       <c r="B57" s="1" t="s">
         <v>68</v>
       </c>
@@ -1807,7 +1813,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="18" t="s">
+      <c r="A60" s="21" t="s">
         <v>127</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -1821,7 +1827,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="18"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="1" t="s">
         <v>112</v>
       </c>
@@ -1831,27 +1837,27 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A62" s="17" t="s">
+      <c r="A62" s="16" t="s">
         <v>70</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C62" s="1"/>
-      <c r="D62" s="16" t="s">
+      <c r="D62" s="17" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A63" s="17"/>
+      <c r="A63" s="16"/>
       <c r="B63" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C63" s="1"/>
-      <c r="D63" s="16"/>
+      <c r="D63" s="17"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A64" s="17" t="s">
+      <c r="A64" s="16" t="s">
         <v>71</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -1863,25 +1869,25 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="17"/>
+      <c r="A65" s="16"/>
       <c r="B65" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C65" s="1"/>
-      <c r="D65" s="16" t="s">
+      <c r="D65" s="17" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="17"/>
+      <c r="A66" s="16"/>
       <c r="B66" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C66" s="1"/>
-      <c r="D66" s="16"/>
+      <c r="D66" s="17"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="17"/>
+      <c r="A67" s="16"/>
       <c r="B67" s="1" t="s">
         <v>81</v>
       </c>
@@ -1891,7 +1897,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="17"/>
+      <c r="A68" s="16"/>
       <c r="B68" s="1" t="s">
         <v>85</v>
       </c>
@@ -1901,7 +1907,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="17" t="s">
+      <c r="A69" s="16" t="s">
         <v>123</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -1913,7 +1919,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="17"/>
+      <c r="A70" s="16"/>
       <c r="B70" s="1" t="s">
         <v>129</v>
       </c>
@@ -1925,6 +1931,15 @@
   </sheetData>
   <autoFilter ref="A1:D68"/>
   <mergeCells count="25">
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A47:A55"/>
     <mergeCell ref="A69:A70"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A5:A7"/>
@@ -1941,15 +1956,6 @@
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="A41:A44"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A47:A55"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 20250807 part 8
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="170">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -547,14 +547,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>酷9JS脚本</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PHP脚本</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>所有脚本均在本地和Github远程存储</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -677,6 +669,18 @@
   </si>
   <si>
     <t>beijing.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hunan.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>酷9JS脚本名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PHP脚本名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -856,10 +860,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -869,9 +876,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1194,52 +1198,52 @@
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D2" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="19"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="17"/>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="20"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1251,7 +1255,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="16"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1261,7 +1265,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="16"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1278,7 +1282,7 @@
         <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>21</v>
@@ -1286,14 +1290,14 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1305,7 +1309,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="16"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="1" t="s">
         <v>121</v>
       </c>
@@ -1315,7 +1319,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="17" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1327,7 +1331,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="16"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1337,7 +1341,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="17" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1349,7 +1353,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="16"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
@@ -1360,12 +1364,12 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
@@ -1382,30 +1386,30 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="17" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="16"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="1" t="s">
         <v>50</v>
       </c>
@@ -1415,39 +1419,39 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="16"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="16" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="16"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="17"/>
+      <c r="D23" s="16"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="16"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1457,7 +1461,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="16"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="1" t="s">
         <v>45</v>
       </c>
@@ -1467,57 +1471,59 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="16"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="16" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="16"/>
+      <c r="A27" s="17"/>
       <c r="B27" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="17"/>
+      <c r="D27" s="16"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="17" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="D30" s="8" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="16"/>
+      <c r="A31" s="17"/>
       <c r="B31" s="1" t="s">
         <v>55</v>
       </c>
@@ -1528,14 +1534,14 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="19" t="s">
         <v>102</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1547,17 +1553,17 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="20"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="17" t="s">
         <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1569,7 +1575,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="16"/>
+      <c r="A36" s="17"/>
       <c r="B36" s="1" t="s">
         <v>60</v>
       </c>
@@ -1592,7 +1598,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1600,46 +1606,46 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="17" t="s">
         <v>62</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C41" s="1"/>
-      <c r="D41" s="17" t="s">
+      <c r="D41" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="16"/>
+      <c r="A42" s="17"/>
       <c r="B42" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C42" s="1"/>
-      <c r="D42" s="17"/>
+      <c r="D42" s="16"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="16"/>
+      <c r="A43" s="17"/>
       <c r="B43" s="1" t="s">
         <v>91</v>
       </c>
@@ -1649,7 +1655,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="16"/>
+      <c r="A44" s="17"/>
       <c r="B44" s="1" t="s">
         <v>92</v>
       </c>
@@ -1659,7 +1665,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="17" t="s">
         <v>95</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1671,7 +1677,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="16"/>
+      <c r="A46" s="17"/>
       <c r="B46" s="1" t="s">
         <v>96</v>
       </c>
@@ -1681,35 +1687,35 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="19" t="s">
         <v>63</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C47" s="1"/>
-      <c r="D47" s="17" t="s">
+      <c r="D47" s="16" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="19"/>
+      <c r="A48" s="20"/>
       <c r="B48" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="17"/>
+      <c r="D48" s="16"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="19"/>
+      <c r="A49" s="20"/>
       <c r="B49" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C49" s="1"/>
-      <c r="D49" s="17"/>
+      <c r="D49" s="16"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="19"/>
+      <c r="A50" s="20"/>
       <c r="B50" s="1" t="s">
         <v>99</v>
       </c>
@@ -1719,7 +1725,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="19"/>
+      <c r="A51" s="20"/>
       <c r="B51" s="1" t="s">
         <v>101</v>
       </c>
@@ -1729,7 +1735,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="19"/>
+      <c r="A52" s="20"/>
       <c r="B52" s="1" t="s">
         <v>110</v>
       </c>
@@ -1739,37 +1745,37 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="19"/>
+      <c r="A53" s="20"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="19"/>
+      <c r="A54" s="20"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="20"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="16" t="s">
+      <c r="A56" s="17" t="s">
         <v>67</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -1781,12 +1787,12 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="16"/>
+      <c r="A57" s="17"/>
       <c r="B57" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>69</v>
@@ -1794,7 +1800,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A58" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1813,21 +1819,21 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="21" t="s">
+      <c r="A60" s="18" t="s">
         <v>127</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D60" s="10" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="21"/>
+      <c r="A61" s="18"/>
       <c r="B61" s="1" t="s">
         <v>112</v>
       </c>
@@ -1837,27 +1843,27 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A62" s="16" t="s">
+      <c r="A62" s="17" t="s">
         <v>70</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C62" s="1"/>
-      <c r="D62" s="17" t="s">
+      <c r="D62" s="16" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A63" s="16"/>
+      <c r="A63" s="17"/>
       <c r="B63" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C63" s="1"/>
-      <c r="D63" s="17"/>
+      <c r="D63" s="16"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A64" s="16" t="s">
+      <c r="A64" s="17" t="s">
         <v>71</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -1869,25 +1875,25 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="16"/>
+      <c r="A65" s="17"/>
       <c r="B65" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C65" s="1"/>
-      <c r="D65" s="17" t="s">
+      <c r="D65" s="16" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="16"/>
+      <c r="A66" s="17"/>
       <c r="B66" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C66" s="1"/>
-      <c r="D66" s="17"/>
+      <c r="D66" s="16"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="16"/>
+      <c r="A67" s="17"/>
       <c r="B67" s="1" t="s">
         <v>81</v>
       </c>
@@ -1897,7 +1903,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="16"/>
+      <c r="A68" s="17"/>
       <c r="B68" s="1" t="s">
         <v>85</v>
       </c>
@@ -1907,7 +1913,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="16" t="s">
+      <c r="A69" s="17" t="s">
         <v>123</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -1919,7 +1925,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="16"/>
+      <c r="A70" s="17"/>
       <c r="B70" s="1" t="s">
         <v>129</v>
       </c>
@@ -1931,15 +1937,6 @@
   </sheetData>
   <autoFilter ref="A1:D68"/>
   <mergeCells count="25">
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A47:A55"/>
     <mergeCell ref="A69:A70"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A5:A7"/>
@@ -1956,6 +1953,15 @@
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="A41:A44"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A47:A55"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1973,7 +1979,7 @@
   <cols>
     <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="43.375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1983,16 +1989,16 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Update on 20250807 part 9
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="171">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -681,6 +681,10 @@
   </si>
   <si>
     <t>PHP脚本名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官网提供卫视,内蒙古自治区频道在线观看,可使用酷9JS脚本的Webview方式观看*</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -860,22 +864,22 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1211,7 +1215,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1220,20 +1224,20 @@
       <c r="C2" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="17" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="20"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="16"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="21"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>149</v>
@@ -1243,7 +1247,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1255,7 +1259,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="17"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1265,7 +1269,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="17"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1297,7 +1301,7 @@
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1309,7 +1313,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="17"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="1" t="s">
         <v>121</v>
       </c>
@@ -1319,7 +1323,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1331,7 +1335,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="17"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1341,7 +1345,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1353,7 +1357,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="17"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
@@ -1395,7 +1399,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="16" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1409,7 +1413,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="17"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="1" t="s">
         <v>50</v>
       </c>
@@ -1419,7 +1423,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="16" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1433,25 +1437,25 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="17"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="17" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="17"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="16"/>
+      <c r="D23" s="17"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="17"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1461,7 +1465,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="17"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="1" t="s">
         <v>45</v>
       </c>
@@ -1471,22 +1475,22 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="17"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="17" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="17"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="16"/>
+      <c r="D27" s="17"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="s">
@@ -1509,7 +1513,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="16" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1523,7 +1527,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="17"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="1" t="s">
         <v>55</v>
       </c>
@@ -1541,7 +1545,7 @@
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="18" t="s">
         <v>102</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1553,7 +1557,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="21"/>
+      <c r="A34" s="20"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
         <v>140</v>
@@ -1563,7 +1567,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="17" t="s">
+      <c r="A35" s="16" t="s">
         <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1575,7 +1579,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="17"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="1" t="s">
         <v>60</v>
       </c>
@@ -1602,7 +1606,9 @@
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
+      <c r="D38" s="15" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="12" t="s">
@@ -1625,27 +1631,27 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="16" t="s">
         <v>62</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C41" s="1"/>
-      <c r="D41" s="16" t="s">
+      <c r="D41" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="17"/>
+      <c r="A42" s="16"/>
       <c r="B42" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C42" s="1"/>
-      <c r="D42" s="16"/>
+      <c r="D42" s="17"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="17"/>
+      <c r="A43" s="16"/>
       <c r="B43" s="1" t="s">
         <v>91</v>
       </c>
@@ -1655,7 +1661,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="17"/>
+      <c r="A44" s="16"/>
       <c r="B44" s="1" t="s">
         <v>92</v>
       </c>
@@ -1665,7 +1671,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="16" t="s">
         <v>95</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1677,7 +1683,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="17"/>
+      <c r="A46" s="16"/>
       <c r="B46" s="1" t="s">
         <v>96</v>
       </c>
@@ -1687,35 +1693,35 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="18" t="s">
         <v>63</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C47" s="1"/>
-      <c r="D47" s="16" t="s">
+      <c r="D47" s="17" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="20"/>
+      <c r="A48" s="19"/>
       <c r="B48" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="16"/>
+      <c r="D48" s="17"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="20"/>
+      <c r="A49" s="19"/>
       <c r="B49" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C49" s="1"/>
-      <c r="D49" s="16"/>
+      <c r="D49" s="17"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="20"/>
+      <c r="A50" s="19"/>
       <c r="B50" s="1" t="s">
         <v>99</v>
       </c>
@@ -1725,7 +1731,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="20"/>
+      <c r="A51" s="19"/>
       <c r="B51" s="1" t="s">
         <v>101</v>
       </c>
@@ -1735,7 +1741,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="20"/>
+      <c r="A52" s="19"/>
       <c r="B52" s="1" t="s">
         <v>110</v>
       </c>
@@ -1745,7 +1751,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="20"/>
+      <c r="A53" s="19"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
         <v>143</v>
@@ -1755,7 +1761,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="20"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
         <v>144</v>
@@ -1765,7 +1771,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="21"/>
+      <c r="A55" s="20"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
         <v>145</v>
@@ -1775,7 +1781,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="16" t="s">
         <v>67</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -1787,7 +1793,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="17"/>
+      <c r="A57" s="16"/>
       <c r="B57" s="1" t="s">
         <v>68</v>
       </c>
@@ -1819,7 +1825,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="18" t="s">
+      <c r="A60" s="21" t="s">
         <v>127</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -1833,7 +1839,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="18"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="1" t="s">
         <v>112</v>
       </c>
@@ -1843,27 +1849,27 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A62" s="17" t="s">
+      <c r="A62" s="16" t="s">
         <v>70</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C62" s="1"/>
-      <c r="D62" s="16" t="s">
+      <c r="D62" s="17" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A63" s="17"/>
+      <c r="A63" s="16"/>
       <c r="B63" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C63" s="1"/>
-      <c r="D63" s="16"/>
+      <c r="D63" s="17"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A64" s="17" t="s">
+      <c r="A64" s="16" t="s">
         <v>71</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -1875,25 +1881,25 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="17"/>
+      <c r="A65" s="16"/>
       <c r="B65" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C65" s="1"/>
-      <c r="D65" s="16" t="s">
+      <c r="D65" s="17" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="17"/>
+      <c r="A66" s="16"/>
       <c r="B66" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C66" s="1"/>
-      <c r="D66" s="16"/>
+      <c r="D66" s="17"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="17"/>
+      <c r="A67" s="16"/>
       <c r="B67" s="1" t="s">
         <v>81</v>
       </c>
@@ -1903,7 +1909,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="17"/>
+      <c r="A68" s="16"/>
       <c r="B68" s="1" t="s">
         <v>85</v>
       </c>
@@ -1913,7 +1919,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="17" t="s">
+      <c r="A69" s="16" t="s">
         <v>123</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -1925,7 +1931,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="17"/>
+      <c r="A70" s="16"/>
       <c r="B70" s="1" t="s">
         <v>129</v>
       </c>
@@ -1937,6 +1943,15 @@
   </sheetData>
   <autoFilter ref="A1:D68"/>
   <mergeCells count="25">
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A47:A55"/>
     <mergeCell ref="A69:A70"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A5:A7"/>
@@ -1953,15 +1968,6 @@
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="A41:A44"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A47:A55"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 20250808 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="172">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -685,6 +685,10 @@
   </si>
   <si>
     <t>官网提供卫视,内蒙古自治区频道在线观看,可使用酷9JS脚本的Webview方式观看*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gzstv.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -864,10 +868,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -877,9 +884,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1215,7 +1219,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1224,20 +1228,20 @@
       <c r="C2" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="19"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="17"/>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="20"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>149</v>
@@ -1247,7 +1251,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1259,7 +1263,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="16"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1269,7 +1273,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="16"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1301,7 +1305,7 @@
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1313,7 +1317,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="16"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="1" t="s">
         <v>121</v>
       </c>
@@ -1323,7 +1327,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="17" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1335,7 +1339,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="16"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1345,7 +1349,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="17" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1357,7 +1361,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="16"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
@@ -1383,7 +1387,9 @@
       <c r="B17" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>171</v>
+      </c>
       <c r="D17" s="1" t="s">
         <v>132</v>
       </c>
@@ -1399,7 +1405,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="17" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1413,7 +1419,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="16"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="1" t="s">
         <v>50</v>
       </c>
@@ -1423,7 +1429,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1437,25 +1443,25 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="16"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="16" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="16"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="17"/>
+      <c r="D23" s="16"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="16"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1465,7 +1471,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="16"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="1" t="s">
         <v>45</v>
       </c>
@@ -1475,22 +1481,22 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="16"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="16" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="16"/>
+      <c r="A27" s="17"/>
       <c r="B27" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="17"/>
+      <c r="D27" s="16"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="s">
@@ -1513,7 +1519,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="17" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1527,7 +1533,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="16"/>
+      <c r="A31" s="17"/>
       <c r="B31" s="1" t="s">
         <v>55</v>
       </c>
@@ -1545,7 +1551,7 @@
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="19" t="s">
         <v>102</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1557,7 +1563,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="20"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
         <v>140</v>
@@ -1567,7 +1573,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="17" t="s">
         <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1579,7 +1585,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="16"/>
+      <c r="A36" s="17"/>
       <c r="B36" s="1" t="s">
         <v>60</v>
       </c>
@@ -1631,27 +1637,27 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="17" t="s">
         <v>62</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C41" s="1"/>
-      <c r="D41" s="17" t="s">
+      <c r="D41" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="16"/>
+      <c r="A42" s="17"/>
       <c r="B42" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C42" s="1"/>
-      <c r="D42" s="17"/>
+      <c r="D42" s="16"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="16"/>
+      <c r="A43" s="17"/>
       <c r="B43" s="1" t="s">
         <v>91</v>
       </c>
@@ -1661,7 +1667,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="16"/>
+      <c r="A44" s="17"/>
       <c r="B44" s="1" t="s">
         <v>92</v>
       </c>
@@ -1671,7 +1677,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="17" t="s">
         <v>95</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1683,7 +1689,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="16"/>
+      <c r="A46" s="17"/>
       <c r="B46" s="1" t="s">
         <v>96</v>
       </c>
@@ -1693,35 +1699,35 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="19" t="s">
         <v>63</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C47" s="1"/>
-      <c r="D47" s="17" t="s">
+      <c r="D47" s="16" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="19"/>
+      <c r="A48" s="20"/>
       <c r="B48" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="17"/>
+      <c r="D48" s="16"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="19"/>
+      <c r="A49" s="20"/>
       <c r="B49" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C49" s="1"/>
-      <c r="D49" s="17"/>
+      <c r="D49" s="16"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="19"/>
+      <c r="A50" s="20"/>
       <c r="B50" s="1" t="s">
         <v>99</v>
       </c>
@@ -1731,7 +1737,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="19"/>
+      <c r="A51" s="20"/>
       <c r="B51" s="1" t="s">
         <v>101</v>
       </c>
@@ -1741,7 +1747,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="19"/>
+      <c r="A52" s="20"/>
       <c r="B52" s="1" t="s">
         <v>110</v>
       </c>
@@ -1751,7 +1757,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="19"/>
+      <c r="A53" s="20"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
         <v>143</v>
@@ -1761,7 +1767,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="19"/>
+      <c r="A54" s="20"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
         <v>144</v>
@@ -1771,7 +1777,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="20"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
         <v>145</v>
@@ -1781,7 +1787,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="16" t="s">
+      <c r="A56" s="17" t="s">
         <v>67</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -1793,7 +1799,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="16"/>
+      <c r="A57" s="17"/>
       <c r="B57" s="1" t="s">
         <v>68</v>
       </c>
@@ -1825,7 +1831,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="21" t="s">
+      <c r="A60" s="18" t="s">
         <v>127</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -1839,7 +1845,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="21"/>
+      <c r="A61" s="18"/>
       <c r="B61" s="1" t="s">
         <v>112</v>
       </c>
@@ -1849,27 +1855,27 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A62" s="16" t="s">
+      <c r="A62" s="17" t="s">
         <v>70</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C62" s="1"/>
-      <c r="D62" s="17" t="s">
+      <c r="D62" s="16" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A63" s="16"/>
+      <c r="A63" s="17"/>
       <c r="B63" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C63" s="1"/>
-      <c r="D63" s="17"/>
+      <c r="D63" s="16"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A64" s="16" t="s">
+      <c r="A64" s="17" t="s">
         <v>71</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -1881,25 +1887,25 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="16"/>
+      <c r="A65" s="17"/>
       <c r="B65" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C65" s="1"/>
-      <c r="D65" s="17" t="s">
+      <c r="D65" s="16" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="16"/>
+      <c r="A66" s="17"/>
       <c r="B66" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C66" s="1"/>
-      <c r="D66" s="17"/>
+      <c r="D66" s="16"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="16"/>
+      <c r="A67" s="17"/>
       <c r="B67" s="1" t="s">
         <v>81</v>
       </c>
@@ -1909,7 +1915,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="16"/>
+      <c r="A68" s="17"/>
       <c r="B68" s="1" t="s">
         <v>85</v>
       </c>
@@ -1919,7 +1925,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="16" t="s">
+      <c r="A69" s="17" t="s">
         <v>123</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -1931,7 +1937,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="16"/>
+      <c r="A70" s="17"/>
       <c r="B70" s="1" t="s">
         <v>129</v>
       </c>
@@ -1943,15 +1949,6 @@
   </sheetData>
   <autoFilter ref="A1:D68"/>
   <mergeCells count="25">
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A47:A55"/>
     <mergeCell ref="A69:A70"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A5:A7"/>
@@ -1968,6 +1965,15 @@
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="A41:A44"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A47:A55"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 20250808 part 5
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="173">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -689,6 +689,10 @@
   </si>
   <si>
     <t>gzstv.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fjtv.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -868,22 +872,22 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1219,7 +1223,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1228,20 +1232,20 @@
       <c r="C2" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="17" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="20"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="16"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="21"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>149</v>
@@ -1251,7 +1255,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1263,7 +1267,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="17"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1273,7 +1277,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="17"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1305,19 +1309,21 @@
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>172</v>
+      </c>
       <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="17"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="1" t="s">
         <v>121</v>
       </c>
@@ -1327,7 +1333,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1339,7 +1345,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="17"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1349,7 +1355,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1361,7 +1367,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="17"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
@@ -1405,7 +1411,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="16" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1419,7 +1425,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="17"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="1" t="s">
         <v>50</v>
       </c>
@@ -1429,7 +1435,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="16" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1443,25 +1449,25 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="17"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="17" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="17"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="16"/>
+      <c r="D23" s="17"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="17"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1471,7 +1477,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="17"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="1" t="s">
         <v>45</v>
       </c>
@@ -1481,22 +1487,22 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="17"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="17" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="17"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="16"/>
+      <c r="D27" s="17"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="s">
@@ -1519,7 +1525,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="16" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1533,7 +1539,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="17"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="1" t="s">
         <v>55</v>
       </c>
@@ -1551,7 +1557,7 @@
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="18" t="s">
         <v>102</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1563,7 +1569,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="21"/>
+      <c r="A34" s="20"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
         <v>140</v>
@@ -1573,7 +1579,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="17" t="s">
+      <c r="A35" s="16" t="s">
         <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1585,7 +1591,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="17"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="1" t="s">
         <v>60</v>
       </c>
@@ -1637,27 +1643,27 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="16" t="s">
         <v>62</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C41" s="1"/>
-      <c r="D41" s="16" t="s">
+      <c r="D41" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="17"/>
+      <c r="A42" s="16"/>
       <c r="B42" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C42" s="1"/>
-      <c r="D42" s="16"/>
+      <c r="D42" s="17"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="17"/>
+      <c r="A43" s="16"/>
       <c r="B43" s="1" t="s">
         <v>91</v>
       </c>
@@ -1667,7 +1673,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="17"/>
+      <c r="A44" s="16"/>
       <c r="B44" s="1" t="s">
         <v>92</v>
       </c>
@@ -1677,7 +1683,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="16" t="s">
         <v>95</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1689,7 +1695,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="17"/>
+      <c r="A46" s="16"/>
       <c r="B46" s="1" t="s">
         <v>96</v>
       </c>
@@ -1699,35 +1705,35 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="18" t="s">
         <v>63</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C47" s="1"/>
-      <c r="D47" s="16" t="s">
+      <c r="D47" s="17" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="20"/>
+      <c r="A48" s="19"/>
       <c r="B48" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="16"/>
+      <c r="D48" s="17"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="20"/>
+      <c r="A49" s="19"/>
       <c r="B49" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C49" s="1"/>
-      <c r="D49" s="16"/>
+      <c r="D49" s="17"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="20"/>
+      <c r="A50" s="19"/>
       <c r="B50" s="1" t="s">
         <v>99</v>
       </c>
@@ -1737,7 +1743,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="20"/>
+      <c r="A51" s="19"/>
       <c r="B51" s="1" t="s">
         <v>101</v>
       </c>
@@ -1747,7 +1753,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="20"/>
+      <c r="A52" s="19"/>
       <c r="B52" s="1" t="s">
         <v>110</v>
       </c>
@@ -1757,7 +1763,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="20"/>
+      <c r="A53" s="19"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
         <v>143</v>
@@ -1767,7 +1773,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="20"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
         <v>144</v>
@@ -1777,7 +1783,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="21"/>
+      <c r="A55" s="20"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
         <v>145</v>
@@ -1787,7 +1793,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="16" t="s">
         <v>67</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -1799,7 +1805,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="17"/>
+      <c r="A57" s="16"/>
       <c r="B57" s="1" t="s">
         <v>68</v>
       </c>
@@ -1831,7 +1837,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="18" t="s">
+      <c r="A60" s="21" t="s">
         <v>127</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -1845,7 +1851,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="18"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="1" t="s">
         <v>112</v>
       </c>
@@ -1855,27 +1861,27 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A62" s="17" t="s">
+      <c r="A62" s="16" t="s">
         <v>70</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C62" s="1"/>
-      <c r="D62" s="16" t="s">
+      <c r="D62" s="17" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A63" s="17"/>
+      <c r="A63" s="16"/>
       <c r="B63" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C63" s="1"/>
-      <c r="D63" s="16"/>
+      <c r="D63" s="17"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A64" s="17" t="s">
+      <c r="A64" s="16" t="s">
         <v>71</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -1887,25 +1893,25 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="17"/>
+      <c r="A65" s="16"/>
       <c r="B65" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C65" s="1"/>
-      <c r="D65" s="16" t="s">
+      <c r="D65" s="17" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="17"/>
+      <c r="A66" s="16"/>
       <c r="B66" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C66" s="1"/>
-      <c r="D66" s="16"/>
+      <c r="D66" s="17"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="17"/>
+      <c r="A67" s="16"/>
       <c r="B67" s="1" t="s">
         <v>81</v>
       </c>
@@ -1915,7 +1921,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="17"/>
+      <c r="A68" s="16"/>
       <c r="B68" s="1" t="s">
         <v>85</v>
       </c>
@@ -1925,7 +1931,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="17" t="s">
+      <c r="A69" s="16" t="s">
         <v>123</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -1937,7 +1943,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="17"/>
+      <c r="A70" s="16"/>
       <c r="B70" s="1" t="s">
         <v>129</v>
       </c>
@@ -1949,6 +1955,15 @@
   </sheetData>
   <autoFilter ref="A1:D68"/>
   <mergeCells count="25">
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A47:A55"/>
     <mergeCell ref="A69:A70"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A5:A7"/>
@@ -1965,15 +1980,6 @@
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="A41:A44"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A47:A55"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 20250808 part 6
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="174">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -693,6 +693,10 @@
   </si>
   <si>
     <t>fjtv.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xizang.php,xztv.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -872,10 +876,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -885,9 +892,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1198,7 +1202,7 @@
   <cols>
     <col min="1" max="1" width="19.375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="111.875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="3"/>
     <col min="6" max="6" width="43.375" style="3" bestFit="1" customWidth="1"/>
@@ -1223,7 +1227,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1232,20 +1236,20 @@
       <c r="C2" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="19"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="17"/>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="20"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>149</v>
@@ -1255,7 +1259,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1267,7 +1271,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="16"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1277,7 +1281,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="16"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1309,7 +1313,7 @@
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1323,7 +1327,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="16"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="1" t="s">
         <v>121</v>
       </c>
@@ -1333,7 +1337,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="17" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1345,7 +1349,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="16"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1355,7 +1359,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="17" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1367,7 +1371,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="16"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
@@ -1411,7 +1415,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="17" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1425,7 +1429,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="16"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="1" t="s">
         <v>50</v>
       </c>
@@ -1435,7 +1439,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1449,25 +1453,25 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="16"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="16" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="16"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="17"/>
+      <c r="D23" s="16"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="16"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1477,7 +1481,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="16"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="1" t="s">
         <v>45</v>
       </c>
@@ -1487,22 +1491,22 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="16"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="16" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="16"/>
+      <c r="A27" s="17"/>
       <c r="B27" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="17"/>
+      <c r="D27" s="16"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="s">
@@ -1525,7 +1529,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="17" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1539,7 +1543,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="16"/>
+      <c r="A31" s="17"/>
       <c r="B31" s="1" t="s">
         <v>55</v>
       </c>
@@ -1557,7 +1561,7 @@
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="19" t="s">
         <v>102</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1569,7 +1573,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="20"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
         <v>140</v>
@@ -1579,7 +1583,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="17" t="s">
         <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1591,7 +1595,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="16"/>
+      <c r="A36" s="17"/>
       <c r="B36" s="1" t="s">
         <v>60</v>
       </c>
@@ -1643,27 +1647,27 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="17" t="s">
         <v>62</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C41" s="1"/>
-      <c r="D41" s="17" t="s">
+      <c r="D41" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="16"/>
+      <c r="A42" s="17"/>
       <c r="B42" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C42" s="1"/>
-      <c r="D42" s="17"/>
+      <c r="D42" s="16"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="16"/>
+      <c r="A43" s="17"/>
       <c r="B43" s="1" t="s">
         <v>91</v>
       </c>
@@ -1673,7 +1677,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="16"/>
+      <c r="A44" s="17"/>
       <c r="B44" s="1" t="s">
         <v>92</v>
       </c>
@@ -1683,7 +1687,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="17" t="s">
         <v>95</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1695,7 +1699,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="16"/>
+      <c r="A46" s="17"/>
       <c r="B46" s="1" t="s">
         <v>96</v>
       </c>
@@ -1705,35 +1709,35 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="19" t="s">
         <v>63</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C47" s="1"/>
-      <c r="D47" s="17" t="s">
+      <c r="D47" s="16" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="19"/>
+      <c r="A48" s="20"/>
       <c r="B48" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="17"/>
+      <c r="D48" s="16"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="19"/>
+      <c r="A49" s="20"/>
       <c r="B49" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C49" s="1"/>
-      <c r="D49" s="17"/>
+      <c r="D49" s="16"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="19"/>
+      <c r="A50" s="20"/>
       <c r="B50" s="1" t="s">
         <v>99</v>
       </c>
@@ -1743,7 +1747,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="19"/>
+      <c r="A51" s="20"/>
       <c r="B51" s="1" t="s">
         <v>101</v>
       </c>
@@ -1753,7 +1757,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="19"/>
+      <c r="A52" s="20"/>
       <c r="B52" s="1" t="s">
         <v>110</v>
       </c>
@@ -1763,7 +1767,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="19"/>
+      <c r="A53" s="20"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
         <v>143</v>
@@ -1773,7 +1777,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="19"/>
+      <c r="A54" s="20"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
         <v>144</v>
@@ -1783,7 +1787,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="20"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
         <v>145</v>
@@ -1793,7 +1797,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="16" t="s">
+      <c r="A56" s="17" t="s">
         <v>67</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -1805,7 +1809,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="16"/>
+      <c r="A57" s="17"/>
       <c r="B57" s="1" t="s">
         <v>68</v>
       </c>
@@ -1831,13 +1835,15 @@
       <c r="B59" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C59" s="1"/>
+      <c r="C59" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="D59" s="1" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="21" t="s">
+      <c r="A60" s="18" t="s">
         <v>127</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -1851,7 +1857,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="21"/>
+      <c r="A61" s="18"/>
       <c r="B61" s="1" t="s">
         <v>112</v>
       </c>
@@ -1861,27 +1867,27 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A62" s="16" t="s">
+      <c r="A62" s="17" t="s">
         <v>70</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C62" s="1"/>
-      <c r="D62" s="17" t="s">
+      <c r="D62" s="16" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A63" s="16"/>
+      <c r="A63" s="17"/>
       <c r="B63" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C63" s="1"/>
-      <c r="D63" s="17"/>
+      <c r="D63" s="16"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A64" s="16" t="s">
+      <c r="A64" s="17" t="s">
         <v>71</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -1893,25 +1899,25 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="16"/>
+      <c r="A65" s="17"/>
       <c r="B65" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C65" s="1"/>
-      <c r="D65" s="17" t="s">
+      <c r="D65" s="16" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="16"/>
+      <c r="A66" s="17"/>
       <c r="B66" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C66" s="1"/>
-      <c r="D66" s="17"/>
+      <c r="D66" s="16"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="16"/>
+      <c r="A67" s="17"/>
       <c r="B67" s="1" t="s">
         <v>81</v>
       </c>
@@ -1921,7 +1927,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="16"/>
+      <c r="A68" s="17"/>
       <c r="B68" s="1" t="s">
         <v>85</v>
       </c>
@@ -1931,7 +1937,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="16" t="s">
+      <c r="A69" s="17" t="s">
         <v>123</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -1943,7 +1949,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="16"/>
+      <c r="A70" s="17"/>
       <c r="B70" s="1" t="s">
         <v>129</v>
       </c>
@@ -1955,15 +1961,6 @@
   </sheetData>
   <autoFilter ref="A1:D68"/>
   <mergeCells count="25">
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A47:A55"/>
     <mergeCell ref="A69:A70"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A5:A7"/>
@@ -1980,6 +1977,15 @@
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="A41:A44"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A47:A55"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 20250810 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="177">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -705,6 +705,10 @@
   </si>
   <si>
     <t>neimenggu.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jinan.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -884,10 +888,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -897,9 +904,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1235,7 +1239,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1244,20 +1248,20 @@
       <c r="C2" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="19"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="17"/>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="20"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>149</v>
@@ -1267,7 +1271,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1279,7 +1283,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="16"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1289,7 +1293,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="16"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1321,7 +1325,7 @@
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1335,7 +1339,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="16"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="1" t="s">
         <v>121</v>
       </c>
@@ -1345,7 +1349,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="17" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1357,7 +1361,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="16"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1367,7 +1371,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="17" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1379,7 +1383,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="16"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
@@ -1425,7 +1429,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="17" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1439,7 +1443,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="16"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="1" t="s">
         <v>50</v>
       </c>
@@ -1449,7 +1453,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1463,25 +1467,25 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="16"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="16" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="16"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="17"/>
+      <c r="D23" s="16"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="16"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1491,7 +1495,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="16"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="1" t="s">
         <v>45</v>
       </c>
@@ -1501,22 +1505,22 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="16"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="16" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="16"/>
+      <c r="A27" s="17"/>
       <c r="B27" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="17"/>
+      <c r="D27" s="16"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="s">
@@ -1539,7 +1543,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="17" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1553,7 +1557,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="16"/>
+      <c r="A31" s="17"/>
       <c r="B31" s="1" t="s">
         <v>55</v>
       </c>
@@ -1571,7 +1575,7 @@
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="19" t="s">
         <v>102</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1583,7 +1587,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="20"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
         <v>140</v>
@@ -1593,7 +1597,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="17" t="s">
         <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1605,7 +1609,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="16"/>
+      <c r="A36" s="17"/>
       <c r="B36" s="1" t="s">
         <v>60</v>
       </c>
@@ -1659,27 +1663,27 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="17" t="s">
         <v>62</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C41" s="1"/>
-      <c r="D41" s="17" t="s">
+      <c r="D41" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="16"/>
+      <c r="A42" s="17"/>
       <c r="B42" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C42" s="1"/>
-      <c r="D42" s="17"/>
+      <c r="D42" s="16"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="16"/>
+      <c r="A43" s="17"/>
       <c r="B43" s="1" t="s">
         <v>91</v>
       </c>
@@ -1689,7 +1693,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="16"/>
+      <c r="A44" s="17"/>
       <c r="B44" s="1" t="s">
         <v>92</v>
       </c>
@@ -1699,7 +1703,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="17" t="s">
         <v>95</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1711,45 +1715,47 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="16"/>
+      <c r="A46" s="17"/>
       <c r="B46" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C46" s="1"/>
+      <c r="C46" s="1" t="s">
+        <v>176</v>
+      </c>
       <c r="D46" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="19" t="s">
         <v>63</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C47" s="1"/>
-      <c r="D47" s="17" t="s">
+      <c r="D47" s="16" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="19"/>
+      <c r="A48" s="20"/>
       <c r="B48" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="17"/>
+      <c r="D48" s="16"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="19"/>
+      <c r="A49" s="20"/>
       <c r="B49" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C49" s="1"/>
-      <c r="D49" s="17"/>
+      <c r="D49" s="16"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="19"/>
+      <c r="A50" s="20"/>
       <c r="B50" s="1" t="s">
         <v>99</v>
       </c>
@@ -1759,7 +1765,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="19"/>
+      <c r="A51" s="20"/>
       <c r="B51" s="1" t="s">
         <v>101</v>
       </c>
@@ -1769,7 +1775,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="19"/>
+      <c r="A52" s="20"/>
       <c r="B52" s="1" t="s">
         <v>110</v>
       </c>
@@ -1779,7 +1785,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="19"/>
+      <c r="A53" s="20"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
         <v>143</v>
@@ -1789,7 +1795,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="19"/>
+      <c r="A54" s="20"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
         <v>144</v>
@@ -1799,7 +1805,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="20"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
         <v>145</v>
@@ -1809,7 +1815,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="16" t="s">
+      <c r="A56" s="17" t="s">
         <v>67</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -1821,7 +1827,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="16"/>
+      <c r="A57" s="17"/>
       <c r="B57" s="1" t="s">
         <v>68</v>
       </c>
@@ -1855,7 +1861,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="21" t="s">
+      <c r="A60" s="18" t="s">
         <v>127</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -1869,7 +1875,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="21"/>
+      <c r="A61" s="18"/>
       <c r="B61" s="1" t="s">
         <v>112</v>
       </c>
@@ -1879,27 +1885,27 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A62" s="16" t="s">
+      <c r="A62" s="17" t="s">
         <v>70</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C62" s="1"/>
-      <c r="D62" s="17" t="s">
+      <c r="D62" s="16" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A63" s="16"/>
+      <c r="A63" s="17"/>
       <c r="B63" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C63" s="1"/>
-      <c r="D63" s="17"/>
+      <c r="D63" s="16"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A64" s="16" t="s">
+      <c r="A64" s="17" t="s">
         <v>71</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -1911,25 +1917,25 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="16"/>
+      <c r="A65" s="17"/>
       <c r="B65" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C65" s="1"/>
-      <c r="D65" s="17" t="s">
+      <c r="D65" s="16" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="16"/>
+      <c r="A66" s="17"/>
       <c r="B66" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C66" s="1"/>
-      <c r="D66" s="17"/>
+      <c r="D66" s="16"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="16"/>
+      <c r="A67" s="17"/>
       <c r="B67" s="1" t="s">
         <v>81</v>
       </c>
@@ -1939,7 +1945,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="16"/>
+      <c r="A68" s="17"/>
       <c r="B68" s="1" t="s">
         <v>85</v>
       </c>
@@ -1949,7 +1955,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="16" t="s">
+      <c r="A69" s="17" t="s">
         <v>123</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -1961,7 +1967,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="16"/>
+      <c r="A70" s="17"/>
       <c r="B70" s="1" t="s">
         <v>129</v>
       </c>
@@ -1973,15 +1979,6 @@
   </sheetData>
   <autoFilter ref="A1:D68"/>
   <mergeCells count="25">
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A47:A55"/>
     <mergeCell ref="A69:A70"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A5:A7"/>
@@ -1998,6 +1995,15 @@
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="A41:A44"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A47:A55"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 20250810 part 3
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="178">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -709,6 +709,10 @@
   </si>
   <si>
     <t>jinan.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhengzhou.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -888,22 +892,22 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1239,7 +1243,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1248,20 +1252,20 @@
       <c r="C2" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="17" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="20"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="16"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="21"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>149</v>
@@ -1271,7 +1275,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1283,7 +1287,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="17"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1293,7 +1297,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="17"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1325,7 +1329,7 @@
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1339,7 +1343,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="17"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="1" t="s">
         <v>121</v>
       </c>
@@ -1349,7 +1353,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1361,7 +1365,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="17"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1371,7 +1375,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1383,7 +1387,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="17"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
@@ -1429,7 +1433,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="16" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1443,7 +1447,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="17"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="1" t="s">
         <v>50</v>
       </c>
@@ -1453,7 +1457,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="16" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1467,25 +1471,27 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="17"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="16" t="s">
+      <c r="C22" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D22" s="17" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="17"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="16"/>
+      <c r="D23" s="17"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="17"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1495,7 +1501,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="17"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="1" t="s">
         <v>45</v>
       </c>
@@ -1505,22 +1511,22 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="17"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="17" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="17"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="16"/>
+      <c r="D27" s="17"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="s">
@@ -1543,7 +1549,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="16" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1557,7 +1563,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="17"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="1" t="s">
         <v>55</v>
       </c>
@@ -1575,7 +1581,7 @@
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="18" t="s">
         <v>102</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1587,7 +1593,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="21"/>
+      <c r="A34" s="20"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
         <v>140</v>
@@ -1597,7 +1603,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="17" t="s">
+      <c r="A35" s="16" t="s">
         <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1609,7 +1615,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="17"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="1" t="s">
         <v>60</v>
       </c>
@@ -1663,27 +1669,27 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="16" t="s">
         <v>62</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C41" s="1"/>
-      <c r="D41" s="16" t="s">
+      <c r="D41" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="17"/>
+      <c r="A42" s="16"/>
       <c r="B42" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C42" s="1"/>
-      <c r="D42" s="16"/>
+      <c r="D42" s="17"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="17"/>
+      <c r="A43" s="16"/>
       <c r="B43" s="1" t="s">
         <v>91</v>
       </c>
@@ -1693,7 +1699,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="17"/>
+      <c r="A44" s="16"/>
       <c r="B44" s="1" t="s">
         <v>92</v>
       </c>
@@ -1703,7 +1709,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="16" t="s">
         <v>95</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1715,7 +1721,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="17"/>
+      <c r="A46" s="16"/>
       <c r="B46" s="1" t="s">
         <v>96</v>
       </c>
@@ -1727,35 +1733,35 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="18" t="s">
         <v>63</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C47" s="1"/>
-      <c r="D47" s="16" t="s">
+      <c r="D47" s="17" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="20"/>
+      <c r="A48" s="19"/>
       <c r="B48" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="16"/>
+      <c r="D48" s="17"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="20"/>
+      <c r="A49" s="19"/>
       <c r="B49" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C49" s="1"/>
-      <c r="D49" s="16"/>
+      <c r="D49" s="17"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="20"/>
+      <c r="A50" s="19"/>
       <c r="B50" s="1" t="s">
         <v>99</v>
       </c>
@@ -1765,7 +1771,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="20"/>
+      <c r="A51" s="19"/>
       <c r="B51" s="1" t="s">
         <v>101</v>
       </c>
@@ -1775,7 +1781,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="20"/>
+      <c r="A52" s="19"/>
       <c r="B52" s="1" t="s">
         <v>110</v>
       </c>
@@ -1785,7 +1791,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="20"/>
+      <c r="A53" s="19"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
         <v>143</v>
@@ -1795,7 +1801,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="20"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
         <v>144</v>
@@ -1805,7 +1811,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="21"/>
+      <c r="A55" s="20"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
         <v>145</v>
@@ -1815,7 +1821,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="16" t="s">
         <v>67</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -1827,7 +1833,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="17"/>
+      <c r="A57" s="16"/>
       <c r="B57" s="1" t="s">
         <v>68</v>
       </c>
@@ -1861,7 +1867,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="18" t="s">
+      <c r="A60" s="21" t="s">
         <v>127</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -1875,7 +1881,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="18"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="1" t="s">
         <v>112</v>
       </c>
@@ -1885,27 +1891,27 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A62" s="17" t="s">
+      <c r="A62" s="16" t="s">
         <v>70</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C62" s="1"/>
-      <c r="D62" s="16" t="s">
+      <c r="D62" s="17" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A63" s="17"/>
+      <c r="A63" s="16"/>
       <c r="B63" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C63" s="1"/>
-      <c r="D63" s="16"/>
+      <c r="D63" s="17"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A64" s="17" t="s">
+      <c r="A64" s="16" t="s">
         <v>71</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -1917,25 +1923,25 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="17"/>
+      <c r="A65" s="16"/>
       <c r="B65" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C65" s="1"/>
-      <c r="D65" s="16" t="s">
+      <c r="D65" s="17" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="17"/>
+      <c r="A66" s="16"/>
       <c r="B66" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C66" s="1"/>
-      <c r="D66" s="16"/>
+      <c r="D66" s="17"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="17"/>
+      <c r="A67" s="16"/>
       <c r="B67" s="1" t="s">
         <v>81</v>
       </c>
@@ -1945,7 +1951,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="17"/>
+      <c r="A68" s="16"/>
       <c r="B68" s="1" t="s">
         <v>85</v>
       </c>
@@ -1955,7 +1961,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="17" t="s">
+      <c r="A69" s="16" t="s">
         <v>123</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -1967,7 +1973,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="17"/>
+      <c r="A70" s="16"/>
       <c r="B70" s="1" t="s">
         <v>129</v>
       </c>
@@ -1979,6 +1985,15 @@
   </sheetData>
   <autoFilter ref="A1:D68"/>
   <mergeCells count="25">
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A47:A55"/>
     <mergeCell ref="A69:A70"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A5:A7"/>
@@ -1995,15 +2010,6 @@
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="A41:A44"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A47:A55"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 20250810 part 4
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="179">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -713,6 +713,10 @@
   </si>
   <si>
     <t>zhengzhou.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shaanxi.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -892,10 +896,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -905,9 +912,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1243,7 +1247,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1252,20 +1256,20 @@
       <c r="C2" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="19"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="17"/>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="20"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>149</v>
@@ -1275,7 +1279,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1287,7 +1291,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="16"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1297,7 +1301,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="16"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1329,7 +1333,7 @@
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1343,7 +1347,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="16"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="1" t="s">
         <v>121</v>
       </c>
@@ -1353,7 +1357,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="17" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1365,7 +1369,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="16"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1375,7 +1379,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="17" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1387,7 +1391,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="16"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
@@ -1433,7 +1437,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="17" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1447,7 +1451,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="16"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="1" t="s">
         <v>50</v>
       </c>
@@ -1457,7 +1461,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1471,27 +1475,27 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="16"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="16" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="16"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="17"/>
+      <c r="D23" s="16"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="16"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1501,7 +1505,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="16"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="1" t="s">
         <v>45</v>
       </c>
@@ -1511,22 +1515,22 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="16"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="16" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="16"/>
+      <c r="A27" s="17"/>
       <c r="B27" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="17"/>
+      <c r="D27" s="16"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="s">
@@ -1549,7 +1553,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="17" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1563,7 +1567,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="16"/>
+      <c r="A31" s="17"/>
       <c r="B31" s="1" t="s">
         <v>55</v>
       </c>
@@ -1581,7 +1585,7 @@
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="19" t="s">
         <v>102</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1593,7 +1597,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="20"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
         <v>140</v>
@@ -1603,7 +1607,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="17" t="s">
         <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1615,7 +1619,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="16"/>
+      <c r="A36" s="17"/>
       <c r="B36" s="1" t="s">
         <v>60</v>
       </c>
@@ -1669,27 +1673,29 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="17" t="s">
         <v>62</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C41" s="1"/>
-      <c r="D41" s="17" t="s">
+      <c r="C41" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D41" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="16"/>
+      <c r="A42" s="17"/>
       <c r="B42" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C42" s="1"/>
-      <c r="D42" s="17"/>
+      <c r="D42" s="16"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="16"/>
+      <c r="A43" s="17"/>
       <c r="B43" s="1" t="s">
         <v>91</v>
       </c>
@@ -1699,7 +1705,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="16"/>
+      <c r="A44" s="17"/>
       <c r="B44" s="1" t="s">
         <v>92</v>
       </c>
@@ -1709,7 +1715,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="17" t="s">
         <v>95</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1721,7 +1727,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="16"/>
+      <c r="A46" s="17"/>
       <c r="B46" s="1" t="s">
         <v>96</v>
       </c>
@@ -1733,35 +1739,35 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="19" t="s">
         <v>63</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C47" s="1"/>
-      <c r="D47" s="17" t="s">
+      <c r="D47" s="16" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="19"/>
+      <c r="A48" s="20"/>
       <c r="B48" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="17"/>
+      <c r="D48" s="16"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="19"/>
+      <c r="A49" s="20"/>
       <c r="B49" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C49" s="1"/>
-      <c r="D49" s="17"/>
+      <c r="D49" s="16"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="19"/>
+      <c r="A50" s="20"/>
       <c r="B50" s="1" t="s">
         <v>99</v>
       </c>
@@ -1771,7 +1777,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="19"/>
+      <c r="A51" s="20"/>
       <c r="B51" s="1" t="s">
         <v>101</v>
       </c>
@@ -1781,7 +1787,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="19"/>
+      <c r="A52" s="20"/>
       <c r="B52" s="1" t="s">
         <v>110</v>
       </c>
@@ -1791,7 +1797,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="19"/>
+      <c r="A53" s="20"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
         <v>143</v>
@@ -1801,7 +1807,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="19"/>
+      <c r="A54" s="20"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
         <v>144</v>
@@ -1811,7 +1817,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="20"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
         <v>145</v>
@@ -1821,7 +1827,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="16" t="s">
+      <c r="A56" s="17" t="s">
         <v>67</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -1833,7 +1839,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="16"/>
+      <c r="A57" s="17"/>
       <c r="B57" s="1" t="s">
         <v>68</v>
       </c>
@@ -1867,7 +1873,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="21" t="s">
+      <c r="A60" s="18" t="s">
         <v>127</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -1881,7 +1887,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="21"/>
+      <c r="A61" s="18"/>
       <c r="B61" s="1" t="s">
         <v>112</v>
       </c>
@@ -1891,27 +1897,27 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A62" s="16" t="s">
+      <c r="A62" s="17" t="s">
         <v>70</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C62" s="1"/>
-      <c r="D62" s="17" t="s">
+      <c r="D62" s="16" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A63" s="16"/>
+      <c r="A63" s="17"/>
       <c r="B63" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C63" s="1"/>
-      <c r="D63" s="17"/>
+      <c r="D63" s="16"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A64" s="16" t="s">
+      <c r="A64" s="17" t="s">
         <v>71</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -1923,25 +1929,25 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="16"/>
+      <c r="A65" s="17"/>
       <c r="B65" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C65" s="1"/>
-      <c r="D65" s="17" t="s">
+      <c r="D65" s="16" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="16"/>
+      <c r="A66" s="17"/>
       <c r="B66" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C66" s="1"/>
-      <c r="D66" s="17"/>
+      <c r="D66" s="16"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="16"/>
+      <c r="A67" s="17"/>
       <c r="B67" s="1" t="s">
         <v>81</v>
       </c>
@@ -1951,7 +1957,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="16"/>
+      <c r="A68" s="17"/>
       <c r="B68" s="1" t="s">
         <v>85</v>
       </c>
@@ -1961,7 +1967,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="16" t="s">
+      <c r="A69" s="17" t="s">
         <v>123</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -1973,7 +1979,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="16"/>
+      <c r="A70" s="17"/>
       <c r="B70" s="1" t="s">
         <v>129</v>
       </c>
@@ -1985,15 +1991,6 @@
   </sheetData>
   <autoFilter ref="A1:D68"/>
   <mergeCells count="25">
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A47:A55"/>
     <mergeCell ref="A69:A70"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A5:A7"/>
@@ -2010,6 +2007,15 @@
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="A41:A44"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A47:A55"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 20250810 part 8
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="182">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -717,6 +717,18 @@
   </si>
   <si>
     <t>shaanxi.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>延边朝鲜族自治州卫视和州频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ybtv.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhejiang_zsj.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1581,8 +1593,12 @@
         <v>155</v>
       </c>
       <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="C32" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="19" t="s">
@@ -1923,7 +1939,9 @@
       <c r="B64" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C64" s="1"/>
+      <c r="C64" s="1" t="s">
+        <v>181</v>
+      </c>
       <c r="D64" s="1" t="s">
         <v>77</v>
       </c>

</xml_diff>

<commit_message>
Update on 20250810 part 9
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -908,22 +908,22 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1259,7 +1259,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1268,20 +1268,20 @@
       <c r="C2" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="17" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="20"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="16"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="21"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>149</v>
@@ -1291,7 +1291,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1303,7 +1303,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="17"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1313,7 +1313,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="17"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1345,7 +1345,7 @@
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1359,7 +1359,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="17"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="1" t="s">
         <v>121</v>
       </c>
@@ -1369,7 +1369,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1381,7 +1381,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="17"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1391,7 +1391,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1403,7 +1403,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="17"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
@@ -1449,7 +1449,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="16" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1463,7 +1463,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="17"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="1" t="s">
         <v>50</v>
       </c>
@@ -1473,7 +1473,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="16" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1487,27 +1487,27 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="17"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="17" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="17"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="16"/>
+      <c r="D23" s="17"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="17"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1517,7 +1517,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="17"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="1" t="s">
         <v>45</v>
       </c>
@@ -1527,22 +1527,22 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="17"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="17" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="17"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="16"/>
+      <c r="D27" s="17"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="s">
@@ -1565,7 +1565,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="16" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1579,7 +1579,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="17"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="1" t="s">
         <v>55</v>
       </c>
@@ -1601,7 +1601,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="18" t="s">
         <v>102</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1613,7 +1613,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="21"/>
+      <c r="A34" s="20"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
         <v>140</v>
@@ -1623,7 +1623,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="17" t="s">
+      <c r="A35" s="16" t="s">
         <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1635,7 +1635,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="17"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="1" t="s">
         <v>60</v>
       </c>
@@ -1689,7 +1689,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="16" t="s">
         <v>62</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1698,20 +1698,20 @@
       <c r="C41" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D41" s="16" t="s">
+      <c r="D41" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="17"/>
+      <c r="A42" s="16"/>
       <c r="B42" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C42" s="1"/>
-      <c r="D42" s="16"/>
+      <c r="D42" s="17"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="17"/>
+      <c r="A43" s="16"/>
       <c r="B43" s="1" t="s">
         <v>91</v>
       </c>
@@ -1721,7 +1721,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="17"/>
+      <c r="A44" s="16"/>
       <c r="B44" s="1" t="s">
         <v>92</v>
       </c>
@@ -1731,7 +1731,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="16" t="s">
         <v>95</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1743,7 +1743,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="17"/>
+      <c r="A46" s="16"/>
       <c r="B46" s="1" t="s">
         <v>96</v>
       </c>
@@ -1755,35 +1755,35 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="18" t="s">
         <v>63</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C47" s="1"/>
-      <c r="D47" s="16" t="s">
+      <c r="D47" s="17" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="20"/>
+      <c r="A48" s="19"/>
       <c r="B48" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="16"/>
+      <c r="D48" s="17"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="20"/>
+      <c r="A49" s="19"/>
       <c r="B49" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C49" s="1"/>
-      <c r="D49" s="16"/>
+      <c r="D49" s="17"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="20"/>
+      <c r="A50" s="19"/>
       <c r="B50" s="1" t="s">
         <v>99</v>
       </c>
@@ -1793,7 +1793,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="20"/>
+      <c r="A51" s="19"/>
       <c r="B51" s="1" t="s">
         <v>101</v>
       </c>
@@ -1803,7 +1803,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="20"/>
+      <c r="A52" s="19"/>
       <c r="B52" s="1" t="s">
         <v>110</v>
       </c>
@@ -1813,7 +1813,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="20"/>
+      <c r="A53" s="19"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
         <v>143</v>
@@ -1823,7 +1823,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="20"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
         <v>144</v>
@@ -1833,7 +1833,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="21"/>
+      <c r="A55" s="20"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
         <v>145</v>
@@ -1843,7 +1843,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="16" t="s">
         <v>67</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -1855,7 +1855,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="17"/>
+      <c r="A57" s="16"/>
       <c r="B57" s="1" t="s">
         <v>68</v>
       </c>
@@ -1889,7 +1889,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="18" t="s">
+      <c r="A60" s="21" t="s">
         <v>127</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -1903,7 +1903,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="18"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="1" t="s">
         <v>112</v>
       </c>
@@ -1913,27 +1913,27 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A62" s="17" t="s">
+      <c r="A62" s="16" t="s">
         <v>70</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C62" s="1"/>
-      <c r="D62" s="16" t="s">
+      <c r="D62" s="17" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A63" s="17"/>
+      <c r="A63" s="16"/>
       <c r="B63" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C63" s="1"/>
-      <c r="D63" s="16"/>
+      <c r="D63" s="17"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A64" s="17" t="s">
+      <c r="A64" s="16" t="s">
         <v>71</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -1947,25 +1947,25 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="17"/>
+      <c r="A65" s="16"/>
       <c r="B65" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C65" s="1"/>
-      <c r="D65" s="16" t="s">
+      <c r="D65" s="17" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="17"/>
+      <c r="A66" s="16"/>
       <c r="B66" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C66" s="1"/>
-      <c r="D66" s="16"/>
+      <c r="D66" s="17"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="17"/>
+      <c r="A67" s="16"/>
       <c r="B67" s="1" t="s">
         <v>81</v>
       </c>
@@ -1975,7 +1975,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="17"/>
+      <c r="A68" s="16"/>
       <c r="B68" s="1" t="s">
         <v>85</v>
       </c>
@@ -1985,7 +1985,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="17" t="s">
+      <c r="A69" s="16" t="s">
         <v>123</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -1997,7 +1997,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="17"/>
+      <c r="A70" s="16"/>
       <c r="B70" s="1" t="s">
         <v>129</v>
       </c>
@@ -2009,6 +2009,15 @@
   </sheetData>
   <autoFilter ref="A1:D68"/>
   <mergeCells count="25">
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A47:A55"/>
     <mergeCell ref="A69:A70"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A5:A7"/>
@@ -2025,15 +2034,6 @@
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="A41:A44"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A47:A55"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 20250810 part 10
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -575,10 +575,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>cdtv.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Shanxi_tyxl.php</t>
   </si>
   <si>
@@ -688,10 +684,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>xizang.php,xztv.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>hainan.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -729,6 +721,16 @@
   </si>
   <si>
     <t>zhejiang_zsj.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xizang.php
+xztv.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cdtv.php
+cdtv2.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -858,7 +860,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -908,10 +910,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -923,7 +928,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1246,10 +1251,10 @@
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -1259,7 +1264,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1268,30 +1273,30 @@
       <c r="C2" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="19"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="17"/>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="20"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1303,7 +1308,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="16"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1313,7 +1318,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="16"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1330,7 +1335,7 @@
         <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>21</v>
@@ -1338,28 +1343,28 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="16"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="1" t="s">
         <v>121</v>
       </c>
@@ -1369,7 +1374,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="17" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1381,7 +1386,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="16"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1391,7 +1396,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="17" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1403,7 +1408,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="16"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
@@ -1414,12 +1419,12 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
@@ -1430,7 +1435,7 @@
         <v>133</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>132</v>
@@ -1438,18 +1443,18 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="17" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1463,7 +1468,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="16"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="1" t="s">
         <v>50</v>
       </c>
@@ -1473,7 +1478,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1487,27 +1492,27 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="16"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D22" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D22" s="16" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="16"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="17"/>
+      <c r="D23" s="16"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="16"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1517,7 +1522,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="16"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="1" t="s">
         <v>45</v>
       </c>
@@ -1527,59 +1532,59 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="16"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="16" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="16"/>
+      <c r="A27" s="17"/>
       <c r="B27" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="17"/>
+      <c r="D27" s="16"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="17" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="16"/>
+      <c r="A31" s="17"/>
       <c r="B31" s="1" t="s">
         <v>55</v>
       </c>
@@ -1590,18 +1595,18 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="19" t="s">
         <v>102</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1613,7 +1618,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="20"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
         <v>140</v>
@@ -1623,7 +1628,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="17" t="s">
         <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1635,7 +1640,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="16"/>
+      <c r="A36" s="17"/>
       <c r="B36" s="1" t="s">
         <v>60</v>
       </c>
@@ -1658,60 +1663,60 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="17" t="s">
         <v>62</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D41" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D41" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="16"/>
+      <c r="A42" s="17"/>
       <c r="B42" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C42" s="1"/>
-      <c r="D42" s="17"/>
+      <c r="D42" s="16"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="16"/>
+      <c r="A43" s="17"/>
       <c r="B43" s="1" t="s">
         <v>91</v>
       </c>
@@ -1721,7 +1726,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="16"/>
+      <c r="A44" s="17"/>
       <c r="B44" s="1" t="s">
         <v>92</v>
       </c>
@@ -1731,7 +1736,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="17" t="s">
         <v>95</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1743,47 +1748,47 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="16"/>
+      <c r="A46" s="17"/>
       <c r="B46" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="19" t="s">
         <v>63</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C47" s="1"/>
-      <c r="D47" s="17" t="s">
+      <c r="D47" s="16" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="19"/>
+      <c r="A48" s="20"/>
       <c r="B48" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="17"/>
+      <c r="D48" s="16"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="19"/>
+      <c r="A49" s="20"/>
       <c r="B49" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C49" s="1"/>
-      <c r="D49" s="17"/>
+      <c r="D49" s="16"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="19"/>
+      <c r="A50" s="20"/>
       <c r="B50" s="1" t="s">
         <v>99</v>
       </c>
@@ -1793,7 +1798,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="19"/>
+      <c r="A51" s="20"/>
       <c r="B51" s="1" t="s">
         <v>101</v>
       </c>
@@ -1803,7 +1808,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="19"/>
+      <c r="A52" s="20"/>
       <c r="B52" s="1" t="s">
         <v>110</v>
       </c>
@@ -1813,37 +1818,37 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="19"/>
+      <c r="A53" s="20"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="19"/>
+      <c r="A54" s="20"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="20"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="16" t="s">
+      <c r="A56" s="17" t="s">
         <v>67</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -1854,13 +1859,13 @@
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="16"/>
+    <row r="57" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
+      <c r="A57" s="17"/>
       <c r="B57" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>142</v>
+      <c r="C57" s="22" t="s">
+        <v>181</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>69</v>
@@ -1868,28 +1873,28 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A58" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
       <c r="A59" s="6" t="s">
         <v>126</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>171</v>
+      <c r="C59" s="22" t="s">
+        <v>180</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="21" t="s">
+      <c r="A60" s="18" t="s">
         <v>127</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -1903,7 +1908,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="21"/>
+      <c r="A61" s="18"/>
       <c r="B61" s="1" t="s">
         <v>112</v>
       </c>
@@ -1913,59 +1918,59 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A62" s="16" t="s">
+      <c r="A62" s="17" t="s">
         <v>70</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C62" s="1"/>
-      <c r="D62" s="17" t="s">
+      <c r="D62" s="16" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A63" s="16"/>
+      <c r="A63" s="17"/>
       <c r="B63" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C63" s="1"/>
-      <c r="D63" s="17"/>
+      <c r="D63" s="16"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A64" s="16" t="s">
+      <c r="A64" s="17" t="s">
         <v>71</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>76</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="16"/>
+      <c r="A65" s="17"/>
       <c r="B65" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C65" s="1"/>
-      <c r="D65" s="17" t="s">
+      <c r="D65" s="16" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="16"/>
+      <c r="A66" s="17"/>
       <c r="B66" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C66" s="1"/>
-      <c r="D66" s="17"/>
+      <c r="D66" s="16"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="16"/>
+      <c r="A67" s="17"/>
       <c r="B67" s="1" t="s">
         <v>81</v>
       </c>
@@ -1975,7 +1980,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="16"/>
+      <c r="A68" s="17"/>
       <c r="B68" s="1" t="s">
         <v>85</v>
       </c>
@@ -1985,7 +1990,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="16" t="s">
+      <c r="A69" s="17" t="s">
         <v>123</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -1997,7 +2002,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="16"/>
+      <c r="A70" s="17"/>
       <c r="B70" s="1" t="s">
         <v>129</v>
       </c>
@@ -2009,15 +2014,6 @@
   </sheetData>
   <autoFilter ref="A1:D68"/>
   <mergeCells count="25">
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A47:A55"/>
     <mergeCell ref="A69:A70"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A5:A7"/>
@@ -2034,6 +2030,15 @@
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="A41:A44"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A47:A55"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2061,10 +2066,10 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Update on 20250810 part 11
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -596,10 +596,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Shanghai_setv.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>重庆</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -731,6 +727,11 @@
   <si>
     <t>cdtv.php
 cdtv2.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shanghai_setv.php
+Shanghai_setv2.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -910,13 +911,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -928,7 +929,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1251,10 +1252,10 @@
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -1273,7 +1274,7 @@
       <c r="C2" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="18" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1283,13 +1284,13 @@
         <v>3</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="16"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="D3" s="18"/>
+    </row>
+    <row r="4" spans="1:6" ht="37.5" x14ac:dyDescent="0.15">
       <c r="A4" s="21"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
-        <v>148</v>
+      <c r="C4" s="16" t="s">
+        <v>181</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>136</v>
@@ -1335,7 +1336,7 @@
         <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>21</v>
@@ -1343,7 +1344,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1357,7 +1358,7 @@
         <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>24</v>
@@ -1419,12 +1420,12 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
@@ -1435,7 +1436,7 @@
         <v>133</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>132</v>
@@ -1443,14 +1444,14 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
@@ -1497,9 +1498,9 @@
         <v>40</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D22" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D22" s="18" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1509,7 +1510,7 @@
         <v>42</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="16"/>
+      <c r="D23" s="18"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="17"/>
@@ -1537,7 +1538,7 @@
         <v>47</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="18" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1547,26 +1548,26 @@
         <v>48</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="16"/>
+      <c r="D27" s="18"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
@@ -1577,7 +1578,7 @@
         <v>53</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>54</v>
@@ -1595,14 +1596,14 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
@@ -1663,34 +1664,34 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
@@ -1701,9 +1702,9 @@
         <v>64</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D41" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="D41" s="18" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1713,7 +1714,7 @@
         <v>90</v>
       </c>
       <c r="C42" s="1"/>
-      <c r="D42" s="16"/>
+      <c r="D42" s="18"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" s="17"/>
@@ -1753,7 +1754,7 @@
         <v>96</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>97</v>
@@ -1767,7 +1768,7 @@
         <v>88</v>
       </c>
       <c r="C47" s="1"/>
-      <c r="D47" s="16" t="s">
+      <c r="D47" s="18" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1777,7 +1778,7 @@
         <v>98</v>
       </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="16"/>
+      <c r="D48" s="18"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" s="20"/>
@@ -1785,7 +1786,7 @@
         <v>118</v>
       </c>
       <c r="C49" s="1"/>
-      <c r="D49" s="16"/>
+      <c r="D49" s="18"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A50" s="20"/>
@@ -1864,8 +1865,8 @@
       <c r="B57" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C57" s="22" t="s">
-        <v>181</v>
+      <c r="C57" s="16" t="s">
+        <v>180</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>69</v>
@@ -1873,7 +1874,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A58" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1886,15 +1887,15 @@
       <c r="B59" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C59" s="22" t="s">
-        <v>180</v>
+      <c r="C59" s="16" t="s">
+        <v>179</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="18" t="s">
+      <c r="A60" s="22" t="s">
         <v>127</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -1908,7 +1909,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="18"/>
+      <c r="A61" s="22"/>
       <c r="B61" s="1" t="s">
         <v>112</v>
       </c>
@@ -1925,7 +1926,7 @@
         <v>73</v>
       </c>
       <c r="C62" s="1"/>
-      <c r="D62" s="16" t="s">
+      <c r="D62" s="18" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1935,7 +1936,7 @@
         <v>74</v>
       </c>
       <c r="C63" s="1"/>
-      <c r="D63" s="16"/>
+      <c r="D63" s="18"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A64" s="17" t="s">
@@ -1945,7 +1946,7 @@
         <v>76</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>77</v>
@@ -1957,7 +1958,7 @@
         <v>78</v>
       </c>
       <c r="C65" s="1"/>
-      <c r="D65" s="16" t="s">
+      <c r="D65" s="18" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1967,7 +1968,7 @@
         <v>80</v>
       </c>
       <c r="C66" s="1"/>
-      <c r="D66" s="16"/>
+      <c r="D66" s="18"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A67" s="17"/>
@@ -2014,6 +2015,15 @@
   </sheetData>
   <autoFilter ref="A1:D68"/>
   <mergeCells count="25">
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A47:A55"/>
     <mergeCell ref="A69:A70"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A5:A7"/>
@@ -2030,15 +2040,6 @@
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="A41:A44"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A47:A55"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2066,10 +2067,10 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Update on 20250810 part 14
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -730,8 +730,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Shanghai_setv.php
-Shanghai_setv2.php</t>
+    <t>Shanghai_setv.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -914,10 +913,13 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -927,9 +929,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1265,7 +1264,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1274,20 +1273,20 @@
       <c r="C2" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="20"/>
+      <c r="A3" s="21"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="18"/>
-    </row>
-    <row r="4" spans="1:6" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A4" s="21"/>
+      <c r="D3" s="17"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="22"/>
       <c r="B4" s="1"/>
       <c r="C4" s="16" t="s">
         <v>181</v>
@@ -1297,7 +1296,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1309,7 +1308,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="17"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1319,7 +1318,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="17"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1351,7 +1350,7 @@
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="18" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1365,7 +1364,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="17"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="1" t="s">
         <v>121</v>
       </c>
@@ -1375,7 +1374,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="18" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1387,7 +1386,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="17"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1397,7 +1396,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="18" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1409,7 +1408,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="17"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
@@ -1455,7 +1454,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="18" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1469,7 +1468,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="17"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="1" t="s">
         <v>50</v>
       </c>
@@ -1479,7 +1478,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="18" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1493,27 +1492,27 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="17"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="17" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="17"/>
+      <c r="A23" s="18"/>
       <c r="B23" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="18"/>
+      <c r="D23" s="17"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="17"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1523,7 +1522,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="17"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="1" t="s">
         <v>45</v>
       </c>
@@ -1533,22 +1532,22 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="17"/>
+      <c r="A26" s="18"/>
       <c r="B26" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="18" t="s">
+      <c r="D26" s="17" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="17"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="18"/>
+      <c r="D27" s="17"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="s">
@@ -1571,7 +1570,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="18" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1585,7 +1584,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="17"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="1" t="s">
         <v>55</v>
       </c>
@@ -1607,7 +1606,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="20" t="s">
         <v>102</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1619,7 +1618,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="21"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
         <v>140</v>
@@ -1629,7 +1628,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="17" t="s">
+      <c r="A35" s="18" t="s">
         <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1641,7 +1640,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="17"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="1" t="s">
         <v>60</v>
       </c>
@@ -1695,7 +1694,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="18" t="s">
         <v>62</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1704,20 +1703,20 @@
       <c r="C41" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="D41" s="18" t="s">
+      <c r="D41" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="17"/>
+      <c r="A42" s="18"/>
       <c r="B42" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C42" s="1"/>
-      <c r="D42" s="18"/>
+      <c r="D42" s="17"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="17"/>
+      <c r="A43" s="18"/>
       <c r="B43" s="1" t="s">
         <v>91</v>
       </c>
@@ -1727,7 +1726,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="17"/>
+      <c r="A44" s="18"/>
       <c r="B44" s="1" t="s">
         <v>92</v>
       </c>
@@ -1737,7 +1736,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="18" t="s">
         <v>95</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1749,7 +1748,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="17"/>
+      <c r="A46" s="18"/>
       <c r="B46" s="1" t="s">
         <v>96</v>
       </c>
@@ -1761,35 +1760,35 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="20" t="s">
         <v>63</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C47" s="1"/>
-      <c r="D47" s="18" t="s">
+      <c r="D47" s="17" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="20"/>
+      <c r="A48" s="21"/>
       <c r="B48" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="18"/>
+      <c r="D48" s="17"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="20"/>
+      <c r="A49" s="21"/>
       <c r="B49" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C49" s="1"/>
-      <c r="D49" s="18"/>
+      <c r="D49" s="17"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="20"/>
+      <c r="A50" s="21"/>
       <c r="B50" s="1" t="s">
         <v>99</v>
       </c>
@@ -1799,7 +1798,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="20"/>
+      <c r="A51" s="21"/>
       <c r="B51" s="1" t="s">
         <v>101</v>
       </c>
@@ -1809,7 +1808,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="20"/>
+      <c r="A52" s="21"/>
       <c r="B52" s="1" t="s">
         <v>110</v>
       </c>
@@ -1819,7 +1818,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="20"/>
+      <c r="A53" s="21"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
         <v>142</v>
@@ -1829,7 +1828,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="20"/>
+      <c r="A54" s="21"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
         <v>143</v>
@@ -1839,7 +1838,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="21"/>
+      <c r="A55" s="22"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
         <v>144</v>
@@ -1849,7 +1848,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="18" t="s">
         <v>67</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -1861,7 +1860,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A57" s="17"/>
+      <c r="A57" s="18"/>
       <c r="B57" s="1" t="s">
         <v>68</v>
       </c>
@@ -1895,7 +1894,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="22" t="s">
+      <c r="A60" s="19" t="s">
         <v>127</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -1909,7 +1908,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="22"/>
+      <c r="A61" s="19"/>
       <c r="B61" s="1" t="s">
         <v>112</v>
       </c>
@@ -1919,27 +1918,27 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A62" s="17" t="s">
+      <c r="A62" s="18" t="s">
         <v>70</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C62" s="1"/>
-      <c r="D62" s="18" t="s">
+      <c r="D62" s="17" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A63" s="17"/>
+      <c r="A63" s="18"/>
       <c r="B63" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C63" s="1"/>
-      <c r="D63" s="18"/>
+      <c r="D63" s="17"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A64" s="17" t="s">
+      <c r="A64" s="18" t="s">
         <v>71</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -1953,25 +1952,25 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="17"/>
+      <c r="A65" s="18"/>
       <c r="B65" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C65" s="1"/>
-      <c r="D65" s="18" t="s">
+      <c r="D65" s="17" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="17"/>
+      <c r="A66" s="18"/>
       <c r="B66" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C66" s="1"/>
-      <c r="D66" s="18"/>
+      <c r="D66" s="17"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="17"/>
+      <c r="A67" s="18"/>
       <c r="B67" s="1" t="s">
         <v>81</v>
       </c>
@@ -1981,7 +1980,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="17"/>
+      <c r="A68" s="18"/>
       <c r="B68" s="1" t="s">
         <v>85</v>
       </c>
@@ -1991,7 +1990,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="17" t="s">
+      <c r="A69" s="18" t="s">
         <v>123</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -2003,7 +2002,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="17"/>
+      <c r="A70" s="18"/>
       <c r="B70" s="1" t="s">
         <v>129</v>
       </c>
@@ -2015,15 +2014,6 @@
   </sheetData>
   <autoFilter ref="A1:D68"/>
   <mergeCells count="25">
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A47:A55"/>
     <mergeCell ref="A69:A70"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A5:A7"/>
@@ -2040,6 +2030,15 @@
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="A41:A44"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A47:A55"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 20250813 part 5
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -11,7 +11,7 @@
     <sheet name="其他JS脚本" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">地方台JS脚本!$A$1:$D$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">地方台JS脚本!$A$2:$D$69</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他JS脚本!$A$1:$D$4</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="188">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -743,6 +743,18 @@
   </si>
   <si>
     <t>中国环球电视网(CGTN)英语,阿拉伯语,法语,俄语,西班牙语,英语纪录频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>极直播</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jzb.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>由博彩网站提供的央视,卫视的频道直播源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -885,62 +897,62 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1243,7 +1255,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1251,806 +1263,808 @@
   <cols>
     <col min="1" max="1" width="19.375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="111.875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="3"/>
     <col min="6" max="6" width="43.375" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D1" s="13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="14" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="19" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="20"/>
-      <c r="B3" s="1" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" s="21"/>
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="18"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="21"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="1"/>
+      <c r="D4" s="17"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" s="22"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="17" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="17"/>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="17"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7" s="18"/>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8" s="18"/>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="7" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" s="12" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="17" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="17"/>
-      <c r="B11" s="1" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A12" s="18"/>
+      <c r="B12" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="17"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" s="18" t="s">
+        <v>25</v>
+      </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="17" t="s">
-        <v>30</v>
-      </c>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14" s="18"/>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="17"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A15" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A16" s="18"/>
+      <c r="B16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A16" s="12" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="15" t="s">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="14" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="9" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="12" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1" t="s">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="17" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A20" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="17"/>
-      <c r="B20" s="1" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A21" s="18"/>
+      <c r="B21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1" t="s">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="17" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A22" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="17"/>
-      <c r="B22" s="1" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A23" s="18"/>
+      <c r="B23" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D23" s="17" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="17"/>
-      <c r="B23" s="1" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A24" s="18"/>
+      <c r="B24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="18"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="17"/>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1"/>
+      <c r="D24" s="17"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A25" s="18"/>
+      <c r="B25" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="17"/>
-      <c r="B25" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A26" s="18"/>
+      <c r="B26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="17"/>
-      <c r="B26" s="1" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A27" s="18"/>
+      <c r="B27" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="18" t="s">
+      <c r="C27" s="1"/>
+      <c r="D27" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="17"/>
-      <c r="B27" s="1" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A28" s="18"/>
+      <c r="B28" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="18"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="12" t="s">
+      <c r="C28" s="1"/>
+      <c r="D28" s="17"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A29" s="11" t="s">
         <v>151</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="12" t="s">
-        <v>152</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="14" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A30" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="14" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="17" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A31" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D31" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="17"/>
-      <c r="B31" s="1" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A32" s="18"/>
+      <c r="B32" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1" t="s">
+      <c r="C32" s="1"/>
+      <c r="D32" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" s="13" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A33" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1" t="s">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="19" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A34" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1" t="s">
+      <c r="C34" s="1"/>
+      <c r="D34" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="21"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A35" s="22"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="17" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A36" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="17"/>
-      <c r="B36" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="7" t="s">
-        <v>86</v>
-      </c>
+      <c r="A37" s="18"/>
       <c r="B37" s="1" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A38" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="12" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A39" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1" t="s">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="12" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A40" s="11" t="s">
         <v>155</v>
-      </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="15" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A40" s="12" t="s">
-        <v>156</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A41" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="14" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="17" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A42" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="D41" s="18" t="s">
+      <c r="D42" s="17" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="17"/>
-      <c r="B42" s="1" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A43" s="18"/>
+      <c r="B43" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C42" s="1"/>
-      <c r="D42" s="18"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="17"/>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="1"/>
+      <c r="D43" s="17"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A44" s="18"/>
+      <c r="B44" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="17"/>
-      <c r="B44" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="17" t="s">
-        <v>95</v>
-      </c>
+      <c r="A45" s="18"/>
       <c r="B45" s="1" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A46" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="17"/>
-      <c r="B46" s="1" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A47" s="18"/>
+      <c r="B47" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="19" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A48" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C47" s="1"/>
-      <c r="D47" s="18" t="s">
+      <c r="C48" s="1"/>
+      <c r="D48" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="20"/>
-      <c r="B48" s="1" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A49" s="21"/>
+      <c r="B49" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C48" s="1"/>
-      <c r="D48" s="18"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="20"/>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="1"/>
+      <c r="D49" s="17"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A50" s="21"/>
+      <c r="B50" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C49" s="1"/>
-      <c r="D49" s="18"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="20"/>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="1"/>
+      <c r="D50" s="17"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A51" s="21"/>
+      <c r="B51" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="20"/>
-      <c r="B51" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="20"/>
+      <c r="A52" s="21"/>
       <c r="B52" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A53" s="21"/>
+      <c r="B53" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="20"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="20"/>
+      <c r="A54" s="21"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A55" s="21"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A56" s="22"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="17" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A57" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1" t="s">
+      <c r="C57" s="1"/>
+      <c r="D57" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A57" s="17"/>
-      <c r="B57" s="1" t="s">
+    <row r="58" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
+      <c r="A58" s="18"/>
+      <c r="B58" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C57" s="16" t="s">
+      <c r="C58" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="12" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A59" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-    </row>
-    <row r="59" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A59" s="6" t="s">
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+    </row>
+    <row r="60" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
+      <c r="A60" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C59" s="16" t="s">
+      <c r="C60" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="22" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A61" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D60" s="10" t="s">
+      <c r="D61" s="9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="22"/>
-      <c r="B61" s="1" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A62" s="19"/>
+      <c r="B62" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C61" s="1"/>
-      <c r="D61" s="8" t="s">
+      <c r="C62" s="1"/>
+      <c r="D62" s="7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A62" s="17" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A63" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C62" s="1"/>
-      <c r="D62" s="18" t="s">
+      <c r="C63" s="1"/>
+      <c r="D63" s="17" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A63" s="17"/>
-      <c r="B63" s="1" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A64" s="18"/>
+      <c r="B64" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C63" s="1"/>
-      <c r="D63" s="18"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A64" s="17" t="s">
+      <c r="C64" s="1"/>
+      <c r="D64" s="17"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A65" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D65" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="17"/>
-      <c r="B65" s="1" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A66" s="18"/>
+      <c r="B66" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C65" s="1"/>
-      <c r="D65" s="18" t="s">
+      <c r="C66" s="1"/>
+      <c r="D66" s="17" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="17"/>
-      <c r="B66" s="1" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A67" s="18"/>
+      <c r="B67" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C66" s="1"/>
-      <c r="D66" s="18"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="17"/>
-      <c r="B67" s="1" t="s">
+      <c r="C67" s="1"/>
+      <c r="D67" s="17"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A68" s="18"/>
+      <c r="B68" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="17"/>
-      <c r="B68" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="17" t="s">
-        <v>123</v>
-      </c>
+      <c r="A69" s="18"/>
       <c r="B69" s="1" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="17"/>
+      <c r="A70" s="18" t="s">
+        <v>123</v>
+      </c>
       <c r="B70" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A71" s="18"/>
+      <c r="B71" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1" t="s">
         <v>130</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D68"/>
+  <autoFilter ref="A2:D69"/>
   <mergeCells count="25">
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A47:A55"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A21:A27"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A70:A71"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="A65:A69"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="D48:D50"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="A48:A56"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2060,7 +2074,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2074,7 +2088,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -2088,7 +2102,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2100,7 +2114,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -2112,7 +2126,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>105</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -2124,7 +2138,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>182</v>
       </c>
       <c r="B5" s="2"/>
@@ -2135,8 +2149,20 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="D8" s="14" t="s">
+    <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
+      <c r="A6" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
+      <c r="D9" s="13" t="s">
         <v>134</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update on 20250817 part 6
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -12,14 +12,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">地方台JS脚本!$A$2:$D$69</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他JS脚本!$A$1:$D$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他JS脚本!$A$1:$D$5</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="190">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -41,10 +41,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CCTV-6,1905极限反转(国内电影)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>HuyaAndDouyu.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -653,10 +649,6 @@
   </si>
   <si>
     <t>官网提供卫视,青海省频道在线观看,可使用酷9JS脚本的Webview方式观看*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>beijing.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -755,6 +747,24 @@
   </si>
   <si>
     <t>由博彩网站提供的央视,卫视的频道直播源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>beijing.php
+beijing_app.php
+beijing_web.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1905.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCTV-6,1905极限反转(国内电影)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1905极限反转(国内电影)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -884,7 +894,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -937,21 +947,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1272,634 +1288,634 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D1" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>14</v>
+        <v>134</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="21"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="17"/>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="22"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="1"/>
       <c r="C5" s="15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7" s="17"/>
+      <c r="B7" s="1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="18"/>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="18"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="56.25" x14ac:dyDescent="0.15">
+      <c r="A9" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="6" t="s">
+      <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="18"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14" s="17"/>
+      <c r="B14" s="1" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="18"/>
-      <c r="B14" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A15" s="17" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="18" t="s">
+      <c r="B15" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="18"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="18"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D22" s="1" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A23" s="17"/>
+      <c r="B23" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="18"/>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D23" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D23" s="17" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A24" s="17"/>
+      <c r="B24" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="18"/>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1"/>
+      <c r="D24" s="18"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A25" s="17"/>
+      <c r="B25" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="17"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="18"/>
-      <c r="B25" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A26" s="17"/>
+      <c r="B26" s="1" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="18"/>
-      <c r="B26" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A27" s="17"/>
+      <c r="B27" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="18"/>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1"/>
+      <c r="D27" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A28" s="17"/>
+      <c r="B28" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="18"/>
-      <c r="B28" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="17"/>
+      <c r="D28" s="18"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D31" s="7" t="s">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A32" s="17"/>
+      <c r="B32" s="1" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" s="18"/>
-      <c r="B32" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="22"/>
+      <c r="A35" s="21"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>141</v>
-      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A37" s="17"/>
+      <c r="B37" s="1" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="18"/>
-      <c r="B37" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="18" t="s">
-        <v>62</v>
+      <c r="A42" s="17" t="s">
+        <v>61</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D42" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="18"/>
+      <c r="A43" s="17"/>
       <c r="B43" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="1"/>
+      <c r="D43" s="18"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A44" s="17"/>
+      <c r="B44" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="17"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="18"/>
-      <c r="B44" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="18"/>
+      <c r="A45" s="17"/>
       <c r="B45" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A46" s="17" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="18" t="s">
-        <v>95</v>
-      </c>
       <c r="B46" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="18"/>
+      <c r="A47" s="17"/>
       <c r="B47" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D47" s="1" t="s">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A48" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A49" s="20"/>
+      <c r="B49" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C48" s="1"/>
-      <c r="D48" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="21"/>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="1"/>
+      <c r="D49" s="18"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A50" s="20"/>
+      <c r="B50" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" s="18"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A51" s="20"/>
+      <c r="B51" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="C49" s="1"/>
-      <c r="D49" s="17"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="21"/>
-      <c r="B50" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C50" s="1"/>
-      <c r="D50" s="17"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="21"/>
-      <c r="B51" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A52" s="20"/>
+      <c r="B52" s="1" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="21"/>
-      <c r="B52" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="21"/>
+      <c r="A53" s="20"/>
       <c r="B53" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="21"/>
+      <c r="A54" s="20"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="21"/>
+      <c r="A55" s="20"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="22"/>
+      <c r="A56" s="21"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="18" t="s">
-        <v>67</v>
+      <c r="A57" s="17" t="s">
+        <v>66</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A58" s="18"/>
+      <c r="A58" s="17"/>
       <c r="B58" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="C58" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A59" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1907,139 +1923,148 @@
     </row>
     <row r="60" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
       <c r="A60" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A61" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C60" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="19" t="s">
-        <v>127</v>
-      </c>
       <c r="B61" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A62" s="19"/>
+      <c r="A62" s="22"/>
       <c r="B62" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A63" s="18" t="s">
+      <c r="A63" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C63" s="1"/>
+      <c r="D63" s="18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A64" s="17"/>
+      <c r="B64" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C64" s="1"/>
+      <c r="D64" s="18"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A65" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C63" s="1"/>
-      <c r="D63" s="17" t="s">
+      <c r="B65" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A64" s="18"/>
-      <c r="B64" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C64" s="1"/>
-      <c r="D64" s="17"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="B65" s="1" t="s">
+      <c r="C65" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D65" s="1" t="s">
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A66" s="17"/>
+      <c r="B66" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="18"/>
-      <c r="B66" s="1" t="s">
+      <c r="C66" s="1"/>
+      <c r="D66" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="C66" s="1"/>
-      <c r="D66" s="17" t="s">
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A67" s="17"/>
+      <c r="B67" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="18"/>
-      <c r="B67" s="1" t="s">
+      <c r="C67" s="1"/>
+      <c r="D67" s="18"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A68" s="17"/>
+      <c r="B68" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C67" s="1"/>
-      <c r="D67" s="17"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="18"/>
-      <c r="B68" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="18"/>
+      <c r="A69" s="17"/>
       <c r="B69" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="18" t="s">
+      <c r="A70" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A71" s="18"/>
+      <c r="A71" s="17"/>
       <c r="B71" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:D69"/>
   <mergeCells count="25">
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="A65:A69"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="D48:D50"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="A48:A56"/>
     <mergeCell ref="A70:A71"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A6:A8"/>
@@ -2056,15 +2081,6 @@
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="D42:D43"/>
     <mergeCell ref="A42:A45"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="A65:A69"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="D48:D50"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="A48:A56"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2074,7 +2090,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2089,85 +2105,98 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A1" s="16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A2" s="4" t="s">
-        <v>7</v>
+      <c r="A2" s="23" t="s">
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>187</v>
+      </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>105</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>107</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>106</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>183</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>184</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="D9" s="13" t="s">
-        <v>134</v>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
+      <c r="D10" s="13" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D4"/>
+  <autoFilter ref="A1:D5"/>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update on 20250817 part 9
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -11,7 +11,7 @@
     <sheet name="其他JS脚本" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">地方台JS脚本!$A$2:$D$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">地方台JS脚本!$A$2:$D$71</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他JS脚本!$A$1:$D$5</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="195">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -766,6 +766,24 @@
   <si>
     <t>1905极限反转(国内电影)</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shandong_qilu.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shandong_shandian.php</t>
+  </si>
+  <si>
+    <t>卫视,山东省频道和部分山东地方频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拉萨市频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lhasa.php</t>
   </si>
 </sst>
 </file>
@@ -894,7 +912,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -911,19 +929,37 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -931,44 +967,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1271,7 +1292,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1279,7 +1300,7 @@
   <cols>
     <col min="1" max="1" width="19.375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="111.875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="3"/>
     <col min="6" max="6" width="43.375" style="3" bestFit="1" customWidth="1"/>
@@ -1287,12 +1308,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1315,7 +1336,7 @@
       <c r="C3" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="16" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1325,15 +1346,15 @@
         <v>3</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="18"/>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="21"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1370,13 +1391,13 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="56.25" x14ac:dyDescent="0.15">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>186</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1384,7 +1405,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>147</v>
       </c>
       <c r="B10" s="1"/>
@@ -1460,17 +1481,17 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>148</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="13" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>130</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1484,7 +1505,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>149</v>
       </c>
       <c r="B19" s="1"/>
@@ -1541,7 +1562,7 @@
       <c r="C23" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="16" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1551,7 +1572,7 @@
         <v>41</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="18"/>
+      <c r="D24" s="16"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="17"/>
@@ -1579,7 +1600,7 @@
         <v>46</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="16" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1589,25 +1610,25 @@
         <v>47</v>
       </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="18"/>
+      <c r="D28" s="16"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="10" t="s">
         <v>150</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="13" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="10" t="s">
         <v>151</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="13" t="s">
         <v>159</v>
       </c>
     </row>
@@ -1621,7 +1642,7 @@
       <c r="C31" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="6" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1636,7 +1657,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="11" t="s">
         <v>152</v>
       </c>
       <c r="B33" s="1"/>
@@ -1692,7 +1713,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="5" t="s">
         <v>85</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1704,7 +1725,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="10" t="s">
         <v>153</v>
       </c>
       <c r="B39" s="1"/>
@@ -1716,22 +1737,22 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="10" t="s">
         <v>154</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="14" t="s">
+      <c r="D40" s="13" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="10" t="s">
         <v>155</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="14" t="s">
+      <c r="D41" s="13" t="s">
         <v>161</v>
       </c>
     </row>
@@ -1745,7 +1766,7 @@
       <c r="C42" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D42" s="18" t="s">
+      <c r="D42" s="16" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1755,7 +1776,7 @@
         <v>89</v>
       </c>
       <c r="C43" s="1"/>
-      <c r="D43" s="18"/>
+      <c r="D43" s="16"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" s="17"/>
@@ -1784,288 +1805,301 @@
       <c r="B46" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C46" s="1"/>
+      <c r="C46" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="D46" s="1" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47" s="17"/>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="1"/>
+      <c r="C47" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A48" s="17"/>
+      <c r="B48" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="19" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A49" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C48" s="1"/>
-      <c r="D48" s="18" t="s">
+      <c r="C49" s="1"/>
+      <c r="D49" s="16" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="20"/>
-      <c r="B49" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C49" s="1"/>
-      <c r="D49" s="18"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A50" s="20"/>
       <c r="B50" s="1" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="C50" s="1"/>
-      <c r="D50" s="18"/>
+      <c r="D50" s="16"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A51" s="20"/>
       <c r="B51" s="1" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="C51" s="1"/>
-      <c r="D51" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="D51" s="16"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A52" s="20"/>
       <c r="B52" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A53" s="20"/>
       <c r="B53" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A54" s="20"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1" t="s">
-        <v>141</v>
-      </c>
+      <c r="B54" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A55" s="20"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="21"/>
+      <c r="A56" s="20"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A57" s="21"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="17" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A58" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1" t="s">
+      <c r="C58" s="1"/>
+      <c r="D58" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A58" s="17"/>
-      <c r="B58" s="1" t="s">
+    <row r="59" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
+      <c r="A59" s="17"/>
+      <c r="B59" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="C59" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" s="11" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A60" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-    </row>
-    <row r="60" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A60" s="5" t="s">
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+    </row>
+    <row r="61" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
+      <c r="A61" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C60" s="15" t="s">
+      <c r="C61" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="22" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A62" s="25"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A63" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D61" s="9" t="s">
+      <c r="D63" s="8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A62" s="22"/>
-      <c r="B62" s="1" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A64" s="18"/>
+      <c r="B64" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C62" s="1"/>
-      <c r="D62" s="7" t="s">
+      <c r="C64" s="1"/>
+      <c r="D64" s="6" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A63" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C63" s="1"/>
-      <c r="D63" s="18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A64" s="17"/>
-      <c r="B64" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C64" s="1"/>
-      <c r="D64" s="18"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A65" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="C65" s="1"/>
+      <c r="D65" s="16" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A66" s="17"/>
       <c r="B66" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C66" s="1"/>
-      <c r="D66" s="18" t="s">
-        <v>78</v>
-      </c>
+      <c r="D66" s="16"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="17"/>
+      <c r="A67" s="17" t="s">
+        <v>70</v>
+      </c>
       <c r="B67" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C67" s="1"/>
-      <c r="D67" s="18"/>
+        <v>75</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A68" s="17"/>
       <c r="B68" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C68" s="1"/>
-      <c r="D68" s="1" t="s">
-        <v>81</v>
+      <c r="D68" s="16" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A69" s="17"/>
       <c r="B69" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C69" s="1"/>
-      <c r="D69" s="1" t="s">
-        <v>83</v>
-      </c>
+      <c r="D69" s="16"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="17" t="s">
-        <v>122</v>
-      </c>
+      <c r="A70" s="17"/>
       <c r="B70" s="1" t="s">
-        <v>123</v>
+        <v>80</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
-        <v>124</v>
+        <v>81</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A71" s="17"/>
       <c r="B71" s="1" t="s">
-        <v>128</v>
+        <v>84</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A72" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A73" s="17"/>
+      <c r="B73" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1" t="s">
         <v>129</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D69"/>
-  <mergeCells count="25">
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="A65:A69"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="D48:D50"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="A48:A56"/>
-    <mergeCell ref="A70:A71"/>
+  <autoFilter ref="A2:D71"/>
+  <mergeCells count="26">
+    <mergeCell ref="A72:A73"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="D3:D4"/>
@@ -2081,6 +2115,16 @@
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="D42:D43"/>
     <mergeCell ref="A42:A45"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="A67:A71"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="D49:D51"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="A49:A57"/>
+    <mergeCell ref="A61:A62"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2104,7 +2148,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -2118,7 +2162,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2130,7 +2174,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A3" s="24"/>
+      <c r="A3" s="23"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
         <v>187</v>
@@ -2188,7 +2232,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>133</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update on 20250818 part 5
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -11,7 +11,7 @@
     <sheet name="其他JS脚本" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">地方台JS脚本!$A$2:$D$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">地方台JS脚本!$A$2:$D$73</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他JS脚本!$A$1:$D$5</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="200">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -747,6 +747,48 @@
   </si>
   <si>
     <t>由博彩网站提供的央视,卫视的频道直播源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1905.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCTV-6,1905极限反转(国内电影)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1905极限反转(国内电影)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shandong_qilu.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shandong_shandian.php</t>
+  </si>
+  <si>
+    <t>卫视,山东省频道和部分山东地方频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拉萨市频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lhasa.php</t>
+  </si>
+  <si>
+    <t>shenzhen.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>henan_daxiang.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卫视,河南省频道,部分河南地方频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -756,37 +798,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1905.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCTV-6,1905极限反转(国内电影)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1905极限反转(国内电影)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>shandong_qilu.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>shandong_shandian.php</t>
-  </si>
-  <si>
-    <t>卫视,山东省频道和部分山东地方频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>拉萨市频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lhasa.php</t>
-  </si>
-  <si>
-    <t>shenzhen.php</t>
+    <t>feidong.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>肥东县频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -966,10 +982,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -979,9 +998,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1296,7 +1312,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1331,7 +1347,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1340,20 +1356,20 @@
       <c r="C3" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="19"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="17"/>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="20"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
         <v>179</v>
@@ -1363,7 +1379,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="19" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1375,7 +1391,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="16"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1385,7 +1401,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="16"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1394,743 +1410,763 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="56.25" x14ac:dyDescent="0.15">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" s="21"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="56.25" x14ac:dyDescent="0.15">
+      <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="C10" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="10" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="16" t="s">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A12" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="16"/>
-      <c r="B12" s="1" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" s="17"/>
+      <c r="B13" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="16"/>
+      <c r="A14" s="17" t="s">
+        <v>24</v>
+      </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="16" t="s">
-        <v>29</v>
-      </c>
+      <c r="A15" s="17"/>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A16" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="16"/>
-      <c r="B16" s="1" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17" s="17"/>
+      <c r="B17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A20" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A21" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A22" s="17"/>
+      <c r="B22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A23" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A24" s="17"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="13" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="16"/>
-      <c r="B21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="16"/>
-      <c r="B23" s="1" t="s">
+      <c r="D24" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A25" s="17"/>
+      <c r="B25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D25" s="16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="16"/>
-      <c r="B24" s="1" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A26" s="17"/>
+      <c r="B26" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="17"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="16"/>
-      <c r="B25" s="1" t="s">
+      <c r="C26" s="1"/>
+      <c r="D26" s="16"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A27" s="17"/>
+      <c r="B27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1" t="s">
+      <c r="C27" s="1"/>
+      <c r="D27" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="16"/>
-      <c r="B26" s="1" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A28" s="17"/>
+      <c r="B28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1" t="s">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="16"/>
-      <c r="B27" s="1" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A29" s="17"/>
+      <c r="B29" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="17" t="s">
+      <c r="C29" s="1"/>
+      <c r="D29" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="16"/>
-      <c r="B28" s="1" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A30" s="17"/>
+      <c r="B30" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="17"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="10" t="s">
+      <c r="C30" s="1"/>
+      <c r="D30" s="16"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A31" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="13" t="s">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="13" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="10" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A32" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="13" t="s">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="13" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="16" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A33" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D33" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" s="16"/>
-      <c r="B32" s="1" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A34" s="17"/>
+      <c r="B34" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
-        <v>103</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="20"/>
+      <c r="A35" s="11" t="s">
+        <v>152</v>
+      </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>139</v>
+        <v>175</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="16" t="s">
-        <v>56</v>
+      <c r="A36" s="19" t="s">
+        <v>101</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="16"/>
-      <c r="B37" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C37" s="1"/>
+      <c r="A37" s="21"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="D37" s="1" t="s">
-        <v>60</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="5" t="s">
-        <v>85</v>
+      <c r="A38" s="17" t="s">
+        <v>56</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A39" s="17"/>
+      <c r="B39" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A40" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A40" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="13" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A42" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A43" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="13" t="s">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="13" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="16" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A44" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D42" s="17" t="s">
+      <c r="D44" s="16" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="16"/>
-      <c r="B43" s="1" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A45" s="17"/>
+      <c r="B45" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="17"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="16"/>
-      <c r="B44" s="1" t="s">
+      <c r="C45" s="1"/>
+      <c r="D45" s="16"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A46" s="17"/>
+      <c r="B46" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1" t="s">
+      <c r="C46" s="1"/>
+      <c r="D46" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="16"/>
-      <c r="B45" s="1" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A47" s="17"/>
+      <c r="B47" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1" t="s">
+      <c r="C47" s="1"/>
+      <c r="D47" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="16" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A48" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C48" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A49" s="17"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="16"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="16"/>
-      <c r="B48" s="1" t="s">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A50" s="17"/>
+      <c r="B50" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="18" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A51" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C49" s="1"/>
-      <c r="D49" s="17" t="s">
+      <c r="C51" s="1"/>
+      <c r="D51" s="16" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="19"/>
-      <c r="B50" s="1" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A52" s="20"/>
+      <c r="B52" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C50" s="1"/>
-      <c r="D50" s="17"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="19"/>
-      <c r="B51" s="1" t="s">
+      <c r="C52" s="1"/>
+      <c r="D52" s="16"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A53" s="20"/>
+      <c r="B53" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C51" s="1"/>
-      <c r="D51" s="17"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="19"/>
-      <c r="B52" s="1" t="s">
+      <c r="C53" s="1"/>
+      <c r="D53" s="16"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A54" s="20"/>
+      <c r="B54" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="19"/>
-      <c r="B53" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="19"/>
-      <c r="B54" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A55" s="20"/>
+      <c r="B55" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A56" s="20"/>
+      <c r="B56" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="19"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="19"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A57" s="20"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A58" s="20"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A59" s="21"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="16" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A60" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1" t="s">
+      <c r="C60" s="1"/>
+      <c r="D60" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A59" s="16"/>
-      <c r="B59" s="1" t="s">
+    <row r="61" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
+      <c r="A61" s="17"/>
+      <c r="B61" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C59" s="14" t="s">
+      <c r="C61" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="10" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A62" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-    </row>
-    <row r="61" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A61" s="22" t="s">
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+    </row>
+    <row r="63" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
+      <c r="A63" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C61" s="14" t="s">
+      <c r="C63" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D63" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A62" s="23"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="D62" s="1" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A64" s="23"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="14" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A63" s="21" t="s">
+      <c r="D64" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A65" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D63" s="8" t="s">
+      <c r="D65" s="8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A64" s="21"/>
-      <c r="B64" s="1" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A66" s="18"/>
+      <c r="B66" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C64" s="1"/>
-      <c r="D64" s="6" t="s">
+      <c r="C66" s="1"/>
+      <c r="D66" s="6" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="16" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A67" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C65" s="1"/>
-      <c r="D65" s="17" t="s">
+      <c r="C67" s="1"/>
+      <c r="D67" s="16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="16"/>
-      <c r="B66" s="1" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A68" s="17"/>
+      <c r="B68" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C66" s="1"/>
-      <c r="D66" s="17"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="16" t="s">
+      <c r="C68" s="1"/>
+      <c r="D68" s="16"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A69" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D69" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="16"/>
-      <c r="B68" s="1" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A70" s="17"/>
+      <c r="B70" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C68" s="1"/>
-      <c r="D68" s="17" t="s">
+      <c r="C70" s="1"/>
+      <c r="D70" s="16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="16"/>
-      <c r="B69" s="1" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A71" s="17"/>
+      <c r="B71" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C69" s="1"/>
-      <c r="D69" s="17"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="16"/>
-      <c r="B70" s="1" t="s">
+      <c r="C71" s="1"/>
+      <c r="D71" s="16"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A72" s="17"/>
+      <c r="B72" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A71" s="16"/>
-      <c r="B71" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A72" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>124</v>
+        <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A73" s="16"/>
+      <c r="A73" s="17"/>
       <c r="B73" s="1" t="s">
-        <v>128</v>
+        <v>84</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A74" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A75" s="17"/>
+      <c r="B75" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1" t="s">
         <v>129</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D71"/>
+  <autoFilter ref="A2:D73"/>
   <mergeCells count="26">
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="A67:A71"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="D49:D51"/>
-    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A23:A30"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="A69:A73"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="D67:D68"/>
     <mergeCell ref="A65:A66"/>
-    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="A51:A59"/>
     <mergeCell ref="A63:A64"/>
-    <mergeCell ref="A49:A57"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A22:A28"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="A42:A45"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2176,17 +2212,17 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A3" s="25"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Update on 20250818 part 10
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="202">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -803,6 +803,14 @@
   </si>
   <si>
     <t>肥东县频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shijiazhuang.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ningbo.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -981,23 +989,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1347,7 +1355,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1356,20 +1364,20 @@
       <c r="C3" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="20" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="20"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="16"/>
+      <c r="D4" s="20"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="21"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
         <v>179</v>
@@ -1379,7 +1387,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1391,7 +1399,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="20"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1401,7 +1409,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="20"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1411,7 +1419,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="21"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>198</v>
@@ -1443,7 +1451,7 @@
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="19" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1457,7 +1465,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="17"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="1" t="s">
         <v>120</v>
       </c>
@@ -1467,7 +1475,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="19" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1479,7 +1487,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="17"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1489,7 +1497,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="19" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1501,7 +1509,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="17"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="1" t="s">
         <v>31</v>
       </c>
@@ -1549,7 +1557,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="19" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1563,17 +1571,19 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="17"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>200</v>
+      </c>
       <c r="D22" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="19" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1587,7 +1597,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="17"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
         <v>195</v>
@@ -1597,27 +1607,27 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="17"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="20" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="17"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="16"/>
+      <c r="D26" s="20"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="17"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="1" t="s">
         <v>42</v>
       </c>
@@ -1627,7 +1637,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="17"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="1" t="s">
         <v>44</v>
       </c>
@@ -1637,22 +1647,22 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="17"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="16" t="s">
+      <c r="D29" s="20" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="17"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="16"/>
+      <c r="D30" s="20"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="10" t="s">
@@ -1675,7 +1685,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="19" t="s">
         <v>51</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1689,7 +1699,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="17"/>
+      <c r="A34" s="19"/>
       <c r="B34" s="1" t="s">
         <v>54</v>
       </c>
@@ -1711,7 +1721,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="16" t="s">
         <v>101</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1723,7 +1733,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="21"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
         <v>139</v>
@@ -1733,7 +1743,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="19" t="s">
         <v>56</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1745,7 +1755,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="17"/>
+      <c r="A39" s="19"/>
       <c r="B39" s="1" t="s">
         <v>59</v>
       </c>
@@ -1799,7 +1809,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="19" t="s">
         <v>61</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -1808,20 +1818,20 @@
       <c r="C44" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D44" s="16" t="s">
+      <c r="D44" s="20" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="17"/>
+      <c r="A45" s="19"/>
       <c r="B45" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C45" s="1"/>
-      <c r="D45" s="16"/>
+      <c r="D45" s="20"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="17"/>
+      <c r="A46" s="19"/>
       <c r="B46" s="1" t="s">
         <v>90</v>
       </c>
@@ -1831,7 +1841,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="17"/>
+      <c r="A47" s="19"/>
       <c r="B47" s="1" t="s">
         <v>91</v>
       </c>
@@ -1841,7 +1851,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="17" t="s">
+      <c r="A48" s="19" t="s">
         <v>94</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -1855,7 +1865,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="17"/>
+      <c r="A49" s="19"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
         <v>190</v>
@@ -1865,7 +1875,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="17"/>
+      <c r="A50" s="19"/>
       <c r="B50" s="1" t="s">
         <v>95</v>
       </c>
@@ -1877,35 +1887,35 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="19" t="s">
+      <c r="A51" s="16" t="s">
         <v>62</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C51" s="1"/>
-      <c r="D51" s="16" t="s">
+      <c r="D51" s="20" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="20"/>
+      <c r="A52" s="17"/>
       <c r="B52" s="1" t="s">
         <v>97</v>
       </c>
       <c r="C52" s="1"/>
-      <c r="D52" s="16"/>
+      <c r="D52" s="20"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="20"/>
+      <c r="A53" s="17"/>
       <c r="B53" s="1" t="s">
         <v>117</v>
       </c>
       <c r="C53" s="1"/>
-      <c r="D53" s="16"/>
+      <c r="D53" s="20"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="20"/>
+      <c r="A54" s="17"/>
       <c r="B54" s="1" t="s">
         <v>98</v>
       </c>
@@ -1915,7 +1925,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="20"/>
+      <c r="A55" s="17"/>
       <c r="B55" s="1" t="s">
         <v>100</v>
       </c>
@@ -1925,7 +1935,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="20"/>
+      <c r="A56" s="17"/>
       <c r="B56" s="1" t="s">
         <v>109</v>
       </c>
@@ -1935,7 +1945,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="20"/>
+      <c r="A57" s="17"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
         <v>141</v>
@@ -1945,7 +1955,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="20"/>
+      <c r="A58" s="17"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
         <v>142</v>
@@ -1955,7 +1965,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" s="21"/>
+      <c r="A59" s="18"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
         <v>143</v>
@@ -1965,7 +1975,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="17" t="s">
+      <c r="A60" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -1977,7 +1987,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A61" s="17"/>
+      <c r="A61" s="19"/>
       <c r="B61" s="1" t="s">
         <v>67</v>
       </c>
@@ -2021,7 +2031,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="18" t="s">
+      <c r="A65" s="21" t="s">
         <v>126</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -2035,7 +2045,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="18"/>
+      <c r="A66" s="21"/>
       <c r="B66" s="1" t="s">
         <v>111</v>
       </c>
@@ -2045,27 +2055,27 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="17" t="s">
+      <c r="A67" s="19" t="s">
         <v>69</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C67" s="1"/>
-      <c r="D67" s="16" t="s">
+      <c r="D67" s="20" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="17"/>
+      <c r="A68" s="19"/>
       <c r="B68" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C68" s="1"/>
-      <c r="D68" s="16"/>
+      <c r="D68" s="20"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="17" t="s">
+      <c r="A69" s="19" t="s">
         <v>70</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -2079,35 +2089,37 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="17"/>
+      <c r="A70" s="19"/>
       <c r="B70" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C70" s="1"/>
-      <c r="D70" s="16" t="s">
+      <c r="D70" s="20" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A71" s="17"/>
+      <c r="A71" s="19"/>
       <c r="B71" s="1" t="s">
         <v>79</v>
       </c>
       <c r="C71" s="1"/>
-      <c r="D71" s="16"/>
+      <c r="D71" s="20"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A72" s="17"/>
+      <c r="A72" s="19"/>
       <c r="B72" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C72" s="1"/>
+      <c r="C72" s="1" t="s">
+        <v>201</v>
+      </c>
       <c r="D72" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A73" s="17"/>
+      <c r="A73" s="19"/>
       <c r="B73" s="1" t="s">
         <v>84</v>
       </c>
@@ -2117,7 +2129,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A74" s="17" t="s">
+      <c r="A74" s="19" t="s">
         <v>122</v>
       </c>
       <c r="B74" s="1" t="s">
@@ -2129,7 +2141,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A75" s="17"/>
+      <c r="A75" s="19"/>
       <c r="B75" s="1" t="s">
         <v>128</v>
       </c>
@@ -2141,6 +2153,16 @@
   </sheetData>
   <autoFilter ref="A2:D73"/>
   <mergeCells count="26">
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="A69:A73"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A51:A59"/>
+    <mergeCell ref="A63:A64"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A74:A75"/>
     <mergeCell ref="A14:A15"/>
@@ -2157,16 +2179,6 @@
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="A44:A47"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="A69:A73"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A51:A59"/>
-    <mergeCell ref="A63:A64"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 20250818 part 13
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="203">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -811,6 +811,10 @@
   </si>
   <si>
     <t>ningbo.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jiangsulitchi_app.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -989,6 +993,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -997,15 +1010,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1355,7 +1359,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1364,20 +1368,20 @@
       <c r="C3" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="17"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="20"/>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="18"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
         <v>179</v>
@@ -1387,7 +1391,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="19" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1399,7 +1403,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="17"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1409,7 +1413,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="17"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1419,7 +1423,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="18"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>198</v>
@@ -1451,7 +1455,7 @@
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="17" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1465,7 +1469,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="19"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="1" t="s">
         <v>120</v>
       </c>
@@ -1475,7 +1479,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1487,7 +1491,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="19"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1497,7 +1501,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="17" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1509,7 +1513,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="19"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="1" t="s">
         <v>31</v>
       </c>
@@ -1557,7 +1561,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="17" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1571,7 +1575,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="19"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="1" t="s">
         <v>49</v>
       </c>
@@ -1583,7 +1587,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="17" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1597,7 +1601,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="19"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
         <v>195</v>
@@ -1607,27 +1611,27 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="19"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="16" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="19"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="20"/>
+      <c r="D26" s="16"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="19"/>
+      <c r="A27" s="17"/>
       <c r="B27" s="1" t="s">
         <v>42</v>
       </c>
@@ -1637,7 +1641,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="19"/>
+      <c r="A28" s="17"/>
       <c r="B28" s="1" t="s">
         <v>44</v>
       </c>
@@ -1647,22 +1651,22 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="19"/>
+      <c r="A29" s="17"/>
       <c r="B29" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="16" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="19"/>
+      <c r="A30" s="17"/>
       <c r="B30" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="20"/>
+      <c r="D30" s="16"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="10" t="s">
@@ -1685,7 +1689,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="17" t="s">
         <v>51</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1699,7 +1703,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="19"/>
+      <c r="A34" s="17"/>
       <c r="B34" s="1" t="s">
         <v>54</v>
       </c>
@@ -1721,19 +1725,21 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="19" t="s">
         <v>101</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="D36" s="1" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="18"/>
+      <c r="A37" s="21"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
         <v>139</v>
@@ -1743,7 +1749,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="17" t="s">
         <v>56</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1755,7 +1761,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="19"/>
+      <c r="A39" s="17"/>
       <c r="B39" s="1" t="s">
         <v>59</v>
       </c>
@@ -1809,7 +1815,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="17" t="s">
         <v>61</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -1818,20 +1824,20 @@
       <c r="C44" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D44" s="20" t="s">
+      <c r="D44" s="16" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="19"/>
+      <c r="A45" s="17"/>
       <c r="B45" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C45" s="1"/>
-      <c r="D45" s="20"/>
+      <c r="D45" s="16"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="19"/>
+      <c r="A46" s="17"/>
       <c r="B46" s="1" t="s">
         <v>90</v>
       </c>
@@ -1841,7 +1847,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="19"/>
+      <c r="A47" s="17"/>
       <c r="B47" s="1" t="s">
         <v>91</v>
       </c>
@@ -1851,7 +1857,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="19" t="s">
+      <c r="A48" s="17" t="s">
         <v>94</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -1865,7 +1871,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="19"/>
+      <c r="A49" s="17"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
         <v>190</v>
@@ -1875,7 +1881,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="19"/>
+      <c r="A50" s="17"/>
       <c r="B50" s="1" t="s">
         <v>95</v>
       </c>
@@ -1887,35 +1893,35 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="16" t="s">
+      <c r="A51" s="19" t="s">
         <v>62</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C51" s="1"/>
-      <c r="D51" s="20" t="s">
+      <c r="D51" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="17"/>
+      <c r="A52" s="20"/>
       <c r="B52" s="1" t="s">
         <v>97</v>
       </c>
       <c r="C52" s="1"/>
-      <c r="D52" s="20"/>
+      <c r="D52" s="16"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="17"/>
+      <c r="A53" s="20"/>
       <c r="B53" s="1" t="s">
         <v>117</v>
       </c>
       <c r="C53" s="1"/>
-      <c r="D53" s="20"/>
+      <c r="D53" s="16"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="17"/>
+      <c r="A54" s="20"/>
       <c r="B54" s="1" t="s">
         <v>98</v>
       </c>
@@ -1925,7 +1931,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="17"/>
+      <c r="A55" s="20"/>
       <c r="B55" s="1" t="s">
         <v>100</v>
       </c>
@@ -1935,7 +1941,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="17"/>
+      <c r="A56" s="20"/>
       <c r="B56" s="1" t="s">
         <v>109</v>
       </c>
@@ -1945,7 +1951,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="17"/>
+      <c r="A57" s="20"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
         <v>141</v>
@@ -1955,7 +1961,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="17"/>
+      <c r="A58" s="20"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
         <v>142</v>
@@ -1965,7 +1971,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" s="18"/>
+      <c r="A59" s="21"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
         <v>143</v>
@@ -1975,7 +1981,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="19" t="s">
+      <c r="A60" s="17" t="s">
         <v>66</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -1987,7 +1993,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A61" s="19"/>
+      <c r="A61" s="17"/>
       <c r="B61" s="1" t="s">
         <v>67</v>
       </c>
@@ -2031,7 +2037,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="21" t="s">
+      <c r="A65" s="18" t="s">
         <v>126</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -2045,7 +2051,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="21"/>
+      <c r="A66" s="18"/>
       <c r="B66" s="1" t="s">
         <v>111</v>
       </c>
@@ -2055,27 +2061,27 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="19" t="s">
+      <c r="A67" s="17" t="s">
         <v>69</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C67" s="1"/>
-      <c r="D67" s="20" t="s">
+      <c r="D67" s="16" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="19"/>
+      <c r="A68" s="17"/>
       <c r="B68" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C68" s="1"/>
-      <c r="D68" s="20"/>
+      <c r="D68" s="16"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="19" t="s">
+      <c r="A69" s="17" t="s">
         <v>70</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -2089,25 +2095,25 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="19"/>
+      <c r="A70" s="17"/>
       <c r="B70" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C70" s="1"/>
-      <c r="D70" s="20" t="s">
+      <c r="D70" s="16" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A71" s="19"/>
+      <c r="A71" s="17"/>
       <c r="B71" s="1" t="s">
         <v>79</v>
       </c>
       <c r="C71" s="1"/>
-      <c r="D71" s="20"/>
+      <c r="D71" s="16"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A72" s="19"/>
+      <c r="A72" s="17"/>
       <c r="B72" s="1" t="s">
         <v>80</v>
       </c>
@@ -2119,7 +2125,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A73" s="19"/>
+      <c r="A73" s="17"/>
       <c r="B73" s="1" t="s">
         <v>84</v>
       </c>
@@ -2129,7 +2135,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A74" s="19" t="s">
+      <c r="A74" s="17" t="s">
         <v>122</v>
       </c>
       <c r="B74" s="1" t="s">
@@ -2141,7 +2147,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A75" s="19"/>
+      <c r="A75" s="17"/>
       <c r="B75" s="1" t="s">
         <v>128</v>
       </c>
@@ -2153,16 +2159,6 @@
   </sheetData>
   <autoFilter ref="A2:D73"/>
   <mergeCells count="26">
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="A69:A73"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A51:A59"/>
-    <mergeCell ref="A63:A64"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A74:A75"/>
     <mergeCell ref="A14:A15"/>
@@ -2179,6 +2175,16 @@
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="A44:A47"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="A69:A73"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A51:A59"/>
+    <mergeCell ref="A63:A64"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 20250819 part 5
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -9,17 +9,19 @@
   <sheets>
     <sheet name="地方台JS脚本" sheetId="1" r:id="rId1"/>
     <sheet name="其他JS脚本" sheetId="2" r:id="rId2"/>
+    <sheet name="省份统计" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">地方台JS脚本!$A$2:$D$73</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他JS脚本!$A$1:$D$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">省份统计!$A$1:$C$33</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="209">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -464,10 +466,6 @@
   </si>
   <si>
     <t>卫视,新疆维吾尔自治区频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>西藏自治区频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -815,6 +813,34 @@
   </si>
   <si>
     <t>jiangsulitchi_app.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JS或PHP脚本是否包含省级和卫视频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>√</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>广东省下属深圳市有脚本可看省级和卫视频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吉林省下属延边朝鲜族自治州有脚本可看省级和卫视频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卫视,西藏自治区频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑龙江移动提供该省卫视和省级频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -944,7 +970,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -993,23 +1019,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1022,6 +1048,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1341,7 +1379,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D1" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -1349,49 +1387,49 @@
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D3" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="20" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="20"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="16"/>
+      <c r="D4" s="20"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="21"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1403,7 +1441,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="20"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1413,7 +1451,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="20"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1423,13 +1461,13 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="21"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="56.25" x14ac:dyDescent="0.15">
@@ -1440,7 +1478,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>20</v>
@@ -1448,38 +1486,38 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="19" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="17"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="19" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1491,7 +1529,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="17"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1501,7 +1539,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="19" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1513,12 +1551,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="17"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>107</v>
@@ -1526,112 +1564,112 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>168</v>
-      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="19" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="17"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="19" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="17"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>196</v>
-      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="17"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D25" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="D25" s="20" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="17"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="16"/>
+      <c r="D26" s="20"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="17"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="1" t="s">
         <v>42</v>
       </c>
@@ -1641,7 +1679,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="17"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="1" t="s">
         <v>44</v>
       </c>
@@ -1651,59 +1689,59 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="17"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="16" t="s">
+      <c r="D29" s="20" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="17"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="16"/>
+      <c r="D30" s="20"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="19" t="s">
         <v>51</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="17"/>
+      <c r="A34" s="19"/>
       <c r="B34" s="1" t="s">
         <v>54</v>
       </c>
@@ -1714,42 +1752,42 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="16" t="s">
         <v>101</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="21"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>140</v>
-      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="19" t="s">
         <v>56</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1761,7 +1799,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="17"/>
+      <c r="A39" s="19"/>
       <c r="B39" s="1" t="s">
         <v>59</v>
       </c>
@@ -1784,60 +1822,60 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="19" t="s">
         <v>61</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>63</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D44" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="D44" s="20" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="17"/>
+      <c r="A45" s="19"/>
       <c r="B45" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C45" s="1"/>
-      <c r="D45" s="16"/>
+      <c r="D45" s="20"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="17"/>
+      <c r="A46" s="19"/>
       <c r="B46" s="1" t="s">
         <v>90</v>
       </c>
@@ -1847,7 +1885,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="17"/>
+      <c r="A47" s="19"/>
       <c r="B47" s="1" t="s">
         <v>91</v>
       </c>
@@ -1857,71 +1895,71 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="17" t="s">
+      <c r="A48" s="19" t="s">
         <v>94</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="17"/>
+      <c r="A49" s="19"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>191</v>
-      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="17"/>
+      <c r="A50" s="19"/>
       <c r="B50" s="1" t="s">
         <v>95</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="19" t="s">
+      <c r="A51" s="16" t="s">
         <v>62</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C51" s="1"/>
-      <c r="D51" s="16" t="s">
+      <c r="D51" s="20" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="20"/>
+      <c r="A52" s="17"/>
       <c r="B52" s="1" t="s">
         <v>97</v>
       </c>
       <c r="C52" s="1"/>
-      <c r="D52" s="16"/>
+      <c r="D52" s="20"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="20"/>
+      <c r="A53" s="17"/>
       <c r="B53" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C53" s="1"/>
-      <c r="D53" s="16"/>
+      <c r="D53" s="20"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="20"/>
+      <c r="A54" s="17"/>
       <c r="B54" s="1" t="s">
         <v>98</v>
       </c>
@@ -1931,17 +1969,17 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="20"/>
+      <c r="A55" s="17"/>
       <c r="B55" s="1" t="s">
         <v>100</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="20"/>
+      <c r="A56" s="17"/>
       <c r="B56" s="1" t="s">
         <v>109</v>
       </c>
@@ -1951,54 +1989,54 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="20"/>
+      <c r="A57" s="17"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="20"/>
+      <c r="A58" s="17"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" s="21"/>
+      <c r="A59" s="18"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="17" t="s">
+      <c r="A60" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A61" s="17"/>
+      <c r="A61" s="19"/>
       <c r="B61" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>68</v>
@@ -2006,7 +2044,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A62" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2014,44 +2052,44 @@
     </row>
     <row r="63" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
       <c r="A63" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>114</v>
+        <v>207</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A64" s="23"/>
       <c r="B64" s="1"/>
       <c r="C64" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="18" t="s">
-        <v>126</v>
+      <c r="A65" s="21" t="s">
+        <v>125</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D65" s="8" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="18"/>
+      <c r="A66" s="21"/>
       <c r="B66" s="1" t="s">
         <v>111</v>
       </c>
@@ -2061,71 +2099,71 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="17" t="s">
+      <c r="A67" s="19" t="s">
         <v>69</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C67" s="1"/>
-      <c r="D67" s="16" t="s">
+      <c r="D67" s="20" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="17"/>
+      <c r="A68" s="19"/>
       <c r="B68" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C68" s="1"/>
-      <c r="D68" s="16"/>
+      <c r="D68" s="20"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="17" t="s">
+      <c r="A69" s="19" t="s">
         <v>70</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="17"/>
+      <c r="A70" s="19"/>
       <c r="B70" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C70" s="1"/>
-      <c r="D70" s="16" t="s">
+      <c r="D70" s="20" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A71" s="17"/>
+      <c r="A71" s="19"/>
       <c r="B71" s="1" t="s">
         <v>79</v>
       </c>
       <c r="C71" s="1"/>
-      <c r="D71" s="16"/>
+      <c r="D71" s="20"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A72" s="17"/>
+      <c r="A72" s="19"/>
       <c r="B72" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A73" s="17"/>
+      <c r="A73" s="19"/>
       <c r="B73" s="1" t="s">
         <v>84</v>
       </c>
@@ -2135,30 +2173,40 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A74" s="17" t="s">
+      <c r="A74" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A75" s="17"/>
+      <c r="A75" s="19"/>
       <c r="B75" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:D73"/>
   <mergeCells count="26">
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="A69:A73"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A51:A59"/>
+    <mergeCell ref="A63:A64"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A74:A75"/>
     <mergeCell ref="A14:A15"/>
@@ -2175,16 +2223,6 @@
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="A44:A47"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="A69:A73"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A51:A59"/>
-    <mergeCell ref="A63:A64"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2212,10 +2250,10 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -2230,17 +2268,17 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A3" s="25"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
@@ -2269,31 +2307,31 @@
     </row>
     <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="D10" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2305,4 +2343,309 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="17.375" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.625" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.625" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="26"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A20" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A21" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A22" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A24" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A25" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A29" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A30" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A31" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A32" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A33" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C33" s="2"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C33"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update on 20250819 part 6
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -630,10 +630,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>黑龙江移动提供的源可看*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>官网提供卫视,广西自治区和部分广西地方频道在线观看,可使用酷9JS脚本的Webview方式观看*</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -841,6 +837,10 @@
   </si>
   <si>
     <t>黑龙江移动提供该省卫视和省级频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官网提供卫视,黑龙江省频道在线观看,可使用酷9JS脚本的Webview方式观看*</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1019,6 +1019,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1028,15 +1049,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1048,18 +1060,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1387,17 +1387,17 @@
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1411,7 +1411,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="17"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1419,17 +1419,17 @@
       <c r="D4" s="20"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="18"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="23" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1441,7 +1441,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="17"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1451,7 +1451,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="17"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1461,13 +1461,13 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="18"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="56.25" x14ac:dyDescent="0.15">
@@ -1478,7 +1478,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>20</v>
@@ -1493,21 +1493,21 @@
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="21" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="19"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="1" t="s">
         <v>119</v>
       </c>
@@ -1517,7 +1517,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="21" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1529,7 +1529,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="19"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1539,7 +1539,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="21" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1551,12 +1551,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="19"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>107</v>
@@ -1569,7 +1569,7 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
@@ -1580,7 +1580,7 @@
         <v>131</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>130</v>
@@ -1592,14 +1592,14 @@
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>167</v>
-      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="21" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1613,19 +1613,19 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="19"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="21" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1639,29 +1639,29 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="19"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>195</v>
-      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="19"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D25" s="20" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="19"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="1" t="s">
         <v>41</v>
       </c>
@@ -1669,7 +1669,7 @@
       <c r="D26" s="20"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="19"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="1" t="s">
         <v>42</v>
       </c>
@@ -1679,7 +1679,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="19"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="1" t="s">
         <v>44</v>
       </c>
@@ -1689,7 +1689,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="19"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="1" t="s">
         <v>46</v>
       </c>
@@ -1699,7 +1699,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="19"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="1" t="s">
         <v>47</v>
       </c>
@@ -1713,7 +1713,7 @@
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="13" t="s">
-        <v>156</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
@@ -1723,25 +1723,25 @@
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="21" t="s">
         <v>51</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="19"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="1" t="s">
         <v>54</v>
       </c>
@@ -1756,28 +1756,28 @@
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="23" t="s">
         <v>101</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="18"/>
+      <c r="A37" s="25"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
         <v>138</v>
@@ -1787,7 +1787,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="21" t="s">
         <v>56</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1799,7 +1799,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="19"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="1" t="s">
         <v>59</v>
       </c>
@@ -1826,10 +1826,10 @@
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
@@ -1839,7 +1839,7 @@
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
@@ -1849,25 +1849,25 @@
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="21" t="s">
         <v>61</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>63</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D44" s="20" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="19"/>
+      <c r="A45" s="21"/>
       <c r="B45" s="1" t="s">
         <v>89</v>
       </c>
@@ -1875,7 +1875,7 @@
       <c r="D45" s="20"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="19"/>
+      <c r="A46" s="21"/>
       <c r="B46" s="1" t="s">
         <v>90</v>
       </c>
@@ -1885,7 +1885,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="19"/>
+      <c r="A47" s="21"/>
       <c r="B47" s="1" t="s">
         <v>91</v>
       </c>
@@ -1895,43 +1895,43 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="19" t="s">
+      <c r="A48" s="21" t="s">
         <v>94</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>117</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="19"/>
+      <c r="A49" s="21"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>190</v>
-      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="19"/>
+      <c r="A50" s="21"/>
       <c r="B50" s="1" t="s">
         <v>95</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="16" t="s">
+      <c r="A51" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -1943,7 +1943,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="17"/>
+      <c r="A52" s="24"/>
       <c r="B52" s="1" t="s">
         <v>97</v>
       </c>
@@ -1951,7 +1951,7 @@
       <c r="D52" s="20"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="17"/>
+      <c r="A53" s="24"/>
       <c r="B53" s="1" t="s">
         <v>116</v>
       </c>
@@ -1959,7 +1959,7 @@
       <c r="D53" s="20"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="17"/>
+      <c r="A54" s="24"/>
       <c r="B54" s="1" t="s">
         <v>98</v>
       </c>
@@ -1969,7 +1969,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="17"/>
+      <c r="A55" s="24"/>
       <c r="B55" s="1" t="s">
         <v>100</v>
       </c>
@@ -1979,7 +1979,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="17"/>
+      <c r="A56" s="24"/>
       <c r="B56" s="1" t="s">
         <v>109</v>
       </c>
@@ -1989,7 +1989,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="17"/>
+      <c r="A57" s="24"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
         <v>140</v>
@@ -1999,7 +1999,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="17"/>
+      <c r="A58" s="24"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
         <v>141</v>
@@ -2009,7 +2009,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" s="18"/>
+      <c r="A59" s="25"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
         <v>142</v>
@@ -2019,7 +2019,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="19" t="s">
+      <c r="A60" s="21" t="s">
         <v>66</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -2031,12 +2031,12 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A61" s="19"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>68</v>
@@ -2051,31 +2051,31 @@
       <c r="D62" s="1"/>
     </row>
     <row r="63" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A63" s="22" t="s">
+      <c r="A63" s="26" t="s">
         <v>124</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A64" s="23"/>
+      <c r="A64" s="27"/>
       <c r="B64" s="1"/>
       <c r="C64" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="21" t="s">
+      <c r="A65" s="22" t="s">
         <v>125</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -2089,7 +2089,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="21"/>
+      <c r="A66" s="22"/>
       <c r="B66" s="1" t="s">
         <v>111</v>
       </c>
@@ -2099,7 +2099,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="19" t="s">
+      <c r="A67" s="21" t="s">
         <v>69</v>
       </c>
       <c r="B67" s="1" t="s">
@@ -2111,7 +2111,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="19"/>
+      <c r="A68" s="21"/>
       <c r="B68" s="1" t="s">
         <v>73</v>
       </c>
@@ -2119,21 +2119,21 @@
       <c r="D68" s="20"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="19" t="s">
+      <c r="A69" s="21" t="s">
         <v>70</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="19"/>
+      <c r="A70" s="21"/>
       <c r="B70" s="1" t="s">
         <v>77</v>
       </c>
@@ -2143,7 +2143,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A71" s="19"/>
+      <c r="A71" s="21"/>
       <c r="B71" s="1" t="s">
         <v>79</v>
       </c>
@@ -2151,19 +2151,19 @@
       <c r="D71" s="20"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A72" s="19"/>
+      <c r="A72" s="21"/>
       <c r="B72" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A73" s="19"/>
+      <c r="A73" s="21"/>
       <c r="B73" s="1" t="s">
         <v>84</v>
       </c>
@@ -2173,7 +2173,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A74" s="19" t="s">
+      <c r="A74" s="21" t="s">
         <v>121</v>
       </c>
       <c r="B74" s="1" t="s">
@@ -2185,7 +2185,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A75" s="19"/>
+      <c r="A75" s="21"/>
       <c r="B75" s="1" t="s">
         <v>127</v>
       </c>
@@ -2197,16 +2197,6 @@
   </sheetData>
   <autoFilter ref="A2:D73"/>
   <mergeCells count="26">
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="A69:A73"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A51:A59"/>
-    <mergeCell ref="A63:A64"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A74:A75"/>
     <mergeCell ref="A14:A15"/>
@@ -2223,6 +2213,16 @@
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="A44:A47"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="A69:A73"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A51:A59"/>
+    <mergeCell ref="A63:A64"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2250,17 +2250,17 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="28" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2268,17 +2268,17 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A3" s="25"/>
+      <c r="A3" s="29"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
@@ -2307,26 +2307,26 @@
     </row>
     <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
@@ -2353,10 +2353,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.375" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.625" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.625" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="26"/>
+    <col min="1" max="1" width="17.375" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.625" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.625" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
@@ -2364,27 +2364,27 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>203</v>
-      </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -2393,7 +2393,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -2405,30 +2405,30 @@
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="18" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="18" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="18" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
@@ -2443,7 +2443,7 @@
         <v>129</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -2452,25 +2452,25 @@
         <v>148</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="18" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="18" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C13" s="2"/>
     </row>
@@ -2480,7 +2480,7 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
@@ -2491,34 +2491,34 @@
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="18" t="s">
         <v>51</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="18" t="s">
         <v>151</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="18" t="s">
         <v>101</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="18" t="s">
         <v>56</v>
       </c>
       <c r="B19" s="2"/>
@@ -2536,7 +2536,7 @@
         <v>152</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C21" s="2"/>
     </row>
@@ -2555,38 +2555,38 @@
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="18" t="s">
         <v>61</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="18" t="s">
         <v>94</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="18" t="s">
         <v>62</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="18" t="s">
         <v>66</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C27" s="2"/>
     </row>
@@ -2598,47 +2598,47 @@
       <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="19" t="s">
         <v>124</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="19" t="s">
         <v>125</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A31" s="28" t="s">
+      <c r="A31" s="18" t="s">
         <v>69</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="18" t="s">
         <v>70</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="18" t="s">
         <v>121</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C33" s="2"/>
     </row>

</xml_diff>

<commit_message>
Update on 20250819 part 11
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -706,11 +706,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>xizang.php
-xztv.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>cdtv.php
 cdtv2.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -841,6 +836,11 @@
   </si>
   <si>
     <t>官网提供卫视,黑龙江省频道在线观看,可使用酷9JS脚本的Webview方式观看*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tibet.php
+TibetTV.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1031,23 +1031,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1397,7 +1397,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1406,30 +1406,30 @@
       <c r="C3" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="24" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="24"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="20"/>
+      <c r="D4" s="24"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="25"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="20" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1441,7 +1441,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="24"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1451,7 +1451,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="24"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1461,13 +1461,13 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="25"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="56.25" x14ac:dyDescent="0.15">
@@ -1478,7 +1478,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>20</v>
@@ -1493,7 +1493,7 @@
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="23" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1507,7 +1507,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="21"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="1" t="s">
         <v>119</v>
       </c>
@@ -1517,7 +1517,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="23" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1529,7 +1529,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="21"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1539,7 +1539,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="23" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1551,12 +1551,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="21"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>107</v>
@@ -1599,7 +1599,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="23" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1613,19 +1613,19 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="21"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="23" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1639,37 +1639,37 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="21"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>194</v>
-      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="21"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="24" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="21"/>
+      <c r="A26" s="23"/>
       <c r="B26" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="20"/>
+      <c r="D26" s="24"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="21"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="1" t="s">
         <v>42</v>
       </c>
@@ -1679,7 +1679,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="21"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="1" t="s">
         <v>44</v>
       </c>
@@ -1689,22 +1689,22 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="21"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="24" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="21"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="20"/>
+      <c r="D30" s="24"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="10" t="s">
@@ -1713,7 +1713,7 @@
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
@@ -1727,7 +1727,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="23" t="s">
         <v>51</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1741,7 +1741,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="21"/>
+      <c r="A34" s="23"/>
       <c r="B34" s="1" t="s">
         <v>54</v>
       </c>
@@ -1763,21 +1763,21 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="20" t="s">
         <v>101</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="25"/>
+      <c r="A37" s="22"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
         <v>138</v>
@@ -1787,7 +1787,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="21" t="s">
+      <c r="A38" s="23" t="s">
         <v>56</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1799,7 +1799,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="21"/>
+      <c r="A39" s="23"/>
       <c r="B39" s="1" t="s">
         <v>59</v>
       </c>
@@ -1853,7 +1853,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="21" t="s">
+      <c r="A44" s="23" t="s">
         <v>61</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -1862,20 +1862,20 @@
       <c r="C44" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D44" s="20" t="s">
+      <c r="D44" s="24" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="21"/>
+      <c r="A45" s="23"/>
       <c r="B45" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C45" s="1"/>
-      <c r="D45" s="20"/>
+      <c r="D45" s="24"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="21"/>
+      <c r="A46" s="23"/>
       <c r="B46" s="1" t="s">
         <v>90</v>
       </c>
@@ -1885,7 +1885,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="21"/>
+      <c r="A47" s="23"/>
       <c r="B47" s="1" t="s">
         <v>91</v>
       </c>
@@ -1895,31 +1895,31 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="21" t="s">
+      <c r="A48" s="23" t="s">
         <v>94</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>117</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="21"/>
+      <c r="A49" s="23"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>189</v>
-      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="21"/>
+      <c r="A50" s="23"/>
       <c r="B50" s="1" t="s">
         <v>95</v>
       </c>
@@ -1931,35 +1931,35 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="23" t="s">
+      <c r="A51" s="20" t="s">
         <v>62</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C51" s="1"/>
-      <c r="D51" s="20" t="s">
+      <c r="D51" s="24" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="24"/>
+      <c r="A52" s="21"/>
       <c r="B52" s="1" t="s">
         <v>97</v>
       </c>
       <c r="C52" s="1"/>
-      <c r="D52" s="20"/>
+      <c r="D52" s="24"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="24"/>
+      <c r="A53" s="21"/>
       <c r="B53" s="1" t="s">
         <v>116</v>
       </c>
       <c r="C53" s="1"/>
-      <c r="D53" s="20"/>
+      <c r="D53" s="24"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="24"/>
+      <c r="A54" s="21"/>
       <c r="B54" s="1" t="s">
         <v>98</v>
       </c>
@@ -1969,7 +1969,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="24"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="1" t="s">
         <v>100</v>
       </c>
@@ -1979,7 +1979,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="24"/>
+      <c r="A56" s="21"/>
       <c r="B56" s="1" t="s">
         <v>109</v>
       </c>
@@ -1989,7 +1989,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="24"/>
+      <c r="A57" s="21"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
         <v>140</v>
@@ -1999,7 +1999,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="24"/>
+      <c r="A58" s="21"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
         <v>141</v>
@@ -2009,7 +2009,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" s="25"/>
+      <c r="A59" s="22"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
         <v>142</v>
@@ -2019,7 +2019,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="21" t="s">
+      <c r="A60" s="23" t="s">
         <v>66</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -2031,12 +2031,12 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A61" s="21"/>
+      <c r="A61" s="23"/>
       <c r="B61" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>68</v>
@@ -2058,24 +2058,24 @@
         <v>108</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>175</v>
+        <v>208</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A64" s="27"/>
       <c r="B64" s="1"/>
       <c r="C64" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="22" t="s">
+      <c r="A65" s="25" t="s">
         <v>125</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -2089,7 +2089,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="22"/>
+      <c r="A66" s="25"/>
       <c r="B66" s="1" t="s">
         <v>111</v>
       </c>
@@ -2099,27 +2099,27 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="21" t="s">
+      <c r="A67" s="23" t="s">
         <v>69</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C67" s="1"/>
-      <c r="D67" s="20" t="s">
+      <c r="D67" s="24" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="21"/>
+      <c r="A68" s="23"/>
       <c r="B68" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C68" s="1"/>
-      <c r="D68" s="20"/>
+      <c r="D68" s="24"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="21" t="s">
+      <c r="A69" s="23" t="s">
         <v>70</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -2133,37 +2133,37 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="21"/>
+      <c r="A70" s="23"/>
       <c r="B70" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C70" s="1"/>
-      <c r="D70" s="20" t="s">
+      <c r="D70" s="24" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A71" s="21"/>
+      <c r="A71" s="23"/>
       <c r="B71" s="1" t="s">
         <v>79</v>
       </c>
       <c r="C71" s="1"/>
-      <c r="D71" s="20"/>
+      <c r="D71" s="24"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A72" s="21"/>
+      <c r="A72" s="23"/>
       <c r="B72" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A73" s="21"/>
+      <c r="A73" s="23"/>
       <c r="B73" s="1" t="s">
         <v>84</v>
       </c>
@@ -2173,7 +2173,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A74" s="21" t="s">
+      <c r="A74" s="23" t="s">
         <v>121</v>
       </c>
       <c r="B74" s="1" t="s">
@@ -2185,7 +2185,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A75" s="21"/>
+      <c r="A75" s="23"/>
       <c r="B75" s="1" t="s">
         <v>127</v>
       </c>
@@ -2197,6 +2197,16 @@
   </sheetData>
   <autoFilter ref="A2:D73"/>
   <mergeCells count="26">
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="A69:A73"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A51:A59"/>
+    <mergeCell ref="A63:A64"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A74:A75"/>
     <mergeCell ref="A14:A15"/>
@@ -2213,16 +2223,6 @@
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="A44:A47"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="A69:A73"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A51:A59"/>
-    <mergeCell ref="A63:A64"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2268,17 +2268,17 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A3" s="29"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
@@ -2307,26 +2307,26 @@
     </row>
     <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
@@ -2364,10 +2364,10 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -2375,7 +2375,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -2384,7 +2384,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -2393,7 +2393,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -2409,7 +2409,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -2418,7 +2418,7 @@
         <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -2428,7 +2428,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
@@ -2443,7 +2443,7 @@
         <v>129</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -2452,7 +2452,7 @@
         <v>148</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -2461,7 +2461,7 @@
         <v>34</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -2470,7 +2470,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C13" s="2"/>
     </row>
@@ -2480,7 +2480,7 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
@@ -2495,7 +2495,7 @@
         <v>51</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C16" s="2"/>
     </row>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
@@ -2513,7 +2513,7 @@
         <v>101</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C18" s="2"/>
     </row>
@@ -2536,7 +2536,7 @@
         <v>152</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C21" s="2"/>
     </row>
@@ -2559,7 +2559,7 @@
         <v>61</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C24" s="2"/>
     </row>
@@ -2568,7 +2568,7 @@
         <v>94</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C25" s="2"/>
     </row>
@@ -2577,7 +2577,7 @@
         <v>62</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C26" s="2"/>
     </row>
@@ -2586,7 +2586,7 @@
         <v>66</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C27" s="2"/>
     </row>
@@ -2602,7 +2602,7 @@
         <v>124</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C29" s="2"/>
     </row>
@@ -2611,7 +2611,7 @@
         <v>125</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C30" s="2"/>
     </row>
@@ -2620,7 +2620,7 @@
         <v>69</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C31" s="2"/>
     </row>
@@ -2629,7 +2629,7 @@
         <v>70</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C32" s="2"/>
     </row>
@@ -2638,7 +2638,7 @@
         <v>121</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C33" s="2"/>
     </row>

</xml_diff>

<commit_message>
Update on 20250820 part 4
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -839,8 +839,8 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Tibet.php
-TibetTV.php</t>
+    <t>xizang.php
+xztv.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1031,6 +1031,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1039,15 +1048,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1397,7 +1397,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1406,20 +1406,20 @@
       <c r="C3" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="20" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="21"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="24"/>
+      <c r="D4" s="20"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="22"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
         <v>176</v>
@@ -1429,7 +1429,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="23" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1441,7 +1441,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="21"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1451,7 +1451,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="21"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1461,7 +1461,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="22"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>195</v>
@@ -1493,7 +1493,7 @@
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="21" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1507,7 +1507,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="23"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="1" t="s">
         <v>119</v>
       </c>
@@ -1517,7 +1517,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="21" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1529,7 +1529,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="23"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1539,7 +1539,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="21" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1551,7 +1551,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="23"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="1" t="s">
         <v>31</v>
       </c>
@@ -1599,7 +1599,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="21" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1613,7 +1613,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="23"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="1" t="s">
         <v>49</v>
       </c>
@@ -1625,7 +1625,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="21" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1639,7 +1639,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="23"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
         <v>192</v>
@@ -1649,27 +1649,27 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="23"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="20" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="23"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="24"/>
+      <c r="D26" s="20"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="23"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="1" t="s">
         <v>42</v>
       </c>
@@ -1679,7 +1679,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="23"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="1" t="s">
         <v>44</v>
       </c>
@@ -1689,22 +1689,22 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="23"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="24" t="s">
+      <c r="D29" s="20" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="23"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="24"/>
+      <c r="D30" s="20"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="10" t="s">
@@ -1727,7 +1727,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="23" t="s">
+      <c r="A33" s="21" t="s">
         <v>51</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1741,7 +1741,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="23"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="1" t="s">
         <v>54</v>
       </c>
@@ -1763,7 +1763,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="23" t="s">
         <v>101</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1777,7 +1777,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="22"/>
+      <c r="A37" s="25"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
         <v>138</v>
@@ -1787,7 +1787,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="21" t="s">
         <v>56</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1799,7 +1799,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="23"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="1" t="s">
         <v>59</v>
       </c>
@@ -1853,7 +1853,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="21" t="s">
         <v>61</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -1862,20 +1862,20 @@
       <c r="C44" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D44" s="24" t="s">
+      <c r="D44" s="20" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="23"/>
+      <c r="A45" s="21"/>
       <c r="B45" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C45" s="1"/>
-      <c r="D45" s="24"/>
+      <c r="D45" s="20"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="23"/>
+      <c r="A46" s="21"/>
       <c r="B46" s="1" t="s">
         <v>90</v>
       </c>
@@ -1885,7 +1885,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="23"/>
+      <c r="A47" s="21"/>
       <c r="B47" s="1" t="s">
         <v>91</v>
       </c>
@@ -1895,7 +1895,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="21" t="s">
         <v>94</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -1909,7 +1909,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="23"/>
+      <c r="A49" s="21"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
         <v>187</v>
@@ -1919,7 +1919,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="23"/>
+      <c r="A50" s="21"/>
       <c r="B50" s="1" t="s">
         <v>95</v>
       </c>
@@ -1931,35 +1931,35 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="20" t="s">
+      <c r="A51" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C51" s="1"/>
-      <c r="D51" s="24" t="s">
+      <c r="D51" s="20" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="21"/>
+      <c r="A52" s="24"/>
       <c r="B52" s="1" t="s">
         <v>97</v>
       </c>
       <c r="C52" s="1"/>
-      <c r="D52" s="24"/>
+      <c r="D52" s="20"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="21"/>
+      <c r="A53" s="24"/>
       <c r="B53" s="1" t="s">
         <v>116</v>
       </c>
       <c r="C53" s="1"/>
-      <c r="D53" s="24"/>
+      <c r="D53" s="20"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="21"/>
+      <c r="A54" s="24"/>
       <c r="B54" s="1" t="s">
         <v>98</v>
       </c>
@@ -1969,7 +1969,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="21"/>
+      <c r="A55" s="24"/>
       <c r="B55" s="1" t="s">
         <v>100</v>
       </c>
@@ -1979,7 +1979,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="21"/>
+      <c r="A56" s="24"/>
       <c r="B56" s="1" t="s">
         <v>109</v>
       </c>
@@ -1989,7 +1989,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="21"/>
+      <c r="A57" s="24"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
         <v>140</v>
@@ -1999,7 +1999,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="21"/>
+      <c r="A58" s="24"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
         <v>141</v>
@@ -2009,7 +2009,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" s="22"/>
+      <c r="A59" s="25"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
         <v>142</v>
@@ -2019,7 +2019,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="23" t="s">
+      <c r="A60" s="21" t="s">
         <v>66</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -2031,7 +2031,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A61" s="23"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="1" t="s">
         <v>67</v>
       </c>
@@ -2075,7 +2075,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="25" t="s">
+      <c r="A65" s="22" t="s">
         <v>125</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -2089,7 +2089,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="25"/>
+      <c r="A66" s="22"/>
       <c r="B66" s="1" t="s">
         <v>111</v>
       </c>
@@ -2099,27 +2099,27 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="23" t="s">
+      <c r="A67" s="21" t="s">
         <v>69</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C67" s="1"/>
-      <c r="D67" s="24" t="s">
+      <c r="D67" s="20" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="23"/>
+      <c r="A68" s="21"/>
       <c r="B68" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C68" s="1"/>
-      <c r="D68" s="24"/>
+      <c r="D68" s="20"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="23" t="s">
+      <c r="A69" s="21" t="s">
         <v>70</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -2133,25 +2133,25 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="23"/>
+      <c r="A70" s="21"/>
       <c r="B70" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C70" s="1"/>
-      <c r="D70" s="24" t="s">
+      <c r="D70" s="20" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A71" s="23"/>
+      <c r="A71" s="21"/>
       <c r="B71" s="1" t="s">
         <v>79</v>
       </c>
       <c r="C71" s="1"/>
-      <c r="D71" s="24"/>
+      <c r="D71" s="20"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A72" s="23"/>
+      <c r="A72" s="21"/>
       <c r="B72" s="1" t="s">
         <v>80</v>
       </c>
@@ -2163,7 +2163,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A73" s="23"/>
+      <c r="A73" s="21"/>
       <c r="B73" s="1" t="s">
         <v>84</v>
       </c>
@@ -2173,7 +2173,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A74" s="23" t="s">
+      <c r="A74" s="21" t="s">
         <v>121</v>
       </c>
       <c r="B74" s="1" t="s">
@@ -2185,7 +2185,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A75" s="23"/>
+      <c r="A75" s="21"/>
       <c r="B75" s="1" t="s">
         <v>127</v>
       </c>
@@ -2197,16 +2197,6 @@
   </sheetData>
   <autoFilter ref="A2:D73"/>
   <mergeCells count="26">
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="A69:A73"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A51:A59"/>
-    <mergeCell ref="A63:A64"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A74:A75"/>
     <mergeCell ref="A14:A15"/>
@@ -2223,6 +2213,16 @@
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="A44:A47"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="A69:A73"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A51:A59"/>
+    <mergeCell ref="A63:A64"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 20250827 part 3
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -12,7 +12,7 @@
     <sheet name="省份统计" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他JS脚本!$A$1:$D$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他JS脚本!$A$1:$D$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">省份JS脚本!$A$2:$D$74</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">省份统计!$A$1:$C$33</definedName>
   </definedNames>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="215">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -52,14 +52,6 @@
   </si>
   <si>
     <t>平台</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>虎牙,斗鱼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>虎牙,斗鱼平台的直播间</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -857,6 +849,26 @@
   </si>
   <si>
     <t>卫视,辽宁省频道和辽宁地方频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>虎牙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>斗鱼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>虎牙平台直播间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>斗鱼平台直播间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>huya.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1047,23 +1059,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1395,684 +1407,684 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D1" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>13</v>
+        <v>131</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="24"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="20"/>
+      <c r="D4" s="24"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="25"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="23" t="s">
-        <v>10</v>
+      <c r="A6" s="20" t="s">
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="24"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="24"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="25"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="56.25" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="21"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="21" t="s">
-        <v>24</v>
+      <c r="A14" s="23" t="s">
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="21"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="75" x14ac:dyDescent="0.15">
+      <c r="A16" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="75" x14ac:dyDescent="0.15">
-      <c r="A16" s="21" t="s">
+      <c r="C16" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17" s="23"/>
+      <c r="B17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="21"/>
-      <c r="B17" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="C19" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A22" s="23"/>
+      <c r="B22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A23" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D21" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="21"/>
-      <c r="B22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="21" t="s">
+      <c r="C23" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="21"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="21"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A26" s="23"/>
+      <c r="B26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D25" s="20" t="s">
+      <c r="C26" s="1"/>
+      <c r="D26" s="24"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A27" s="23"/>
+      <c r="B27" s="1" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="21"/>
-      <c r="B26" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="20"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="21"/>
-      <c r="B27" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="21"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A29" s="23"/>
+      <c r="B29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A30" s="23"/>
+      <c r="B30" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="21"/>
-      <c r="B29" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="21"/>
-      <c r="B30" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="20"/>
+      <c r="D30" s="24"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="1" t="s">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A34" s="23"/>
+      <c r="B34" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="21"/>
-      <c r="B34" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>103</v>
-      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="25"/>
+      <c r="A37" s="21"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="21" t="s">
-        <v>56</v>
+      <c r="A38" s="23" t="s">
+        <v>54</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="21"/>
+      <c r="A39" s="23"/>
       <c r="B39" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="56.25" x14ac:dyDescent="0.15">
-      <c r="A40" s="23" t="s">
-        <v>85</v>
+      <c r="A40" s="20" t="s">
+        <v>83</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="25"/>
+      <c r="A41" s="21"/>
       <c r="B41" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="21" t="s">
+      <c r="A45" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="C45" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D45" s="20" t="s">
-        <v>64</v>
+        <v>169</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="21"/>
+      <c r="A46" s="23"/>
       <c r="B46" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C46" s="1"/>
-      <c r="D46" s="20"/>
+      <c r="D46" s="24"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="21"/>
+      <c r="A47" s="23"/>
       <c r="B47" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="21"/>
+      <c r="A48" s="23"/>
       <c r="B48" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="21" t="s">
-        <v>94</v>
+      <c r="A49" s="23" t="s">
+        <v>92</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="21"/>
+      <c r="A50" s="23"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="21"/>
+      <c r="A51" s="23"/>
       <c r="B51" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A52" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A53" s="22"/>
+      <c r="B53" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D51" s="1" t="s">
+      <c r="C53" s="1"/>
+      <c r="D53" s="24"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A54" s="22"/>
+      <c r="B54" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="24"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A55" s="22"/>
+      <c r="B55" s="1" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C52" s="1"/>
-      <c r="D52" s="20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="24"/>
-      <c r="B53" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C53" s="1"/>
-      <c r="D53" s="20"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="24"/>
-      <c r="B54" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C54" s="1"/>
-      <c r="D54" s="20"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="24"/>
-      <c r="B55" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="24"/>
+      <c r="A56" s="22"/>
       <c r="B56" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="24"/>
+      <c r="A57" s="22"/>
       <c r="B57" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="24"/>
+      <c r="A58" s="22"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" s="24"/>
+      <c r="A59" s="22"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="25"/>
+      <c r="A60" s="21"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="21" t="s">
-        <v>66</v>
+      <c r="A61" s="23" t="s">
+        <v>64</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A62" s="21"/>
+      <c r="A62" s="23"/>
       <c r="B62" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A63" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2080,151 +2092,162 @@
     </row>
     <row r="64" spans="1:4" ht="75" x14ac:dyDescent="0.15">
       <c r="A64" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A65" s="27"/>
       <c r="B65" s="1"/>
       <c r="C65" s="14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="22" t="s">
-        <v>125</v>
+      <c r="A66" s="25" t="s">
+        <v>123</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="22"/>
+      <c r="A67" s="25"/>
       <c r="B67" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="21" t="s">
-        <v>69</v>
+      <c r="A68" s="23" t="s">
+        <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C68" s="1"/>
+      <c r="D68" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="C68" s="1"/>
-      <c r="D68" s="20" t="s">
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A69" s="23"/>
+      <c r="B69" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C69" s="1"/>
+      <c r="D69" s="24"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A70" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="21"/>
-      <c r="B69" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C69" s="1"/>
-      <c r="D69" s="20"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B70" s="1" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A71" s="23"/>
+      <c r="B71" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D70" s="1" t="s">
+      <c r="C71" s="1"/>
+      <c r="D71" s="24" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A71" s="21"/>
-      <c r="B71" s="1" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A72" s="23"/>
+      <c r="B72" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C71" s="1"/>
-      <c r="D71" s="20" t="s">
+      <c r="C72" s="1"/>
+      <c r="D72" s="24"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A73" s="23"/>
+      <c r="B73" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A72" s="21"/>
-      <c r="B72" s="1" t="s">
+      <c r="C73" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C72" s="1"/>
-      <c r="D72" s="20"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A73" s="21"/>
-      <c r="B73" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A74" s="21"/>
+      <c r="A74" s="23"/>
       <c r="B74" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A75" s="21" t="s">
-        <v>121</v>
+      <c r="A75" s="23" t="s">
+        <v>119</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A76" s="21"/>
+      <c r="A76" s="23"/>
       <c r="B76" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:D74"/>
   <mergeCells count="27">
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="A70:A74"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="A52:A60"/>
+    <mergeCell ref="A64:A65"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A75:A76"/>
@@ -2241,17 +2264,6 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="D45:D46"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="A70:A74"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="D52:D54"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="A52:A60"/>
-    <mergeCell ref="A64:A65"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2261,7 +2273,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2279,10 +2291,10 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -2297,74 +2309,88 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A3" s="29"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>8</v>
+        <v>210</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>214</v>
+      </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>104</v>
+        <v>211</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>106</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>105</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
-        <v>178</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>179</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="D10" s="12" t="s">
-        <v>132</v>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
+      <c r="A8" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
+      <c r="D11" s="12" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D5"/>
+  <autoFilter ref="A1:D6"/>
   <mergeCells count="1">
     <mergeCell ref="A2:A3"/>
   </mergeCells>
@@ -2390,13 +2416,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -2404,272 +2430,272 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C33" s="2"/>
     </row>

</xml_diff>

<commit_message>
Update on 20250827 part 4
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="216">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -869,6 +869,10 @@
   </si>
   <si>
     <t>huya.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>douyu.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1059,23 +1063,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1425,7 +1429,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1434,20 +1438,20 @@
       <c r="C3" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="21" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="22"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="24"/>
+      <c r="D4" s="21"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="21"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
         <v>174</v>
@@ -1457,7 +1461,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1469,7 +1473,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="22"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1479,7 +1483,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="22"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1489,7 +1493,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="21"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>193</v>
@@ -1521,7 +1525,7 @@
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1535,7 +1539,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="23"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="1" t="s">
         <v>117</v>
       </c>
@@ -1545,7 +1549,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="20" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1557,7 +1561,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="23"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
@@ -1567,7 +1571,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="75" x14ac:dyDescent="0.15">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="20" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1581,7 +1585,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="23"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="1" t="s">
         <v>29</v>
       </c>
@@ -1629,7 +1633,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="20" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1643,7 +1647,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="23"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="1" t="s">
         <v>47</v>
       </c>
@@ -1655,7 +1659,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1669,7 +1673,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="23"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
         <v>190</v>
@@ -1679,27 +1683,27 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="23"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="21" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="23"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="24"/>
+      <c r="D26" s="21"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="23"/>
+      <c r="A27" s="20"/>
       <c r="B27" s="1" t="s">
         <v>40</v>
       </c>
@@ -1709,7 +1713,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="23"/>
+      <c r="A28" s="20"/>
       <c r="B28" s="1" t="s">
         <v>42</v>
       </c>
@@ -1719,22 +1723,22 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="23"/>
+      <c r="A29" s="20"/>
       <c r="B29" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="24" t="s">
+      <c r="D29" s="21" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="23"/>
+      <c r="A30" s="20"/>
       <c r="B30" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="24"/>
+      <c r="D30" s="21"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="10" t="s">
@@ -1757,7 +1761,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="23" t="s">
+      <c r="A33" s="20" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1771,7 +1775,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="23"/>
+      <c r="A34" s="20"/>
       <c r="B34" s="1" t="s">
         <v>52</v>
       </c>
@@ -1793,7 +1797,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="23" t="s">
         <v>99</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1807,7 +1811,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="21"/>
+      <c r="A37" s="25"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
         <v>136</v>
@@ -1817,7 +1821,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1829,7 +1833,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="23"/>
+      <c r="A39" s="20"/>
       <c r="B39" s="1" t="s">
         <v>57</v>
       </c>
@@ -1839,7 +1843,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="56.25" x14ac:dyDescent="0.15">
-      <c r="A40" s="20" t="s">
+      <c r="A40" s="23" t="s">
         <v>83</v>
       </c>
       <c r="B40" s="1"/>
@@ -1851,7 +1855,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="21"/>
+      <c r="A41" s="25"/>
       <c r="B41" s="1" t="s">
         <v>84</v>
       </c>
@@ -1893,7 +1897,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="20" t="s">
         <v>59</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1902,20 +1906,20 @@
       <c r="C45" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D45" s="24" t="s">
+      <c r="D45" s="21" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="23"/>
+      <c r="A46" s="20"/>
       <c r="B46" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C46" s="1"/>
-      <c r="D46" s="24"/>
+      <c r="D46" s="21"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="23"/>
+      <c r="A47" s="20"/>
       <c r="B47" s="1" t="s">
         <v>88</v>
       </c>
@@ -1925,7 +1929,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="23"/>
+      <c r="A48" s="20"/>
       <c r="B48" s="1" t="s">
         <v>89</v>
       </c>
@@ -1935,7 +1939,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="23" t="s">
+      <c r="A49" s="20" t="s">
         <v>92</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -1949,7 +1953,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="23"/>
+      <c r="A50" s="20"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
         <v>185</v>
@@ -1959,7 +1963,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="23"/>
+      <c r="A51" s="20"/>
       <c r="B51" s="1" t="s">
         <v>93</v>
       </c>
@@ -1971,35 +1975,35 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="20" t="s">
+      <c r="A52" s="23" t="s">
         <v>60</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C52" s="1"/>
-      <c r="D52" s="24" t="s">
+      <c r="D52" s="21" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="22"/>
+      <c r="A53" s="24"/>
       <c r="B53" s="1" t="s">
         <v>95</v>
       </c>
       <c r="C53" s="1"/>
-      <c r="D53" s="24"/>
+      <c r="D53" s="21"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="22"/>
+      <c r="A54" s="24"/>
       <c r="B54" s="1" t="s">
         <v>114</v>
       </c>
       <c r="C54" s="1"/>
-      <c r="D54" s="24"/>
+      <c r="D54" s="21"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="22"/>
+      <c r="A55" s="24"/>
       <c r="B55" s="1" t="s">
         <v>96</v>
       </c>
@@ -2009,7 +2013,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="22"/>
+      <c r="A56" s="24"/>
       <c r="B56" s="1" t="s">
         <v>98</v>
       </c>
@@ -2019,7 +2023,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="22"/>
+      <c r="A57" s="24"/>
       <c r="B57" s="1" t="s">
         <v>107</v>
       </c>
@@ -2029,7 +2033,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="22"/>
+      <c r="A58" s="24"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
         <v>138</v>
@@ -2039,7 +2043,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" s="22"/>
+      <c r="A59" s="24"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
         <v>139</v>
@@ -2049,7 +2053,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="21"/>
+      <c r="A60" s="25"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1" t="s">
         <v>140</v>
@@ -2059,7 +2063,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="23" t="s">
+      <c r="A61" s="20" t="s">
         <v>64</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -2071,7 +2075,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A62" s="23"/>
+      <c r="A62" s="20"/>
       <c r="B62" s="1" t="s">
         <v>65</v>
       </c>
@@ -2115,7 +2119,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="25" t="s">
+      <c r="A66" s="22" t="s">
         <v>123</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -2129,7 +2133,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="25"/>
+      <c r="A67" s="22"/>
       <c r="B67" s="1" t="s">
         <v>109</v>
       </c>
@@ -2139,27 +2143,27 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="23" t="s">
+      <c r="A68" s="20" t="s">
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C68" s="1"/>
-      <c r="D68" s="24" t="s">
+      <c r="D68" s="21" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="23"/>
+      <c r="A69" s="20"/>
       <c r="B69" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C69" s="1"/>
-      <c r="D69" s="24"/>
+      <c r="D69" s="21"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="23" t="s">
+      <c r="A70" s="20" t="s">
         <v>68</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -2173,25 +2177,25 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A71" s="23"/>
+      <c r="A71" s="20"/>
       <c r="B71" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C71" s="1"/>
-      <c r="D71" s="24" t="s">
+      <c r="D71" s="21" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A72" s="23"/>
+      <c r="A72" s="20"/>
       <c r="B72" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C72" s="1"/>
-      <c r="D72" s="24"/>
+      <c r="D72" s="21"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A73" s="23"/>
+      <c r="A73" s="20"/>
       <c r="B73" s="1" t="s">
         <v>78</v>
       </c>
@@ -2203,7 +2207,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A74" s="23"/>
+      <c r="A74" s="20"/>
       <c r="B74" s="1" t="s">
         <v>82</v>
       </c>
@@ -2213,7 +2217,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A75" s="23" t="s">
+      <c r="A75" s="20" t="s">
         <v>119</v>
       </c>
       <c r="B75" s="1" t="s">
@@ -2225,7 +2229,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A76" s="23"/>
+      <c r="A76" s="20"/>
       <c r="B76" s="1" t="s">
         <v>125</v>
       </c>
@@ -2237,17 +2241,6 @@
   </sheetData>
   <autoFilter ref="A2:D74"/>
   <mergeCells count="27">
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="A70:A74"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="D52:D54"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="A52:A60"/>
-    <mergeCell ref="A64:A65"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A75:A76"/>
@@ -2264,6 +2257,17 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="D45:D46"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="A70:A74"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="A52:A60"/>
+    <mergeCell ref="A64:A65"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2343,7 +2347,9 @@
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>215</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>213</v>
       </c>

</xml_diff>

<commit_message>
Update on 20250827 part 10
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="219">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -860,19 +860,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>虎牙平台直播间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>斗鱼平台直播间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>huya.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>douyu.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>哔哩哔哩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bilibili.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>虎牙直播间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>斗鱼直播间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B站哔哩哔哩直播间</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1063,6 +1075,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1071,15 +1092,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1429,7 +1441,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1438,20 +1450,20 @@
       <c r="C3" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="24" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="24"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="21"/>
+      <c r="D4" s="24"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="25"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
         <v>174</v>
@@ -1461,7 +1473,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1473,7 +1485,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="24"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1483,7 +1495,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="24"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1493,7 +1505,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="25"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>193</v>
@@ -1525,7 +1537,7 @@
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1539,7 +1551,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="20"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="1" t="s">
         <v>117</v>
       </c>
@@ -1549,7 +1561,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="23" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1561,7 +1573,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="20"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
@@ -1571,7 +1583,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="75" x14ac:dyDescent="0.15">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="23" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1585,7 +1597,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="20"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="1" t="s">
         <v>29</v>
       </c>
@@ -1633,7 +1645,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="23" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1647,7 +1659,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="20"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="1" t="s">
         <v>47</v>
       </c>
@@ -1659,7 +1671,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="23" t="s">
         <v>34</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1673,7 +1685,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="20"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
         <v>190</v>
@@ -1683,27 +1695,27 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="20"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="D25" s="24" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="20"/>
+      <c r="A26" s="23"/>
       <c r="B26" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="21"/>
+      <c r="D26" s="24"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="20"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="1" t="s">
         <v>40</v>
       </c>
@@ -1713,7 +1725,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="20"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="1" t="s">
         <v>42</v>
       </c>
@@ -1723,22 +1735,22 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="20"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="21" t="s">
+      <c r="D29" s="24" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="20"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="21"/>
+      <c r="D30" s="24"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="10" t="s">
@@ -1761,7 +1773,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="23" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1775,7 +1787,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="20"/>
+      <c r="A34" s="23"/>
       <c r="B34" s="1" t="s">
         <v>52</v>
       </c>
@@ -1797,7 +1809,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="20" t="s">
         <v>99</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1811,7 +1823,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="25"/>
+      <c r="A37" s="21"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
         <v>136</v>
@@ -1821,7 +1833,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="20" t="s">
+      <c r="A38" s="23" t="s">
         <v>54</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1833,7 +1845,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="20"/>
+      <c r="A39" s="23"/>
       <c r="B39" s="1" t="s">
         <v>57</v>
       </c>
@@ -1843,7 +1855,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="56.25" x14ac:dyDescent="0.15">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="20" t="s">
         <v>83</v>
       </c>
       <c r="B40" s="1"/>
@@ -1855,7 +1867,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="25"/>
+      <c r="A41" s="21"/>
       <c r="B41" s="1" t="s">
         <v>84</v>
       </c>
@@ -1897,7 +1909,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="20" t="s">
+      <c r="A45" s="23" t="s">
         <v>59</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1906,20 +1918,20 @@
       <c r="C45" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D45" s="21" t="s">
+      <c r="D45" s="24" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="20"/>
+      <c r="A46" s="23"/>
       <c r="B46" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C46" s="1"/>
-      <c r="D46" s="21"/>
+      <c r="D46" s="24"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="20"/>
+      <c r="A47" s="23"/>
       <c r="B47" s="1" t="s">
         <v>88</v>
       </c>
@@ -1929,7 +1941,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="20"/>
+      <c r="A48" s="23"/>
       <c r="B48" s="1" t="s">
         <v>89</v>
       </c>
@@ -1939,7 +1951,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="20" t="s">
+      <c r="A49" s="23" t="s">
         <v>92</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -1953,7 +1965,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="20"/>
+      <c r="A50" s="23"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
         <v>185</v>
@@ -1963,7 +1975,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="20"/>
+      <c r="A51" s="23"/>
       <c r="B51" s="1" t="s">
         <v>93</v>
       </c>
@@ -1975,35 +1987,35 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="23" t="s">
+      <c r="A52" s="20" t="s">
         <v>60</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C52" s="1"/>
-      <c r="D52" s="21" t="s">
+      <c r="D52" s="24" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="24"/>
+      <c r="A53" s="22"/>
       <c r="B53" s="1" t="s">
         <v>95</v>
       </c>
       <c r="C53" s="1"/>
-      <c r="D53" s="21"/>
+      <c r="D53" s="24"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="24"/>
+      <c r="A54" s="22"/>
       <c r="B54" s="1" t="s">
         <v>114</v>
       </c>
       <c r="C54" s="1"/>
-      <c r="D54" s="21"/>
+      <c r="D54" s="24"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="24"/>
+      <c r="A55" s="22"/>
       <c r="B55" s="1" t="s">
         <v>96</v>
       </c>
@@ -2013,7 +2025,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="24"/>
+      <c r="A56" s="22"/>
       <c r="B56" s="1" t="s">
         <v>98</v>
       </c>
@@ -2023,7 +2035,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="24"/>
+      <c r="A57" s="22"/>
       <c r="B57" s="1" t="s">
         <v>107</v>
       </c>
@@ -2033,7 +2045,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="24"/>
+      <c r="A58" s="22"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
         <v>138</v>
@@ -2043,7 +2055,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" s="24"/>
+      <c r="A59" s="22"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
         <v>139</v>
@@ -2053,7 +2065,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="25"/>
+      <c r="A60" s="21"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1" t="s">
         <v>140</v>
@@ -2063,7 +2075,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="20" t="s">
+      <c r="A61" s="23" t="s">
         <v>64</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -2075,7 +2087,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A62" s="20"/>
+      <c r="A62" s="23"/>
       <c r="B62" s="1" t="s">
         <v>65</v>
       </c>
@@ -2119,7 +2131,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="22" t="s">
+      <c r="A66" s="25" t="s">
         <v>123</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -2133,7 +2145,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="22"/>
+      <c r="A67" s="25"/>
       <c r="B67" s="1" t="s">
         <v>109</v>
       </c>
@@ -2143,27 +2155,27 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="20" t="s">
+      <c r="A68" s="23" t="s">
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C68" s="1"/>
-      <c r="D68" s="21" t="s">
+      <c r="D68" s="24" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="20"/>
+      <c r="A69" s="23"/>
       <c r="B69" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C69" s="1"/>
-      <c r="D69" s="21"/>
+      <c r="D69" s="24"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="20" t="s">
+      <c r="A70" s="23" t="s">
         <v>68</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -2177,25 +2189,25 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A71" s="20"/>
+      <c r="A71" s="23"/>
       <c r="B71" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C71" s="1"/>
-      <c r="D71" s="21" t="s">
+      <c r="D71" s="24" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A72" s="20"/>
+      <c r="A72" s="23"/>
       <c r="B72" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C72" s="1"/>
-      <c r="D72" s="21"/>
+      <c r="D72" s="24"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A73" s="20"/>
+      <c r="A73" s="23"/>
       <c r="B73" s="1" t="s">
         <v>78</v>
       </c>
@@ -2207,7 +2219,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A74" s="20"/>
+      <c r="A74" s="23"/>
       <c r="B74" s="1" t="s">
         <v>82</v>
       </c>
@@ -2217,7 +2229,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A75" s="20" t="s">
+      <c r="A75" s="23" t="s">
         <v>119</v>
       </c>
       <c r="B75" s="1" t="s">
@@ -2229,7 +2241,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A76" s="20"/>
+      <c r="A76" s="23"/>
       <c r="B76" s="1" t="s">
         <v>125</v>
       </c>
@@ -2241,6 +2253,17 @@
   </sheetData>
   <autoFilter ref="A2:D74"/>
   <mergeCells count="27">
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="A70:A74"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="A52:A60"/>
+    <mergeCell ref="A64:A65"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A75:A76"/>
@@ -2257,17 +2280,6 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="D45:D46"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="A70:A74"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="D52:D54"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="A52:A60"/>
-    <mergeCell ref="A64:A65"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2277,7 +2289,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2334,10 +2346,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
@@ -2348,10 +2360,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
@@ -2368,30 +2380,42 @@
     </row>
     <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>175</v>
+        <v>214</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>176</v>
+        <v>215</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>177</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
+      <c r="A9" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="D11" s="12" t="s">
+    <row r="12" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
+      <c r="D12" s="12" t="s">
         <v>130</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update on 20250827 part 11
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="222">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -885,6 +885,18 @@
   </si>
   <si>
     <t>B站哔哩哔哩直播间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抖音</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>doyin.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抖音直播间</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1075,23 +1087,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1441,7 +1453,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1450,20 +1462,20 @@
       <c r="C3" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="21" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="22"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="24"/>
+      <c r="D4" s="21"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="21"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
         <v>174</v>
@@ -1473,7 +1485,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1485,7 +1497,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="22"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1495,7 +1507,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="22"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1505,7 +1517,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="21"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>193</v>
@@ -1537,7 +1549,7 @@
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1551,7 +1563,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="23"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="1" t="s">
         <v>117</v>
       </c>
@@ -1561,7 +1573,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="20" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1573,7 +1585,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="23"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
@@ -1583,7 +1595,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="75" x14ac:dyDescent="0.15">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="20" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1597,7 +1609,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="23"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="1" t="s">
         <v>29</v>
       </c>
@@ -1645,7 +1657,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="20" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1659,7 +1671,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="23"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="1" t="s">
         <v>47</v>
       </c>
@@ -1671,7 +1683,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1685,7 +1697,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="23"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
         <v>190</v>
@@ -1695,27 +1707,27 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="23"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="21" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="23"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="24"/>
+      <c r="D26" s="21"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="23"/>
+      <c r="A27" s="20"/>
       <c r="B27" s="1" t="s">
         <v>40</v>
       </c>
@@ -1725,7 +1737,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="23"/>
+      <c r="A28" s="20"/>
       <c r="B28" s="1" t="s">
         <v>42</v>
       </c>
@@ -1735,22 +1747,22 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="23"/>
+      <c r="A29" s="20"/>
       <c r="B29" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="24" t="s">
+      <c r="D29" s="21" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="23"/>
+      <c r="A30" s="20"/>
       <c r="B30" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="24"/>
+      <c r="D30" s="21"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="10" t="s">
@@ -1773,7 +1785,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="23" t="s">
+      <c r="A33" s="20" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1787,7 +1799,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="23"/>
+      <c r="A34" s="20"/>
       <c r="B34" s="1" t="s">
         <v>52</v>
       </c>
@@ -1809,7 +1821,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="23" t="s">
         <v>99</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1823,7 +1835,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="21"/>
+      <c r="A37" s="25"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
         <v>136</v>
@@ -1833,7 +1845,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1845,7 +1857,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="23"/>
+      <c r="A39" s="20"/>
       <c r="B39" s="1" t="s">
         <v>57</v>
       </c>
@@ -1855,7 +1867,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="56.25" x14ac:dyDescent="0.15">
-      <c r="A40" s="20" t="s">
+      <c r="A40" s="23" t="s">
         <v>83</v>
       </c>
       <c r="B40" s="1"/>
@@ -1867,7 +1879,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="21"/>
+      <c r="A41" s="25"/>
       <c r="B41" s="1" t="s">
         <v>84</v>
       </c>
@@ -1909,7 +1921,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="20" t="s">
         <v>59</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1918,20 +1930,20 @@
       <c r="C45" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D45" s="24" t="s">
+      <c r="D45" s="21" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="23"/>
+      <c r="A46" s="20"/>
       <c r="B46" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C46" s="1"/>
-      <c r="D46" s="24"/>
+      <c r="D46" s="21"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="23"/>
+      <c r="A47" s="20"/>
       <c r="B47" s="1" t="s">
         <v>88</v>
       </c>
@@ -1941,7 +1953,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="23"/>
+      <c r="A48" s="20"/>
       <c r="B48" s="1" t="s">
         <v>89</v>
       </c>
@@ -1951,7 +1963,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="23" t="s">
+      <c r="A49" s="20" t="s">
         <v>92</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -1965,7 +1977,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="23"/>
+      <c r="A50" s="20"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
         <v>185</v>
@@ -1975,7 +1987,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="23"/>
+      <c r="A51" s="20"/>
       <c r="B51" s="1" t="s">
         <v>93</v>
       </c>
@@ -1987,35 +1999,35 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="20" t="s">
+      <c r="A52" s="23" t="s">
         <v>60</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C52" s="1"/>
-      <c r="D52" s="24" t="s">
+      <c r="D52" s="21" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="22"/>
+      <c r="A53" s="24"/>
       <c r="B53" s="1" t="s">
         <v>95</v>
       </c>
       <c r="C53" s="1"/>
-      <c r="D53" s="24"/>
+      <c r="D53" s="21"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="22"/>
+      <c r="A54" s="24"/>
       <c r="B54" s="1" t="s">
         <v>114</v>
       </c>
       <c r="C54" s="1"/>
-      <c r="D54" s="24"/>
+      <c r="D54" s="21"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="22"/>
+      <c r="A55" s="24"/>
       <c r="B55" s="1" t="s">
         <v>96</v>
       </c>
@@ -2025,7 +2037,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="22"/>
+      <c r="A56" s="24"/>
       <c r="B56" s="1" t="s">
         <v>98</v>
       </c>
@@ -2035,7 +2047,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="22"/>
+      <c r="A57" s="24"/>
       <c r="B57" s="1" t="s">
         <v>107</v>
       </c>
@@ -2045,7 +2057,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="22"/>
+      <c r="A58" s="24"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
         <v>138</v>
@@ -2055,7 +2067,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" s="22"/>
+      <c r="A59" s="24"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
         <v>139</v>
@@ -2065,7 +2077,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="21"/>
+      <c r="A60" s="25"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1" t="s">
         <v>140</v>
@@ -2075,7 +2087,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="23" t="s">
+      <c r="A61" s="20" t="s">
         <v>64</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -2087,7 +2099,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A62" s="23"/>
+      <c r="A62" s="20"/>
       <c r="B62" s="1" t="s">
         <v>65</v>
       </c>
@@ -2131,7 +2143,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="25" t="s">
+      <c r="A66" s="22" t="s">
         <v>123</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -2145,7 +2157,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="25"/>
+      <c r="A67" s="22"/>
       <c r="B67" s="1" t="s">
         <v>109</v>
       </c>
@@ -2155,27 +2167,27 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="23" t="s">
+      <c r="A68" s="20" t="s">
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C68" s="1"/>
-      <c r="D68" s="24" t="s">
+      <c r="D68" s="21" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="23"/>
+      <c r="A69" s="20"/>
       <c r="B69" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C69" s="1"/>
-      <c r="D69" s="24"/>
+      <c r="D69" s="21"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="23" t="s">
+      <c r="A70" s="20" t="s">
         <v>68</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -2189,25 +2201,25 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A71" s="23"/>
+      <c r="A71" s="20"/>
       <c r="B71" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C71" s="1"/>
-      <c r="D71" s="24" t="s">
+      <c r="D71" s="21" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A72" s="23"/>
+      <c r="A72" s="20"/>
       <c r="B72" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C72" s="1"/>
-      <c r="D72" s="24"/>
+      <c r="D72" s="21"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A73" s="23"/>
+      <c r="A73" s="20"/>
       <c r="B73" s="1" t="s">
         <v>78</v>
       </c>
@@ -2219,7 +2231,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A74" s="23"/>
+      <c r="A74" s="20"/>
       <c r="B74" s="1" t="s">
         <v>82</v>
       </c>
@@ -2229,7 +2241,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A75" s="23" t="s">
+      <c r="A75" s="20" t="s">
         <v>119</v>
       </c>
       <c r="B75" s="1" t="s">
@@ -2241,7 +2253,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A76" s="23"/>
+      <c r="A76" s="20"/>
       <c r="B76" s="1" t="s">
         <v>125</v>
       </c>
@@ -2253,17 +2265,6 @@
   </sheetData>
   <autoFilter ref="A2:D74"/>
   <mergeCells count="27">
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="A70:A74"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="D52:D54"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="A52:A60"/>
-    <mergeCell ref="A64:A65"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A75:A76"/>
@@ -2280,6 +2281,17 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="D45:D46"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="A70:A74"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="A52:A60"/>
+    <mergeCell ref="A64:A65"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2289,7 +2301,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2392,30 +2404,42 @@
     </row>
     <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>175</v>
+        <v>219</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>176</v>
+        <v>220</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>177</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
+      <c r="A10" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="D12" s="12" t="s">
+    <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
+      <c r="D13" s="12" t="s">
         <v>130</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update on 20250828 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="225">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -630,23 +630,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>官网提供卫视,宁夏自治区频道在线观看,可使用酷9JS脚本的Webview方式观看*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>官网提供卫视,青海省频道在线观看,可使用酷9JS脚本的Webview方式观看*</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>hunan.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>酷9JS脚本名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PHP脚本名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -720,10 +708,6 @@
   </si>
   <si>
     <t>jzb.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>由博彩网站提供的央视,卫视的频道直播源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -889,11 +873,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ningxia.php
-(仅中国大陆可访问)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>hangzhou.php
 (仅中国大陆可访问)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -907,6 +886,22 @@
   <si>
     <t>Shanghai_setv.php
 (仅中国大陆可访问)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>酷9JS脚本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PHP脚本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ningxia.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>由伟大合法的菠菜平台提供的央视,卫视的频道直播源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1105,6 +1100,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1113,15 +1117,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1461,17 +1456,17 @@
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1480,30 +1475,30 @@
       <c r="C3" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="24" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="24"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="21"/>
+      <c r="D4" s="24"/>
     </row>
     <row r="5" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A5" s="25"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1515,7 +1510,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="24"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1525,7 +1520,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="24"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1535,13 +1530,13 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="25"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="56.25" x14ac:dyDescent="0.15">
@@ -1552,7 +1547,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>18</v>
@@ -1567,21 +1562,21 @@
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="20"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="1" t="s">
         <v>117</v>
       </c>
@@ -1591,7 +1586,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="23" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1603,7 +1598,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="20"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
@@ -1613,26 +1608,26 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="56.25" x14ac:dyDescent="0.15">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="23" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="20"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>105</v>
@@ -1656,7 +1651,7 @@
         <v>129</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>128</v>
@@ -1668,14 +1663,14 @@
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="23" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1689,19 +1684,19 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="20"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="23" t="s">
         <v>34</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1715,37 +1710,37 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="20"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="20"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D25" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="D25" s="24" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="20"/>
+      <c r="A26" s="23"/>
       <c r="B26" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="21"/>
+      <c r="D26" s="24"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="20"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="1" t="s">
         <v>40</v>
       </c>
@@ -1755,7 +1750,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="20"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="1" t="s">
         <v>42</v>
       </c>
@@ -1765,22 +1760,22 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="20"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="21" t="s">
+      <c r="D29" s="24" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="20"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="21"/>
+      <c r="D30" s="24"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="10" t="s">
@@ -1789,7 +1784,7 @@
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="13" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
@@ -1803,21 +1798,21 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="23" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="20"/>
+      <c r="A34" s="23"/>
       <c r="B34" s="1" t="s">
         <v>52</v>
       </c>
@@ -1832,28 +1827,28 @@
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="20" t="s">
         <v>99</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>100</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="25"/>
+      <c r="A37" s="21"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
         <v>136</v>
@@ -1863,7 +1858,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="20" t="s">
+      <c r="A38" s="23" t="s">
         <v>54</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1875,7 +1870,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="20"/>
+      <c r="A39" s="23"/>
       <c r="B39" s="1" t="s">
         <v>57</v>
       </c>
@@ -1885,19 +1880,19 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="20" t="s">
         <v>83</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="14" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="25"/>
+      <c r="A41" s="21"/>
       <c r="B41" s="1" t="s">
         <v>84</v>
       </c>
@@ -1912,23 +1907,21 @@
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" s="10" t="s">
         <v>151</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="14" t="s">
-        <v>220</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>156</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="D43" s="13"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" s="10" t="s">
@@ -1937,33 +1930,33 @@
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="20" t="s">
+      <c r="A45" s="23" t="s">
         <v>59</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D45" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="D45" s="24" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="20"/>
+      <c r="A46" s="23"/>
       <c r="B46" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C46" s="1"/>
-      <c r="D46" s="21"/>
+      <c r="D46" s="24"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="20"/>
+      <c r="A47" s="23"/>
       <c r="B47" s="1" t="s">
         <v>88</v>
       </c>
@@ -1973,7 +1966,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="20"/>
+      <c r="A48" s="23"/>
       <c r="B48" s="1" t="s">
         <v>89</v>
       </c>
@@ -1983,71 +1976,71 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="20" t="s">
+      <c r="A49" s="23" t="s">
         <v>92</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="20"/>
+      <c r="A50" s="23"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="20"/>
+      <c r="A51" s="23"/>
       <c r="B51" s="1" t="s">
         <v>93</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="23" t="s">
+      <c r="A52" s="20" t="s">
         <v>60</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C52" s="1"/>
-      <c r="D52" s="21" t="s">
+      <c r="D52" s="24" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="24"/>
+      <c r="A53" s="22"/>
       <c r="B53" s="1" t="s">
         <v>95</v>
       </c>
       <c r="C53" s="1"/>
-      <c r="D53" s="21"/>
+      <c r="D53" s="24"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="24"/>
+      <c r="A54" s="22"/>
       <c r="B54" s="1" t="s">
         <v>114</v>
       </c>
       <c r="C54" s="1"/>
-      <c r="D54" s="21"/>
+      <c r="D54" s="24"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="24"/>
+      <c r="A55" s="22"/>
       <c r="B55" s="1" t="s">
         <v>96</v>
       </c>
@@ -2057,7 +2050,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="24"/>
+      <c r="A56" s="22"/>
       <c r="B56" s="1" t="s">
         <v>98</v>
       </c>
@@ -2067,7 +2060,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="24"/>
+      <c r="A57" s="22"/>
       <c r="B57" s="1" t="s">
         <v>107</v>
       </c>
@@ -2077,7 +2070,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="24"/>
+      <c r="A58" s="22"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
         <v>138</v>
@@ -2087,7 +2080,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" s="24"/>
+      <c r="A59" s="22"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
         <v>139</v>
@@ -2097,7 +2090,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="25"/>
+      <c r="A60" s="21"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1" t="s">
         <v>140</v>
@@ -2107,7 +2100,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="20" t="s">
+      <c r="A61" s="23" t="s">
         <v>64</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -2119,12 +2112,12 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A62" s="20"/>
+      <c r="A62" s="23"/>
       <c r="B62" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>66</v>
@@ -2146,24 +2139,24 @@
         <v>106</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A65" s="27"/>
       <c r="B65" s="1"/>
       <c r="C65" s="14" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="22" t="s">
+      <c r="A66" s="25" t="s">
         <v>123</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -2177,7 +2170,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="22"/>
+      <c r="A67" s="25"/>
       <c r="B67" s="1" t="s">
         <v>109</v>
       </c>
@@ -2187,73 +2180,73 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="20" t="s">
+      <c r="A68" s="23" t="s">
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C68" s="1"/>
-      <c r="D68" s="21" t="s">
+      <c r="D68" s="24" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="20"/>
+      <c r="A69" s="23"/>
       <c r="B69" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C69" s="1"/>
-      <c r="D69" s="21"/>
+      <c r="D69" s="24"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="20" t="s">
+      <c r="A70" s="23" t="s">
         <v>68</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A71" s="20"/>
+      <c r="A71" s="23"/>
       <c r="B71" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>221</v>
-      </c>
-      <c r="D71" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="D71" s="24" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A72" s="20"/>
+      <c r="A72" s="23"/>
       <c r="B72" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C72" s="1"/>
-      <c r="D72" s="21"/>
+      <c r="D72" s="24"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A73" s="20"/>
+      <c r="A73" s="23"/>
       <c r="B73" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A74" s="20"/>
+      <c r="A74" s="23"/>
       <c r="B74" s="1" t="s">
         <v>82</v>
       </c>
@@ -2263,7 +2256,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A75" s="20" t="s">
+      <c r="A75" s="23" t="s">
         <v>119</v>
       </c>
       <c r="B75" s="1" t="s">
@@ -2275,7 +2268,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A76" s="20"/>
+      <c r="A76" s="23"/>
       <c r="B76" s="1" t="s">
         <v>125</v>
       </c>
@@ -2287,6 +2280,17 @@
   </sheetData>
   <autoFilter ref="A2:D74"/>
   <mergeCells count="27">
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="A70:A74"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="A52:A60"/>
+    <mergeCell ref="A64:A65"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A75:A76"/>
@@ -2303,17 +2307,6 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="D45:D46"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="A70:A74"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="D52:D54"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="A52:A60"/>
-    <mergeCell ref="A64:A65"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2341,10 +2334,10 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>159</v>
+        <v>223</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>160</v>
+        <v>224</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -2359,45 +2352,45 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A3" s="29"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
@@ -2414,50 +2407,50 @@
     </row>
     <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>179</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
@@ -2495,10 +2488,10 @@
         <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -2506,7 +2499,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -2515,7 +2508,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -2524,7 +2517,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -2540,7 +2533,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -2549,7 +2542,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -2559,7 +2552,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
@@ -2574,7 +2567,7 @@
         <v>127</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -2583,7 +2576,7 @@
         <v>146</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -2592,7 +2585,7 @@
         <v>32</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -2601,7 +2594,7 @@
         <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C13" s="2"/>
     </row>
@@ -2611,7 +2604,7 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
@@ -2626,7 +2619,7 @@
         <v>49</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C16" s="2"/>
     </row>
@@ -2636,7 +2629,7 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
@@ -2644,7 +2637,7 @@
         <v>99</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C18" s="2"/>
     </row>
@@ -2660,7 +2653,7 @@
         <v>83</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C20" s="2"/>
     </row>
@@ -2669,7 +2662,7 @@
         <v>150</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C21" s="2"/>
     </row>
@@ -2678,7 +2671,7 @@
         <v>151</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C22" s="2"/>
     </row>
@@ -2694,7 +2687,7 @@
         <v>59</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C24" s="2"/>
     </row>
@@ -2703,7 +2696,7 @@
         <v>92</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C25" s="2"/>
     </row>
@@ -2712,7 +2705,7 @@
         <v>60</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C26" s="2"/>
     </row>
@@ -2721,7 +2714,7 @@
         <v>64</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C27" s="2"/>
     </row>
@@ -2737,7 +2730,7 @@
         <v>122</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C29" s="2"/>
     </row>
@@ -2746,7 +2739,7 @@
         <v>123</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C30" s="2"/>
     </row>
@@ -2755,7 +2748,7 @@
         <v>67</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C31" s="2"/>
     </row>
@@ -2764,7 +2757,7 @@
         <v>68</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C32" s="2"/>
     </row>
@@ -2773,7 +2766,7 @@
         <v>119</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C33" s="2"/>
     </row>

</xml_diff>

<commit_message>
Update on 20250828 part 3
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -13,7 +13,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他JS脚本!$A$1:$D$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">省份JS脚本!$A$2:$D$74</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">省份JS脚本!$A$2:$E$74</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">省份统计!$A$1:$C$33</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="227">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -863,61 +863,65 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>xizang.php
+    <t>酷9JS脚本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PHP脚本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ningxia.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>由伟大合法的菠菜平台提供的央视,卫视的频道直播源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>酷9JS脚本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PHP脚本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PHP脚本仅中国大陆可访问</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shanghai_setv.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">guangzhou.php
+gztv.php 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liaoning_bfgd.php
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xizang.php
 xztv.php
-(仅中国大陆可访问)</t>
-  </si>
-  <si>
-    <t>liaoning_bfgd.php
-(仅中国大陆可访问)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hangzhou.php
-(仅中国大陆可访问)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>guangzhou.php
-gztv.php 
-(仅中国大陆可访问)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shanghai_setv.php
-(仅中国大陆可访问)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>酷9JS脚本</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PHP脚本</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ningxia.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>由伟大合法的菠菜平台提供的央视,卫视的频道直播源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>酷9JS脚本</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PHP脚本</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hangzhou.php
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -950,8 +954,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
-      <sz val="14"/>
+      <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <family val="3"/>
@@ -1039,54 +1059,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
@@ -1094,41 +1072,68 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1431,882 +1436,974 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D76"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="19.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="111.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" style="3"/>
-    <col min="6" max="6" width="43.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="3"/>
+    <col min="1" max="1" width="16.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="93.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="1"/>
+    <col min="7" max="7" width="43.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="D1" s="12" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="22"/>
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="17"/>
+      <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="24"/>
-    </row>
-    <row r="5" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A5" s="21"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="16"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="11"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="E5" s="18" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="20" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="22"/>
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="17"/>
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="22"/>
-      <c r="B8" s="1" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" s="17"/>
+      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="21"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" s="11"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="56.25" x14ac:dyDescent="0.15">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="23" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="23"/>
-      <c r="B13" s="1" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="19"/>
+      <c r="B13" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1" t="s">
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="23" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1" t="s">
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="23"/>
-      <c r="B15" s="1" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="19"/>
+      <c r="B15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1" t="s">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="56.25" x14ac:dyDescent="0.15">
-      <c r="A16" s="23" t="s">
+    <row r="16" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A16" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="C16" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="23"/>
-      <c r="B17" s="1" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" s="19"/>
+      <c r="B17" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="5"/>
+      <c r="E17" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="10" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="13" t="s">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="20" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="7" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="5"/>
+      <c r="E19" s="5" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="10" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A20" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1" t="s">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="5"/>
+      <c r="E20" s="5" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="23" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="5"/>
+      <c r="E21" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="23"/>
-      <c r="B22" s="1" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A22" s="19"/>
+      <c r="B22" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="5"/>
+      <c r="E22" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="23" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A23" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="5"/>
+      <c r="E23" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="23"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A24" s="19"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="5"/>
+      <c r="E24" s="5" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="23"/>
-      <c r="B25" s="1" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A25" s="19"/>
+      <c r="B25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="5"/>
+      <c r="E25" s="16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="23"/>
-      <c r="B26" s="1" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A26" s="19"/>
+      <c r="B26" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="24"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="23"/>
-      <c r="B27" s="1" t="s">
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="16"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A27" s="19"/>
+      <c r="B27" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1" t="s">
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="23"/>
-      <c r="B28" s="1" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A28" s="19"/>
+      <c r="B28" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1" t="s">
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="23"/>
-      <c r="B29" s="1" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A29" s="19"/>
+      <c r="B29" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="24" t="s">
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="23"/>
-      <c r="B30" s="1" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A30" s="19"/>
+      <c r="B30" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="24"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="10" t="s">
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="16"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A31" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="13" t="s">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="20" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" s="10" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A32" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="13" t="s">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="20" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="23" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A33" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="5"/>
+      <c r="E33" s="18" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="23"/>
-      <c r="B34" s="1" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A34" s="19"/>
+      <c r="B34" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1" t="s">
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="11" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A35" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1" t="s">
+      <c r="B35" s="5"/>
+      <c r="C35" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="5"/>
+      <c r="E35" s="5" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="20" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A36" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="5"/>
+      <c r="E36" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="21"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A37" s="11"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="5"/>
+      <c r="E37" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="23" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A38" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1" t="s">
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="23"/>
-      <c r="B39" s="1" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A39" s="19"/>
+      <c r="B39" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1" t="s">
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A40" s="20" t="s">
+    <row r="40" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A40" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="D40" s="1" t="s">
+      <c r="B40" s="5"/>
+      <c r="C40" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="E40" s="5" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="21"/>
-      <c r="B41" s="1" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A41" s="11"/>
+      <c r="B41" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1" t="s">
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="10" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A42" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1" t="s">
+      <c r="B42" s="5"/>
+      <c r="C42" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" s="5"/>
+      <c r="E42" s="5" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="10" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A43" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="14" t="s">
+      <c r="B43" s="5"/>
+      <c r="C43" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="D43" s="7"/>
+      <c r="E43" s="20"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A44" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="20" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A45" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D45" s="5"/>
+      <c r="E45" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A46" s="19"/>
+      <c r="B46" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="16"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A47" s="19"/>
+      <c r="B47" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A48" s="19"/>
+      <c r="B48" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A49" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A50" s="19"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A51" s="19"/>
+      <c r="B51" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A52" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A53" s="17"/>
+      <c r="B53" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="16"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A54" s="17"/>
+      <c r="B54" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="16"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A55" s="17"/>
+      <c r="B55" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A56" s="17"/>
+      <c r="B56" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A57" s="17"/>
+      <c r="B57" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A58" s="17"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A59" s="17"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A60" s="11"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A61" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A62" s="19"/>
+      <c r="B62" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D62" s="7"/>
+      <c r="E62" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A63" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+    </row>
+    <row r="64" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A64" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D64" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="D43" s="13"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="13" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D45" s="24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="23"/>
-      <c r="B46" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C46" s="1"/>
-      <c r="D46" s="24"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="23"/>
-      <c r="B47" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="23"/>
-      <c r="B48" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="23"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="23"/>
-      <c r="B51" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C52" s="1"/>
-      <c r="D52" s="24" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="22"/>
-      <c r="B53" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C53" s="1"/>
-      <c r="D53" s="24"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="22"/>
-      <c r="B54" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C54" s="1"/>
-      <c r="D54" s="24"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="22"/>
-      <c r="B55" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="22"/>
-      <c r="B56" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="22"/>
-      <c r="B57" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="22"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" s="22"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="21"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A62" s="23"/>
-      <c r="B62" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C62" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A63" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-    </row>
-    <row r="64" spans="1:4" ht="56.25" x14ac:dyDescent="0.15">
-      <c r="A64" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C64" s="14" t="s">
-        <v>214</v>
-      </c>
-      <c r="D64" s="1" t="s">
+      <c r="E64" s="5" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="27"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="14" t="s">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A65" s="23"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D65" s="7"/>
+      <c r="E65" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66" s="25" t="s">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A66" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="D66" s="8" t="s">
+      <c r="D66" s="5"/>
+      <c r="E66" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67" s="25"/>
-      <c r="B67" s="1" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A67" s="24"/>
+      <c r="B67" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C67" s="1"/>
-      <c r="D67" s="6" t="s">
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="18" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="23" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A68" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C68" s="1"/>
-      <c r="D68" s="24" t="s">
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="23"/>
-      <c r="B69" s="1" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A69" s="19"/>
+      <c r="B69" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C69" s="1"/>
-      <c r="D69" s="24"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="23" t="s">
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="16"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A70" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D70" s="5"/>
+      <c r="E70" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A71" s="23"/>
-      <c r="B71" s="1" t="s">
+    <row r="71" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A71" s="19"/>
+      <c r="B71" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C71" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="D71" s="24" t="s">
+      <c r="C71" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="E71" s="16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A72" s="23"/>
-      <c r="B72" s="1" t="s">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A72" s="19"/>
+      <c r="B72" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C72" s="1"/>
-      <c r="D72" s="24"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A73" s="23"/>
-      <c r="B73" s="1" t="s">
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="16"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A73" s="19"/>
+      <c r="B73" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D73" s="5"/>
+      <c r="E73" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A74" s="23"/>
-      <c r="B74" s="1" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A74" s="19"/>
+      <c r="B74" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1" t="s">
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A75" s="23" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A75" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1" t="s">
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A76" s="23"/>
-      <c r="B76" s="1" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A76" s="19"/>
+      <c r="B76" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1" t="s">
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5" t="s">
         <v>126</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D74"/>
+  <autoFilter ref="A2:E74"/>
   <mergeCells count="27">
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="A70:A74"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="D52:D54"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="A52:A60"/>
-    <mergeCell ref="A64:A65"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A75:A76"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E25:E26"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="A23:A30"/>
     <mergeCell ref="A21:A22"/>
-    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A36:A37"/>
-    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="A70:A74"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="E52:E54"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="A52:A60"/>
+    <mergeCell ref="A64:A65"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2320,141 +2417,143 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="87.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.25" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="9"/>
+    <col min="6" max="6" width="43.375" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A3" s="29"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" s="11"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="5" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="5" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="5" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="5" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="D13" s="12" t="s">
+      <c r="D10" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D13" s="13" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2477,298 +2576,298 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.375" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.625" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.625" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="16"/>
+    <col min="1" max="1" width="14.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2" t="s">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C21" s="2"/>
+      <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C26" s="2"/>
+      <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C27" s="2"/>
+      <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C29" s="2"/>
+      <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C30" s="2"/>
+      <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C31" s="2"/>
+      <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C32" s="2"/>
+      <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C33" s="2"/>
+      <c r="C33" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C33"/>

</xml_diff>

<commit_message>
Update on 20250828 part 5
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="228">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -915,6 +915,10 @@
   <si>
     <t xml:space="preserve">hangzhou.php
 </t>
+  </si>
+  <si>
+    <t>gansu.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1090,12 +1094,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1111,15 +1109,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1127,12 +1116,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1453,16 +1457,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15" t="s">
+      <c r="A1" s="12"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="13" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1479,7 +1483,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1489,21 +1493,21 @@
         <v>131</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="21" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="17"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="16"/>
+      <c r="E4" s="21"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="11"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="5"/>
       <c r="C5" s="7" t="s">
         <v>222</v>
@@ -1511,12 +1515,12 @@
       <c r="D5" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="14" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1529,7 +1533,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="17"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1540,7 +1544,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="17"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1551,7 +1555,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="11"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
         <v>188</v>
@@ -1562,7 +1566,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1577,7 +1581,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="10" t="s">
         <v>144</v>
       </c>
       <c r="B11" s="5"/>
@@ -1586,7 +1590,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1601,7 +1605,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="19"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="5" t="s">
         <v>117</v>
       </c>
@@ -1612,20 +1616,24 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="20" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>221</v>
+      </c>
       <c r="E14" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="19"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="5" t="s">
         <v>25</v>
       </c>
@@ -1636,7 +1644,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="20" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1653,7 +1661,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="19"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="5" t="s">
         <v>29</v>
       </c>
@@ -1666,18 +1674,18 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="10" t="s">
         <v>145</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="15" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="10" t="s">
         <v>127</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -1692,7 +1700,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="10" t="s">
         <v>146</v>
       </c>
       <c r="B20" s="5"/>
@@ -1705,7 +1713,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="20" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -1720,7 +1728,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="19"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="5" t="s">
         <v>47</v>
       </c>
@@ -1733,7 +1741,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1748,7 +1756,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="19"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5" t="s">
         <v>185</v>
@@ -1759,7 +1767,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="19"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="5" t="s">
         <v>37</v>
       </c>
@@ -1767,21 +1775,21 @@
         <v>165</v>
       </c>
       <c r="D25" s="5"/>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="21" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="19"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="16"/>
+      <c r="E26" s="21"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="19"/>
+      <c r="A27" s="20"/>
       <c r="B27" s="5" t="s">
         <v>40</v>
       </c>
@@ -1792,7 +1800,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="19"/>
+      <c r="A28" s="20"/>
       <c r="B28" s="5" t="s">
         <v>42</v>
       </c>
@@ -1803,49 +1811,49 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="19"/>
+      <c r="A29" s="20"/>
       <c r="B29" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="E29" s="16" t="s">
+      <c r="E29" s="21" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="19"/>
+      <c r="A30" s="20"/>
       <c r="B30" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="16"/>
+      <c r="E30" s="21"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="10" t="s">
         <v>147</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="20" t="s">
+      <c r="E31" s="15" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="10" t="s">
         <v>148</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="20" t="s">
+      <c r="E32" s="15" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="20" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="5" t="s">
@@ -1855,12 +1863,12 @@
         <v>157</v>
       </c>
       <c r="D33" s="5"/>
-      <c r="E33" s="18" t="s">
+      <c r="E33" s="14" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" s="19"/>
+      <c r="A34" s="20"/>
       <c r="B34" s="5" t="s">
         <v>52</v>
       </c>
@@ -1871,7 +1879,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="16" t="s">
         <v>149</v>
       </c>
       <c r="B35" s="5"/>
@@ -1884,7 +1892,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="17" t="s">
         <v>99</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -1899,7 +1907,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="11"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5" t="s">
         <v>136</v>
@@ -1910,7 +1918,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -1923,7 +1931,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="19"/>
+      <c r="A39" s="20"/>
       <c r="B39" s="5" t="s">
         <v>57</v>
       </c>
@@ -1934,7 +1942,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="17" t="s">
         <v>83</v>
       </c>
       <c r="B40" s="5"/>
@@ -1949,7 +1957,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="11"/>
+      <c r="A41" s="18"/>
       <c r="B41" s="5" t="s">
         <v>84</v>
       </c>
@@ -1960,7 +1968,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="10" t="s">
         <v>150</v>
       </c>
       <c r="B42" s="5"/>
@@ -1973,7 +1981,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="12" t="s">
+      <c r="A43" s="10" t="s">
         <v>151</v>
       </c>
       <c r="B43" s="5"/>
@@ -1981,21 +1989,21 @@
         <v>216</v>
       </c>
       <c r="D43" s="7"/>
-      <c r="E43" s="20"/>
+      <c r="E43" s="15"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="12" t="s">
+      <c r="A44" s="10" t="s">
         <v>152</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
-      <c r="E44" s="20" t="s">
+      <c r="E44" s="15" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="19" t="s">
+      <c r="A45" s="20" t="s">
         <v>59</v>
       </c>
       <c r="B45" s="5" t="s">
@@ -2005,21 +2013,21 @@
         <v>166</v>
       </c>
       <c r="D45" s="5"/>
-      <c r="E45" s="16" t="s">
+      <c r="E45" s="21" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="19"/>
+      <c r="A46" s="20"/>
       <c r="B46" s="5" t="s">
         <v>87</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
-      <c r="E46" s="16"/>
+      <c r="E46" s="21"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="19"/>
+      <c r="A47" s="20"/>
       <c r="B47" s="5" t="s">
         <v>88</v>
       </c>
@@ -2030,7 +2038,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="19"/>
+      <c r="A48" s="20"/>
       <c r="B48" s="5" t="s">
         <v>89</v>
       </c>
@@ -2041,7 +2049,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A49" s="19" t="s">
+      <c r="A49" s="20" t="s">
         <v>92</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -2056,7 +2064,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A50" s="19"/>
+      <c r="A50" s="20"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
         <v>180</v>
@@ -2067,7 +2075,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A51" s="19"/>
+      <c r="A51" s="20"/>
       <c r="B51" s="5" t="s">
         <v>93</v>
       </c>
@@ -2080,7 +2088,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A52" s="10" t="s">
+      <c r="A52" s="17" t="s">
         <v>60</v>
       </c>
       <c r="B52" s="5" t="s">
@@ -2088,30 +2096,30 @@
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
-      <c r="E52" s="16" t="s">
+      <c r="E52" s="21" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A53" s="17"/>
+      <c r="A53" s="19"/>
       <c r="B53" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
-      <c r="E53" s="16"/>
+      <c r="E53" s="21"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A54" s="17"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="5" t="s">
         <v>114</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
-      <c r="E54" s="16"/>
+      <c r="E54" s="21"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A55" s="17"/>
+      <c r="A55" s="19"/>
       <c r="B55" s="5" t="s">
         <v>96</v>
       </c>
@@ -2122,7 +2130,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" s="17"/>
+      <c r="A56" s="19"/>
       <c r="B56" s="5" t="s">
         <v>98</v>
       </c>
@@ -2133,7 +2141,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A57" s="17"/>
+      <c r="A57" s="19"/>
       <c r="B57" s="5" t="s">
         <v>107</v>
       </c>
@@ -2144,7 +2152,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A58" s="17"/>
+      <c r="A58" s="19"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
         <v>138</v>
@@ -2155,7 +2163,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A59" s="17"/>
+      <c r="A59" s="19"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
         <v>139</v>
@@ -2166,7 +2174,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60" s="11"/>
+      <c r="A60" s="18"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
         <v>140</v>
@@ -2177,7 +2185,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A61" s="19" t="s">
+      <c r="A61" s="20" t="s">
         <v>64</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -2190,7 +2198,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A62" s="19"/>
+      <c r="A62" s="20"/>
       <c r="B62" s="5" t="s">
         <v>65</v>
       </c>
@@ -2203,7 +2211,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A63" s="12" t="s">
+      <c r="A63" s="10" t="s">
         <v>153</v>
       </c>
       <c r="B63" s="5"/>
@@ -2212,7 +2220,7 @@
       <c r="E63" s="5"/>
     </row>
     <row r="64" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A64" s="22" t="s">
+      <c r="A64" s="23" t="s">
         <v>122</v>
       </c>
       <c r="B64" s="5" t="s">
@@ -2229,7 +2237,7 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A65" s="23"/>
+      <c r="A65" s="24"/>
       <c r="B65" s="5"/>
       <c r="C65" s="7" t="s">
         <v>183</v>
@@ -2240,7 +2248,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A66" s="24" t="s">
+      <c r="A66" s="22" t="s">
         <v>123</v>
       </c>
       <c r="B66" s="5" t="s">
@@ -2255,18 +2263,18 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A67" s="24"/>
+      <c r="A67" s="22"/>
       <c r="B67" s="5" t="s">
         <v>109</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
-      <c r="E67" s="18" t="s">
+      <c r="E67" s="14" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A68" s="19" t="s">
+      <c r="A68" s="20" t="s">
         <v>67</v>
       </c>
       <c r="B68" s="5" t="s">
@@ -2274,21 +2282,21 @@
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
-      <c r="E68" s="16" t="s">
+      <c r="E68" s="21" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A69" s="19"/>
+      <c r="A69" s="20"/>
       <c r="B69" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
-      <c r="E69" s="16"/>
+      <c r="E69" s="21"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A70" s="19" t="s">
+      <c r="A70" s="20" t="s">
         <v>68</v>
       </c>
       <c r="B70" s="5" t="s">
@@ -2303,7 +2311,7 @@
       </c>
     </row>
     <row r="71" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A71" s="19"/>
+      <c r="A71" s="20"/>
       <c r="B71" s="5" t="s">
         <v>75</v>
       </c>
@@ -2313,21 +2321,21 @@
       <c r="D71" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="E71" s="16" t="s">
+      <c r="E71" s="21" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A72" s="19"/>
+      <c r="A72" s="20"/>
       <c r="B72" s="5" t="s">
         <v>77</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
-      <c r="E72" s="16"/>
+      <c r="E72" s="21"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A73" s="19"/>
+      <c r="A73" s="20"/>
       <c r="B73" s="5" t="s">
         <v>78</v>
       </c>
@@ -2340,7 +2348,7 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A74" s="19"/>
+      <c r="A74" s="20"/>
       <c r="B74" s="5" t="s">
         <v>82</v>
       </c>
@@ -2351,7 +2359,7 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A75" s="19" t="s">
+      <c r="A75" s="20" t="s">
         <v>119</v>
       </c>
       <c r="B75" s="5" t="s">
@@ -2364,7 +2372,7 @@
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A76" s="19"/>
+      <c r="A76" s="20"/>
       <c r="B76" s="5" t="s">
         <v>125</v>
       </c>
@@ -2377,6 +2385,17 @@
   </sheetData>
   <autoFilter ref="A2:E74"/>
   <mergeCells count="27">
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="A70:A74"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="E52:E54"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="A52:A60"/>
+    <mergeCell ref="A64:A65"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A75:A76"/>
@@ -2393,17 +2412,6 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="E45:E46"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="A70:A74"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="E52:E54"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="A52:A60"/>
-    <mergeCell ref="A64:A65"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2443,7 +2451,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2455,7 +2463,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="11"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
         <v>176</v>
@@ -2465,7 +2473,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="10" t="s">
         <v>202</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -2479,7 +2487,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="10" t="s">
         <v>203</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -2493,7 +2501,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="10" t="s">
         <v>102</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -2505,7 +2513,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="10" t="s">
         <v>206</v>
       </c>
       <c r="B7" s="5"/>
@@ -2517,7 +2525,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="10" t="s">
         <v>211</v>
       </c>
       <c r="B8" s="5"/>
@@ -2529,7 +2537,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="10" t="s">
         <v>171</v>
       </c>
       <c r="B9" s="5"/>
@@ -2541,7 +2549,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>174</v>
       </c>
       <c r="B10" s="5"/>
@@ -2553,7 +2561,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="11" t="s">
         <v>130</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update on 20250828 part 8
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -13,7 +13,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他JS脚本!$A$1:$D$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">省份JS脚本!$A$2:$E$74</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">省份JS脚本!$A$2:$E$76</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">省份统计!$A$1:$C$33</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -908,16 +908,16 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">xizang.php
-xztv.php
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hangzhou.php
-</t>
-  </si>
-  <si>
     <t>gansu.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hangzhou.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xizang.php
+xztv.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1115,15 +1115,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1132,6 +1123,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1483,7 +1483,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1493,21 +1493,21 @@
         <v>131</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="19"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="21"/>
+      <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="18"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="5"/>
       <c r="C5" s="7" t="s">
         <v>222</v>
@@ -1520,7 +1520,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1533,7 +1533,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="19"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1544,7 +1544,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="19"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1555,7 +1555,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="18"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
         <v>188</v>
@@ -1590,7 +1590,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1605,7 +1605,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="20"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="5" t="s">
         <v>117</v>
       </c>
@@ -1616,14 +1616,14 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>221</v>
@@ -1633,7 +1633,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="20"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="5" t="s">
         <v>25</v>
       </c>
@@ -1644,7 +1644,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="17" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1661,7 +1661,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="20"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="5" t="s">
         <v>29</v>
       </c>
@@ -1713,7 +1713,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="17" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -1728,7 +1728,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="20"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="5" t="s">
         <v>47</v>
       </c>
@@ -1741,7 +1741,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="17" t="s">
         <v>34</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1756,7 +1756,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="20"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5" t="s">
         <v>185</v>
@@ -1767,7 +1767,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="20"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="5" t="s">
         <v>37</v>
       </c>
@@ -1775,21 +1775,21 @@
         <v>165</v>
       </c>
       <c r="D25" s="5"/>
-      <c r="E25" s="21" t="s">
+      <c r="E25" s="18" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="20"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="21"/>
+      <c r="E26" s="18"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="20"/>
+      <c r="A27" s="17"/>
       <c r="B27" s="5" t="s">
         <v>40</v>
       </c>
@@ -1800,7 +1800,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="20"/>
+      <c r="A28" s="17"/>
       <c r="B28" s="5" t="s">
         <v>42</v>
       </c>
@@ -1811,24 +1811,24 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="20"/>
+      <c r="A29" s="17"/>
       <c r="B29" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="E29" s="21" t="s">
+      <c r="E29" s="18" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="20"/>
+      <c r="A30" s="17"/>
       <c r="B30" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="21"/>
+      <c r="E30" s="18"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="10" t="s">
@@ -1853,7 +1853,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="17" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="5" t="s">
@@ -1868,7 +1868,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" s="20"/>
+      <c r="A34" s="17"/>
       <c r="B34" s="5" t="s">
         <v>52</v>
       </c>
@@ -1892,7 +1892,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="20" t="s">
         <v>99</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -1907,7 +1907,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="18"/>
+      <c r="A37" s="22"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5" t="s">
         <v>136</v>
@@ -1918,7 +1918,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="20" t="s">
+      <c r="A38" s="17" t="s">
         <v>54</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -1931,7 +1931,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="20"/>
+      <c r="A39" s="17"/>
       <c r="B39" s="5" t="s">
         <v>57</v>
       </c>
@@ -1942,7 +1942,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="20" t="s">
         <v>83</v>
       </c>
       <c r="B40" s="5"/>
@@ -1957,7 +1957,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="18"/>
+      <c r="A41" s="22"/>
       <c r="B41" s="5" t="s">
         <v>84</v>
       </c>
@@ -2003,7 +2003,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="20" t="s">
+      <c r="A45" s="17" t="s">
         <v>59</v>
       </c>
       <c r="B45" s="5" t="s">
@@ -2013,21 +2013,21 @@
         <v>166</v>
       </c>
       <c r="D45" s="5"/>
-      <c r="E45" s="21" t="s">
+      <c r="E45" s="18" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="20"/>
+      <c r="A46" s="17"/>
       <c r="B46" s="5" t="s">
         <v>87</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
-      <c r="E46" s="21"/>
+      <c r="E46" s="18"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="20"/>
+      <c r="A47" s="17"/>
       <c r="B47" s="5" t="s">
         <v>88</v>
       </c>
@@ -2038,7 +2038,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="20"/>
+      <c r="A48" s="17"/>
       <c r="B48" s="5" t="s">
         <v>89</v>
       </c>
@@ -2049,7 +2049,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A49" s="20" t="s">
+      <c r="A49" s="17" t="s">
         <v>92</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -2064,7 +2064,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A50" s="20"/>
+      <c r="A50" s="17"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
         <v>180</v>
@@ -2075,7 +2075,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A51" s="20"/>
+      <c r="A51" s="17"/>
       <c r="B51" s="5" t="s">
         <v>93</v>
       </c>
@@ -2088,7 +2088,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A52" s="17" t="s">
+      <c r="A52" s="20" t="s">
         <v>60</v>
       </c>
       <c r="B52" s="5" t="s">
@@ -2096,30 +2096,30 @@
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
-      <c r="E52" s="21" t="s">
+      <c r="E52" s="18" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A53" s="19"/>
+      <c r="A53" s="21"/>
       <c r="B53" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
-      <c r="E53" s="21"/>
+      <c r="E53" s="18"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A54" s="19"/>
+      <c r="A54" s="21"/>
       <c r="B54" s="5" t="s">
         <v>114</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
-      <c r="E54" s="21"/>
+      <c r="E54" s="18"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A55" s="19"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="5" t="s">
         <v>96</v>
       </c>
@@ -2130,7 +2130,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" s="19"/>
+      <c r="A56" s="21"/>
       <c r="B56" s="5" t="s">
         <v>98</v>
       </c>
@@ -2141,7 +2141,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A57" s="19"/>
+      <c r="A57" s="21"/>
       <c r="B57" s="5" t="s">
         <v>107</v>
       </c>
@@ -2152,7 +2152,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A58" s="19"/>
+      <c r="A58" s="21"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
         <v>138</v>
@@ -2163,7 +2163,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A59" s="19"/>
+      <c r="A59" s="21"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
         <v>139</v>
@@ -2174,7 +2174,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60" s="18"/>
+      <c r="A60" s="22"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
         <v>140</v>
@@ -2185,7 +2185,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A61" s="20" t="s">
+      <c r="A61" s="17" t="s">
         <v>64</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -2198,7 +2198,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A62" s="20"/>
+      <c r="A62" s="17"/>
       <c r="B62" s="5" t="s">
         <v>65</v>
       </c>
@@ -2219,7 +2219,7 @@
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
     </row>
-    <row r="64" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A64" s="23" t="s">
         <v>122</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>106</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>221</v>
@@ -2248,7 +2248,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A66" s="22" t="s">
+      <c r="A66" s="19" t="s">
         <v>123</v>
       </c>
       <c r="B66" s="5" t="s">
@@ -2263,7 +2263,7 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A67" s="22"/>
+      <c r="A67" s="19"/>
       <c r="B67" s="5" t="s">
         <v>109</v>
       </c>
@@ -2274,7 +2274,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A68" s="20" t="s">
+      <c r="A68" s="17" t="s">
         <v>67</v>
       </c>
       <c r="B68" s="5" t="s">
@@ -2282,21 +2282,21 @@
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
-      <c r="E68" s="21" t="s">
+      <c r="E68" s="18" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A69" s="20"/>
+      <c r="A69" s="17"/>
       <c r="B69" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
-      <c r="E69" s="21"/>
+      <c r="E69" s="18"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A70" s="20" t="s">
+      <c r="A70" s="17" t="s">
         <v>68</v>
       </c>
       <c r="B70" s="5" t="s">
@@ -2310,8 +2310,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A71" s="20"/>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A71" s="17"/>
       <c r="B71" s="5" t="s">
         <v>75</v>
       </c>
@@ -2321,21 +2321,21 @@
       <c r="D71" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="E71" s="21" t="s">
+      <c r="E71" s="18" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A72" s="20"/>
+      <c r="A72" s="17"/>
       <c r="B72" s="5" t="s">
         <v>77</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
-      <c r="E72" s="21"/>
+      <c r="E72" s="18"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A73" s="20"/>
+      <c r="A73" s="17"/>
       <c r="B73" s="5" t="s">
         <v>78</v>
       </c>
@@ -2348,7 +2348,7 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A74" s="20"/>
+      <c r="A74" s="17"/>
       <c r="B74" s="5" t="s">
         <v>82</v>
       </c>
@@ -2359,7 +2359,7 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A75" s="20" t="s">
+      <c r="A75" s="17" t="s">
         <v>119</v>
       </c>
       <c r="B75" s="5" t="s">
@@ -2372,7 +2372,7 @@
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A76" s="20"/>
+      <c r="A76" s="17"/>
       <c r="B76" s="5" t="s">
         <v>125</v>
       </c>
@@ -2383,19 +2383,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E74"/>
+  <autoFilter ref="A2:E76"/>
   <mergeCells count="27">
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="A70:A74"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="E52:E54"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="A52:A60"/>
-    <mergeCell ref="A64:A65"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A75:A76"/>
@@ -2412,6 +2401,17 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="E45:E46"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="A70:A74"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="E52:E54"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="A52:A60"/>
+    <mergeCell ref="A64:A65"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2451,7 +2451,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2463,7 +2463,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="18"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
         <v>176</v>

</xml_diff>

<commit_message>
Update on 20250902 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="227">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -901,10 +901,6 @@
   <si>
     <t xml:space="preserve">guangzhou.php
 gztv.php 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">liaoning_bfgd.php
 </t>
   </si>
   <si>
@@ -1115,6 +1111,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1123,15 +1128,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1483,7 +1479,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1493,21 +1489,21 @@
         <v>131</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="21" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="21"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="18"/>
+      <c r="E4" s="21"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="22"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="5"/>
       <c r="C5" s="7" t="s">
         <v>222</v>
@@ -1520,7 +1516,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1533,7 +1529,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="21"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1544,7 +1540,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="21"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1555,7 +1551,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="22"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
         <v>188</v>
@@ -1590,7 +1586,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1605,7 +1601,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="17"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="5" t="s">
         <v>117</v>
       </c>
@@ -1616,14 +1612,14 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="20" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>221</v>
@@ -1633,7 +1629,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="17"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="5" t="s">
         <v>25</v>
       </c>
@@ -1644,7 +1640,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="20" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1661,7 +1657,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="17"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="5" t="s">
         <v>29</v>
       </c>
@@ -1713,7 +1709,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="20" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -1728,7 +1724,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="17"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="5" t="s">
         <v>47</v>
       </c>
@@ -1741,7 +1737,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1756,7 +1752,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="17"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5" t="s">
         <v>185</v>
@@ -1767,7 +1763,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="17"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="5" t="s">
         <v>37</v>
       </c>
@@ -1775,21 +1771,21 @@
         <v>165</v>
       </c>
       <c r="D25" s="5"/>
-      <c r="E25" s="18" t="s">
+      <c r="E25" s="21" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="17"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="18"/>
+      <c r="E26" s="21"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="17"/>
+      <c r="A27" s="20"/>
       <c r="B27" s="5" t="s">
         <v>40</v>
       </c>
@@ -1800,7 +1796,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="17"/>
+      <c r="A28" s="20"/>
       <c r="B28" s="5" t="s">
         <v>42</v>
       </c>
@@ -1811,24 +1807,24 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="17"/>
+      <c r="A29" s="20"/>
       <c r="B29" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="E29" s="18" t="s">
+      <c r="E29" s="21" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="17"/>
+      <c r="A30" s="20"/>
       <c r="B30" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="18"/>
+      <c r="E30" s="21"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="10" t="s">
@@ -1853,7 +1849,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="20" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="5" t="s">
@@ -1868,7 +1864,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" s="17"/>
+      <c r="A34" s="20"/>
       <c r="B34" s="5" t="s">
         <v>52</v>
       </c>
@@ -1892,7 +1888,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="17" t="s">
         <v>99</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -1907,7 +1903,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="22"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5" t="s">
         <v>136</v>
@@ -1918,7 +1914,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -1931,7 +1927,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="17"/>
+      <c r="A39" s="20"/>
       <c r="B39" s="5" t="s">
         <v>57</v>
       </c>
@@ -1941,23 +1937,19 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A40" s="20" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A40" s="17" t="s">
         <v>83</v>
       </c>
       <c r="B40" s="5"/>
-      <c r="C40" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>221</v>
-      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
       <c r="E40" s="5" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="22"/>
+      <c r="A41" s="18"/>
       <c r="B41" s="5" t="s">
         <v>84</v>
       </c>
@@ -2003,7 +1995,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="20" t="s">
         <v>59</v>
       </c>
       <c r="B45" s="5" t="s">
@@ -2013,21 +2005,21 @@
         <v>166</v>
       </c>
       <c r="D45" s="5"/>
-      <c r="E45" s="18" t="s">
+      <c r="E45" s="21" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="17"/>
+      <c r="A46" s="20"/>
       <c r="B46" s="5" t="s">
         <v>87</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
-      <c r="E46" s="18"/>
+      <c r="E46" s="21"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="17"/>
+      <c r="A47" s="20"/>
       <c r="B47" s="5" t="s">
         <v>88</v>
       </c>
@@ -2038,7 +2030,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="17"/>
+      <c r="A48" s="20"/>
       <c r="B48" s="5" t="s">
         <v>89</v>
       </c>
@@ -2049,7 +2041,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A49" s="17" t="s">
+      <c r="A49" s="20" t="s">
         <v>92</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -2064,7 +2056,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A50" s="17"/>
+      <c r="A50" s="20"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
         <v>180</v>
@@ -2075,7 +2067,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A51" s="17"/>
+      <c r="A51" s="20"/>
       <c r="B51" s="5" t="s">
         <v>93</v>
       </c>
@@ -2088,7 +2080,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A52" s="20" t="s">
+      <c r="A52" s="17" t="s">
         <v>60</v>
       </c>
       <c r="B52" s="5" t="s">
@@ -2096,30 +2088,30 @@
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
-      <c r="E52" s="18" t="s">
+      <c r="E52" s="21" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A53" s="21"/>
+      <c r="A53" s="19"/>
       <c r="B53" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
-      <c r="E53" s="18"/>
+      <c r="E53" s="21"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A54" s="21"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="5" t="s">
         <v>114</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
-      <c r="E54" s="18"/>
+      <c r="E54" s="21"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A55" s="21"/>
+      <c r="A55" s="19"/>
       <c r="B55" s="5" t="s">
         <v>96</v>
       </c>
@@ -2130,7 +2122,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" s="21"/>
+      <c r="A56" s="19"/>
       <c r="B56" s="5" t="s">
         <v>98</v>
       </c>
@@ -2141,7 +2133,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A57" s="21"/>
+      <c r="A57" s="19"/>
       <c r="B57" s="5" t="s">
         <v>107</v>
       </c>
@@ -2152,7 +2144,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A58" s="21"/>
+      <c r="A58" s="19"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
         <v>138</v>
@@ -2163,7 +2155,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A59" s="21"/>
+      <c r="A59" s="19"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
         <v>139</v>
@@ -2174,7 +2166,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60" s="22"/>
+      <c r="A60" s="18"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
         <v>140</v>
@@ -2185,7 +2177,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A61" s="17" t="s">
+      <c r="A61" s="20" t="s">
         <v>64</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -2198,7 +2190,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A62" s="17"/>
+      <c r="A62" s="20"/>
       <c r="B62" s="5" t="s">
         <v>65</v>
       </c>
@@ -2227,7 +2219,7 @@
         <v>106</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>221</v>
@@ -2248,7 +2240,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A66" s="19" t="s">
+      <c r="A66" s="22" t="s">
         <v>123</v>
       </c>
       <c r="B66" s="5" t="s">
@@ -2263,7 +2255,7 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A67" s="19"/>
+      <c r="A67" s="22"/>
       <c r="B67" s="5" t="s">
         <v>109</v>
       </c>
@@ -2274,7 +2266,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A68" s="17" t="s">
+      <c r="A68" s="20" t="s">
         <v>67</v>
       </c>
       <c r="B68" s="5" t="s">
@@ -2282,21 +2274,21 @@
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
-      <c r="E68" s="18" t="s">
+      <c r="E68" s="21" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A69" s="17"/>
+      <c r="A69" s="20"/>
       <c r="B69" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
-      <c r="E69" s="18"/>
+      <c r="E69" s="21"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A70" s="17" t="s">
+      <c r="A70" s="20" t="s">
         <v>68</v>
       </c>
       <c r="B70" s="5" t="s">
@@ -2311,31 +2303,31 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A71" s="17"/>
+      <c r="A71" s="20"/>
       <c r="B71" s="5" t="s">
         <v>75</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D71" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="E71" s="18" t="s">
+      <c r="E71" s="21" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A72" s="17"/>
+      <c r="A72" s="20"/>
       <c r="B72" s="5" t="s">
         <v>77</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
-      <c r="E72" s="18"/>
+      <c r="E72" s="21"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A73" s="17"/>
+      <c r="A73" s="20"/>
       <c r="B73" s="5" t="s">
         <v>78</v>
       </c>
@@ -2348,7 +2340,7 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A74" s="17"/>
+      <c r="A74" s="20"/>
       <c r="B74" s="5" t="s">
         <v>82</v>
       </c>
@@ -2359,7 +2351,7 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A75" s="17" t="s">
+      <c r="A75" s="20" t="s">
         <v>119</v>
       </c>
       <c r="B75" s="5" t="s">
@@ -2372,7 +2364,7 @@
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A76" s="17"/>
+      <c r="A76" s="20"/>
       <c r="B76" s="5" t="s">
         <v>125</v>
       </c>
@@ -2385,6 +2377,17 @@
   </sheetData>
   <autoFilter ref="A2:E76"/>
   <mergeCells count="27">
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="A70:A74"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="E52:E54"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="A52:A60"/>
+    <mergeCell ref="A64:A65"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A75:A76"/>
@@ -2401,17 +2404,6 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="E45:E46"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="A70:A74"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="E52:E54"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="A52:A60"/>
-    <mergeCell ref="A64:A65"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2451,7 +2443,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2463,7 +2455,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="22"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
         <v>176</v>
@@ -2759,9 +2751,7 @@
       <c r="A20" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>194</v>
-      </c>
+      <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Update on 20250903 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="250">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -867,10 +867,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>由伟大合法的菠菜平台提供的央视,卫视的频道直播源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>酷9JS脚本</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -909,10 +905,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1905a.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1905.php
 1905a.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1007,6 +999,14 @@
   </si>
   <si>
     <t>重庆新闻频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>由伟大合法的博彩平台提供的央视,卫视的频道直播源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1905a.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1210,15 +1210,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1227,6 +1218,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1571,14 +1571,14 @@
         <v>213</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1588,51 +1588,51 @@
         <v>131</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="23" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="23"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="19"/>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="24"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="5"/>
       <c r="C5" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="23"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1643,7 +1643,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="23"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1654,7 +1654,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="24"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
         <v>186</v>
@@ -1685,17 +1685,17 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>249</v>
-      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1710,20 +1710,20 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="20"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>241</v>
-      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="20"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="5" t="s">
         <v>117</v>
       </c>
@@ -1734,24 +1734,24 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="22" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="20"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="5" t="s">
         <v>25</v>
       </c>
@@ -1762,24 +1762,24 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="22" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="20"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="5" t="s">
         <v>29</v>
       </c>
@@ -1831,7 +1831,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="22" t="s">
         <v>32</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -1846,7 +1846,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="20"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="5" t="s">
         <v>47</v>
       </c>
@@ -1859,7 +1859,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="22" t="s">
         <v>34</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -1874,7 +1874,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="20"/>
+      <c r="A25" s="22"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5" t="s">
         <v>183</v>
@@ -1885,7 +1885,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="20"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="5" t="s">
         <v>37</v>
       </c>
@@ -1893,21 +1893,21 @@
         <v>164</v>
       </c>
       <c r="D26" s="5"/>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="20"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="19"/>
+      <c r="E27" s="23"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="20"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="5" t="s">
         <v>40</v>
       </c>
@@ -1918,7 +1918,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="20"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="5" t="s">
         <v>42</v>
       </c>
@@ -1929,24 +1929,24 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="20"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="19" t="s">
+      <c r="E30" s="23" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="20"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="19"/>
+      <c r="E31" s="23"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="10" t="s">
@@ -1965,28 +1965,28 @@
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="18"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="20" t="s">
+      <c r="A35" s="22" t="s">
         <v>49</v>
       </c>
       <c r="B35" s="5" t="s">
@@ -2001,7 +2001,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="20"/>
+      <c r="A36" s="22"/>
       <c r="B36" s="5" t="s">
         <v>52</v>
       </c>
@@ -2025,7 +2025,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="22" t="s">
+      <c r="A38" s="19" t="s">
         <v>99</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -2040,7 +2040,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="24"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5" t="s">
         <v>136</v>
@@ -2051,14 +2051,14 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="22" t="s">
+      <c r="A40" s="19" t="s">
         <v>54</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="5" t="s">
@@ -2066,7 +2066,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="23"/>
+      <c r="A41" s="20"/>
       <c r="B41" s="5" t="s">
         <v>57</v>
       </c>
@@ -2077,20 +2077,20 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="24"/>
+      <c r="A42" s="21"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="19" t="s">
         <v>83</v>
       </c>
       <c r="B43" s="5"/>
@@ -2101,7 +2101,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="24"/>
+      <c r="A44" s="21"/>
       <c r="B44" s="5" t="s">
         <v>84</v>
       </c>
@@ -2147,7 +2147,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="20" t="s">
+      <c r="A48" s="22" t="s">
         <v>59</v>
       </c>
       <c r="B48" s="5" t="s">
@@ -2157,21 +2157,21 @@
         <v>165</v>
       </c>
       <c r="D48" s="5"/>
-      <c r="E48" s="19" t="s">
+      <c r="E48" s="23" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A49" s="20"/>
+      <c r="A49" s="22"/>
       <c r="B49" s="5" t="s">
         <v>87</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
-      <c r="E49" s="19"/>
+      <c r="E49" s="23"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A50" s="20"/>
+      <c r="A50" s="22"/>
       <c r="B50" s="5" t="s">
         <v>88</v>
       </c>
@@ -2182,7 +2182,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A51" s="20"/>
+      <c r="A51" s="22"/>
       <c r="B51" s="5" t="s">
         <v>89</v>
       </c>
@@ -2193,7 +2193,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A52" s="20" t="s">
+      <c r="A52" s="22" t="s">
         <v>92</v>
       </c>
       <c r="B52" s="5" t="s">
@@ -2208,7 +2208,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A53" s="20"/>
+      <c r="A53" s="22"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5" t="s">
         <v>178</v>
@@ -2219,7 +2219,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A54" s="20"/>
+      <c r="A54" s="22"/>
       <c r="B54" s="5" t="s">
         <v>93</v>
       </c>
@@ -2232,7 +2232,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A55" s="22" t="s">
+      <c r="A55" s="19" t="s">
         <v>60</v>
       </c>
       <c r="B55" s="5" t="s">
@@ -2240,34 +2240,34 @@
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
-      <c r="E55" s="19" t="s">
+      <c r="E55" s="23" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" s="23"/>
+      <c r="A56" s="20"/>
       <c r="B56" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="E56" s="19"/>
+        <v>232</v>
+      </c>
+      <c r="E56" s="23"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A57" s="23"/>
+      <c r="A57" s="20"/>
       <c r="B57" s="5" t="s">
         <v>114</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
-      <c r="E57" s="19"/>
+      <c r="E57" s="23"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A58" s="23"/>
+      <c r="A58" s="20"/>
       <c r="B58" s="5" t="s">
         <v>96</v>
       </c>
@@ -2278,7 +2278,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A59" s="23"/>
+      <c r="A59" s="20"/>
       <c r="B59" s="5" t="s">
         <v>98</v>
       </c>
@@ -2289,7 +2289,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60" s="23"/>
+      <c r="A60" s="20"/>
       <c r="B60" s="5" t="s">
         <v>107</v>
       </c>
@@ -2300,7 +2300,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A61" s="23"/>
+      <c r="A61" s="20"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
         <v>138</v>
@@ -2311,7 +2311,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A62" s="23"/>
+      <c r="A62" s="20"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
         <v>139</v>
@@ -2322,7 +2322,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A63" s="24"/>
+      <c r="A63" s="21"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
         <v>140</v>
@@ -2333,24 +2333,24 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A64" s="20" t="s">
+      <c r="A64" s="22" t="s">
         <v>64</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>112</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A65" s="20"/>
+      <c r="A65" s="22"/>
       <c r="B65" s="5" t="s">
         <v>65</v>
       </c>
@@ -2379,10 +2379,10 @@
         <v>106</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>196</v>
@@ -2400,7 +2400,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A69" s="21" t="s">
+      <c r="A69" s="24" t="s">
         <v>123</v>
       </c>
       <c r="B69" s="5" t="s">
@@ -2415,12 +2415,12 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A70" s="21"/>
+      <c r="A70" s="24"/>
       <c r="B70" s="5" t="s">
         <v>109</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="14" t="s">
@@ -2428,33 +2428,33 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A71" s="20" t="s">
+      <c r="A71" s="22" t="s">
         <v>67</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>70</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="E71" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="E71" s="23" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A72" s="20"/>
+      <c r="A72" s="22"/>
       <c r="B72" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
-      <c r="E72" s="19"/>
+      <c r="E72" s="23"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A73" s="20" t="s">
+      <c r="A73" s="22" t="s">
         <v>68</v>
       </c>
       <c r="B73" s="5" t="s">
@@ -2469,31 +2469,31 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A74" s="20"/>
+      <c r="A74" s="22"/>
       <c r="B74" s="5" t="s">
         <v>75</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="E74" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="E74" s="23" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A75" s="20"/>
+      <c r="A75" s="22"/>
       <c r="B75" s="5" t="s">
         <v>77</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
-      <c r="E75" s="19"/>
+      <c r="E75" s="23"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A76" s="20"/>
+      <c r="A76" s="22"/>
       <c r="B76" s="5" t="s">
         <v>78</v>
       </c>
@@ -2506,7 +2506,7 @@
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A77" s="20"/>
+      <c r="A77" s="22"/>
       <c r="B77" s="5" t="s">
         <v>82</v>
       </c>
@@ -2517,7 +2517,7 @@
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A78" s="20" t="s">
+      <c r="A78" s="22" t="s">
         <v>119</v>
       </c>
       <c r="B78" s="5" t="s">
@@ -2530,7 +2530,7 @@
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A79" s="20"/>
+      <c r="A79" s="22"/>
       <c r="B79" s="5" t="s">
         <v>125</v>
       </c>
@@ -2543,21 +2543,6 @@
   </sheetData>
   <autoFilter ref="A2:E79"/>
   <mergeCells count="27">
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A24:A31"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="A3:A5"/>
     <mergeCell ref="E48:E49"/>
     <mergeCell ref="A48:A51"/>
     <mergeCell ref="E74:E75"/>
@@ -2570,6 +2555,21 @@
     <mergeCell ref="A69:A70"/>
     <mergeCell ref="A55:A63"/>
     <mergeCell ref="A67:A68"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A24:A31"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A38:A39"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2587,8 +2587,8 @@
   <cols>
     <col min="1" max="1" width="11.625" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.25" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="13.875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="26.125" style="9" customWidth="1"/>
     <col min="5" max="5" width="72.625" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="9"/>
     <col min="7" max="7" width="43.375" style="9" bestFit="1" customWidth="1"/>
@@ -2600,10 +2600,10 @@
         <v>7</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>216</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>217</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>193</v>
@@ -2613,30 +2613,30 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>225</v>
+        <v>249</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A3" s="20"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="5"/>
       <c r="C3" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>176</v>
@@ -2732,24 +2732,26 @@
       <c r="C10" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="7" t="s">
+        <v>218</v>
+      </c>
       <c r="E10" s="5" t="s">
-        <v>215</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A11" s="17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>227</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Update on 20250903 part 3
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="250">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -887,11 +887,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">guangzhou.php
-gztv.php 
-</t>
-  </si>
-  <si>
     <t>gansu.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -934,10 +929,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>shanxi_huang.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PHP脚本仅中国大陆可访问</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1007,6 +998,15 @@
   </si>
   <si>
     <t>1905a.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">guangzhou.php
+gztv.php </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shanxi_huanghe.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1152,7 +1152,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1208,7 +1208,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1219,20 +1225,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1578,7 +1581,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1588,21 +1591,21 @@
         <v>131</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="20"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="23"/>
+      <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="21"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="5"/>
       <c r="C5" s="7" t="s">
         <v>219</v>
@@ -1615,24 +1618,24 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="20"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1643,7 +1646,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="20"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1654,7 +1657,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="21"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
         <v>186</v>
@@ -1685,17 +1688,17 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>247</v>
-      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1710,20 +1713,20 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="22"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>239</v>
-      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="22"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="5" t="s">
         <v>117</v>
       </c>
@@ -1734,14 +1737,14 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="19" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>218</v>
@@ -1751,7 +1754,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="22"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="5" t="s">
         <v>25</v>
       </c>
@@ -1761,15 +1764,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A17" s="22" t="s">
+    <row r="17" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A17" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>220</v>
+        <v>248</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>218</v>
@@ -1779,7 +1782,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="22"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="5" t="s">
         <v>29</v>
       </c>
@@ -1831,7 +1834,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="19" t="s">
         <v>32</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -1846,7 +1849,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="22"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="5" t="s">
         <v>47</v>
       </c>
@@ -1859,10 +1862,10 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C24" s="5" t="s">
@@ -1874,8 +1877,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="22"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="27"/>
       <c r="C25" s="5" t="s">
         <v>183</v>
       </c>
@@ -1885,7 +1888,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="22"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="5" t="s">
         <v>37</v>
       </c>
@@ -1893,21 +1896,21 @@
         <v>164</v>
       </c>
       <c r="D26" s="5"/>
-      <c r="E26" s="23" t="s">
+      <c r="E26" s="18" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="22"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="23"/>
+      <c r="E27" s="18"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="22"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="5" t="s">
         <v>40</v>
       </c>
@@ -1918,7 +1921,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="22"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="5" t="s">
         <v>42</v>
       </c>
@@ -1929,24 +1932,24 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="22"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="23" t="s">
+      <c r="E30" s="18" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="22"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="23"/>
+      <c r="E31" s="18"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="10" t="s">
@@ -1960,33 +1963,33 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="21" t="s">
         <v>148</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" s="18"/>
+      <c r="A34" s="23"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="22" t="s">
+      <c r="A35" s="19" t="s">
         <v>49</v>
       </c>
       <c r="B35" s="5" t="s">
@@ -2001,7 +2004,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="22"/>
+      <c r="A36" s="19"/>
       <c r="B36" s="5" t="s">
         <v>52</v>
       </c>
@@ -2025,7 +2028,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="21" t="s">
         <v>99</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -2040,25 +2043,27 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="21"/>
+      <c r="A39" s="23"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D39" s="5"/>
+      <c r="D39" s="7" t="s">
+        <v>218</v>
+      </c>
       <c r="E39" s="5" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="19" t="s">
+      <c r="A40" s="21" t="s">
         <v>54</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="5" t="s">
@@ -2066,7 +2071,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="20"/>
+      <c r="A41" s="22"/>
       <c r="B41" s="5" t="s">
         <v>57</v>
       </c>
@@ -2077,20 +2082,20 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="21"/>
+      <c r="A42" s="23"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>218</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="19" t="s">
+      <c r="A43" s="21" t="s">
         <v>83</v>
       </c>
       <c r="B43" s="5"/>
@@ -2101,7 +2106,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="21"/>
+      <c r="A44" s="23"/>
       <c r="B44" s="5" t="s">
         <v>84</v>
       </c>
@@ -2147,7 +2152,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="22" t="s">
+      <c r="A48" s="19" t="s">
         <v>59</v>
       </c>
       <c r="B48" s="5" t="s">
@@ -2157,21 +2162,21 @@
         <v>165</v>
       </c>
       <c r="D48" s="5"/>
-      <c r="E48" s="23" t="s">
+      <c r="E48" s="18" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A49" s="22"/>
+      <c r="A49" s="19"/>
       <c r="B49" s="5" t="s">
         <v>87</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
-      <c r="E49" s="23"/>
+      <c r="E49" s="18"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A50" s="22"/>
+      <c r="A50" s="19"/>
       <c r="B50" s="5" t="s">
         <v>88</v>
       </c>
@@ -2182,7 +2187,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A51" s="22"/>
+      <c r="A51" s="19"/>
       <c r="B51" s="5" t="s">
         <v>89</v>
       </c>
@@ -2193,7 +2198,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A52" s="22" t="s">
+      <c r="A52" s="19" t="s">
         <v>92</v>
       </c>
       <c r="B52" s="5" t="s">
@@ -2208,7 +2213,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A53" s="22"/>
+      <c r="A53" s="19"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5" t="s">
         <v>178</v>
@@ -2219,7 +2224,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A54" s="22"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="5" t="s">
         <v>93</v>
       </c>
@@ -2232,7 +2237,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A55" s="19" t="s">
+      <c r="A55" s="21" t="s">
         <v>60</v>
       </c>
       <c r="B55" s="5" t="s">
@@ -2240,34 +2245,34 @@
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
-      <c r="E55" s="23" t="s">
+      <c r="E55" s="18" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" s="20"/>
+      <c r="A56" s="22"/>
       <c r="B56" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>231</v>
+        <v>249</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="E56" s="23"/>
+        <v>230</v>
+      </c>
+      <c r="E56" s="18"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A57" s="20"/>
+      <c r="A57" s="22"/>
       <c r="B57" s="5" t="s">
         <v>114</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
-      <c r="E57" s="23"/>
+      <c r="E57" s="18"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A58" s="20"/>
+      <c r="A58" s="22"/>
       <c r="B58" s="5" t="s">
         <v>96</v>
       </c>
@@ -2278,7 +2283,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A59" s="20"/>
+      <c r="A59" s="22"/>
       <c r="B59" s="5" t="s">
         <v>98</v>
       </c>
@@ -2289,7 +2294,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60" s="20"/>
+      <c r="A60" s="22"/>
       <c r="B60" s="5" t="s">
         <v>107</v>
       </c>
@@ -2300,7 +2305,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A61" s="20"/>
+      <c r="A61" s="22"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
         <v>138</v>
@@ -2311,7 +2316,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A62" s="20"/>
+      <c r="A62" s="22"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
         <v>139</v>
@@ -2322,7 +2327,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A63" s="21"/>
+      <c r="A63" s="23"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
         <v>140</v>
@@ -2333,24 +2338,24 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A64" s="22" t="s">
+      <c r="A64" s="19" t="s">
         <v>64</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>112</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A65" s="22"/>
+      <c r="A65" s="19"/>
       <c r="B65" s="5" t="s">
         <v>65</v>
       </c>
@@ -2372,14 +2377,14 @@
       <c r="E66" s="5"/>
     </row>
     <row r="67" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A67" s="25" t="s">
+      <c r="A67" s="24" t="s">
         <v>122</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>106</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D67" s="7" t="s">
         <v>218</v>
@@ -2389,7 +2394,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A68" s="26"/>
+      <c r="A68" s="25"/>
       <c r="B68" s="5"/>
       <c r="C68" s="7" t="s">
         <v>181</v>
@@ -2400,7 +2405,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A69" s="24" t="s">
+      <c r="A69" s="20" t="s">
         <v>123</v>
       </c>
       <c r="B69" s="5" t="s">
@@ -2415,12 +2420,12 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A70" s="24"/>
+      <c r="A70" s="20"/>
       <c r="B70" s="5" t="s">
         <v>109</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="14" t="s">
@@ -2428,33 +2433,33 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A71" s="22" t="s">
+      <c r="A71" s="19" t="s">
         <v>67</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>70</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="E71" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="E71" s="18" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A72" s="22"/>
+      <c r="A72" s="19"/>
       <c r="B72" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
-      <c r="E72" s="23"/>
+      <c r="E72" s="18"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A73" s="22" t="s">
+      <c r="A73" s="19" t="s">
         <v>68</v>
       </c>
       <c r="B73" s="5" t="s">
@@ -2469,31 +2474,31 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A74" s="22"/>
+      <c r="A74" s="19"/>
       <c r="B74" s="5" t="s">
         <v>75</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="E74" s="23" t="s">
+      <c r="E74" s="18" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A75" s="22"/>
+      <c r="A75" s="19"/>
       <c r="B75" s="5" t="s">
         <v>77</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
-      <c r="E75" s="23"/>
+      <c r="E75" s="18"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A76" s="22"/>
+      <c r="A76" s="19"/>
       <c r="B76" s="5" t="s">
         <v>78</v>
       </c>
@@ -2506,7 +2511,7 @@
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A77" s="22"/>
+      <c r="A77" s="19"/>
       <c r="B77" s="5" t="s">
         <v>82</v>
       </c>
@@ -2517,7 +2522,7 @@
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A78" s="22" t="s">
+      <c r="A78" s="19" t="s">
         <v>119</v>
       </c>
       <c r="B78" s="5" t="s">
@@ -2530,7 +2535,7 @@
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A79" s="22"/>
+      <c r="A79" s="19"/>
       <c r="B79" s="5" t="s">
         <v>125</v>
       </c>
@@ -2542,7 +2547,24 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:E79"/>
-  <mergeCells count="27">
+  <mergeCells count="29">
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A24:A31"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B24:B25"/>
     <mergeCell ref="E48:E49"/>
     <mergeCell ref="A48:A51"/>
     <mergeCell ref="E74:E75"/>
@@ -2555,21 +2577,6 @@
     <mergeCell ref="A69:A70"/>
     <mergeCell ref="A55:A63"/>
     <mergeCell ref="A67:A68"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A24:A31"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A38:A39"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2612,15 +2619,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>218</v>
@@ -2630,10 +2637,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A3" s="22"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="5"/>
       <c r="C3" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>218</v>
@@ -2736,22 +2743,22 @@
         <v>218</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>218</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
@@ -2774,7 +2781,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>

<commit_message>
Update on 20250905 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -13,7 +13,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他JS脚本!$A$1:$E$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">省份JS脚本!$A$2:$E$79</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">省份JS脚本!$A$2:$E$80</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">省份统计!$A$1:$C$33</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="255">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1018,6 +1018,14 @@
   </si>
   <si>
     <t>1905.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hubei.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卫视,湖北省频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1194,9 +1202,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1206,17 +1211,29 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1227,26 +1244,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1549,7 +1557,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1566,16 +1574,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" s="12"/>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13" t="s">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="12" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1592,7 +1600,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1602,21 +1610,21 @@
         <v>131</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="19"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="22"/>
+      <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="20"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="5"/>
       <c r="C5" s="7" t="s">
         <v>219</v>
@@ -1624,12 +1632,12 @@
       <c r="D5" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="17" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1646,7 +1654,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="19"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1657,7 +1665,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="19"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1668,7 +1676,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="20"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
         <v>186</v>
@@ -1679,7 +1687,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1694,7 +1702,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="16" t="s">
         <v>144</v>
       </c>
       <c r="B11" s="5"/>
@@ -1709,7 +1717,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1724,7 +1732,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="21"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
         <v>235</v>
@@ -1737,7 +1745,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="21"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="5" t="s">
         <v>117</v>
       </c>
@@ -1748,7 +1756,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="19" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -1765,7 +1773,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="21"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="5" t="s">
         <v>25</v>
       </c>
@@ -1776,7 +1784,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1793,7 +1801,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="21"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="5" t="s">
         <v>29</v>
       </c>
@@ -1806,18 +1814,18 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="16" t="s">
         <v>145</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="13" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="16" t="s">
         <v>127</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -1832,7 +1840,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="16" t="s">
         <v>146</v>
       </c>
       <c r="B21" s="5"/>
@@ -1845,7 +1853,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="19" t="s">
         <v>32</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -1860,7 +1868,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="21"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="5" t="s">
         <v>47</v>
       </c>
@@ -1873,10 +1881,10 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C24" s="5" t="s">
@@ -1888,8 +1896,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="21"/>
-      <c r="B25" s="24"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="27"/>
       <c r="C25" s="5" t="s">
         <v>183</v>
       </c>
@@ -1899,7 +1907,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="21"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="5" t="s">
         <v>37</v>
       </c>
@@ -1907,21 +1915,21 @@
         <v>164</v>
       </c>
       <c r="D26" s="5"/>
-      <c r="E26" s="22" t="s">
+      <c r="E26" s="18" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="21"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="22"/>
+      <c r="E27" s="18"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="21"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="5" t="s">
         <v>40</v>
       </c>
@@ -1932,7 +1940,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="21"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="5" t="s">
         <v>42</v>
       </c>
@@ -1943,651 +1951,664 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="21"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="22" t="s">
+      <c r="E30" s="18" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="21"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="22"/>
+      <c r="E31" s="18"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="16" t="s">
         <v>147</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="13" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="21" t="s">
         <v>148</v>
       </c>
       <c r="B33" s="5"/>
-      <c r="C33" s="5" t="s">
-        <v>231</v>
+      <c r="C33" s="9" t="s">
+        <v>253</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>229</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>232</v>
+        <v>254</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" s="20"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A35" s="23"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5" t="s">
+      <c r="D35" s="5"/>
+      <c r="E35" s="5" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="21" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A36" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B36" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C36" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="D35" s="5"/>
-      <c r="E35" s="14" t="s">
+      <c r="D36" s="5"/>
+      <c r="E36" s="17" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="21"/>
-      <c r="B36" s="5" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A37" s="19"/>
+      <c r="B37" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5" t="s">
-        <v>167</v>
-      </c>
+      <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5" t="s">
-        <v>166</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="A38" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B38" s="5"/>
       <c r="C38" s="5" t="s">
-        <v>190</v>
+        <v>167</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A39" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="20"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A40" s="23"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D40" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E40" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="18" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A41" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B41" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C41" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="D40" s="7"/>
-      <c r="E40" s="5" t="s">
+      <c r="D41" s="7"/>
+      <c r="E41" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="19"/>
-      <c r="B41" s="5" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A42" s="22"/>
+      <c r="B42" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5" t="s">
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="20"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A43" s="23"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D43" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E43" s="5" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="18" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A44" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="5" t="s">
+      <c r="B44" s="5"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="5" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="20"/>
-      <c r="B44" s="5" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A45" s="23"/>
+      <c r="B45" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5" t="s">
-        <v>162</v>
-      </c>
+      <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A46" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="10" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A47" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="7" t="s">
+      <c r="B47" s="5"/>
+      <c r="C47" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="D46" s="7"/>
-      <c r="E46" s="15"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="10" t="s">
+      <c r="D47" s="7"/>
+      <c r="E47" s="13"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A48" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="15" t="s">
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="13" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="21" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A49" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B49" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C49" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="D48" s="5"/>
-      <c r="E48" s="22" t="s">
+      <c r="D49" s="5"/>
+      <c r="E49" s="18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A49" s="21"/>
-      <c r="B49" s="5" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A50" s="19"/>
+      <c r="B50" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="22"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A50" s="21"/>
-      <c r="B50" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
-      <c r="E50" s="5" t="s">
-        <v>90</v>
-      </c>
+      <c r="E50" s="18"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A51" s="21"/>
+      <c r="A51" s="19"/>
       <c r="B51" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A52" s="21" t="s">
-        <v>92</v>
-      </c>
+      <c r="A52" s="19"/>
       <c r="B52" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>177</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A53" s="21"/>
-      <c r="B53" s="5"/>
+      <c r="A53" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="C53" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5" t="s">
-        <v>179</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A54" s="21"/>
-      <c r="B54" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="A54" s="19"/>
+      <c r="B54" s="5"/>
       <c r="C54" s="5" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A55" s="19"/>
+      <c r="B55" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A55" s="18" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A56" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B56" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="22" t="s">
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="18" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" s="19"/>
-      <c r="B56" s="5" t="s">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A57" s="22"/>
+      <c r="B57" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C57" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="D57" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="E56" s="22"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A57" s="19"/>
-      <c r="B57" s="5" t="s">
+      <c r="E57" s="18"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A58" s="22"/>
+      <c r="B58" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="22"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A58" s="19"/>
-      <c r="B58" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
-      <c r="E58" s="5" t="s">
-        <v>97</v>
-      </c>
+      <c r="E58" s="18"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A59" s="19"/>
+      <c r="A59" s="22"/>
       <c r="B59" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60" s="19"/>
+      <c r="A60" s="22"/>
       <c r="B60" s="5" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A61" s="19"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5" t="s">
-        <v>138</v>
-      </c>
+      <c r="A61" s="22"/>
+      <c r="B61" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A62" s="19"/>
+      <c r="A62" s="22"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A63" s="20"/>
+      <c r="A63" s="22"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A64" s="23"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A64" s="21" t="s">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A65" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B65" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C65" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="D65" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="E64" s="5" t="s">
+      <c r="E65" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A65" s="21"/>
-      <c r="B65" s="5" t="s">
+    <row r="66" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A66" s="19"/>
+      <c r="B66" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C66" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="D65" s="7"/>
-      <c r="E65" s="5" t="s">
+      <c r="D66" s="7"/>
+      <c r="E66" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A66" s="10" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A67" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-    </row>
-    <row r="67" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A67" s="26" t="s">
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+    </row>
+    <row r="68" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A68" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B68" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C67" s="7" t="s">
+      <c r="C68" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="D67" s="7" t="s">
+      <c r="D68" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="E67" s="5" t="s">
+      <c r="E68" s="5" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A68" s="27"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="7" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A69" s="25"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D68" s="7"/>
-      <c r="E68" s="5" t="s">
+      <c r="D69" s="7"/>
+      <c r="E69" s="5" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A69" s="25" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A70" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B70" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C70" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="D69" s="5"/>
-      <c r="E69" s="6" t="s">
+      <c r="D70" s="5"/>
+      <c r="E70" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A70" s="25"/>
-      <c r="B70" s="5" t="s">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A71" s="20"/>
+      <c r="B71" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C71" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="D70" s="5"/>
-      <c r="E70" s="14" t="s">
+      <c r="D71" s="5"/>
+      <c r="E71" s="17" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A71" s="21" t="s">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A72" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B72" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C71" s="5" t="s">
+      <c r="C72" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="D71" s="5" t="s">
+      <c r="D72" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="E71" s="22" t="s">
+      <c r="E72" s="18" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A72" s="21"/>
-      <c r="B72" s="5" t="s">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A73" s="19"/>
+      <c r="B73" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
-      <c r="E72" s="22"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A73" s="21" t="s">
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="18"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A74" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B74" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C74" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5" t="s">
+      <c r="D74" s="5"/>
+      <c r="E74" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A74" s="21"/>
-      <c r="B74" s="5" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A75" s="19"/>
+      <c r="B75" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C74" s="7" t="s">
+      <c r="C75" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="D74" s="7" t="s">
+      <c r="D75" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="E74" s="22" t="s">
+      <c r="E75" s="18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A75" s="21"/>
-      <c r="B75" s="5" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A76" s="19"/>
+      <c r="B76" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
-      <c r="E75" s="22"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A76" s="21"/>
-      <c r="B76" s="5" t="s">
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="18"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A77" s="19"/>
+      <c r="B77" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C77" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A77" s="21"/>
-      <c r="B77" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C77" s="5"/>
       <c r="D77" s="5"/>
       <c r="E77" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A78" s="21" t="s">
-        <v>119</v>
-      </c>
+      <c r="A78" s="19"/>
       <c r="B78" s="5" t="s">
-        <v>120</v>
+        <v>82</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A79" s="21"/>
+      <c r="A79" s="19" t="s">
+        <v>119</v>
+      </c>
       <c r="B79" s="5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A80" s="19"/>
+      <c r="B80" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5" t="s">
         <v>126</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E79"/>
+  <autoFilter ref="A2:E80"/>
   <mergeCells count="29">
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="A73:A77"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="E55:E57"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="A55:A63"/>
-    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A33:A35"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="E26:E27"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A36:A37"/>
     <mergeCell ref="A24:A31"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="E30:E31"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="A74:A78"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="E56:E58"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="A70:A71"/>
+    <mergeCell ref="A56:A64"/>
+    <mergeCell ref="A68:A69"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2631,7 +2652,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2648,7 +2669,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="21"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="5"/>
       <c r="C3" s="7" t="s">
         <v>252</v>
@@ -2661,7 +2682,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="14" t="s">
         <v>200</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -2676,7 +2697,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="14" t="s">
         <v>201</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -2691,7 +2712,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="14" t="s">
         <v>102</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -2704,7 +2725,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="14" t="s">
         <v>204</v>
       </c>
       <c r="B7" s="5"/>
@@ -2717,7 +2738,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="14" t="s">
         <v>209</v>
       </c>
       <c r="B8" s="5"/>
@@ -2730,7 +2751,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="14" t="s">
         <v>170</v>
       </c>
       <c r="B9" s="5"/>
@@ -2743,7 +2764,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="14" t="s">
         <v>173</v>
       </c>
       <c r="B10" s="5"/>
@@ -2758,7 +2779,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="14" t="s">
         <v>224</v>
       </c>
       <c r="B11" s="5"/>
@@ -2773,7 +2794,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="14" t="s">
         <v>250</v>
       </c>
       <c r="B12" s="5"/>
@@ -2788,7 +2809,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="10" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2807,9 +2828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2947,7 +2966,9 @@
       <c r="A15" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="5" t="s">
+        <v>192</v>
+      </c>
       <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Update on 20250913 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="257">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -623,10 +623,6 @@
   </si>
   <si>
     <t>官网提供卫视,广西自治区和部分广西地方频道在线观看,可使用酷9JS脚本的Webview方式观看*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>官网提供卫视,青海省频道在线观看,可使用酷9JS脚本的Webview方式观看*</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1026,6 +1022,18 @@
   </si>
   <si>
     <t>卫视,湖北省频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qinghai.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>liaoning_bfgd.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PHP脚本仅中国大陆可访问</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1587,13 +1595,13 @@
         <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>213</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>0</v>
@@ -1627,10 +1635,10 @@
       <c r="A5" s="23"/>
       <c r="B5" s="5"/>
       <c r="C5" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>132</v>
@@ -1644,10 +1652,10 @@
         <v>9</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>233</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>234</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>12</v>
@@ -1679,11 +1687,11 @@
       <c r="A9" s="23"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
@@ -1694,7 +1702,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="5" t="s">
@@ -1707,13 +1715,13 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>243</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
@@ -1724,7 +1732,7 @@
         <v>20</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="s">
@@ -1735,13 +1743,13 @@
       <c r="A13" s="19"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>235</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
@@ -1763,10 +1771,10 @@
         <v>23</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>24</v>
@@ -1791,10 +1799,10 @@
         <v>28</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>30</v>
@@ -1806,7 +1814,7 @@
         <v>29</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5" t="s">
@@ -1832,7 +1840,7 @@
         <v>129</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5" t="s">
@@ -1845,11 +1853,11 @@
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
@@ -1873,7 +1881,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
@@ -1899,11 +1907,11 @@
       <c r="A25" s="19"/>
       <c r="B25" s="27"/>
       <c r="C25" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
@@ -1912,7 +1920,7 @@
         <v>37</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="18" t="s">
@@ -1978,7 +1986,7 @@
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
@@ -1987,37 +1995,37 @@
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>253</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="22"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>231</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="23"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
@@ -2028,7 +2036,7 @@
         <v>50</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="17" t="s">
@@ -2052,11 +2060,11 @@
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
@@ -2067,7 +2075,7 @@
         <v>100</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="5" t="s">
@@ -2081,7 +2089,7 @@
         <v>136</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>137</v>
@@ -2095,7 +2103,7 @@
         <v>55</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="5" t="s">
@@ -2117,13 +2125,13 @@
       <c r="A43" s="23"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>227</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
@@ -2131,10 +2139,14 @@
         <v>83</v>
       </c>
       <c r="B44" s="5"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
+      <c r="C44" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>256</v>
+      </c>
       <c r="E44" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
@@ -2154,11 +2166,11 @@
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
@@ -2167,7 +2179,7 @@
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="13"/>
@@ -2177,11 +2189,11 @@
         <v>152</v>
       </c>
       <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
+      <c r="C48" s="5" t="s">
+        <v>254</v>
+      </c>
       <c r="D48" s="5"/>
-      <c r="E48" s="13" t="s">
-        <v>155</v>
-      </c>
+      <c r="E48" s="13"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" s="19" t="s">
@@ -2191,7 +2203,7 @@
         <v>61</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="18" t="s">
@@ -2237,7 +2249,7 @@
         <v>115</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5" t="s">
@@ -2248,11 +2260,11 @@
       <c r="A54" s="19"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
@@ -2261,7 +2273,7 @@
         <v>93</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5" t="s">
@@ -2287,10 +2299,10 @@
         <v>95</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E57" s="18"/>
     </row>
@@ -2377,10 +2389,10 @@
         <v>112</v>
       </c>
       <c r="C65" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D65" s="5" t="s">
         <v>237</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>238</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>113</v>
@@ -2392,7 +2404,7 @@
         <v>65</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="5" t="s">
@@ -2416,24 +2428,24 @@
         <v>106</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A69" s="25"/>
       <c r="B69" s="5"/>
       <c r="C69" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D69" s="7"/>
       <c r="E69" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.15">
@@ -2457,7 +2469,7 @@
         <v>109</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="17" t="s">
@@ -2472,10 +2484,10 @@
         <v>70</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E72" s="18" t="s">
         <v>72</v>
@@ -2498,7 +2510,7 @@
         <v>73</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="5" t="s">
@@ -2511,10 +2523,10 @@
         <v>75</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E75" s="18" t="s">
         <v>76</v>
@@ -2535,7 +2547,7 @@
         <v>78</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D77" s="5"/>
       <c r="E77" s="5" t="s">
@@ -2639,13 +2651,13 @@
         <v>7</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>216</v>
-      </c>
       <c r="D1" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>0</v>
@@ -2659,56 +2671,56 @@
         <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="19"/>
       <c r="B3" s="5"/>
       <c r="C3" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -2726,86 +2738,86 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
@@ -2843,10 +2855,10 @@
         <v>10</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -2854,7 +2866,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -2863,7 +2875,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -2872,7 +2884,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -2888,7 +2900,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C6" s="5"/>
     </row>
@@ -2897,7 +2909,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C7" s="5"/>
     </row>
@@ -2907,7 +2919,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
@@ -2922,7 +2934,7 @@
         <v>127</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C10" s="5"/>
     </row>
@@ -2931,7 +2943,7 @@
         <v>146</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C11" s="5"/>
     </row>
@@ -2940,7 +2952,7 @@
         <v>32</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C12" s="5"/>
     </row>
@@ -2949,7 +2961,7 @@
         <v>34</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C13" s="5"/>
     </row>
@@ -2959,7 +2971,7 @@
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
@@ -2967,7 +2979,7 @@
         <v>148</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C15" s="5"/>
     </row>
@@ -2976,7 +2988,7 @@
         <v>49</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C16" s="5"/>
     </row>
@@ -2986,7 +2998,7 @@
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
@@ -2994,7 +3006,7 @@
         <v>99</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C18" s="5"/>
     </row>
@@ -3009,7 +3021,9 @@
       <c r="A20" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B20" s="5"/>
+      <c r="B20" s="5" t="s">
+        <v>191</v>
+      </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
@@ -3017,7 +3031,7 @@
         <v>150</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C21" s="5"/>
     </row>
@@ -3026,7 +3040,7 @@
         <v>151</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C22" s="5"/>
     </row>
@@ -3034,7 +3048,9 @@
       <c r="A23" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B23" s="5"/>
+      <c r="B23" s="5" t="s">
+        <v>191</v>
+      </c>
       <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
@@ -3042,7 +3058,7 @@
         <v>59</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C24" s="5"/>
     </row>
@@ -3051,7 +3067,7 @@
         <v>92</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C25" s="5"/>
     </row>
@@ -3060,7 +3076,7 @@
         <v>60</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C26" s="5"/>
     </row>
@@ -3069,7 +3085,7 @@
         <v>64</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C27" s="5"/>
     </row>
@@ -3085,7 +3101,7 @@
         <v>122</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C29" s="5"/>
     </row>
@@ -3094,7 +3110,7 @@
         <v>123</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C30" s="5"/>
     </row>
@@ -3103,7 +3119,7 @@
         <v>67</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C31" s="5"/>
     </row>
@@ -3112,7 +3128,7 @@
         <v>68</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C32" s="5"/>
     </row>
@@ -3121,7 +3137,7 @@
         <v>119</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C33" s="5"/>
     </row>

</xml_diff>

<commit_message>
Update on 20250915 part 4
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -883,10 +883,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>gansu.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>hangzhou.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1034,6 +1030,11 @@
   </si>
   <si>
     <t>PHP脚本仅中国大陆可访问</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gansu_app.php
+gansu.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1234,15 +1235,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1252,17 +1244,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1608,7 +1609,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1618,21 +1619,21 @@
         <v>131</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="22" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="22"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="18"/>
+      <c r="E4" s="22"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="23"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="5"/>
       <c r="C5" s="7" t="s">
         <v>218</v>
@@ -1645,24 +1646,24 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>232</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>233</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="22"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1673,7 +1674,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="22"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1684,7 +1685,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="23"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
         <v>185</v>
@@ -1715,17 +1716,17 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>243</v>
-      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1740,20 +1741,20 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="19"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>235</v>
-      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="19"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="5" t="s">
         <v>117</v>
       </c>
@@ -1763,15 +1764,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="19" t="s">
+    <row r="15" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A15" s="21" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>219</v>
+      <c r="C15" s="7" t="s">
+        <v>256</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>217</v>
@@ -1781,7 +1782,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="19"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="5" t="s">
         <v>25</v>
       </c>
@@ -1792,14 +1793,14 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="21" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>217</v>
@@ -1809,7 +1810,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="19"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="5" t="s">
         <v>29</v>
       </c>
@@ -1861,7 +1862,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="21" t="s">
         <v>32</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -1876,7 +1877,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="19"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="5" t="s">
         <v>47</v>
       </c>
@@ -1889,10 +1890,10 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="23" t="s">
         <v>35</v>
       </c>
       <c r="C24" s="5" t="s">
@@ -1904,8 +1905,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="19"/>
-      <c r="B25" s="27"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="24"/>
       <c r="C25" s="5" t="s">
         <v>182</v>
       </c>
@@ -1915,7 +1916,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="19"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="5" t="s">
         <v>37</v>
       </c>
@@ -1923,21 +1924,21 @@
         <v>163</v>
       </c>
       <c r="D26" s="5"/>
-      <c r="E26" s="18" t="s">
+      <c r="E26" s="22" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="19"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="18"/>
+      <c r="E27" s="22"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="19"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="5" t="s">
         <v>40</v>
       </c>
@@ -1948,7 +1949,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="19"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="5" t="s">
         <v>42</v>
       </c>
@@ -1959,24 +1960,24 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="19"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="18" t="s">
+      <c r="E30" s="22" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="19"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="18"/>
+      <c r="E31" s="22"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="16" t="s">
@@ -1990,46 +1991,46 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="18" t="s">
         <v>148</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>253</v>
-      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" s="22"/>
+      <c r="A34" s="19"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>217</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="23"/>
+      <c r="A35" s="20"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -2044,7 +2045,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="19"/>
+      <c r="A37" s="21"/>
       <c r="B37" s="5" t="s">
         <v>52</v>
       </c>
@@ -2068,7 +2069,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="21" t="s">
+      <c r="A39" s="18" t="s">
         <v>99</v>
       </c>
       <c r="B39" s="5" t="s">
@@ -2083,7 +2084,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="23"/>
+      <c r="A40" s="20"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5" t="s">
         <v>136</v>
@@ -2096,14 +2097,14 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="21" t="s">
+      <c r="A41" s="18" t="s">
         <v>54</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="5" t="s">
@@ -2111,7 +2112,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="22"/>
+      <c r="A42" s="19"/>
       <c r="B42" s="5" t="s">
         <v>57</v>
       </c>
@@ -2122,35 +2123,35 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="23"/>
+      <c r="A43" s="20"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>217</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="21" t="s">
+      <c r="A44" s="18" t="s">
         <v>83</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="D44" s="7" t="s">
         <v>255</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>256</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="23"/>
+      <c r="A45" s="20"/>
       <c r="B45" s="5" t="s">
         <v>84</v>
       </c>
@@ -2190,13 +2191,13 @@
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="13"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A49" s="19" t="s">
+      <c r="A49" s="21" t="s">
         <v>59</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -2206,21 +2207,21 @@
         <v>164</v>
       </c>
       <c r="D49" s="5"/>
-      <c r="E49" s="18" t="s">
+      <c r="E49" s="22" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A50" s="19"/>
+      <c r="A50" s="21"/>
       <c r="B50" s="5" t="s">
         <v>87</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
-      <c r="E50" s="18"/>
+      <c r="E50" s="22"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A51" s="19"/>
+      <c r="A51" s="21"/>
       <c r="B51" s="5" t="s">
         <v>88</v>
       </c>
@@ -2231,7 +2232,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A52" s="19"/>
+      <c r="A52" s="21"/>
       <c r="B52" s="5" t="s">
         <v>89</v>
       </c>
@@ -2242,7 +2243,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A53" s="19" t="s">
+      <c r="A53" s="21" t="s">
         <v>92</v>
       </c>
       <c r="B53" s="5" t="s">
@@ -2257,7 +2258,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A54" s="19"/>
+      <c r="A54" s="21"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5" t="s">
         <v>177</v>
@@ -2268,7 +2269,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A55" s="19"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="5" t="s">
         <v>93</v>
       </c>
@@ -2281,7 +2282,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="18" t="s">
         <v>60</v>
       </c>
       <c r="B56" s="5" t="s">
@@ -2289,34 +2290,34 @@
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
-      <c r="E56" s="18" t="s">
+      <c r="E56" s="22" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A57" s="22"/>
+      <c r="A57" s="19"/>
       <c r="B57" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="E57" s="18"/>
+        <v>227</v>
+      </c>
+      <c r="E57" s="22"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A58" s="22"/>
+      <c r="A58" s="19"/>
       <c r="B58" s="5" t="s">
         <v>114</v>
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
-      <c r="E58" s="18"/>
+      <c r="E58" s="22"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A59" s="22"/>
+      <c r="A59" s="19"/>
       <c r="B59" s="5" t="s">
         <v>96</v>
       </c>
@@ -2327,7 +2328,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60" s="22"/>
+      <c r="A60" s="19"/>
       <c r="B60" s="5" t="s">
         <v>98</v>
       </c>
@@ -2338,7 +2339,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A61" s="22"/>
+      <c r="A61" s="19"/>
       <c r="B61" s="5" t="s">
         <v>107</v>
       </c>
@@ -2349,7 +2350,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A62" s="22"/>
+      <c r="A62" s="19"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
         <v>138</v>
@@ -2360,7 +2361,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A63" s="22"/>
+      <c r="A63" s="19"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
         <v>139</v>
@@ -2371,7 +2372,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A64" s="23"/>
+      <c r="A64" s="20"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5" t="s">
         <v>140</v>
@@ -2382,24 +2383,24 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A65" s="19" t="s">
+      <c r="A65" s="21" t="s">
         <v>64</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>112</v>
       </c>
       <c r="C65" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="D65" s="5" t="s">
         <v>236</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>237</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A66" s="19"/>
+      <c r="A66" s="21"/>
       <c r="B66" s="5" t="s">
         <v>65</v>
       </c>
@@ -2421,14 +2422,14 @@
       <c r="E67" s="5"/>
     </row>
     <row r="68" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A68" s="24" t="s">
+      <c r="A68" s="26" t="s">
         <v>122</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>106</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>217</v>
@@ -2438,7 +2439,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A69" s="25"/>
+      <c r="A69" s="27"/>
       <c r="B69" s="5"/>
       <c r="C69" s="7" t="s">
         <v>180</v>
@@ -2449,7 +2450,7 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A70" s="20" t="s">
+      <c r="A70" s="25" t="s">
         <v>123</v>
       </c>
       <c r="B70" s="5" t="s">
@@ -2464,12 +2465,12 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A71" s="20"/>
+      <c r="A71" s="25"/>
       <c r="B71" s="5" t="s">
         <v>109</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="17" t="s">
@@ -2477,33 +2478,33 @@
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A72" s="19" t="s">
+      <c r="A72" s="21" t="s">
         <v>67</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>70</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="E72" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="E72" s="22" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A73" s="19"/>
+      <c r="A73" s="21"/>
       <c r="B73" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
-      <c r="E73" s="18"/>
+      <c r="E73" s="22"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A74" s="19" t="s">
+      <c r="A74" s="21" t="s">
         <v>68</v>
       </c>
       <c r="B74" s="5" t="s">
@@ -2518,31 +2519,31 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A75" s="19"/>
+      <c r="A75" s="21"/>
       <c r="B75" s="5" t="s">
         <v>75</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D75" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="E75" s="18" t="s">
+      <c r="E75" s="22" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A76" s="19"/>
+      <c r="A76" s="21"/>
       <c r="B76" s="5" t="s">
         <v>77</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
-      <c r="E76" s="18"/>
+      <c r="E76" s="22"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A77" s="19"/>
+      <c r="A77" s="21"/>
       <c r="B77" s="5" t="s">
         <v>78</v>
       </c>
@@ -2555,7 +2556,7 @@
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A78" s="19"/>
+      <c r="A78" s="21"/>
       <c r="B78" s="5" t="s">
         <v>82</v>
       </c>
@@ -2566,7 +2567,7 @@
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A79" s="19" t="s">
+      <c r="A79" s="21" t="s">
         <v>119</v>
       </c>
       <c r="B79" s="5" t="s">
@@ -2579,7 +2580,7 @@
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A80" s="19"/>
+      <c r="A80" s="21"/>
       <c r="B80" s="5" t="s">
         <v>125</v>
       </c>
@@ -2592,23 +2593,6 @@
   </sheetData>
   <autoFilter ref="A2:E80"/>
   <mergeCells count="29">
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A24:A31"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B24:B25"/>
     <mergeCell ref="E49:E50"/>
     <mergeCell ref="A49:A52"/>
     <mergeCell ref="E75:E76"/>
@@ -2621,6 +2605,23 @@
     <mergeCell ref="A70:A71"/>
     <mergeCell ref="A56:A64"/>
     <mergeCell ref="A68:A69"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A24:A31"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A33:A35"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2664,14 +2665,14 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>217</v>
@@ -2681,10 +2682,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="19"/>
+      <c r="A3" s="21"/>
       <c r="B3" s="5"/>
       <c r="C3" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>217</v>
@@ -2787,37 +2788,37 @@
         <v>217</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>217</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>217</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Update on 20250922 part 4
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -13,7 +13,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他JS脚本!$A$1:$E$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">省份JS脚本!$A$2:$E$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">省份JS脚本!$A$2:$E$84</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">省份统计!$A$1:$C$33</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="266">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1054,15 +1054,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>吉林省下属延边朝鲜族自治州有脚本可看卫视和省级频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>jiangxi.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>卫视,江西省频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jltv.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PHP脚本仅中国大陆可访问</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卫视,吉林省频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1208,7 +1216,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1254,9 +1262,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1266,35 +1271,35 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1597,7 +1602,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1623,7 +1628,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1640,7 +1645,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1650,21 +1655,21 @@
         <v>131</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="25" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="22"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="19"/>
+      <c r="E4" s="25"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="23"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="5"/>
       <c r="C5" s="7" t="s">
         <v>216</v>
@@ -1672,12 +1677,12 @@
       <c r="D5" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1694,7 +1699,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="22"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1705,7 +1710,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="22"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1716,7 +1721,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="23"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
         <v>185</v>
@@ -1727,7 +1732,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1742,7 +1747,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>144</v>
       </c>
       <c r="B11" s="5"/>
@@ -1757,7 +1762,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1772,7 +1777,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="20"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
         <v>231</v>
@@ -1785,7 +1790,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="20"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="5" t="s">
         <v>117</v>
       </c>
@@ -1796,7 +1801,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="21" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -1813,7 +1818,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="20"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="5" t="s">
         <v>25</v>
       </c>
@@ -1824,7 +1829,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="18" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="5"/>
@@ -1839,7 +1844,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A18" s="22"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="5" t="s">
         <v>28</v>
       </c>
@@ -1854,7 +1859,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="23"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="5" t="s">
         <v>29</v>
       </c>
@@ -1867,7 +1872,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="15" t="s">
         <v>145</v>
       </c>
       <c r="B20" s="5"/>
@@ -1878,7 +1883,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="15" t="s">
         <v>127</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -1893,7 +1898,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="15" t="s">
         <v>146</v>
       </c>
       <c r="B22" s="5"/>
@@ -1906,7 +1911,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="21" t="s">
         <v>32</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1921,7 +1926,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="20"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="5" t="s">
         <v>47</v>
       </c>
@@ -1934,7 +1939,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="21" t="s">
         <v>34</v>
       </c>
       <c r="B25" s="26" t="s">
@@ -1949,7 +1954,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="20"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="27"/>
       <c r="C26" s="5" t="s">
         <v>182</v>
@@ -1960,7 +1965,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="20"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="5" t="s">
         <v>37</v>
       </c>
@@ -1968,21 +1973,21 @@
         <v>163</v>
       </c>
       <c r="D27" s="5"/>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="25" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="20"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="19"/>
+      <c r="E28" s="25"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="20"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="5" t="s">
         <v>40</v>
       </c>
@@ -1993,7 +1998,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="20"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="5" t="s">
         <v>42</v>
       </c>
@@ -2004,27 +2009,27 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="20"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="19" t="s">
+      <c r="E31" s="25" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" s="20"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="19"/>
+      <c r="E32" s="25"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="15" t="s">
         <v>147</v>
       </c>
       <c r="B33" s="5"/>
@@ -2035,7 +2040,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="18" t="s">
         <v>148</v>
       </c>
       <c r="B34" s="5"/>
@@ -2050,7 +2055,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="22"/>
+      <c r="A35" s="20"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
         <v>227</v>
@@ -2063,7 +2068,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="23"/>
+      <c r="A36" s="19"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5" t="s">
         <v>236</v>
@@ -2074,7 +2079,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="20" t="s">
+      <c r="A37" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B37" s="5" t="s">
@@ -2084,12 +2089,12 @@
         <v>155</v>
       </c>
       <c r="D37" s="5"/>
-      <c r="E37" s="17" t="s">
+      <c r="E37" s="16" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="20"/>
+      <c r="A38" s="21"/>
       <c r="B38" s="5" t="s">
         <v>52</v>
       </c>
@@ -2100,575 +2105,591 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="15" t="s">
+      <c r="A39" s="18" t="s">
         <v>149</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A40" s="19"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5" t="s">
         <v>166</v>
-      </c>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>189</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A41" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="23"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="21" t="s">
-        <v>54</v>
-      </c>
+      <c r="A42" s="19"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="D42" s="7"/>
+        <v>136</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>215</v>
+      </c>
       <c r="E42" s="5" t="s">
-        <v>263</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="22"/>
-      <c r="B43" s="5" t="s">
-        <v>55</v>
-      </c>
+      <c r="A43" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A44" s="20"/>
+      <c r="B44" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="D44" s="7"/>
+      <c r="E44" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="22"/>
-      <c r="B44" s="5" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A45" s="20"/>
+      <c r="B45" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5" t="s">
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="23"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A46" s="19"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D46" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E46" s="5" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="21" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A47" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="7" t="s">
+      <c r="B47" s="5"/>
+      <c r="C47" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D47" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E47" s="5" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="23"/>
-      <c r="B47" s="5" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A48" s="19"/>
+      <c r="B48" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5" t="s">
-        <v>161</v>
-      </c>
+      <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A49" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A49" s="16" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A50" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="7" t="s">
+      <c r="B50" s="5"/>
+      <c r="C50" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="D49" s="7"/>
-      <c r="E49" s="13"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A50" s="16" t="s">
+      <c r="D50" s="7"/>
+      <c r="E50" s="13"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A51" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5" t="s">
+      <c r="B51" s="5"/>
+      <c r="C51" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="D50" s="5"/>
-      <c r="E50" s="13"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A51" s="20" t="s">
+      <c r="D51" s="5"/>
+      <c r="E51" s="13"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A52" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B52" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C52" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="D51" s="5"/>
-      <c r="E51" s="19" t="s">
+      <c r="D52" s="5"/>
+      <c r="E52" s="25" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A52" s="20"/>
-      <c r="B52" s="5" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A53" s="21"/>
+      <c r="B53" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="19"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A53" s="20"/>
-      <c r="B53" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
-      <c r="E53" s="5" t="s">
-        <v>90</v>
-      </c>
+      <c r="E53" s="25"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A54" s="20"/>
+      <c r="A54" s="21"/>
       <c r="B54" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A55" s="20" t="s">
-        <v>92</v>
-      </c>
+      <c r="A55" s="21"/>
       <c r="B55" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>176</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" s="20"/>
-      <c r="B56" s="5"/>
+      <c r="A56" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="C56" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5" t="s">
-        <v>178</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A57" s="20"/>
-      <c r="B57" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="A57" s="21"/>
+      <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A58" s="21"/>
+      <c r="B58" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A58" s="21" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A59" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B59" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="19" t="s">
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="25" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A59" s="22"/>
-      <c r="B59" s="5" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A60" s="20"/>
+      <c r="B60" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C60" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D60" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="E59" s="19"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60" s="22"/>
-      <c r="B60" s="5" t="s">
+      <c r="E60" s="25"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A61" s="20"/>
+      <c r="B61" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="19"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A61" s="22"/>
-      <c r="B61" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
-      <c r="E61" s="5" t="s">
-        <v>97</v>
-      </c>
+      <c r="E61" s="25"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A62" s="22"/>
+      <c r="A62" s="20"/>
       <c r="B62" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A63" s="22"/>
+      <c r="A63" s="20"/>
       <c r="B63" s="5" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A64" s="22"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5" t="s">
-        <v>138</v>
-      </c>
+      <c r="A64" s="20"/>
+      <c r="B64" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A65" s="22"/>
+      <c r="A65" s="20"/>
       <c r="B65" s="5"/>
       <c r="C65" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A66" s="23"/>
+      <c r="A66" s="20"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A67" s="19"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A67" s="20" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A68" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B68" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C68" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="D68" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="E67" s="5" t="s">
+      <c r="E68" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A68" s="20"/>
-      <c r="B68" s="5" t="s">
+    <row r="69" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A69" s="21"/>
+      <c r="B69" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="C69" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="D68" s="7"/>
-      <c r="E68" s="5" t="s">
+      <c r="D69" s="7"/>
+      <c r="E69" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A69" s="16" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A70" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-    </row>
-    <row r="70" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A70" s="24" t="s">
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+    </row>
+    <row r="71" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A71" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B71" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="C71" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="D71" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="E70" s="5" t="s">
+      <c r="E71" s="5" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A71" s="25"/>
-      <c r="B71" s="5"/>
-      <c r="C71" s="7" t="s">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A72" s="24"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="D71" s="7"/>
-      <c r="E71" s="5" t="s">
+      <c r="D72" s="7"/>
+      <c r="E72" s="5" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A72" s="24" t="s">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A73" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B73" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C72" s="5" t="s">
+      <c r="C73" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="D72" s="5"/>
-      <c r="E72" s="6" t="s">
+      <c r="D73" s="5"/>
+      <c r="E73" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A73" s="28"/>
-      <c r="B73" s="5" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A74" s="23"/>
+      <c r="B74" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C74" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="D73" s="5"/>
-      <c r="E73" s="17" t="s">
+      <c r="D74" s="5"/>
+      <c r="E74" s="16" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A74" s="25"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A75" s="24"/>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D75" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="E74" s="18" t="s">
+      <c r="E75" s="17" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A75" s="20" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A76" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B76" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="C76" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D76" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="E75" s="19" t="s">
+      <c r="E76" s="25" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A76" s="20"/>
-      <c r="B76" s="5" t="s">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A77" s="21"/>
+      <c r="B77" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
-      <c r="E76" s="19"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A77" s="20" t="s">
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="25"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A78" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B78" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C78" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5" t="s">
+      <c r="D78" s="5"/>
+      <c r="E78" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A78" s="20"/>
-      <c r="B78" s="5" t="s">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A79" s="21"/>
+      <c r="B79" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C78" s="7" t="s">
+      <c r="C79" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="D78" s="7" t="s">
+      <c r="D79" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="E78" s="19" t="s">
+      <c r="E79" s="25" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A79" s="20"/>
-      <c r="B79" s="5" t="s">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A80" s="21"/>
+      <c r="B80" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="19"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A80" s="20"/>
-      <c r="B80" s="5" t="s">
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="25"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A81" s="21"/>
+      <c r="B81" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C80" s="5" t="s">
+      <c r="C81" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A81" s="20"/>
-      <c r="B81" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A82" s="20" t="s">
-        <v>119</v>
-      </c>
+      <c r="A82" s="21"/>
       <c r="B82" s="5" t="s">
-        <v>120</v>
+        <v>82</v>
       </c>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="5" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A83" s="20"/>
+      <c r="A83" s="21" t="s">
+        <v>119</v>
+      </c>
       <c r="B83" s="5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
       <c r="E83" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A84" s="21"/>
+      <c r="B84" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5" t="s">
         <v>126</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E83"/>
-  <mergeCells count="29">
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="A42:A45"/>
+  <autoFilter ref="A2:E84"/>
+  <mergeCells count="30">
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="A78:A82"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="E59:E61"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="E76:E77"/>
+    <mergeCell ref="A59:A67"/>
+    <mergeCell ref="A71:A72"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="E27:E28"/>
     <mergeCell ref="A12:A14"/>
@@ -2679,17 +2700,15 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="A17:A19"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="E78:E79"/>
-    <mergeCell ref="A77:A81"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="E58:E60"/>
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="A58:A66"/>
-    <mergeCell ref="A70:A71"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A39:A40"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2733,7 +2752,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2750,7 +2769,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="20"/>
+      <c r="A3" s="21"/>
       <c r="B3" s="5"/>
       <c r="C3" s="7" t="s">
         <v>248</v>
@@ -3065,10 +3084,10 @@
       <c r="A17" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5" t="s">
-        <v>261</v>
-      </c>
+      <c r="B17" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">

</xml_diff>

<commit_message>
Update on 20251007 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -537,9 +537,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Shanghai_shtv.php</t>
-  </si>
-  <si>
     <t>上海教育电视台</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1084,6 +1081,12 @@
   </si>
   <si>
     <t>长春市频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shanghai_KanDongFang.php
+Shanghai_KanKanNews.php
+Shanghai_shtv.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1284,35 +1287,35 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1623,7 +1626,7 @@
   <cols>
     <col min="1" max="1" width="16.75" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.25" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="93.125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="1"/>
@@ -1645,74 +1648,74 @@
         <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>208</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="18" t="s">
+    <row r="3" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>131</v>
+      <c r="C3" s="7" t="s">
+        <v>268</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="20"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="25"/>
+      <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="19"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="5"/>
       <c r="C5" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>227</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>228</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="20"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1723,7 +1726,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="20"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1734,14 +1737,14 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="19"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
@@ -1752,7 +1755,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="5" t="s">
@@ -1761,28 +1764,28 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>238</v>
-      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="s">
@@ -1790,20 +1793,20 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="21"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>230</v>
-      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="21"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="5" t="s">
         <v>117</v>
       </c>
@@ -1814,24 +1817,24 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="19" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="21"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="5" t="s">
         <v>25</v>
       </c>
@@ -1842,42 +1845,42 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="20" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>258</v>
-      </c>
     </row>
     <row r="18" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A18" s="20"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="19"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5" t="s">
@@ -1886,13 +1889,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
@@ -1903,7 +1906,7 @@
         <v>129</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5" t="s">
@@ -1912,26 +1915,26 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="19" t="s">
         <v>32</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
@@ -1939,12 +1942,12 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="21"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5" t="s">
@@ -1952,14 +1955,14 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5" t="s">
@@ -1967,40 +1970,40 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="21"/>
-      <c r="B26" s="27"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="26"/>
       <c r="C26" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="21"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D27" s="5"/>
-      <c r="E27" s="25" t="s">
+      <c r="E27" s="18" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="21"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="25"/>
+      <c r="E28" s="18"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="21"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="5" t="s">
         <v>40</v>
       </c>
@@ -2011,7 +2014,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="21"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="5" t="s">
         <v>42</v>
       </c>
@@ -2022,84 +2025,84 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="21"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="25" t="s">
+      <c r="E31" s="18" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" s="21"/>
+      <c r="A32" s="19"/>
       <c r="B32" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="25"/>
+      <c r="E32" s="18"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="13" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" s="18" t="s">
-        <v>148</v>
+      <c r="A34" s="20" t="s">
+        <v>147</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>248</v>
-      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="20"/>
+      <c r="A35" s="21"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>226</v>
-      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="19"/>
+      <c r="A36" s="22"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="21" t="s">
+      <c r="A37" s="19" t="s">
         <v>49</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>50</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="16" t="s">
@@ -2107,7 +2110,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="21"/>
+      <c r="A38" s="19"/>
       <c r="B38" s="5" t="s">
         <v>52</v>
       </c>
@@ -2118,51 +2121,51 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="18" t="s">
-        <v>149</v>
+      <c r="A39" s="20" t="s">
+        <v>148</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="E39" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="E39" s="5" t="s">
-        <v>263</v>
-      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="20"/>
+      <c r="A40" s="21"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="19"/>
+      <c r="A41" s="22"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="18" t="s">
+      <c r="A42" s="20" t="s">
         <v>99</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>100</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5" t="s">
@@ -2170,38 +2173,38 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="19"/>
+      <c r="A43" s="22"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D43" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>137</v>
-      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="18" t="s">
+      <c r="A44" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="20"/>
+      <c r="A45" s="21"/>
       <c r="B45" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="5" t="s">
@@ -2209,7 +2212,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="20"/>
+      <c r="A46" s="21"/>
       <c r="B46" s="5" t="s">
         <v>57</v>
       </c>
@@ -2220,35 +2223,35 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="19"/>
+      <c r="A47" s="22"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E47" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="D47" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>222</v>
-      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="20" t="s">
         <v>83</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="D48" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="D48" s="7" t="s">
-        <v>251</v>
-      </c>
       <c r="E48" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A49" s="19"/>
+      <c r="A49" s="22"/>
       <c r="B49" s="5" t="s">
         <v>84</v>
       </c>
@@ -2260,65 +2263,65 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A50" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D51" s="7"/>
       <c r="E51" s="13"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A52" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="13"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A53" s="21" t="s">
+      <c r="A53" s="19" t="s">
         <v>59</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>61</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D53" s="5"/>
-      <c r="E53" s="25" t="s">
+      <c r="E53" s="18" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A54" s="21"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="5" t="s">
         <v>87</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
-      <c r="E54" s="25"/>
+      <c r="E54" s="18"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A55" s="21"/>
+      <c r="A55" s="19"/>
       <c r="B55" s="5" t="s">
         <v>88</v>
       </c>
@@ -2329,7 +2332,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" s="21"/>
+      <c r="A56" s="19"/>
       <c r="B56" s="5" t="s">
         <v>89</v>
       </c>
@@ -2340,14 +2343,14 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A57" s="21" t="s">
+      <c r="A57" s="19" t="s">
         <v>92</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>115</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5" t="s">
@@ -2355,23 +2358,23 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A58" s="21"/>
+      <c r="A58" s="19"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A59" s="21"/>
+      <c r="A59" s="19"/>
       <c r="B59" s="5" t="s">
         <v>93</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="5" t="s">
@@ -2379,7 +2382,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60" s="18" t="s">
+      <c r="A60" s="20" t="s">
         <v>60</v>
       </c>
       <c r="B60" s="5" t="s">
@@ -2387,34 +2390,34 @@
       </c>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
-      <c r="E60" s="25" t="s">
+      <c r="E60" s="18" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A61" s="20"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="E61" s="25"/>
+        <v>222</v>
+      </c>
+      <c r="E61" s="18"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A62" s="20"/>
+      <c r="A62" s="21"/>
       <c r="B62" s="5" t="s">
         <v>114</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
-      <c r="E62" s="25"/>
+      <c r="E62" s="18"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A63" s="20"/>
+      <c r="A63" s="21"/>
       <c r="B63" s="5" t="s">
         <v>96</v>
       </c>
@@ -2425,7 +2428,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A64" s="20"/>
+      <c r="A64" s="21"/>
       <c r="B64" s="5" t="s">
         <v>98</v>
       </c>
@@ -2436,7 +2439,7 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A65" s="20"/>
+      <c r="A65" s="21"/>
       <c r="B65" s="5" t="s">
         <v>107</v>
       </c>
@@ -2447,62 +2450,62 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A66" s="20"/>
+      <c r="A66" s="21"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A67" s="20"/>
+      <c r="A67" s="21"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A68" s="19"/>
+      <c r="A68" s="22"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A69" s="21" t="s">
+      <c r="A69" s="19" t="s">
         <v>64</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>112</v>
       </c>
       <c r="C69" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D69" s="5" t="s">
         <v>231</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>232</v>
       </c>
       <c r="E69" s="5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A70" s="21"/>
+      <c r="A70" s="19"/>
       <c r="B70" s="5" t="s">
         <v>65</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D70" s="7"/>
       <c r="E70" s="5" t="s">
@@ -2511,7 +2514,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A71" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
@@ -2519,42 +2522,42 @@
       <c r="E71" s="5"/>
     </row>
     <row r="72" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A72" s="22" t="s">
+      <c r="A72" s="23" t="s">
         <v>122</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>106</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A73" s="24"/>
       <c r="B73" s="5"/>
       <c r="C73" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D73" s="7"/>
       <c r="E73" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A74" s="22" t="s">
+      <c r="A74" s="23" t="s">
         <v>123</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>69</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="6" t="s">
@@ -2562,12 +2565,12 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A75" s="23"/>
+      <c r="A75" s="27"/>
       <c r="B75" s="5" t="s">
         <v>109</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="16" t="s">
@@ -2578,50 +2581,50 @@
       <c r="A76" s="24"/>
       <c r="B76" s="5"/>
       <c r="C76" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="D76" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="E76" s="17" t="s">
         <v>254</v>
       </c>
-      <c r="E76" s="17" t="s">
-        <v>255</v>
-      </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A77" s="21" t="s">
+      <c r="A77" s="19" t="s">
         <v>67</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>70</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="E77" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="E77" s="18" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A78" s="21"/>
+      <c r="A78" s="19"/>
       <c r="B78" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
-      <c r="E78" s="25"/>
+      <c r="E78" s="18"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A79" s="21" t="s">
+      <c r="A79" s="19" t="s">
         <v>68</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>73</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="5" t="s">
@@ -2629,36 +2632,36 @@
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A80" s="21"/>
+      <c r="A80" s="19"/>
       <c r="B80" s="5" t="s">
         <v>75</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="E80" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="E80" s="18" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A81" s="21"/>
+      <c r="A81" s="19"/>
       <c r="B81" s="5" t="s">
         <v>77</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
-      <c r="E81" s="25"/>
+      <c r="E81" s="18"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A82" s="21"/>
+      <c r="A82" s="19"/>
       <c r="B82" s="5" t="s">
         <v>78</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="5" t="s">
@@ -2666,7 +2669,7 @@
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A83" s="21"/>
+      <c r="A83" s="19"/>
       <c r="B83" s="5" t="s">
         <v>82</v>
       </c>
@@ -2677,7 +2680,7 @@
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A84" s="21" t="s">
+      <c r="A84" s="19" t="s">
         <v>119</v>
       </c>
       <c r="B84" s="5" t="s">
@@ -2690,7 +2693,7 @@
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A85" s="21"/>
+      <c r="A85" s="19"/>
       <c r="B85" s="5" t="s">
         <v>125</v>
       </c>
@@ -2703,6 +2706,25 @@
   </sheetData>
   <autoFilter ref="A2:E85"/>
   <mergeCells count="30">
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A17:A19"/>
     <mergeCell ref="E53:E54"/>
     <mergeCell ref="A53:A56"/>
     <mergeCell ref="E80:E81"/>
@@ -2714,25 +2736,6 @@
     <mergeCell ref="E77:E78"/>
     <mergeCell ref="A60:A68"/>
     <mergeCell ref="A72:A73"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A25:A32"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A39:A41"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2763,76 +2766,76 @@
         <v>7</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>211</v>
-      </c>
       <c r="D1" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="21"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="5"/>
       <c r="C3" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -2850,86 +2853,86 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
@@ -2967,10 +2970,10 @@
         <v>10</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -2978,7 +2981,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -2987,7 +2990,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -2996,17 +2999,17 @@
         <v>16</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
@@ -3014,7 +3017,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C6" s="5"/>
     </row>
@@ -3023,7 +3026,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C7" s="5"/>
     </row>
@@ -3032,13 +3035,13 @@
         <v>27</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -3048,16 +3051,16 @@
         <v>127</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C11" s="5"/>
     </row>
@@ -3066,7 +3069,7 @@
         <v>32</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C12" s="5"/>
     </row>
@@ -3075,25 +3078,25 @@
         <v>34</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C15" s="5"/>
     </row>
@@ -3102,16 +3105,16 @@
         <v>49</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C17" s="5"/>
     </row>
@@ -3120,7 +3123,7 @@
         <v>99</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C18" s="5"/>
     </row>
@@ -3129,7 +3132,7 @@
         <v>54</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C19" s="5"/>
     </row>
@@ -3138,34 +3141,34 @@
         <v>83</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C23" s="5"/>
     </row>
@@ -3174,7 +3177,7 @@
         <v>59</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C24" s="5"/>
     </row>
@@ -3183,7 +3186,7 @@
         <v>92</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C25" s="5"/>
     </row>
@@ -3192,7 +3195,7 @@
         <v>60</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C26" s="5"/>
     </row>
@@ -3201,13 +3204,13 @@
         <v>64</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -3217,7 +3220,7 @@
         <v>122</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C29" s="5"/>
     </row>
@@ -3226,7 +3229,7 @@
         <v>123</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C30" s="5"/>
     </row>
@@ -3235,7 +3238,7 @@
         <v>67</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C31" s="5"/>
     </row>
@@ -3244,7 +3247,7 @@
         <v>68</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C32" s="5"/>
     </row>
@@ -3253,7 +3256,7 @@
         <v>119</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C33" s="5"/>
     </row>

</xml_diff>

<commit_message>
Update on 20251007 part 6
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -13,7 +13,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他JS脚本!$A$1:$E$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">省份JS脚本!$A$2:$E$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">省份JS脚本!$A$2:$E$84</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">省份统计!$A$1:$C$33</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -21,21 +21,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="268">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>上海</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>KanKanNews.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>shanghai.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1087,6 +1079,12 @@
     <t>Shanghai_KanDongFang.php
 Shanghai_KanKanNews.php
 Shanghai_shtv.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KanDongFang.js
+shanghai.js
+KanKanNews.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1232,7 +1230,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1290,32 +1288,35 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1618,7 +1619,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1640,370 +1641,372 @@
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
       <c r="E1" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>2</v>
+      <c r="B3" s="7" t="s">
+        <v>267</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="20"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="21"/>
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="21"/>
-      <c r="B4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="18"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="22"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>227</v>
-      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="21"/>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="21"/>
-      <c r="B8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="5"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5" t="s">
+        <v>182</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A9" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="22"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="D9" s="5"/>
+      <c r="C9" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D9" s="7"/>
       <c r="E9" s="5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="5" t="s">
+      <c r="B11" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>236</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="D11" s="5"/>
       <c r="E11" s="5" t="s">
-        <v>237</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="22"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="22"/>
+      <c r="B13" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A14" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5" t="s">
+      <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="19"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="19"/>
-      <c r="B14" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="C14" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>210</v>
+      </c>
       <c r="E14" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A15" s="19" t="s">
         <v>22</v>
       </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="22"/>
       <c r="B15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>212</v>
-      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="19"/>
-      <c r="B16" s="5" t="s">
+      <c r="A16" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>254</v>
+      </c>
       <c r="E16" s="5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A17" s="21"/>
+      <c r="B17" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="20" t="s">
+      <c r="C17" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" s="20"/>
+      <c r="B18" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A18" s="21"/>
-      <c r="B18" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>212</v>
-      </c>
+      <c r="C18" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D18" s="5"/>
       <c r="E18" s="5" t="s">
-        <v>30</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="22"/>
-      <c r="B19" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>180</v>
-      </c>
+      <c r="A19" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="5" t="s">
-        <v>105</v>
+      <c r="E19" s="13" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
+        <v>125</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>153</v>
+      </c>
       <c r="D20" s="5"/>
-      <c r="E20" s="13" t="s">
-        <v>153</v>
+      <c r="E20" s="5" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>129</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="B21" s="5"/>
       <c r="C21" s="5" t="s">
         <v>155</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="B22" s="5"/>
+      <c r="A22" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="C22" s="5" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5" t="s">
-        <v>158</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="19" t="s">
-        <v>32</v>
-      </c>
+      <c r="A23" s="22"/>
       <c r="B23" s="5" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>132</v>
+        <v>184</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A24" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="27" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="19"/>
-      <c r="B24" s="5" t="s">
-        <v>47</v>
-      </c>
       <c r="C24" s="5" t="s">
-        <v>186</v>
+        <v>131</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>35</v>
-      </c>
+      <c r="A25" s="22"/>
+      <c r="B25" s="28"/>
       <c r="C25" s="5" t="s">
-        <v>133</v>
+        <v>179</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A26" s="22"/>
+      <c r="B26" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="26" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="19"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="19"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>162</v>
-      </c>
+      <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="26"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A28" s="22"/>
+      <c r="B28" s="5" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="19"/>
-      <c r="B28" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="18"/>
+      <c r="E28" s="5" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="19"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="5" t="s">
         <v>40</v>
       </c>
@@ -2014,188 +2017,190 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="19"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A31" s="22"/>
+      <c r="B31" s="5" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="19"/>
-      <c r="B31" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="18" t="s">
-        <v>46</v>
-      </c>
+      <c r="E31" s="26"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" s="19"/>
-      <c r="B32" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="A32" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="18"/>
+      <c r="E32" s="13" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="15" t="s">
-        <v>146</v>
+      <c r="A33" s="19" t="s">
+        <v>145</v>
       </c>
       <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="13" t="s">
-        <v>193</v>
+      <c r="C33" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" s="20" t="s">
-        <v>147</v>
-      </c>
+      <c r="A34" s="21"/>
       <c r="B34" s="5"/>
-      <c r="C34" s="9" t="s">
-        <v>246</v>
+      <c r="C34" s="5" t="s">
+        <v>222</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="21"/>
+      <c r="A35" s="20"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>212</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="D35" s="5"/>
       <c r="E35" s="5" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="22"/>
-      <c r="B36" s="5"/>
+      <c r="A36" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="C36" s="5" t="s">
-        <v>233</v>
+        <v>152</v>
       </c>
       <c r="D36" s="5"/>
-      <c r="E36" s="5" t="s">
-        <v>234</v>
+      <c r="E36" s="16" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="19" t="s">
-        <v>49</v>
-      </c>
+      <c r="A37" s="22"/>
       <c r="B37" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>154</v>
-      </c>
+      <c r="C37" s="5"/>
       <c r="D37" s="5"/>
-      <c r="E37" s="16" t="s">
+      <c r="E37" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="19"/>
-      <c r="B38" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
+      <c r="A38" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>259</v>
+      </c>
       <c r="E38" s="5" t="s">
-        <v>53</v>
+        <v>260</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="20" t="s">
-        <v>148</v>
-      </c>
+      <c r="A39" s="21"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>261</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="D39" s="5"/>
       <c r="E39" s="5" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="21"/>
+      <c r="A40" s="20"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5" t="s">
-        <v>266</v>
+        <v>163</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="5" t="s">
-        <v>267</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="22"/>
-      <c r="B41" s="5"/>
+      <c r="A41" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="C41" s="5" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5" t="s">
-        <v>164</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="A42" s="20"/>
+      <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="D42" s="5"/>
+        <v>133</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>210</v>
+      </c>
       <c r="E42" s="5" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="22"/>
+      <c r="A43" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>212</v>
-      </c>
+        <v>256</v>
+      </c>
+      <c r="D43" s="7"/>
       <c r="E43" s="5" t="s">
-        <v>136</v>
+        <v>257</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B44" s="5"/>
+      <c r="A44" s="21"/>
+      <c r="B44" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="C44" s="5" t="s">
-        <v>258</v>
+        <v>217</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="5" t="s">
-        <v>259</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
@@ -2203,218 +2208,216 @@
       <c r="B45" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="D45" s="7"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
       <c r="E45" s="5" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="21"/>
-      <c r="B46" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
+      <c r="A46" s="20"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>210</v>
+      </c>
       <c r="E46" s="5" t="s">
-        <v>58</v>
+        <v>219</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="22"/>
+      <c r="A47" s="19" t="s">
+        <v>81</v>
+      </c>
       <c r="B47" s="5"/>
-      <c r="C47" s="5" t="s">
-        <v>220</v>
+      <c r="C47" s="7" t="s">
+        <v>247</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>212</v>
+        <v>248</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>221</v>
+        <v>192</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>250</v>
-      </c>
+      <c r="A48" s="20"/>
+      <c r="B48" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
       <c r="E48" s="5" t="s">
-        <v>194</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A49" s="22"/>
-      <c r="B49" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C49" s="5"/>
+      <c r="A49" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5" t="s">
+        <v>158</v>
+      </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5" t="s">
-        <v>86</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A50" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B50" s="5"/>
-      <c r="C50" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5" t="s">
-        <v>159</v>
-      </c>
+      <c r="C50" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="D50" s="7"/>
+      <c r="E50" s="13"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B51" s="5"/>
-      <c r="C51" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="D51" s="7"/>
+      <c r="C51" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D51" s="5"/>
       <c r="E51" s="13"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A52" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="B52" s="5"/>
+      <c r="A52" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="C52" s="5" t="s">
-        <v>248</v>
+        <v>161</v>
       </c>
       <c r="D52" s="5"/>
-      <c r="E52" s="13"/>
+      <c r="E52" s="26" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A53" s="19" t="s">
-        <v>59</v>
-      </c>
+      <c r="A53" s="22"/>
       <c r="B53" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>163</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C53" s="5"/>
       <c r="D53" s="5"/>
-      <c r="E53" s="18" t="s">
-        <v>62</v>
-      </c>
+      <c r="E53" s="26"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A54" s="19"/>
+      <c r="A54" s="22"/>
       <c r="B54" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
-      <c r="E54" s="18"/>
+      <c r="E54" s="5" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A55" s="19"/>
+      <c r="A55" s="22"/>
       <c r="B55" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A56" s="22" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" s="19"/>
       <c r="B56" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C56" s="5"/>
+        <v>113</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>173</v>
+      </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A57" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>115</v>
-      </c>
+      <c r="A57" s="22"/>
+      <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5" t="s">
-        <v>116</v>
+        <v>175</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A58" s="19"/>
-      <c r="B58" s="5"/>
+      <c r="A58" s="22"/>
+      <c r="B58" s="5" t="s">
+        <v>91</v>
+      </c>
       <c r="C58" s="5" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5" t="s">
-        <v>177</v>
+        <v>92</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A59" s="19"/>
+      <c r="A59" s="19" t="s">
+        <v>58</v>
+      </c>
       <c r="B59" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A60" s="21"/>
+      <c r="B60" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="18" t="s">
-        <v>63</v>
-      </c>
+      <c r="C60" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E60" s="26"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A61" s="21"/>
       <c r="B61" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="E61" s="18"/>
+        <v>112</v>
+      </c>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="26"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A62" s="21"/>
       <c r="B62" s="5" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
-      <c r="E62" s="18"/>
+      <c r="E62" s="5" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A63" s="21"/>
@@ -2424,318 +2427,306 @@
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A64" s="21"/>
       <c r="B64" s="5" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A65" s="21"/>
-      <c r="B65" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C65" s="5"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5" t="s">
+        <v>135</v>
+      </c>
       <c r="D65" s="5"/>
       <c r="E65" s="5" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A66" s="21"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A67" s="21"/>
+      <c r="A67" s="20"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A68" s="22"/>
-      <c r="B68" s="5"/>
+      <c r="A68" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>110</v>
+      </c>
       <c r="C68" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="D68" s="5"/>
+        <v>228</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>229</v>
+      </c>
       <c r="E68" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A69" s="19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A69" s="22"/>
+      <c r="B69" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D69" s="7"/>
+      <c r="E69" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B69" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C69" s="5" t="s">
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A70" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+    </row>
+    <row r="71" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A71" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A72" s="25"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D72" s="7"/>
+      <c r="E72" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A73" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D73" s="5"/>
+      <c r="E73" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A74" s="24"/>
+      <c r="B74" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C74" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="D69" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A70" s="19"/>
-      <c r="B70" s="5" t="s">
+      <c r="D74" s="5"/>
+      <c r="E74" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A75" s="25"/>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="E75" s="17" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A76" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="C70" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="D70" s="7"/>
-      <c r="E70" s="5" t="s">
+      <c r="B76" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E76" s="26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A77" s="22"/>
+      <c r="B77" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="26"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A78" s="22" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A71" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-    </row>
-    <row r="72" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A72" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="D72" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A73" s="24"/>
-      <c r="B73" s="5"/>
-      <c r="C73" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="D73" s="7"/>
-      <c r="E73" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A74" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D74" s="5"/>
-      <c r="E74" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A75" s="27"/>
-      <c r="B75" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="D75" s="5"/>
-      <c r="E75" s="16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A76" s="24"/>
-      <c r="B76" s="5"/>
-      <c r="C76" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="E76" s="17" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A77" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="E77" s="18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A78" s="19"/>
       <c r="B78" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C78" s="5"/>
+      <c r="C78" s="5" t="s">
+        <v>164</v>
+      </c>
       <c r="D78" s="5"/>
-      <c r="E78" s="18"/>
+      <c r="E78" s="5" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A79" s="19" t="s">
-        <v>68</v>
-      </c>
+      <c r="A79" s="22"/>
       <c r="B79" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C79" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="D79" s="5"/>
-      <c r="E79" s="5" t="s">
+      <c r="C79" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E79" s="26" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A80" s="19"/>
+      <c r="A80" s="22"/>
       <c r="B80" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C80" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="D80" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="E80" s="18" t="s">
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="26"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A81" s="22"/>
+      <c r="B81" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A81" s="19"/>
-      <c r="B81" s="5" t="s">
+      <c r="C81" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
-      <c r="E81" s="18"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A82" s="19"/>
+      <c r="A82" s="22"/>
       <c r="B82" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>187</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="5" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A83" s="19"/>
+      <c r="A83" s="22" t="s">
+        <v>117</v>
+      </c>
       <c r="B83" s="5" t="s">
-        <v>82</v>
+        <v>118</v>
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
       <c r="E83" s="5" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A84" s="19" t="s">
-        <v>119</v>
-      </c>
+      <c r="A84" s="22"/>
       <c r="B84" s="5" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A85" s="19"/>
-      <c r="B85" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
-      <c r="E85" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E85"/>
-  <mergeCells count="30">
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A25:A32"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="E80:E81"/>
-    <mergeCell ref="A79:A83"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="E60:E62"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="A60:A68"/>
-    <mergeCell ref="A72:A73"/>
+  <autoFilter ref="A2:E84"/>
+  <mergeCells count="29">
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="A78:A82"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="E59:E61"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="E76:E77"/>
+    <mergeCell ref="A59:A67"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A24:A31"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A38:A40"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2763,181 +2754,181 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="19" t="s">
-        <v>6</v>
+      <c r="A2" s="22" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="19"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="5"/>
       <c r="C3" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="14" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>216</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="14" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>242</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="E14" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2967,13 +2958,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>189</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -2981,282 +2972,282 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C33" s="5"/>
     </row>

</xml_diff>

<commit_message>
Update on 20251009 part 4
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="277">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1096,6 +1096,30 @@
   </si>
   <si>
     <t>由不知名平台提供的央视,卫视,电影等频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wsd.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PHP脚本仅中国大陆可访问</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天津市频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>央视新闻</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCTV.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>央视新闻APP提供的部分央视频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1300,21 +1324,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1326,8 +1350,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1673,7 +1697,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -1688,7 +1712,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="21"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="5"/>
       <c r="C4" s="7" t="s">
         <v>211</v>
@@ -1701,7 +1725,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1740,7 +1764,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="21"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
         <v>182</v>
@@ -1781,7 +1805,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="20" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1796,7 +1820,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="19"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
         <v>226</v>
@@ -1809,7 +1833,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="19"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="5" t="s">
         <v>115</v>
       </c>
@@ -1820,7 +1844,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="20" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -1837,7 +1861,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="19"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="5" t="s">
         <v>23</v>
       </c>
@@ -1848,7 +1872,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="21" t="s">
         <v>25</v>
       </c>
       <c r="B16" s="5"/>
@@ -1878,7 +1902,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="21"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="5" t="s">
         <v>27</v>
       </c>
@@ -1930,7 +1954,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="20" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -1945,7 +1969,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="19"/>
+      <c r="A23" s="20"/>
       <c r="B23" s="5" t="s">
         <v>45</v>
       </c>
@@ -1958,7 +1982,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="20" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="26" t="s">
@@ -1973,7 +1997,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="19"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="27"/>
       <c r="C25" s="5" t="s">
         <v>179</v>
@@ -1984,7 +2008,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="19"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="5" t="s">
         <v>35</v>
       </c>
@@ -1992,21 +2016,21 @@
         <v>160</v>
       </c>
       <c r="D26" s="5"/>
-      <c r="E26" s="28" t="s">
+      <c r="E26" s="19" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="19"/>
+      <c r="A27" s="20"/>
       <c r="B27" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="28"/>
+      <c r="E27" s="19"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="19"/>
+      <c r="A28" s="20"/>
       <c r="B28" s="5" t="s">
         <v>38</v>
       </c>
@@ -2017,7 +2041,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="19"/>
+      <c r="A29" s="20"/>
       <c r="B29" s="5" t="s">
         <v>40</v>
       </c>
@@ -2028,24 +2052,24 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="19"/>
+      <c r="A30" s="20"/>
       <c r="B30" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="28" t="s">
+      <c r="E30" s="19" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="19"/>
+      <c r="A31" s="20"/>
       <c r="B31" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="28"/>
+      <c r="E31" s="19"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="14" t="s">
@@ -2059,7 +2083,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="21" t="s">
         <v>145</v>
       </c>
       <c r="B33" s="5"/>
@@ -2087,7 +2111,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="21"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
         <v>231</v>
@@ -2098,7 +2122,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="20" t="s">
         <v>47</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -2113,7 +2137,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="19"/>
+      <c r="A37" s="20"/>
       <c r="B37" s="5" t="s">
         <v>50</v>
       </c>
@@ -2124,7 +2148,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="20" t="s">
+      <c r="A38" s="21" t="s">
         <v>146</v>
       </c>
       <c r="B38" s="5"/>
@@ -2150,7 +2174,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="21"/>
+      <c r="A40" s="23"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5" t="s">
         <v>163</v>
@@ -2161,7 +2185,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="20" t="s">
+      <c r="A41" s="21" t="s">
         <v>97</v>
       </c>
       <c r="B41" s="5" t="s">
@@ -2176,7 +2200,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="21"/>
+      <c r="A42" s="23"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
         <v>133</v>
@@ -2189,7 +2213,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="20" t="s">
+      <c r="A43" s="21" t="s">
         <v>52</v>
       </c>
       <c r="B43" s="5"/>
@@ -2226,7 +2250,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="21"/>
+      <c r="A46" s="23"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5" t="s">
         <v>218</v>
@@ -2239,7 +2263,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="20" t="s">
+      <c r="A47" s="21" t="s">
         <v>81</v>
       </c>
       <c r="B47" s="5"/>
@@ -2254,7 +2278,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="21"/>
+      <c r="A48" s="23"/>
       <c r="B48" s="5" t="s">
         <v>82</v>
       </c>
@@ -2300,7 +2324,7 @@
       <c r="E51" s="13"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A52" s="19" t="s">
+      <c r="A52" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B52" s="5" t="s">
@@ -2310,21 +2334,21 @@
         <v>161</v>
       </c>
       <c r="D52" s="5"/>
-      <c r="E52" s="28" t="s">
+      <c r="E52" s="19" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A53" s="19"/>
+      <c r="A53" s="20"/>
       <c r="B53" s="5" t="s">
         <v>85</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
-      <c r="E53" s="28"/>
+      <c r="E53" s="19"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A54" s="19"/>
+      <c r="A54" s="20"/>
       <c r="B54" s="5" t="s">
         <v>86</v>
       </c>
@@ -2335,7 +2359,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A55" s="19"/>
+      <c r="A55" s="20"/>
       <c r="B55" s="5" t="s">
         <v>87</v>
       </c>
@@ -2346,7 +2370,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" s="19" t="s">
+      <c r="A56" s="20" t="s">
         <v>90</v>
       </c>
       <c r="B56" s="5" t="s">
@@ -2361,7 +2385,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A57" s="19"/>
+      <c r="A57" s="20"/>
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
         <v>174</v>
@@ -2372,7 +2396,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A58" s="19"/>
+      <c r="A58" s="20"/>
       <c r="B58" s="5" t="s">
         <v>91</v>
       </c>
@@ -2385,7 +2409,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A59" s="20" t="s">
+      <c r="A59" s="21" t="s">
         <v>58</v>
       </c>
       <c r="B59" s="5" t="s">
@@ -2393,7 +2417,7 @@
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
-      <c r="E59" s="28" t="s">
+      <c r="E59" s="19" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2408,7 +2432,7 @@
       <c r="D60" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="E60" s="28"/>
+      <c r="E60" s="19"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A61" s="22"/>
@@ -2417,7 +2441,7 @@
       </c>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
-      <c r="E61" s="28"/>
+      <c r="E61" s="19"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A62" s="22"/>
@@ -2475,7 +2499,7 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A67" s="21"/>
+      <c r="A67" s="23"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5" t="s">
         <v>137</v>
@@ -2486,7 +2510,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A68" s="19" t="s">
+      <c r="A68" s="20" t="s">
         <v>62</v>
       </c>
       <c r="B68" s="5" t="s">
@@ -2503,7 +2527,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A69" s="19"/>
+      <c r="A69" s="20"/>
       <c r="B69" s="5" t="s">
         <v>63</v>
       </c>
@@ -2520,12 +2544,18 @@
         <v>150</v>
       </c>
       <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
+      <c r="C70" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="71" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A71" s="23" t="s">
+      <c r="A71" s="24" t="s">
         <v>120</v>
       </c>
       <c r="B71" s="5" t="s">
@@ -2553,7 +2583,7 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A73" s="23" t="s">
+      <c r="A73" s="24" t="s">
         <v>121</v>
       </c>
       <c r="B73" s="5" t="s">
@@ -2568,7 +2598,7 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A74" s="24"/>
+      <c r="A74" s="28"/>
       <c r="B74" s="5" t="s">
         <v>107</v>
       </c>
@@ -2594,7 +2624,7 @@
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A76" s="19" t="s">
+      <c r="A76" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B76" s="5" t="s">
@@ -2606,21 +2636,21 @@
       <c r="D76" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="E76" s="28" t="s">
+      <c r="E76" s="19" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A77" s="19"/>
+      <c r="A77" s="20"/>
       <c r="B77" s="5" t="s">
         <v>69</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
-      <c r="E77" s="28"/>
+      <c r="E77" s="19"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A78" s="19" t="s">
+      <c r="A78" s="20" t="s">
         <v>66</v>
       </c>
       <c r="B78" s="5" t="s">
@@ -2635,7 +2665,7 @@
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A79" s="19"/>
+      <c r="A79" s="20"/>
       <c r="B79" s="5" t="s">
         <v>73</v>
       </c>
@@ -2645,21 +2675,21 @@
       <c r="D79" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="E79" s="28" t="s">
+      <c r="E79" s="19" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A80" s="19"/>
+      <c r="A80" s="20"/>
       <c r="B80" s="5" t="s">
         <v>75</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
-      <c r="E80" s="28"/>
+      <c r="E80" s="19"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A81" s="19"/>
+      <c r="A81" s="20"/>
       <c r="B81" s="5" t="s">
         <v>76</v>
       </c>
@@ -2672,7 +2702,7 @@
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A82" s="19"/>
+      <c r="A82" s="20"/>
       <c r="B82" s="5" t="s">
         <v>80</v>
       </c>
@@ -2683,7 +2713,7 @@
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A83" s="19" t="s">
+      <c r="A83" s="20" t="s">
         <v>117</v>
       </c>
       <c r="B83" s="5" t="s">
@@ -2696,7 +2726,7 @@
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A84" s="19"/>
+      <c r="A84" s="20"/>
       <c r="B84" s="5" t="s">
         <v>123</v>
       </c>
@@ -2709,6 +2739,24 @@
   </sheetData>
   <autoFilter ref="A2:E84"/>
   <mergeCells count="29">
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A24:A31"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="E30:E31"/>
     <mergeCell ref="E52:E53"/>
     <mergeCell ref="A52:A55"/>
     <mergeCell ref="E79:E80"/>
@@ -2720,24 +2768,6 @@
     <mergeCell ref="E76:E77"/>
     <mergeCell ref="A59:A67"/>
     <mergeCell ref="A71:A72"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A24:A31"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A38:A40"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2747,7 +2777,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2781,7 +2811,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2798,7 +2828,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="19"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="5"/>
       <c r="C3" s="7" t="s">
         <v>243</v>
@@ -2950,8 +2980,21 @@
         <v>270</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="E15" s="10" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E16" s="10" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3227,7 +3270,9 @@
       <c r="A28" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B28" s="5"/>
+      <c r="B28" s="5" t="s">
+        <v>188</v>
+      </c>
       <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Update on 20251013 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -13,7 +13,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他脚本!$A$1:$E$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">省份脚本!$A$2:$E$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">省份脚本!$A$2:$E$85</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">省份统计!$A$1:$C$33</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="279">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1121,6 +1121,14 @@
   <si>
     <t>qhtv.php
 qinghai.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baotou.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>包头市频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1325,21 +1333,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1351,8 +1359,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1655,7 +1663,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1698,7 +1706,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -1713,7 +1721,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="21"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="5"/>
       <c r="C4" s="7" t="s">
         <v>210</v>
@@ -1726,7 +1734,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1765,7 +1773,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="21"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
         <v>182</v>
@@ -1806,7 +1814,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="20" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1821,7 +1829,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="19"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
         <v>225</v>
@@ -1834,7 +1842,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="19"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="5" t="s">
         <v>115</v>
       </c>
@@ -1845,7 +1853,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="20" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -1862,7 +1870,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="19"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="5" t="s">
         <v>23</v>
       </c>
@@ -1873,7 +1881,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="21" t="s">
         <v>25</v>
       </c>
       <c r="B16" s="5"/>
@@ -1903,7 +1911,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="21"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="5" t="s">
         <v>27</v>
       </c>
@@ -1955,7 +1963,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="20" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -1970,7 +1978,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="19"/>
+      <c r="A23" s="20"/>
       <c r="B23" s="5" t="s">
         <v>45</v>
       </c>
@@ -1983,7 +1991,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="20" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="26" t="s">
@@ -1998,7 +2006,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="19"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="27"/>
       <c r="C25" s="5" t="s">
         <v>179</v>
@@ -2009,7 +2017,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="19"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="5" t="s">
         <v>35</v>
       </c>
@@ -2017,21 +2025,21 @@
         <v>160</v>
       </c>
       <c r="D26" s="5"/>
-      <c r="E26" s="28" t="s">
+      <c r="E26" s="19" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="19"/>
+      <c r="A27" s="20"/>
       <c r="B27" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="28"/>
+      <c r="E27" s="19"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="19"/>
+      <c r="A28" s="20"/>
       <c r="B28" s="5" t="s">
         <v>38</v>
       </c>
@@ -2042,7 +2050,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="19"/>
+      <c r="A29" s="20"/>
       <c r="B29" s="5" t="s">
         <v>40</v>
       </c>
@@ -2053,24 +2061,24 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="19"/>
+      <c r="A30" s="20"/>
       <c r="B30" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="28" t="s">
+      <c r="E30" s="19" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="19"/>
+      <c r="A31" s="20"/>
       <c r="B31" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="28"/>
+      <c r="E31" s="19"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="14" t="s">
@@ -2084,7 +2092,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="21" t="s">
         <v>145</v>
       </c>
       <c r="B33" s="5"/>
@@ -2112,7 +2120,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="21"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
         <v>230</v>
@@ -2123,7 +2131,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="20" t="s">
         <v>47</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -2138,7 +2146,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="19"/>
+      <c r="A37" s="20"/>
       <c r="B37" s="5" t="s">
         <v>50</v>
       </c>
@@ -2149,7 +2157,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="20" t="s">
+      <c r="A38" s="21" t="s">
         <v>146</v>
       </c>
       <c r="B38" s="5"/>
@@ -2175,7 +2183,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="21"/>
+      <c r="A40" s="23"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5" t="s">
         <v>163</v>
@@ -2186,7 +2194,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="20" t="s">
+      <c r="A41" s="21" t="s">
         <v>97</v>
       </c>
       <c r="B41" s="5" t="s">
@@ -2201,7 +2209,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="21"/>
+      <c r="A42" s="23"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
         <v>133</v>
@@ -2214,7 +2222,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="20" t="s">
+      <c r="A43" s="21" t="s">
         <v>52</v>
       </c>
       <c r="B43" s="5"/>
@@ -2251,7 +2259,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="21"/>
+      <c r="A46" s="23"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5" t="s">
         <v>217</v>
@@ -2264,7 +2272,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="20" t="s">
+      <c r="A47" s="21" t="s">
         <v>81</v>
       </c>
       <c r="B47" s="5"/>
@@ -2279,7 +2287,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="21"/>
+      <c r="A48" s="23"/>
       <c r="B48" s="5" t="s">
         <v>82</v>
       </c>
@@ -2290,7 +2298,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A49" s="14" t="s">
+      <c r="A49" s="21" t="s">
         <v>147</v>
       </c>
       <c r="B49" s="5"/>
@@ -2303,472 +2311,484 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A50" s="14" t="s">
+      <c r="A50" s="23"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A51" s="14" t="s">
         <v>148</v>
-      </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="D50" s="7"/>
-      <c r="E50" s="13"/>
-    </row>
-    <row r="51" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A51" s="14" t="s">
-        <v>149</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="D51" s="7"/>
+      <c r="E51" s="13"/>
+    </row>
+    <row r="52" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A52" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="D51" s="5"/>
-      <c r="E51" s="13"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A52" s="19" t="s">
+      <c r="D52" s="5"/>
+      <c r="E52" s="13"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A53" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B53" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C53" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="D52" s="5"/>
-      <c r="E52" s="28" t="s">
+      <c r="D53" s="5"/>
+      <c r="E53" s="19" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A53" s="19"/>
-      <c r="B53" s="5" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A54" s="20"/>
+      <c r="B54" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="28"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A54" s="19"/>
-      <c r="B54" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
-      <c r="E54" s="5" t="s">
-        <v>88</v>
-      </c>
+      <c r="E54" s="19"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A55" s="19"/>
+      <c r="A55" s="20"/>
       <c r="B55" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" s="19" t="s">
-        <v>90</v>
-      </c>
+      <c r="A56" s="20"/>
       <c r="B56" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>173</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A57" s="19"/>
-      <c r="B57" s="5"/>
+      <c r="A57" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>113</v>
+      </c>
       <c r="C57" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5" t="s">
-        <v>175</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A58" s="19"/>
-      <c r="B58" s="5" t="s">
-        <v>91</v>
-      </c>
+      <c r="A58" s="20"/>
+      <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A59" s="20"/>
+      <c r="B59" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A59" s="20" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A60" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B60" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="28" t="s">
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="19" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60" s="22"/>
-      <c r="B60" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="E60" s="28"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A61" s="22"/>
       <c r="B61" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="28"/>
+        <v>93</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E61" s="19"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A62" s="22"/>
       <c r="B62" s="5" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
-      <c r="E62" s="5" t="s">
-        <v>95</v>
-      </c>
+      <c r="E62" s="19"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A63" s="22"/>
       <c r="B63" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A64" s="22"/>
       <c r="B64" s="5" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A65" s="22"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5" t="s">
-        <v>135</v>
-      </c>
+      <c r="B65" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A66" s="22"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A67" s="21"/>
+      <c r="A67" s="22"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A68" s="23"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A68" s="19" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A69" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B69" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C69" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="D69" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="E68" s="5" t="s">
+      <c r="E69" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A69" s="19"/>
-      <c r="B69" s="5" t="s">
+    <row r="70" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A70" s="20"/>
+      <c r="B70" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C70" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="D69" s="7"/>
-      <c r="E69" s="5" t="s">
+      <c r="D70" s="7"/>
+      <c r="E70" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A70" s="14" t="s">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A71" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5" t="s">
+      <c r="B71" s="5"/>
+      <c r="C71" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="D71" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="E70" s="5" t="s">
+      <c r="E71" s="5" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A71" s="23" t="s">
+    <row r="72" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A72" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B72" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C71" s="7" t="s">
+      <c r="C72" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="D71" s="7" t="s">
+      <c r="D72" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="E71" s="5" t="s">
+      <c r="E72" s="5" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A72" s="25"/>
-      <c r="B72" s="5"/>
-      <c r="C72" s="7" t="s">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A73" s="25"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D72" s="7"/>
-      <c r="E72" s="5" t="s">
+      <c r="D73" s="7"/>
+      <c r="E73" s="5" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A73" s="23" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A74" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B74" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C74" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D73" s="5"/>
-      <c r="E73" s="6" t="s">
+      <c r="D74" s="5"/>
+      <c r="E74" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A74" s="24"/>
-      <c r="B74" s="5" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A75" s="28"/>
+      <c r="B75" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C75" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="D74" s="5"/>
-      <c r="E74" s="15" t="s">
+      <c r="D75" s="5"/>
+      <c r="E75" s="15" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A75" s="25"/>
-      <c r="B75" s="5"/>
-      <c r="C75" s="5" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A76" s="25"/>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D76" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="E75" s="16" t="s">
+      <c r="E76" s="16" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A76" s="19" t="s">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A77" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B77" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C77" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D77" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E76" s="28" t="s">
+      <c r="E77" s="19" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A77" s="19"/>
-      <c r="B77" s="5" t="s">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A78" s="20"/>
+      <c r="B78" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="28"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A78" s="19" t="s">
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="19"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A79" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B79" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C78" s="5" t="s">
+      <c r="C79" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5" t="s">
+      <c r="D79" s="5"/>
+      <c r="E79" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A79" s="19"/>
-      <c r="B79" s="5" t="s">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A80" s="20"/>
+      <c r="B80" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C79" s="7" t="s">
+      <c r="C80" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="D79" s="7" t="s">
+      <c r="D80" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="E79" s="28" t="s">
+      <c r="E80" s="19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A80" s="19"/>
-      <c r="B80" s="5" t="s">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A81" s="20"/>
+      <c r="B81" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
-      <c r="E80" s="28"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A81" s="19"/>
-      <c r="B81" s="5" t="s">
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="19"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A82" s="20"/>
+      <c r="B82" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C81" s="5" t="s">
+      <c r="C82" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A82" s="19"/>
-      <c r="B82" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A83" s="19" t="s">
-        <v>117</v>
-      </c>
+      <c r="A83" s="20"/>
       <c r="B83" s="5" t="s">
-        <v>118</v>
+        <v>80</v>
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
       <c r="E83" s="5" t="s">
-        <v>119</v>
+        <v>79</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A84" s="19"/>
+      <c r="A84" s="20" t="s">
+        <v>117</v>
+      </c>
       <c r="B84" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A85" s="20"/>
+      <c r="B85" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="5" t="s">
         <v>124</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E84"/>
-  <mergeCells count="29">
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="A78:A82"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="E59:E61"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="A76:A77"/>
-    <mergeCell ref="E76:E77"/>
-    <mergeCell ref="A59:A67"/>
-    <mergeCell ref="A71:A72"/>
+  <autoFilter ref="A2:E85"/>
+  <mergeCells count="30">
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A5:A8"/>
     <mergeCell ref="E26:E27"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="A24:A31"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="E30:E31"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="E80:E81"/>
+    <mergeCell ref="A79:A83"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="E60:E62"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="A60:A68"/>
+    <mergeCell ref="A72:A73"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2812,7 +2832,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2829,7 +2849,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="19"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="5"/>
       <c r="C3" s="7" t="s">
         <v>242</v>

</xml_diff>

<commit_message>
Update on 20251015 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="285">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1351,9 +1351,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1367,6 +1364,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1712,7 +1712,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -1727,7 +1727,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="18"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="5"/>
       <c r="C4" s="7" t="s">
         <v>210</v>
@@ -1740,7 +1740,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1757,7 +1757,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="18"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
@@ -1768,7 +1768,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="18"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1779,7 +1779,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="18"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
         <v>182</v>
@@ -1820,7 +1820,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="17" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1835,7 +1835,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="18"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
         <v>225</v>
@@ -1848,7 +1848,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="18"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="5" t="s">
         <v>115</v>
       </c>
@@ -1859,7 +1859,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -1876,7 +1876,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="18"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="5" t="s">
         <v>23</v>
       </c>
@@ -1887,7 +1887,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="17" t="s">
         <v>25</v>
       </c>
       <c r="B16" s="5"/>
@@ -1902,7 +1902,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A17" s="18"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="5" t="s">
         <v>26</v>
       </c>
@@ -1917,7 +1917,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="18"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="5" t="s">
         <v>27</v>
       </c>
@@ -1969,7 +1969,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="17" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -1984,7 +1984,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="18"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="5" t="s">
         <v>45</v>
       </c>
@@ -1997,10 +1997,10 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="22" t="s">
         <v>33</v>
       </c>
       <c r="C24" s="5" t="s">
@@ -2012,8 +2012,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="18"/>
-      <c r="B25" s="17"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="22"/>
       <c r="C25" s="5" t="s">
         <v>179</v>
       </c>
@@ -2023,7 +2023,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="18"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="5" t="s">
         <v>35</v>
       </c>
@@ -2031,21 +2031,21 @@
         <v>160</v>
       </c>
       <c r="D26" s="5"/>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="22" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="18"/>
+      <c r="A27" s="17"/>
       <c r="B27" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="17"/>
+      <c r="E27" s="22"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="18"/>
+      <c r="A28" s="17"/>
       <c r="B28" s="5" t="s">
         <v>38</v>
       </c>
@@ -2056,7 +2056,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="18"/>
+      <c r="A29" s="17"/>
       <c r="B29" s="5" t="s">
         <v>40</v>
       </c>
@@ -2067,24 +2067,24 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="18"/>
+      <c r="A30" s="17"/>
       <c r="B30" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="17" t="s">
+      <c r="E30" s="22" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="18"/>
+      <c r="A31" s="17"/>
       <c r="B31" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="17"/>
+      <c r="E31" s="22"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="15" t="s">
@@ -2098,7 +2098,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="17" t="s">
         <v>145</v>
       </c>
       <c r="B33" s="5"/>
@@ -2111,7 +2111,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" s="18"/>
+      <c r="A34" s="17"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5" t="s">
         <v>243</v>
@@ -2124,7 +2124,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="18"/>
+      <c r="A35" s="17"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
         <v>221</v>
@@ -2137,7 +2137,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="18"/>
+      <c r="A36" s="17"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5" t="s">
         <v>230</v>
@@ -2148,7 +2148,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="18" t="s">
+      <c r="A37" s="17" t="s">
         <v>47</v>
       </c>
       <c r="B37" s="5" t="s">
@@ -2163,7 +2163,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="18"/>
+      <c r="A38" s="17"/>
       <c r="B38" s="5" t="s">
         <v>50</v>
       </c>
@@ -2174,7 +2174,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="18" t="s">
+      <c r="A39" s="17" t="s">
         <v>146</v>
       </c>
       <c r="B39" s="5"/>
@@ -2189,7 +2189,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="18"/>
+      <c r="A40" s="17"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5" t="s">
         <v>262</v>
@@ -2200,7 +2200,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="18"/>
+      <c r="A41" s="17"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5" t="s">
         <v>163</v>
@@ -2211,7 +2211,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="18" t="s">
+      <c r="A42" s="17" t="s">
         <v>97</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -2226,7 +2226,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="18"/>
+      <c r="A43" s="17"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
         <v>133</v>
@@ -2239,7 +2239,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="18" t="s">
+      <c r="A44" s="17" t="s">
         <v>52</v>
       </c>
       <c r="B44" s="5"/>
@@ -2252,7 +2252,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="18"/>
+      <c r="A45" s="17"/>
       <c r="B45" s="5" t="s">
         <v>53</v>
       </c>
@@ -2265,7 +2265,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="18"/>
+      <c r="A46" s="17"/>
       <c r="B46" s="5" t="s">
         <v>55</v>
       </c>
@@ -2276,7 +2276,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="18"/>
+      <c r="A47" s="17"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5" t="s">
         <v>217</v>
@@ -2289,7 +2289,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="17" t="s">
         <v>81</v>
       </c>
       <c r="B48" s="5"/>
@@ -2304,7 +2304,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A49" s="18"/>
+      <c r="A49" s="17"/>
       <c r="B49" s="5" t="s">
         <v>82</v>
       </c>
@@ -2315,7 +2315,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A50" s="18" t="s">
+      <c r="A50" s="17" t="s">
         <v>147</v>
       </c>
       <c r="B50" s="5"/>
@@ -2328,7 +2328,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A51" s="18"/>
+      <c r="A51" s="17"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5" t="s">
         <v>277</v>
@@ -2361,7 +2361,7 @@
       <c r="E53" s="12"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A54" s="18" t="s">
+      <c r="A54" s="17" t="s">
         <v>57</v>
       </c>
       <c r="B54" s="5" t="s">
@@ -2371,21 +2371,21 @@
         <v>161</v>
       </c>
       <c r="D54" s="5"/>
-      <c r="E54" s="17" t="s">
+      <c r="E54" s="22" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A55" s="18"/>
+      <c r="A55" s="17"/>
       <c r="B55" s="5" t="s">
         <v>85</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
-      <c r="E55" s="17"/>
+      <c r="E55" s="22"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" s="18"/>
+      <c r="A56" s="17"/>
       <c r="B56" s="5" t="s">
         <v>86</v>
       </c>
@@ -2400,7 +2400,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A57" s="18"/>
+      <c r="A57" s="17"/>
       <c r="B57" s="5" t="s">
         <v>87</v>
       </c>
@@ -2411,7 +2411,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A58" s="20" t="s">
+      <c r="A58" s="19" t="s">
         <v>90</v>
       </c>
       <c r="B58" s="5" t="s">
@@ -2426,7 +2426,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A59" s="21"/>
+      <c r="A59" s="20"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
         <v>174</v>
@@ -2437,7 +2437,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60" s="21"/>
+      <c r="A60" s="20"/>
       <c r="B60" s="5" t="s">
         <v>91</v>
       </c>
@@ -2450,18 +2450,20 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A61" s="22"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="D61" s="5"/>
+      <c r="D61" s="5" t="s">
+        <v>209</v>
+      </c>
       <c r="E61" s="5" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A62" s="18" t="s">
+      <c r="A62" s="17" t="s">
         <v>58</v>
       </c>
       <c r="B62" s="5" t="s">
@@ -2469,12 +2471,12 @@
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
-      <c r="E62" s="17" t="s">
+      <c r="E62" s="22" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A63" s="18"/>
+      <c r="A63" s="17"/>
       <c r="B63" s="5" t="s">
         <v>93</v>
       </c>
@@ -2484,19 +2486,19 @@
       <c r="D63" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E63" s="17"/>
+      <c r="E63" s="22"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A64" s="18"/>
+      <c r="A64" s="17"/>
       <c r="B64" s="5" t="s">
         <v>112</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
-      <c r="E64" s="17"/>
+      <c r="E64" s="22"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A65" s="18"/>
+      <c r="A65" s="17"/>
       <c r="B65" s="5" t="s">
         <v>94</v>
       </c>
@@ -2507,7 +2509,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A66" s="18"/>
+      <c r="A66" s="17"/>
       <c r="B66" s="5" t="s">
         <v>96</v>
       </c>
@@ -2518,7 +2520,7 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A67" s="18"/>
+      <c r="A67" s="17"/>
       <c r="B67" s="5" t="s">
         <v>105</v>
       </c>
@@ -2529,7 +2531,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A68" s="18"/>
+      <c r="A68" s="17"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5" t="s">
         <v>135</v>
@@ -2540,7 +2542,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A69" s="18"/>
+      <c r="A69" s="17"/>
       <c r="B69" s="5"/>
       <c r="C69" s="5" t="s">
         <v>136</v>
@@ -2551,7 +2553,7 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A70" s="18"/>
+      <c r="A70" s="17"/>
       <c r="B70" s="5"/>
       <c r="C70" s="5" t="s">
         <v>137</v>
@@ -2562,7 +2564,7 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A71" s="18" t="s">
+      <c r="A71" s="17" t="s">
         <v>62</v>
       </c>
       <c r="B71" s="5" t="s">
@@ -2579,7 +2581,7 @@
       </c>
     </row>
     <row r="72" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A72" s="18"/>
+      <c r="A72" s="17"/>
       <c r="B72" s="5" t="s">
         <v>63</v>
       </c>
@@ -2607,7 +2609,7 @@
       </c>
     </row>
     <row r="74" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A74" s="19" t="s">
+      <c r="A74" s="18" t="s">
         <v>120</v>
       </c>
       <c r="B74" s="5" t="s">
@@ -2624,7 +2626,7 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A75" s="19"/>
+      <c r="A75" s="18"/>
       <c r="B75" s="5"/>
       <c r="C75" s="7" t="s">
         <v>177</v>
@@ -2635,7 +2637,7 @@
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A76" s="19" t="s">
+      <c r="A76" s="18" t="s">
         <v>121</v>
       </c>
       <c r="B76" s="5" t="s">
@@ -2650,7 +2652,7 @@
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A77" s="19"/>
+      <c r="A77" s="18"/>
       <c r="B77" s="5" t="s">
         <v>107</v>
       </c>
@@ -2663,7 +2665,7 @@
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A78" s="19"/>
+      <c r="A78" s="18"/>
       <c r="B78" s="5"/>
       <c r="C78" s="5" t="s">
         <v>248</v>
@@ -2676,7 +2678,7 @@
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A79" s="18" t="s">
+      <c r="A79" s="17" t="s">
         <v>65</v>
       </c>
       <c r="B79" s="5" t="s">
@@ -2688,21 +2690,21 @@
       <c r="D79" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E79" s="17" t="s">
+      <c r="E79" s="22" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A80" s="18"/>
+      <c r="A80" s="17"/>
       <c r="B80" s="5" t="s">
         <v>69</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
-      <c r="E80" s="17"/>
+      <c r="E80" s="22"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A81" s="18" t="s">
+      <c r="A81" s="17" t="s">
         <v>66</v>
       </c>
       <c r="B81" s="5" t="s">
@@ -2717,7 +2719,7 @@
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A82" s="18"/>
+      <c r="A82" s="17"/>
       <c r="B82" s="5" t="s">
         <v>73</v>
       </c>
@@ -2727,21 +2729,21 @@
       <c r="D82" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="E82" s="17" t="s">
+      <c r="E82" s="22" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A83" s="18"/>
+      <c r="A83" s="17"/>
       <c r="B83" s="5" t="s">
         <v>75</v>
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
-      <c r="E83" s="17"/>
+      <c r="E83" s="22"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A84" s="18"/>
+      <c r="A84" s="17"/>
       <c r="B84" s="5" t="s">
         <v>76</v>
       </c>
@@ -2754,7 +2756,7 @@
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A85" s="18"/>
+      <c r="A85" s="17"/>
       <c r="B85" s="5" t="s">
         <v>80</v>
       </c>
@@ -2765,7 +2767,7 @@
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A86" s="18" t="s">
+      <c r="A86" s="17" t="s">
         <v>117</v>
       </c>
       <c r="B86" s="5" t="s">
@@ -2778,7 +2780,7 @@
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A87" s="18"/>
+      <c r="A87" s="17"/>
       <c r="B87" s="5" t="s">
         <v>123</v>
       </c>
@@ -2791,26 +2793,6 @@
   </sheetData>
   <autoFilter ref="A2:E87"/>
   <mergeCells count="30">
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A76:A78"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A24:A31"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="A33:A36"/>
     <mergeCell ref="E54:E55"/>
     <mergeCell ref="A54:A57"/>
     <mergeCell ref="E82:E83"/>
@@ -2821,6 +2803,26 @@
     <mergeCell ref="E79:E80"/>
     <mergeCell ref="A62:A70"/>
     <mergeCell ref="A74:A75"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A24:A31"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A76:A78"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A58:A61"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2864,7 +2866,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2881,7 +2883,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="18"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="5"/>
       <c r="C3" s="7" t="s">
         <v>242</v>

</xml_diff>

<commit_message>
Update on 20251019 part 5
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -13,7 +13,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他脚本!$A$1:$E$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">省份脚本!$A$2:$E$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">省份脚本!$A$2:$E$93</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">省份统计!$A$1:$C$33</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="295">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -406,10 +406,6 @@
   </si>
   <si>
     <t>jstv.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>卫视,江苏省频道和江苏地方频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -705,10 +701,6 @@
   </si>
   <si>
     <t>shandong_shandian.php</t>
-  </si>
-  <si>
-    <t>卫视,山东省频道和部分山东地方频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>拉萨市频道</t>
@@ -1023,10 +1015,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>卫视,广东省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>jiangxi.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1161,6 +1149,50 @@
   </si>
   <si>
     <t>yy.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sdqilu.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卫视,山东省频道和部分山东地方频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>部分山东地方频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tengxun.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卫视,广东省频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>由腾讯云提供的广东卫视和省频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>由腾讯云提供的贵州卫视和省频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卫视,江苏省频道和江苏地方频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>由腾讯云提供的江苏卫视,省频道和江苏地方频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>由腾讯云提供的江西卫视,省频道和江西地方频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>由腾讯云提供的内蒙古卫视,省频道和内蒙古地方频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1306,7 +1338,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1349,14 +1381,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1373,8 +1408,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1677,7 +1712,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1694,12 +1729,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
       <c r="E1" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
@@ -1707,65 +1742,65 @@
         <v>8</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="17"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="5"/>
       <c r="C4" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>129</v>
+        <v>207</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="17"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
@@ -1776,7 +1811,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="17"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1787,14 +1822,14 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="17"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
@@ -1805,7 +1840,7 @@
         <v>15</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="5" t="s">
@@ -1814,28 +1849,28 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>234</v>
-      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="18" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="s">
@@ -1843,48 +1878,48 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="17"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>226</v>
-      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="17"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="18" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="17"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="5" t="s">
         <v>23</v>
       </c>
@@ -1895,944 +1930,1011 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="18" t="s">
         <v>25</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>253</v>
+        <v>288</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A17" s="17"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="17"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="5" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" s="18"/>
+      <c r="B19" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>176</v>
+      </c>
       <c r="D19" s="5"/>
-      <c r="E19" s="12" t="s">
-        <v>151</v>
+      <c r="E19" s="5" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>153</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="B21" s="5"/>
       <c r="C21" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="17" t="s">
-        <v>30</v>
-      </c>
+      <c r="A22" s="22"/>
       <c r="B22" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>130</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5" t="s">
-        <v>31</v>
+        <v>290</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="17"/>
-      <c r="B23" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="A23" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
-        <v>46</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>33</v>
+      <c r="A24" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="17"/>
-      <c r="B25" s="22"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="C25" s="5" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5" t="s">
-        <v>180</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="17"/>
-      <c r="B26" s="5" t="s">
+      <c r="A26" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A27" s="18"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A28" s="18"/>
+      <c r="B28" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="22" t="s">
+      <c r="C28" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="17"/>
-      <c r="B27" s="5" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A29" s="18"/>
+      <c r="B29" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="22"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="17"/>
-      <c r="B28" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="17"/>
-      <c r="B29" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="E29" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="E29" s="17"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="17"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="22" t="s">
-        <v>44</v>
+      <c r="E30" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="17"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="22"/>
+      <c r="E31" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="B32" s="5"/>
+      <c r="A32" s="18"/>
+      <c r="B32" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="12" t="s">
-        <v>191</v>
+      <c r="E32" s="17" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="A33" s="18"/>
+      <c r="B33" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="5" t="s">
-        <v>282</v>
-      </c>
+      <c r="E33" s="17"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" s="17"/>
+      <c r="A34" s="15" t="s">
+        <v>143</v>
+      </c>
       <c r="B34" s="5"/>
-      <c r="C34" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>244</v>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="12" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="17"/>
+      <c r="A35" s="18" t="s">
+        <v>144</v>
+      </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>209</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="D35" s="5"/>
       <c r="E35" s="5" t="s">
-        <v>222</v>
+        <v>279</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="17"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="D36" s="5"/>
+        <v>241</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>217</v>
+      </c>
       <c r="E36" s="5" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>48</v>
-      </c>
+      <c r="A37" s="18"/>
+      <c r="B37" s="5"/>
       <c r="C37" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="D37" s="5"/>
-      <c r="E37" s="14" t="s">
-        <v>49</v>
+        <v>219</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="17"/>
-      <c r="B38" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C38" s="5"/>
+      <c r="A38" s="18"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5" t="s">
+        <v>228</v>
+      </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="s">
-        <v>51</v>
+        <v>229</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="B39" s="5"/>
+      <c r="A39" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="C39" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>258</v>
+        <v>151</v>
+      </c>
+      <c r="D39" s="5"/>
+      <c r="E39" s="16" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="17"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5" t="s">
-        <v>262</v>
-      </c>
+      <c r="A40" s="18"/>
+      <c r="B40" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5" t="s">
-        <v>263</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="17"/>
+      <c r="A41" s="18" t="s">
+        <v>145</v>
+      </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="D41" s="5"/>
+        <v>253</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>254</v>
+      </c>
       <c r="E41" s="5" t="s">
-        <v>162</v>
+        <v>255</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>98</v>
-      </c>
+      <c r="A42" s="18"/>
+      <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
-        <v>186</v>
+        <v>259</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5" t="s">
-        <v>99</v>
+        <v>260</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="17"/>
+      <c r="A43" s="18"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A44" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A45" s="21"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="E45" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="D43" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="D44" s="7"/>
-      <c r="E44" s="5" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="17"/>
-      <c r="B45" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="D45" s="7"/>
-      <c r="E45" s="5" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="17"/>
+      <c r="A46" s="22"/>
       <c r="B46" s="5" t="s">
-        <v>55</v>
+        <v>287</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5" t="s">
-        <v>56</v>
+        <v>292</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="17"/>
+      <c r="A47" s="20" t="s">
+        <v>52</v>
+      </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>209</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="D47" s="7"/>
       <c r="E47" s="5" t="s">
-        <v>218</v>
+        <v>252</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>246</v>
-      </c>
+      <c r="A48" s="21"/>
+      <c r="B48" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="D48" s="7"/>
       <c r="E48" s="5" t="s">
-        <v>192</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A49" s="17"/>
+      <c r="A49" s="21"/>
       <c r="B49" s="5" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A50" s="17" t="s">
-        <v>147</v>
-      </c>
+      <c r="A50" s="21"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="D50" s="5"/>
+        <v>215</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>207</v>
+      </c>
       <c r="E50" s="5" t="s">
-        <v>157</v>
+        <v>216</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A51" s="17"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5" t="s">
-        <v>277</v>
-      </c>
+      <c r="A51" s="22"/>
+      <c r="B51" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5" t="s">
-        <v>278</v>
+        <v>293</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A52" s="15" t="s">
-        <v>148</v>
+      <c r="A52" s="18" t="s">
+        <v>81</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A53" s="18"/>
+      <c r="B53" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A54" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A55" s="21"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="D52" s="7"/>
-      <c r="E52" s="12"/>
-    </row>
-    <row r="53" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A53" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="7" t="s">
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A56" s="22"/>
+      <c r="B56" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A57" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="D57" s="7"/>
+      <c r="E57" s="12"/>
+    </row>
+    <row r="58" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A58" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B58" s="5"/>
+      <c r="C58" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="D58" s="5"/>
+      <c r="E58" s="12"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A59" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D59" s="5"/>
+      <c r="E59" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A60" s="18"/>
+      <c r="B60" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="17"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A61" s="18"/>
+      <c r="B61" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C61" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="D53" s="5"/>
-      <c r="E53" s="12"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A54" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="D54" s="5"/>
-      <c r="E54" s="22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A55" s="17"/>
-      <c r="B55" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="22"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" s="17"/>
-      <c r="B56" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="E56" s="5" t="s">
+      <c r="D61" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="E61" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A57" s="17"/>
-      <c r="B57" s="5" t="s">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A62" s="18"/>
+      <c r="B62" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A58" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A59" s="20"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60" s="20"/>
-      <c r="B60" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A61" s="21"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A62" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
-      <c r="E62" s="22" t="s">
-        <v>61</v>
+      <c r="E62" s="5" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A63" s="17"/>
+      <c r="A63" s="18" t="s">
+        <v>90</v>
+      </c>
       <c r="B63" s="5" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="E63" s="22"/>
+        <v>172</v>
+      </c>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A64" s="17"/>
-      <c r="B64" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C64" s="5"/>
+      <c r="A64" s="18"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5" t="s">
+        <v>173</v>
+      </c>
       <c r="D64" s="5"/>
-      <c r="E64" s="22"/>
+      <c r="E64" s="5" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A65" s="17"/>
+      <c r="A65" s="18"/>
       <c r="B65" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C65" s="5"/>
+        <v>91</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>158</v>
+      </c>
       <c r="D65" s="5"/>
       <c r="E65" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A66" s="18"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A67" s="18"/>
+      <c r="B67" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C67" s="5"/>
+      <c r="D67" s="23"/>
+      <c r="E67" s="5" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A68" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A69" s="18"/>
+      <c r="B69" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="E69" s="17"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A70" s="18"/>
+      <c r="B70" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="17"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A71" s="18"/>
+      <c r="B71" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A66" s="17"/>
-      <c r="B66" s="5" t="s">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A72" s="18"/>
+      <c r="B72" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A67" s="17"/>
-      <c r="B67" s="5" t="s">
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A73" s="18"/>
+      <c r="B73" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A68" s="17"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A69" s="17"/>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A70" s="17"/>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5" t="s">
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A74" s="18"/>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A71" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A72" s="17"/>
-      <c r="B72" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="D72" s="7"/>
-      <c r="E72" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A73" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A74" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A75" s="18"/>
       <c r="B75" s="5"/>
-      <c r="C75" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="D75" s="7"/>
+      <c r="C75" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D75" s="5"/>
       <c r="E75" s="5" t="s">
-        <v>176</v>
+        <v>138</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A76" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="B76" s="5" t="s">
+      <c r="A76" s="18"/>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A77" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A78" s="18"/>
+      <c r="B78" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="D78" s="7"/>
+      <c r="E78" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A79" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A80" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A81" s="19"/>
+      <c r="B81" s="5"/>
+      <c r="C81" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D81" s="7"/>
+      <c r="E81" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A82" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="B82" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C76" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D76" s="5"/>
-      <c r="E76" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A77" s="18"/>
-      <c r="B77" s="5" t="s">
+      <c r="C82" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D82" s="5"/>
+      <c r="E82" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A83" s="19"/>
+      <c r="B83" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="D83" s="5"/>
+      <c r="E83" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="C77" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="D77" s="5"/>
-      <c r="E77" s="14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A78" s="18"/>
-      <c r="B78" s="5"/>
-      <c r="C78" s="5" t="s">
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A84" s="19"/>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="E84" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="D78" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="E78" s="14" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A79" s="17" t="s">
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A85" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B85" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C79" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="E79" s="22" t="s">
+      <c r="C85" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="E85" s="17" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A80" s="17"/>
-      <c r="B80" s="5" t="s">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A86" s="18"/>
+      <c r="B86" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
-      <c r="E80" s="22"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A81" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A82" s="17"/>
-      <c r="B82" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="D82" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="E82" s="22" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A83" s="17"/>
-      <c r="B83" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C83" s="5"/>
-      <c r="D83" s="5"/>
-      <c r="E83" s="22"/>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A84" s="17"/>
-      <c r="B84" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="D84" s="5"/>
-      <c r="E84" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A85" s="17"/>
-      <c r="B85" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
-      <c r="E85" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A86" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
-      <c r="E86" s="5" t="s">
-        <v>119</v>
-      </c>
+      <c r="E86" s="17"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A87" s="17"/>
+      <c r="A87" s="18" t="s">
+        <v>66</v>
+      </c>
       <c r="B87" s="5" t="s">
-        <v>123</v>
+        <v>71</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>285</v>
+        <v>163</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="5" t="s">
-        <v>124</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A88" s="18"/>
+      <c r="B88" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="E88" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A89" s="18"/>
+      <c r="B89" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="17"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A90" s="18"/>
+      <c r="B90" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D90" s="5"/>
+      <c r="E90" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A91" s="18"/>
+      <c r="B91" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A92" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A93" s="18"/>
+      <c r="B93" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="D93" s="5"/>
+      <c r="E93" s="5" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E87"/>
-  <mergeCells count="30">
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="A81:A85"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="E62:E64"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="A62:A70"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="E26:E27"/>
+  <autoFilter ref="A2:E93"/>
+  <mergeCells count="31">
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A82:A84"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A63:A67"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="E28:E29"/>
     <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A24:A31"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A76:A78"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A26:A33"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="E88:E89"/>
+    <mergeCell ref="A87:A91"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="E68:E70"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="A68:A76"/>
+    <mergeCell ref="A80:A81"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2863,206 +2965,206 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="17"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="5"/>
       <c r="C3" s="7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A4" s="13" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="13" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="13" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>213</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="13" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>239</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="13" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="5" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="13" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="5" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="E16" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -3095,10 +3197,10 @@
         <v>8</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>187</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -3106,7 +3208,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -3115,7 +3217,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -3124,17 +3226,17 @@
         <v>14</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
@@ -3142,7 +3244,7 @@
         <v>17</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C6" s="5"/>
     </row>
@@ -3151,7 +3253,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C7" s="5"/>
     </row>
@@ -3160,32 +3262,32 @@
         <v>25</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C11" s="5"/>
     </row>
@@ -3194,7 +3296,7 @@
         <v>30</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C12" s="5"/>
     </row>
@@ -3203,25 +3305,25 @@
         <v>32</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C15" s="5"/>
     </row>
@@ -3230,16 +3332,16 @@
         <v>47</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C17" s="5"/>
     </row>
@@ -3248,7 +3350,7 @@
         <v>97</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C18" s="5"/>
     </row>
@@ -3257,7 +3359,7 @@
         <v>52</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C19" s="5"/>
     </row>
@@ -3266,34 +3368,34 @@
         <v>81</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C23" s="5"/>
     </row>
@@ -3302,7 +3404,7 @@
         <v>57</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C24" s="5"/>
     </row>
@@ -3311,7 +3413,7 @@
         <v>90</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C25" s="5"/>
     </row>
@@ -3320,7 +3422,7 @@
         <v>58</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C26" s="5"/>
     </row>
@@ -3329,34 +3431,34 @@
         <v>62</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C30" s="5"/>
     </row>
@@ -3365,7 +3467,7 @@
         <v>65</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C31" s="5"/>
     </row>
@@ -3374,16 +3476,16 @@
         <v>66</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C33" s="5"/>
     </row>

</xml_diff>

<commit_message>
Update on 20251019 part 6
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -59,14 +59,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>卫视,上海市频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>卫视,安徽省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>hefei.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -87,10 +79,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>卫视,北京市频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>福建</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -98,10 +86,6 @@
     <t>fjtv.js</t>
   </si>
   <si>
-    <t>卫视,福建省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>甘肃</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -110,10 +94,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>卫视,甘肃省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>lanzhou.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -146,10 +126,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>卫视,河北省频道,河北地方频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>河南</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -157,10 +133,6 @@
     <t>henan.js</t>
   </si>
   <si>
-    <t>卫视,河南省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>zhengzhou.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -216,10 +188,6 @@
     <t>hunan.js</t>
   </si>
   <si>
-    <t>卫视,湖南省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>hny.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -259,14 +227,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>卫视,陕西省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>卫视,山西省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>四川</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -296,18 +256,10 @@
     <t>yn.js</t>
   </si>
   <si>
-    <t>卫视,云南省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>zhejiang.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>卫视,浙江省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>hangzhou.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -421,10 +373,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>卫视,深圳市,部分广东频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Tibet.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -445,18 +393,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>卫视,新疆维吾尔自治区频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>sichuan1.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>卫视,四川省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>shanxi_new.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -465,10 +405,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>卫视,山东省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>quanzhou.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -485,10 +421,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>卫视</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>西藏</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -513,10 +445,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>贵州省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>gzstv.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -624,14 +552,6 @@
   </si>
   <si>
     <t>hainan.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>卫视,海南省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>卫视,内蒙古自治区和部分内蒙古地方频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -715,10 +635,6 @@
   </si>
   <si>
     <t>henan_daxiang.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>卫视,河南省频道,部分河南地方频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -760,15 +676,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>卫视,西藏自治区频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>官网提供卫视,黑龙江省频道在线观看,可使用酷9JS脚本的Webview方式观看*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>卫视,辽宁省频道和辽宁地方频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -978,10 +886,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>卫视,湖北省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>liaoning_bfgd.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1019,19 +923,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>卫视,江西省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>jltv.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>PHP脚本仅中国大陆可访问</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>卫视,吉林省频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1132,10 +1028,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>卫视,湖北省频道,央视和其他省卫视,劲爆体育</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>qingdao.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1156,10 +1048,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>卫视,山东省频道和部分山东地方频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>部分山东地方频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1168,31 +1056,142 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>卫视,广东省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>由腾讯云提供的广东卫视和省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>由腾讯云提供的贵州卫视和省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>卫视,江苏省频道和江苏地方频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>由腾讯云提供的江苏卫视,省频道和江苏地方频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>由腾讯云提供的江西卫视,省频道和江西地方频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>由腾讯云提供的内蒙古卫视,省频道和内蒙古地方频道</t>
+    <t>上海市频道和卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>安徽省频道和卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>北京市频道和卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>福建省频道和卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>甘肃省频道和卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>广东省频道和卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>由腾讯云提供的广东省频道和卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>深圳市频道和卫视,部分广东频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贵州省频道和卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>由腾讯云提供的贵州省频道和卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>海南省频道和卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>河北省频道和卫视,河北地方频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>河南省频道和卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>河南省频道和卫视,部分河南地方频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>湖北省频道和卫视,央视和其他省卫视,劲爆体育</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>湖北省频道和卫视</t>
+  </si>
+  <si>
+    <t>湖南省频道和卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吉林省频道和卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>江苏省频道和卫视,江苏地方频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>由腾讯云提供的江苏省频道和卫视,江苏地方频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>江西省频道和卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>辽宁省频道和卫视,辽宁地方频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>内蒙古自治区和卫视,部分内蒙古地方频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>由腾讯云提供的内蒙古自治区和卫视,部分内蒙古地方频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>陕西省频道和卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>山东省频道和卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>山东省频道和卫视,部分山东地方频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>山西省频道和卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>四川省频道和卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>西藏自治区频道和卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新疆维吾尔自治区频道和卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>云南省频道和卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>浙江省频道和卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>香港卫视</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1390,8 +1389,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1402,14 +1401,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1734,7 +1733,7 @@
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="11" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
@@ -1742,13 +1741,13 @@
         <v>8</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>202</v>
+        <v>179</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>203</v>
+        <v>180</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>0</v>
@@ -1759,27 +1758,27 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>262</v>
+        <v>236</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>261</v>
+        <v>235</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="16" t="s">
-        <v>9</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="18"/>
       <c r="B4" s="5"/>
       <c r="C4" s="7" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -1790,1141 +1789,1120 @@
         <v>7</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>221</v>
+        <v>198</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>10</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="18"/>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="18"/>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="18"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A9" s="15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="5" t="s">
-        <v>16</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="15" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>232</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="18" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="s">
-        <v>19</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="18"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="18"/>
       <c r="B13" s="5" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A14" s="18" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>245</v>
+        <v>221</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>22</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" s="18"/>
       <c r="B15" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="18" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>288</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A17" s="18"/>
       <c r="B17" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>235</v>
+        <v>212</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="18"/>
       <c r="B18" s="5" t="s">
-        <v>287</v>
+        <v>259</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="5" t="s">
-        <v>289</v>
+        <v>267</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="18"/>
       <c r="B19" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5" t="s">
-        <v>102</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="15" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="12" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="20" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5" t="s">
-        <v>125</v>
+        <v>269</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="22"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="5" t="s">
-        <v>287</v>
+        <v>259</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="15" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
-        <v>155</v>
+        <v>271</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="18" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5" t="s">
-        <v>31</v>
+        <v>272</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" s="18"/>
       <c r="B25" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>33</v>
+        <v>26</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>27</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5" t="s">
-        <v>34</v>
+        <v>273</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="18"/>
-      <c r="B27" s="17"/>
+      <c r="B27" s="23"/>
       <c r="C27" s="5" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5" t="s">
-        <v>178</v>
+        <v>274</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="18"/>
       <c r="B28" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="D28" s="5"/>
-      <c r="E28" s="17" t="s">
-        <v>36</v>
+      <c r="E28" s="23" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="18"/>
       <c r="B29" s="5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="E29" s="17"/>
+      <c r="E29" s="23"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="18"/>
       <c r="B30" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="18"/>
       <c r="B31" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="18"/>
       <c r="B32" s="5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="17" t="s">
-        <v>44</v>
+      <c r="E32" s="23" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" s="18"/>
       <c r="B33" s="5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="17"/>
+      <c r="E33" s="23"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="15" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="12" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="18" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
-        <v>278</v>
+        <v>252</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="18"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>217</v>
+        <v>194</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>242</v>
+        <v>276</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" s="18"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5" t="s">
-        <v>219</v>
+        <v>196</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" s="18"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5" t="s">
-        <v>228</v>
+        <v>205</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" s="18" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="16" t="s">
-        <v>49</v>
+        <v>277</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" s="18"/>
       <c r="B40" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41" s="18" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5" t="s">
-        <v>253</v>
+        <v>228</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>254</v>
+        <v>229</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>255</v>
+        <v>278</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" s="18"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5" t="s">
-        <v>260</v>
+        <v>234</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A43" s="18"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A44" s="20" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="21"/>
+      <c r="A45" s="22"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="22"/>
+      <c r="A46" s="21"/>
       <c r="B46" s="5" t="s">
-        <v>287</v>
+        <v>259</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" s="20" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="5" t="s">
-        <v>252</v>
+        <v>281</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="21"/>
+      <c r="A48" s="22"/>
       <c r="B48" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>214</v>
+        <v>191</v>
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A49" s="21"/>
+      <c r="A49" s="22"/>
       <c r="B49" s="5" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A50" s="21"/>
+      <c r="A50" s="22"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
-        <v>215</v>
+        <v>192</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>216</v>
+        <v>193</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A51" s="22"/>
+      <c r="A51" s="21"/>
       <c r="B51" s="5" t="s">
-        <v>287</v>
+        <v>259</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5" t="s">
-        <v>293</v>
+        <v>260</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A52" s="18" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="7" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>190</v>
+        <v>282</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A53" s="18"/>
       <c r="B53" s="5" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A54" s="20" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="5" t="s">
-        <v>156</v>
+        <v>283</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A55" s="21"/>
+      <c r="A55" s="22"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
-        <v>274</v>
+        <v>248</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5" t="s">
-        <v>275</v>
+        <v>249</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" s="22"/>
+      <c r="A56" s="21"/>
       <c r="B56" s="5" t="s">
-        <v>287</v>
+        <v>259</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A57" s="15" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="7" t="s">
-        <v>272</v>
+        <v>246</v>
       </c>
       <c r="D57" s="7"/>
       <c r="E57" s="12"/>
     </row>
     <row r="58" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A58" s="15" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="7" t="s">
-        <v>273</v>
+        <v>247</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="12"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A59" s="18" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="D59" s="5"/>
-      <c r="E59" s="17" t="s">
-        <v>60</v>
+      <c r="E59" s="23" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A60" s="18"/>
       <c r="B60" s="5" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
-      <c r="E60" s="17"/>
+      <c r="E60" s="23"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A61" s="18"/>
       <c r="B61" s="5" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>276</v>
+        <v>250</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>277</v>
+        <v>251</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A62" s="18"/>
       <c r="B62" s="5" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A63" s="18" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="5" t="s">
-        <v>113</v>
+        <v>286</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A64" s="18"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="5" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A65" s="18"/>
       <c r="B65" s="5" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="5" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A66" s="18"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
-        <v>280</v>
+        <v>253</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>281</v>
+        <v>254</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A67" s="18"/>
       <c r="B67" s="5" t="s">
-        <v>284</v>
+        <v>257</v>
       </c>
       <c r="C67" s="5"/>
-      <c r="D67" s="23"/>
+      <c r="D67" s="17"/>
       <c r="E67" s="5" t="s">
-        <v>286</v>
+        <v>258</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A68" s="18" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
-      <c r="E68" s="17" t="s">
-        <v>61</v>
+      <c r="E68" s="23" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A69" s="18"/>
       <c r="B69" s="5" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>236</v>
+        <v>213</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="E69" s="17"/>
+        <v>194</v>
+      </c>
+      <c r="E69" s="23"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A70" s="18"/>
       <c r="B70" s="5" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
-      <c r="E70" s="17"/>
+      <c r="E70" s="23"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A71" s="18"/>
       <c r="B71" s="5" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A72" s="18"/>
       <c r="B72" s="5" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A73" s="18"/>
       <c r="B73" s="5" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A74" s="18"/>
       <c r="B74" s="5"/>
       <c r="C74" s="5" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="5" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A75" s="18"/>
       <c r="B75" s="5"/>
       <c r="C75" s="5" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="5" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A76" s="18"/>
       <c r="B76" s="5"/>
       <c r="C76" s="5" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="D76" s="5"/>
       <c r="E76" s="5" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A77" s="18" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>225</v>
+        <v>202</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>226</v>
+        <v>203</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>110</v>
+        <v>289</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A78" s="18"/>
       <c r="B78" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="D78" s="7"/>
       <c r="E78" s="5" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A79" s="15" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5" t="s">
-        <v>266</v>
+        <v>240</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>267</v>
+        <v>241</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>268</v>
+        <v>242</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A80" s="19" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>188</v>
+        <v>290</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A81" s="19"/>
       <c r="B81" s="5"/>
       <c r="C81" s="7" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="D81" s="7"/>
       <c r="E81" s="5" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A82" s="19" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="6" t="s">
-        <v>108</v>
+        <v>291</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A83" s="19"/>
       <c r="B83" s="5" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="16" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A84" s="19"/>
       <c r="B84" s="5"/>
       <c r="C84" s="5" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
       <c r="E84" s="16" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A85" s="18" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>218</v>
+        <v>195</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="E85" s="17" t="s">
-        <v>70</v>
+        <v>194</v>
+      </c>
+      <c r="E85" s="23" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A86" s="18"/>
       <c r="B86" s="5" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
-      <c r="E86" s="17"/>
+      <c r="E86" s="23"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A87" s="18" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="5" t="s">
-        <v>72</v>
+        <v>293</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A88" s="18"/>
       <c r="B88" s="5" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="D88" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="E88" s="17" t="s">
-        <v>74</v>
+        <v>184</v>
+      </c>
+      <c r="E88" s="23" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A89" s="18"/>
       <c r="B89" s="5" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
-      <c r="E89" s="17"/>
+      <c r="E89" s="23"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A90" s="18"/>
       <c r="B90" s="5" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="D90" s="5"/>
       <c r="E90" s="5" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A91" s="18"/>
       <c r="B91" s="5" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C91" s="5"/>
       <c r="D91" s="5"/>
       <c r="E91" s="5" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A92" s="18" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
       <c r="E92" s="5" t="s">
-        <v>118</v>
+        <v>294</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A93" s="18"/>
       <c r="B93" s="5" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>282</v>
+        <v>255</v>
       </c>
       <c r="D93" s="5"/>
       <c r="E93" s="5" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:E93"/>
   <mergeCells count="31">
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A82:A84"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A63:A67"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A47:A51"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A26:A33"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="A35:A38"/>
     <mergeCell ref="E59:E60"/>
     <mergeCell ref="A59:A62"/>
     <mergeCell ref="E88:E89"/>
@@ -2935,6 +2913,27 @@
     <mergeCell ref="E85:E86"/>
     <mergeCell ref="A68:A76"/>
     <mergeCell ref="A80:A81"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A26:A33"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A82:A84"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A63:A67"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A54:A56"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2965,13 +2964,13 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>0</v>
@@ -2985,186 +2984,186 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>234</v>
+        <v>211</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="18"/>
       <c r="B3" s="5"/>
       <c r="C3" s="7" t="s">
-        <v>240</v>
+        <v>217</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A4" s="13" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>258</v>
+        <v>232</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="13" t="s">
-        <v>192</v>
+        <v>169</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="13" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>283</v>
+        <v>256</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="13" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>195</v>
+        <v>172</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>198</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="13" t="s">
-        <v>199</v>
+        <v>176</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5" t="s">
-        <v>201</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="13" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="13" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>233</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="13" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="13" t="s">
-        <v>238</v>
+        <v>215</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
-        <v>237</v>
+        <v>214</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="13" t="s">
-        <v>263</v>
+        <v>237</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
-        <v>264</v>
+        <v>238</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="5" t="s">
-        <v>265</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="13" t="s">
-        <v>269</v>
+        <v>243</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
-        <v>270</v>
+        <v>244</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="5" t="s">
-        <v>271</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="E16" s="10" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -3197,10 +3196,10 @@
         <v>8</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -3208,7 +3207,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -3217,275 +3216,275 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="6" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="6" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="7" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="7" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="6" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="6" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C33" s="5"/>
     </row>

</xml_diff>

<commit_message>
Update on 20251020 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="298">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1200,6 +1200,10 @@
   </si>
   <si>
     <t>黑龙江省频道和卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sdqilu.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1401,9 +1405,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1417,6 +1418,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1762,7 +1766,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -1777,7 +1781,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="19"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="5"/>
       <c r="C4" s="7" t="s">
         <v>184</v>
@@ -1790,7 +1794,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1807,7 +1811,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="19"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1818,7 +1822,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="19"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
@@ -1829,7 +1833,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="19"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
         <v>159</v>
@@ -1870,7 +1874,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1885,7 +1889,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="19"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
         <v>199</v>
@@ -1898,7 +1902,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="19"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="5" t="s">
         <v>98</v>
       </c>
@@ -1909,7 +1913,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="18" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -1926,7 +1930,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="19"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="5" t="s">
         <v>18</v>
       </c>
@@ -1937,7 +1941,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="18" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="5"/>
@@ -1952,7 +1956,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A17" s="19"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
@@ -1967,7 +1971,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="19"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="5" t="s">
         <v>258</v>
       </c>
@@ -1978,7 +1982,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="19"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
@@ -2002,7 +2006,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="20" t="s">
         <v>107</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -2017,7 +2021,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="22"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="5" t="s">
         <v>258</v>
       </c>
@@ -2041,7 +2045,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="18" t="s">
         <v>25</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -2056,7 +2060,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="19"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="5" t="s">
         <v>38</v>
       </c>
@@ -2069,10 +2073,10 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="23" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -2084,8 +2088,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="19"/>
-      <c r="B27" s="18"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="23"/>
       <c r="C27" s="5" t="s">
         <v>157</v>
       </c>
@@ -2095,7 +2099,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="19"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="5" t="s">
         <v>28</v>
       </c>
@@ -2103,21 +2107,21 @@
         <v>139</v>
       </c>
       <c r="D28" s="5"/>
-      <c r="E28" s="18" t="s">
+      <c r="E28" s="23" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="19"/>
+      <c r="A29" s="18"/>
       <c r="B29" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="E29" s="18"/>
+      <c r="E29" s="23"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="19"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="5" t="s">
         <v>31</v>
       </c>
@@ -2128,7 +2132,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="19"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="5" t="s">
         <v>33</v>
       </c>
@@ -2139,24 +2143,24 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" s="19"/>
+      <c r="A32" s="18"/>
       <c r="B32" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="18" t="s">
+      <c r="E32" s="23" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="19"/>
+      <c r="A33" s="18"/>
       <c r="B33" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="18"/>
+      <c r="E33" s="23"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="15" t="s">
@@ -2174,7 +2178,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="18" t="s">
         <v>126</v>
       </c>
       <c r="B35" s="5"/>
@@ -2187,7 +2191,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="19"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5" t="s">
         <v>217</v>
@@ -2200,7 +2204,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="19"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5" t="s">
         <v>195</v>
@@ -2213,7 +2217,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="19"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5" t="s">
         <v>204</v>
@@ -2224,7 +2228,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="18" t="s">
         <v>40</v>
       </c>
       <c r="B39" s="5" t="s">
@@ -2239,7 +2243,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="19"/>
+      <c r="A40" s="18"/>
       <c r="B40" s="5" t="s">
         <v>42</v>
       </c>
@@ -2250,7 +2254,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="18" t="s">
         <v>127</v>
       </c>
       <c r="B41" s="5"/>
@@ -2265,7 +2269,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="19"/>
+      <c r="A42" s="18"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
         <v>232</v>
@@ -2276,7 +2280,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="19"/>
+      <c r="A43" s="18"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
         <v>142</v>
@@ -2287,7 +2291,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="21" t="s">
+      <c r="A44" s="20" t="s">
         <v>85</v>
       </c>
       <c r="B44" s="5" t="s">
@@ -2302,7 +2306,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="23"/>
+      <c r="A45" s="22"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5" t="s">
         <v>114</v>
@@ -2315,7 +2319,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="22"/>
+      <c r="A46" s="21"/>
       <c r="B46" s="5" t="s">
         <v>258</v>
       </c>
@@ -2326,7 +2330,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="21" t="s">
+      <c r="A47" s="20" t="s">
         <v>44</v>
       </c>
       <c r="B47" s="5"/>
@@ -2339,7 +2343,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="23"/>
+      <c r="A48" s="22"/>
       <c r="B48" s="5" t="s">
         <v>45</v>
       </c>
@@ -2352,7 +2356,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A49" s="23"/>
+      <c r="A49" s="22"/>
       <c r="B49" s="5" t="s">
         <v>47</v>
       </c>
@@ -2363,7 +2367,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A50" s="23"/>
+      <c r="A50" s="22"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
         <v>191</v>
@@ -2376,7 +2380,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A51" s="22"/>
+      <c r="A51" s="21"/>
       <c r="B51" s="5" t="s">
         <v>258</v>
       </c>
@@ -2387,7 +2391,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A52" s="19" t="s">
+      <c r="A52" s="18" t="s">
         <v>69</v>
       </c>
       <c r="B52" s="5"/>
@@ -2402,7 +2406,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A53" s="19"/>
+      <c r="A53" s="18"/>
       <c r="B53" s="5" t="s">
         <v>70</v>
       </c>
@@ -2413,7 +2417,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A54" s="21" t="s">
+      <c r="A54" s="20" t="s">
         <v>128</v>
       </c>
       <c r="B54" s="5"/>
@@ -2426,7 +2430,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A55" s="23"/>
+      <c r="A55" s="22"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
         <v>247</v>
@@ -2437,7 +2441,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" s="22"/>
+      <c r="A56" s="21"/>
       <c r="B56" s="5" t="s">
         <v>258</v>
       </c>
@@ -2470,7 +2474,7 @@
       <c r="E58" s="12"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A59" s="19" t="s">
+      <c r="A59" s="18" t="s">
         <v>49</v>
       </c>
       <c r="B59" s="5" t="s">
@@ -2480,21 +2484,21 @@
         <v>140</v>
       </c>
       <c r="D59" s="5"/>
-      <c r="E59" s="18" t="s">
+      <c r="E59" s="23" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60" s="19"/>
+      <c r="A60" s="18"/>
       <c r="B60" s="5" t="s">
         <v>73</v>
       </c>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
-      <c r="E60" s="18"/>
+      <c r="E60" s="23"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A61" s="19"/>
+      <c r="A61" s="18"/>
       <c r="B61" s="5" t="s">
         <v>74</v>
       </c>
@@ -2509,7 +2513,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A62" s="19"/>
+      <c r="A62" s="18"/>
       <c r="B62" s="5" t="s">
         <v>75</v>
       </c>
@@ -2520,7 +2524,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A63" s="19" t="s">
+      <c r="A63" s="18" t="s">
         <v>78</v>
       </c>
       <c r="B63" s="5" t="s">
@@ -2535,7 +2539,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A64" s="19"/>
+      <c r="A64" s="18"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5" t="s">
         <v>153</v>
@@ -2546,7 +2550,7 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A65" s="19"/>
+      <c r="A65" s="18"/>
       <c r="B65" s="5" t="s">
         <v>79</v>
       </c>
@@ -2559,7 +2563,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A66" s="19"/>
+      <c r="A66" s="18"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
         <v>252</v>
@@ -2572,18 +2576,20 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A67" s="19"/>
+      <c r="A67" s="18"/>
       <c r="B67" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="C67" s="5"/>
+      <c r="C67" s="5" t="s">
+        <v>297</v>
+      </c>
       <c r="D67" s="17"/>
       <c r="E67" s="5" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A68" s="19" t="s">
+      <c r="A68" s="18" t="s">
         <v>50</v>
       </c>
       <c r="B68" s="5" t="s">
@@ -2591,12 +2597,12 @@
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
-      <c r="E68" s="18" t="s">
+      <c r="E68" s="23" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A69" s="19"/>
+      <c r="A69" s="18"/>
       <c r="B69" s="5" t="s">
         <v>81</v>
       </c>
@@ -2606,19 +2612,19 @@
       <c r="D69" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="E69" s="18"/>
+      <c r="E69" s="23"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A70" s="19"/>
+      <c r="A70" s="18"/>
       <c r="B70" s="5" t="s">
         <v>96</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
-      <c r="E70" s="18"/>
+      <c r="E70" s="23"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A71" s="19"/>
+      <c r="A71" s="18"/>
       <c r="B71" s="5" t="s">
         <v>82</v>
       </c>
@@ -2629,7 +2635,7 @@
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A72" s="19"/>
+      <c r="A72" s="18"/>
       <c r="B72" s="5" t="s">
         <v>84</v>
       </c>
@@ -2640,7 +2646,7 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A73" s="19"/>
+      <c r="A73" s="18"/>
       <c r="B73" s="5" t="s">
         <v>91</v>
       </c>
@@ -2651,7 +2657,7 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A74" s="19"/>
+      <c r="A74" s="18"/>
       <c r="B74" s="5"/>
       <c r="C74" s="5" t="s">
         <v>116</v>
@@ -2662,7 +2668,7 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A75" s="19"/>
+      <c r="A75" s="18"/>
       <c r="B75" s="5"/>
       <c r="C75" s="5" t="s">
         <v>117</v>
@@ -2673,7 +2679,7 @@
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A76" s="19"/>
+      <c r="A76" s="18"/>
       <c r="B76" s="5"/>
       <c r="C76" s="5" t="s">
         <v>118</v>
@@ -2684,7 +2690,7 @@
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A77" s="19" t="s">
+      <c r="A77" s="18" t="s">
         <v>52</v>
       </c>
       <c r="B77" s="5" t="s">
@@ -2701,7 +2707,7 @@
       </c>
     </row>
     <row r="78" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A78" s="19"/>
+      <c r="A78" s="18"/>
       <c r="B78" s="5" t="s">
         <v>53</v>
       </c>
@@ -2729,7 +2735,7 @@
       </c>
     </row>
     <row r="80" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A80" s="20" t="s">
+      <c r="A80" s="19" t="s">
         <v>102</v>
       </c>
       <c r="B80" s="5" t="s">
@@ -2746,7 +2752,7 @@
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A81" s="20"/>
+      <c r="A81" s="19"/>
       <c r="B81" s="5"/>
       <c r="C81" s="7" t="s">
         <v>155</v>
@@ -2757,7 +2763,7 @@
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A82" s="20" t="s">
+      <c r="A82" s="19" t="s">
         <v>103</v>
       </c>
       <c r="B82" s="5" t="s">
@@ -2772,7 +2778,7 @@
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A83" s="20"/>
+      <c r="A83" s="19"/>
       <c r="B83" s="5" t="s">
         <v>93</v>
       </c>
@@ -2785,7 +2791,7 @@
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A84" s="20"/>
+      <c r="A84" s="19"/>
       <c r="B84" s="5"/>
       <c r="C84" s="5" t="s">
         <v>221</v>
@@ -2798,7 +2804,7 @@
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A85" s="19" t="s">
+      <c r="A85" s="18" t="s">
         <v>55</v>
       </c>
       <c r="B85" s="5" t="s">
@@ -2810,21 +2816,21 @@
       <c r="D85" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="E85" s="18" t="s">
+      <c r="E85" s="23" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A86" s="19"/>
+      <c r="A86" s="18"/>
       <c r="B86" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
-      <c r="E86" s="18"/>
+      <c r="E86" s="23"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A87" s="19" t="s">
+      <c r="A87" s="18" t="s">
         <v>56</v>
       </c>
       <c r="B87" s="5" t="s">
@@ -2839,7 +2845,7 @@
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A88" s="19"/>
+      <c r="A88" s="18"/>
       <c r="B88" s="5" t="s">
         <v>61</v>
       </c>
@@ -2849,21 +2855,21 @@
       <c r="D88" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="E88" s="18" t="s">
+      <c r="E88" s="23" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A89" s="19"/>
+      <c r="A89" s="18"/>
       <c r="B89" s="5" t="s">
         <v>63</v>
       </c>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
-      <c r="E89" s="18"/>
+      <c r="E89" s="23"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A90" s="19"/>
+      <c r="A90" s="18"/>
       <c r="B90" s="5" t="s">
         <v>64</v>
       </c>
@@ -2876,7 +2882,7 @@
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A91" s="19"/>
+      <c r="A91" s="18"/>
       <c r="B91" s="5" t="s">
         <v>68</v>
       </c>
@@ -2887,7 +2893,7 @@
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A92" s="19" t="s">
+      <c r="A92" s="18" t="s">
         <v>100</v>
       </c>
       <c r="B92" s="5" t="s">
@@ -2900,7 +2906,7 @@
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A93" s="19"/>
+      <c r="A93" s="18"/>
       <c r="B93" s="5" t="s">
         <v>105</v>
       </c>
@@ -2915,27 +2921,6 @@
   </sheetData>
   <autoFilter ref="A2:E93"/>
   <mergeCells count="31">
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A82:A84"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A63:A67"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A47:A51"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A26:A33"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="A35:A38"/>
     <mergeCell ref="E59:E60"/>
     <mergeCell ref="A59:A62"/>
     <mergeCell ref="E88:E89"/>
@@ -2946,6 +2931,27 @@
     <mergeCell ref="E85:E86"/>
     <mergeCell ref="A68:A76"/>
     <mergeCell ref="A80:A81"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A26:A33"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A82:A84"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A63:A67"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A54:A56"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2989,7 +2995,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -3006,7 +3012,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="19"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="5"/>
       <c r="C3" s="7" t="s">
         <v>216</v>

</xml_diff>

<commit_message>
Update on 20251021 part 4
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/脚本汇总统计.xlsx
@@ -13,7 +13,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他脚本!$A$1:$E$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">省份脚本!$A$2:$E$93</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">省份脚本!$A$2:$E$94</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">省份统计!$A$1:$C$33</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="301">
   <si>
     <t>可看频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1212,6 +1212,10 @@
   </si>
   <si>
     <t>CCTV.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>由腾讯云提供的江西省频道和卫视,江西地方频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1291,7 +1295,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1314,50 +1318,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1403,12 +1370,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1419,16 +1380,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1731,7 +1689,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E93"/>
+  <dimension ref="A1:E94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1757,7 +1715,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1774,7 +1732,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -1789,7 +1747,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="19"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="5"/>
       <c r="C4" s="7" t="s">
         <v>183</v>
@@ -1802,7 +1760,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1819,7 +1777,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="19"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1830,7 +1788,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="19"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
@@ -1841,7 +1799,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="19"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
         <v>158</v>
@@ -1852,7 +1810,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="17" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -1867,7 +1825,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="17" t="s">
         <v>122</v>
       </c>
       <c r="B10" s="5"/>
@@ -1882,7 +1840,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1897,7 +1855,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="19"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
         <v>198</v>
@@ -1910,7 +1868,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="19"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="5" t="s">
         <v>98</v>
       </c>
@@ -1921,7 +1879,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="18" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -1938,7 +1896,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="19"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="5" t="s">
         <v>18</v>
       </c>
@@ -1949,7 +1907,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="18" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="5"/>
@@ -1964,7 +1922,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A17" s="19"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
@@ -1979,7 +1937,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="19"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="5" t="s">
         <v>257</v>
       </c>
@@ -1990,7 +1948,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="19"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
@@ -2003,7 +1961,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="17" t="s">
         <v>123</v>
       </c>
       <c r="B20" s="5"/>
@@ -2016,7 +1974,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="18" t="s">
         <v>107</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -2031,7 +1989,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="22"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="5" t="s">
         <v>257</v>
       </c>
@@ -2042,7 +2000,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="17" t="s">
         <v>124</v>
       </c>
       <c r="B23" s="5"/>
@@ -2055,7 +2013,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="18" t="s">
         <v>25</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -2070,7 +2028,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="19"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="5" t="s">
         <v>38</v>
       </c>
@@ -2083,10 +2041,10 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="20" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -2098,8 +2056,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="19"/>
-      <c r="B27" s="18"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="20"/>
       <c r="C27" s="5" t="s">
         <v>156</v>
       </c>
@@ -2109,7 +2067,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="19"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="5" t="s">
         <v>28</v>
       </c>
@@ -2117,21 +2075,21 @@
         <v>138</v>
       </c>
       <c r="D28" s="5"/>
-      <c r="E28" s="18" t="s">
+      <c r="E28" s="20" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="19"/>
+      <c r="A29" s="18"/>
       <c r="B29" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="E29" s="18"/>
+      <c r="E29" s="20"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="19"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="5" t="s">
         <v>31</v>
       </c>
@@ -2142,7 +2100,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="19"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="5" t="s">
         <v>33</v>
       </c>
@@ -2153,27 +2111,27 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" s="19"/>
+      <c r="A32" s="18"/>
       <c r="B32" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="18" t="s">
+      <c r="E32" s="20" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="19"/>
+      <c r="A33" s="18"/>
       <c r="B33" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="18"/>
+      <c r="E33" s="20"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="17" t="s">
         <v>125</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -2188,7 +2146,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="18" t="s">
         <v>126</v>
       </c>
       <c r="B35" s="5"/>
@@ -2201,7 +2159,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="19"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5" t="s">
         <v>216</v>
@@ -2214,7 +2172,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="19"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5" t="s">
         <v>194</v>
@@ -2227,7 +2185,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="19"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5" t="s">
         <v>203</v>
@@ -2238,7 +2196,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="18" t="s">
         <v>40</v>
       </c>
       <c r="B39" s="5" t="s">
@@ -2253,7 +2211,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="19"/>
+      <c r="A40" s="18"/>
       <c r="B40" s="5" t="s">
         <v>42</v>
       </c>
@@ -2264,7 +2222,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="18" t="s">
         <v>127</v>
       </c>
       <c r="B41" s="5"/>
@@ -2279,7 +2237,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="19"/>
+      <c r="A42" s="18"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
         <v>231</v>
@@ -2290,7 +2248,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="19"/>
+      <c r="A43" s="18"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
         <v>141</v>
@@ -2301,650 +2259,657 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="21" t="s">
+      <c r="A44" s="18" t="s">
         <v>85</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>162</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A45" s="18"/>
+      <c r="B45" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="23"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A46" s="18"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D46" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E46" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="22"/>
-      <c r="B46" s="5" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A47" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A48" s="18"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5" t="s">
         <v>225</v>
-      </c>
-      <c r="D47" s="7"/>
-      <c r="E47" s="5" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="23"/>
-      <c r="B48" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>189</v>
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A49" s="18"/>
+      <c r="B49" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D49" s="7"/>
+      <c r="E49" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A49" s="23"/>
-      <c r="B49" s="5" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A50" s="18"/>
+      <c r="B50" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5" t="s">
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A50" s="23"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A51" s="18"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D51" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="E51" s="5" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A51" s="22"/>
-      <c r="B51" s="5" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A52" s="18"/>
+      <c r="B52" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5" t="s">
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A52" s="19" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A53" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="7" t="s">
+      <c r="B53" s="5"/>
+      <c r="C53" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D53" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="E52" s="5" t="s">
+      <c r="E53" s="5" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A53" s="19"/>
-      <c r="B53" s="5" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A54" s="18"/>
+      <c r="B54" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A54" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5" t="s">
-        <v>136</v>
-      </c>
+      <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5" t="s">
-        <v>281</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A55" s="23"/>
+      <c r="A55" s="18" t="s">
+        <v>128</v>
+      </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
-        <v>246</v>
+        <v>136</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5" t="s">
-        <v>247</v>
+        <v>281</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" s="22"/>
-      <c r="B56" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="C56" s="5"/>
+      <c r="A56" s="18"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5" t="s">
+        <v>246</v>
+      </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A57" s="18"/>
+      <c r="B57" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A57" s="15" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A58" s="17" t="s">
         <v>129</v>
-      </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="D57" s="7"/>
-      <c r="E57" s="12"/>
-    </row>
-    <row r="58" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A58" s="15" t="s">
-        <v>130</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="D58" s="7"/>
+      <c r="E58" s="12"/>
+    </row>
+    <row r="59" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A59" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="D58" s="5"/>
-      <c r="E58" s="12"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A59" s="19" t="s">
+      <c r="D59" s="5"/>
+      <c r="E59" s="12"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A60" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B60" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C60" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D59" s="5"/>
-      <c r="E59" s="18" t="s">
+      <c r="D60" s="5"/>
+      <c r="E60" s="20" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60" s="19"/>
-      <c r="B60" s="5" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A61" s="18"/>
+      <c r="B61" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="18"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A61" s="19"/>
-      <c r="B61" s="5" t="s">
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="20"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A62" s="18"/>
+      <c r="B62" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C62" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D62" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="E61" s="5" t="s">
+      <c r="E62" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A62" s="19"/>
-      <c r="B62" s="5" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A63" s="18"/>
+      <c r="B63" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A63" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>151</v>
-      </c>
+      <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5" t="s">
-        <v>284</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A64" s="19"/>
-      <c r="B64" s="5"/>
+      <c r="A64" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="C64" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A65" s="19"/>
-      <c r="B65" s="5" t="s">
-        <v>79</v>
-      </c>
+      <c r="A65" s="18"/>
+      <c r="B65" s="5"/>
       <c r="C65" s="5" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A66" s="18"/>
+      <c r="B66" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A66" s="19"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A67" s="18"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="D67" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="E66" s="5" t="s">
+      <c r="E67" s="5" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A67" s="19"/>
-      <c r="B67" s="5" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A68" s="18"/>
+      <c r="B68" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C68" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="D67" s="17"/>
-      <c r="E67" s="5" t="s">
+      <c r="D68" s="15"/>
+      <c r="E68" s="5" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A68" s="19" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A69" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B69" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="18" t="s">
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="20" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A69" s="19"/>
-      <c r="B69" s="5" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A70" s="18"/>
+      <c r="B70" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C70" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="D70" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="E69" s="18"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A70" s="19"/>
-      <c r="B70" s="5" t="s">
+      <c r="E70" s="20"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A71" s="18"/>
+      <c r="B71" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="18"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A71" s="19"/>
-      <c r="B71" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
-      <c r="E71" s="5" t="s">
-        <v>83</v>
-      </c>
+      <c r="E71" s="20"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A72" s="19"/>
+      <c r="A72" s="18"/>
       <c r="B72" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A73" s="19"/>
+      <c r="A73" s="18"/>
       <c r="B73" s="5" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A74" s="19"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5" t="s">
-        <v>116</v>
-      </c>
+      <c r="A74" s="18"/>
+      <c r="B74" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A75" s="19"/>
+      <c r="A75" s="18"/>
       <c r="B75" s="5"/>
       <c r="C75" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A76" s="19"/>
+      <c r="A76" s="18"/>
       <c r="B76" s="5"/>
       <c r="C76" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D76" s="5"/>
       <c r="E76" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A77" s="18"/>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A77" s="19" t="s">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A78" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B78" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C78" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D78" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="E77" s="5" t="s">
+      <c r="E78" s="5" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A78" s="19"/>
-      <c r="B78" s="5" t="s">
+    <row r="79" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A79" s="18"/>
+      <c r="B79" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C78" s="7" t="s">
+      <c r="C79" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D78" s="7"/>
-      <c r="E78" s="5" t="s">
+      <c r="D79" s="7"/>
+      <c r="E79" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A79" s="15" t="s">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A80" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="B79" s="5"/>
-      <c r="C79" s="5" t="s">
+      <c r="B80" s="5"/>
+      <c r="C80" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="D79" s="5" t="s">
+      <c r="D80" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="E79" s="5" t="s">
+      <c r="E80" s="5" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A80" s="20" t="s">
+    <row r="81" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A81" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B81" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C80" s="7" t="s">
+      <c r="C81" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="D80" s="7" t="s">
+      <c r="D81" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="E80" s="5" t="s">
+      <c r="E81" s="5" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A81" s="20"/>
-      <c r="B81" s="5"/>
-      <c r="C81" s="7" t="s">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A82" s="19"/>
+      <c r="B82" s="5"/>
+      <c r="C82" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="D81" s="7"/>
-      <c r="E81" s="5" t="s">
+      <c r="D82" s="7"/>
+      <c r="E82" s="5" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A82" s="20" t="s">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A83" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B83" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C82" s="5" t="s">
+      <c r="C83" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D82" s="5"/>
-      <c r="E82" s="6" t="s">
+      <c r="D83" s="5"/>
+      <c r="E83" s="6" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A83" s="20"/>
-      <c r="B83" s="5" t="s">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A84" s="19"/>
+      <c r="B84" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C83" s="5" t="s">
+      <c r="C84" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="D83" s="5"/>
-      <c r="E83" s="16" t="s">
+      <c r="D84" s="5"/>
+      <c r="E84" s="16" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A84" s="20"/>
-      <c r="B84" s="5"/>
-      <c r="C84" s="5" t="s">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A85" s="19"/>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="D85" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="E84" s="16" t="s">
+      <c r="E85" s="16" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A85" s="19" t="s">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A86" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B86" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C85" s="5" t="s">
+      <c r="C86" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="D85" s="5" t="s">
+      <c r="D86" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="E85" s="18" t="s">
+      <c r="E86" s="20" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A86" s="19"/>
-      <c r="B86" s="5" t="s">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A87" s="18"/>
+      <c r="B87" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C86" s="5"/>
-      <c r="D86" s="5"/>
-      <c r="E86" s="18"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A87" s="19" t="s">
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="20"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A88" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B88" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C87" s="5" t="s">
+      <c r="C88" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="D87" s="5"/>
-      <c r="E87" s="5" t="s">
+      <c r="D88" s="5"/>
+      <c r="E88" s="5" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A88" s="19"/>
-      <c r="B88" s="5" t="s">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A89" s="18"/>
+      <c r="B89" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C88" s="7" t="s">
+      <c r="C89" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="D88" s="7" t="s">
+      <c r="D89" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="E88" s="18" t="s">
+      <c r="E89" s="20" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A89" s="19"/>
-      <c r="B89" s="5" t="s">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A90" s="18"/>
+      <c r="B90" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
-      <c r="E89" s="18"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A90" s="19"/>
-      <c r="B90" s="5" t="s">
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="20"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A91" s="18"/>
+      <c r="B91" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C90" s="5" t="s">
+      <c r="C91" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="D90" s="5"/>
-      <c r="E90" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A91" s="19"/>
-      <c r="B91" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C91" s="5"/>
       <c r="D91" s="5"/>
       <c r="E91" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A92" s="19" t="s">
-        <v>100</v>
-      </c>
+      <c r="A92" s="18"/>
       <c r="B92" s="5" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
       <c r="E92" s="5" t="s">
-        <v>292</v>
+        <v>67</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A93" s="19"/>
+      <c r="A93" s="18" t="s">
+        <v>100</v>
+      </c>
       <c r="B93" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C93" s="5" t="s">
-        <v>253</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C93" s="5"/>
       <c r="D93" s="5"/>
       <c r="E93" s="5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A94" s="18"/>
+      <c r="B94" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5" t="s">
         <v>106</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E93"/>
+  <autoFilter ref="A2:E94"/>
   <mergeCells count="31">
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A82:A84"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A63:A67"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A47:A51"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="E89:E90"/>
+    <mergeCell ref="A88:A92"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="E69:E71"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="E86:E87"/>
+    <mergeCell ref="A69:A77"/>
+    <mergeCell ref="A81:A82"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A39:A40"/>
@@ -2952,16 +2917,20 @@
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="E32:E33"/>
     <mergeCell ref="A35:A38"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="E88:E89"/>
-    <mergeCell ref="A87:A91"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="E68:E70"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="E85:E86"/>
-    <mergeCell ref="A68:A76"/>
-    <mergeCell ref="A80:A81"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A47:A52"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A55:A57"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3005,7 +2974,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -3022,7 +2991,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="19"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="5"/>
       <c r="C3" s="7" t="s">
         <v>215</v>

</xml_diff>